<commit_message>
Changed "Ts" in file and class name to "Kt".
</commit_message>
<xml_diff>
--- a/meta/api/BlancoApiPostSample.xlsx
+++ b/meta/api/BlancoApiPostSample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\h-matsumoto\Documents\workspace\cacco_oplux\blancoRestGeneratorTs\meta\api\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\h-matsumoto\Documents\workspace\cacco_oplux\blancoRestGeneratorKt\meta\api\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="206">
   <si>
     <t>項目名</t>
     <rPh sb="0" eb="3">
@@ -2022,10 +2022,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>/blanco/main/typescript</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>本番時にファイルを配置する歳のベースディレクトリ。主にTypeScriptのimport文生成時に使用する事を想定しています。</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -2192,6 +2188,14 @@
   </si>
   <si>
     <t>BlancoApiPostSample</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>/blanco/main/kotlin</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>/blanco/main/kotlin</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -3319,6 +3323,126 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3335,126 +3459,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3923,9 +3927,7 @@
   </sheetPr>
   <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:E8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -3967,147 +3969,147 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A5" s="133" t="s">
+      <c r="A5" s="173" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="133"/>
-      <c r="C5" s="133"/>
-      <c r="D5" s="133"/>
-      <c r="E5" s="133"/>
+      <c r="B5" s="173"/>
+      <c r="C5" s="173"/>
+      <c r="D5" s="173"/>
+      <c r="E5" s="173"/>
       <c r="F5" s="55"/>
       <c r="G5" s="55"/>
       <c r="H5" s="96"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A6" s="136" t="s">
+      <c r="A6" s="176" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="137"/>
-      <c r="C6" s="138"/>
-      <c r="D6" s="134" t="s">
-        <v>203</v>
-      </c>
-      <c r="E6" s="134"/>
+      <c r="B6" s="177"/>
+      <c r="C6" s="178"/>
+      <c r="D6" s="174" t="s">
+        <v>202</v>
+      </c>
+      <c r="E6" s="174"/>
       <c r="F6" s="55"/>
       <c r="G6" s="55"/>
       <c r="H6" s="96"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A7" s="133" t="s">
+      <c r="A7" s="173" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="133"/>
-      <c r="C7" s="133"/>
-      <c r="D7" s="134" t="s">
+      <c r="B7" s="173"/>
+      <c r="C7" s="173"/>
+      <c r="D7" s="174" t="s">
         <v>167</v>
       </c>
-      <c r="E7" s="134"/>
+      <c r="E7" s="174"/>
       <c r="F7" s="55"/>
       <c r="G7" s="55"/>
       <c r="H7" s="96"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A8" s="133" t="s">
+      <c r="A8" s="173" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="133"/>
-      <c r="C8" s="133"/>
-      <c r="D8" s="134" t="s">
-        <v>204</v>
-      </c>
-      <c r="E8" s="134"/>
+      <c r="B8" s="173"/>
+      <c r="C8" s="173"/>
+      <c r="D8" s="174" t="s">
+        <v>203</v>
+      </c>
+      <c r="E8" s="174"/>
       <c r="F8" s="96"/>
       <c r="G8" s="96"/>
       <c r="H8" s="96"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A9" s="133" t="s">
+      <c r="A9" s="173" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="133"/>
-      <c r="C9" s="133"/>
-      <c r="D9" s="134" t="s">
+      <c r="B9" s="173"/>
+      <c r="C9" s="173"/>
+      <c r="D9" s="174" t="s">
         <v>100</v>
       </c>
-      <c r="E9" s="134"/>
+      <c r="E9" s="174"/>
       <c r="F9" s="96"/>
       <c r="G9" s="96"/>
       <c r="H9" s="96"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A10" s="133" t="s">
+      <c r="A10" s="173" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="133"/>
-      <c r="C10" s="133"/>
-      <c r="D10" s="134"/>
-      <c r="E10" s="134"/>
+      <c r="B10" s="173"/>
+      <c r="C10" s="173"/>
+      <c r="D10" s="174"/>
+      <c r="E10" s="174"/>
       <c r="F10" s="96"/>
       <c r="G10" s="96"/>
       <c r="H10" s="96"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A11" s="133" t="s">
+      <c r="A11" s="173" t="s">
         <v>99</v>
       </c>
-      <c r="B11" s="133"/>
-      <c r="C11" s="133"/>
-      <c r="D11" s="134" t="s">
+      <c r="B11" s="173"/>
+      <c r="C11" s="173"/>
+      <c r="D11" s="174" t="s">
         <v>163</v>
       </c>
-      <c r="E11" s="134"/>
+      <c r="E11" s="174"/>
       <c r="F11" s="96"/>
       <c r="G11" s="96"/>
       <c r="H11" s="96"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A12" s="142" t="s">
+      <c r="A12" s="138" t="s">
         <v>180</v>
       </c>
-      <c r="B12" s="142"/>
-      <c r="C12" s="142"/>
-      <c r="D12" s="135" t="s">
+      <c r="B12" s="138"/>
+      <c r="C12" s="138"/>
+      <c r="D12" s="175" t="s">
+        <v>204</v>
+      </c>
+      <c r="E12" s="175"/>
+      <c r="F12" s="96" t="s">
         <v>181</v>
       </c>
-      <c r="E12" s="135"/>
-      <c r="F12" s="96" t="s">
+      <c r="G12" s="54"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A13" s="138" t="s">
         <v>182</v>
       </c>
-      <c r="G12" s="54"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A13" s="142" t="s">
+      <c r="B13" s="138"/>
+      <c r="C13" s="138"/>
+      <c r="D13" s="175" t="s">
         <v>183</v>
       </c>
-      <c r="B13" s="142"/>
-      <c r="C13" s="142"/>
-      <c r="D13" s="135" t="s">
-        <v>184</v>
-      </c>
-      <c r="E13" s="135"/>
+      <c r="E13" s="175"/>
       <c r="F13" s="54"/>
       <c r="G13" s="54"/>
       <c r="H13" s="96"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A14" s="139" t="s">
+      <c r="A14" s="170" t="s">
         <v>143</v>
       </c>
-      <c r="B14" s="140"/>
-      <c r="C14" s="141"/>
+      <c r="B14" s="171"/>
+      <c r="C14" s="172"/>
       <c r="D14" s="115"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A15" s="165" t="s">
-        <v>185</v>
-      </c>
-      <c r="B15" s="166"/>
-      <c r="C15" s="167"/>
+      <c r="A15" s="139" t="s">
+        <v>184</v>
+      </c>
+      <c r="B15" s="140"/>
+      <c r="C15" s="141"/>
       <c r="D15" s="101" t="s">
         <v>141</v>
       </c>
       <c r="E15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F15"/>
       <c r="G15"/>
@@ -4122,19 +4124,19 @@
       <c r="B16" s="6"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A17" s="176" t="s">
-        <v>194</v>
-      </c>
-      <c r="B17" s="177"/>
-      <c r="C17" s="177"/>
-      <c r="D17" s="177"/>
-      <c r="E17" s="177"/>
-      <c r="F17" s="177"/>
-      <c r="G17" s="178"/>
+      <c r="A17" s="152" t="s">
+        <v>193</v>
+      </c>
+      <c r="B17" s="153"/>
+      <c r="C17" s="153"/>
+      <c r="D17" s="153"/>
+      <c r="E17" s="153"/>
+      <c r="F17" s="153"/>
+      <c r="G17" s="154"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A18" s="102" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B18" s="111"/>
       <c r="C18" s="103"/>
@@ -4161,7 +4163,7 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A20" s="99" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B20" s="114"/>
       <c r="C20" s="100"/>
@@ -4174,28 +4176,28 @@
       <c r="C21"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A22" s="175" t="s">
-        <v>195</v>
-      </c>
-      <c r="B22" s="175"/>
-      <c r="C22" s="175"/>
-      <c r="D22" s="175"/>
-      <c r="E22" s="175"/>
-      <c r="F22" s="175"/>
-      <c r="G22" s="175"/>
+      <c r="A22" s="151" t="s">
+        <v>194</v>
+      </c>
+      <c r="B22" s="151"/>
+      <c r="C22" s="151"/>
+      <c r="D22" s="151"/>
+      <c r="E22" s="151"/>
+      <c r="F22" s="151"/>
+      <c r="G22" s="151"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A23" s="116" t="s">
         <v>69</v>
       </c>
-      <c r="B23" s="169" t="s">
-        <v>189</v>
-      </c>
-      <c r="C23" s="170"/>
-      <c r="D23" s="170"/>
-      <c r="E23" s="170"/>
-      <c r="F23" s="170"/>
-      <c r="G23" s="171"/>
+      <c r="B23" s="145" t="s">
+        <v>188</v>
+      </c>
+      <c r="C23" s="146"/>
+      <c r="D23" s="146"/>
+      <c r="E23" s="146"/>
+      <c r="F23" s="146"/>
+      <c r="G23" s="147"/>
       <c r="H23" s="106"/>
       <c r="I23" s="106"/>
       <c r="J23" s="106"/>
@@ -4206,12 +4208,12 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A24" s="117"/>
-      <c r="B24" s="153"/>
-      <c r="C24" s="153"/>
-      <c r="D24" s="153"/>
-      <c r="E24" s="153"/>
-      <c r="F24" s="153"/>
-      <c r="G24" s="153"/>
+      <c r="B24" s="157"/>
+      <c r="C24" s="157"/>
+      <c r="D24" s="157"/>
+      <c r="E24" s="157"/>
+      <c r="F24" s="157"/>
+      <c r="G24" s="157"/>
       <c r="H24" s="113"/>
       <c r="I24" s="113"/>
       <c r="J24" s="113"/>
@@ -4222,12 +4224,12 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A25" s="118"/>
-      <c r="B25" s="155"/>
-      <c r="C25" s="155"/>
-      <c r="D25" s="155"/>
-      <c r="E25" s="155"/>
-      <c r="F25" s="155"/>
-      <c r="G25" s="155"/>
+      <c r="B25" s="158"/>
+      <c r="C25" s="158"/>
+      <c r="D25" s="158"/>
+      <c r="E25" s="158"/>
+      <c r="F25" s="158"/>
+      <c r="G25" s="158"/>
       <c r="H25" s="113"/>
       <c r="I25" s="113"/>
       <c r="J25" s="113"/>
@@ -4238,12 +4240,12 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A26" s="119"/>
-      <c r="B26" s="157"/>
-      <c r="C26" s="157"/>
-      <c r="D26" s="157"/>
-      <c r="E26" s="157"/>
-      <c r="F26" s="157"/>
-      <c r="G26" s="157"/>
+      <c r="B26" s="159"/>
+      <c r="C26" s="159"/>
+      <c r="D26" s="159"/>
+      <c r="E26" s="159"/>
+      <c r="F26" s="159"/>
+      <c r="G26" s="159"/>
       <c r="H26" s="113"/>
       <c r="I26" s="113"/>
       <c r="J26" s="113"/>
@@ -4256,28 +4258,28 @@
       <c r="C27"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A28" s="172" t="s">
-        <v>196</v>
-      </c>
-      <c r="B28" s="173"/>
-      <c r="C28" s="173"/>
-      <c r="D28" s="173"/>
-      <c r="E28" s="173"/>
-      <c r="F28" s="173"/>
-      <c r="G28" s="174"/>
+      <c r="A28" s="148" t="s">
+        <v>195</v>
+      </c>
+      <c r="B28" s="149"/>
+      <c r="C28" s="149"/>
+      <c r="D28" s="149"/>
+      <c r="E28" s="149"/>
+      <c r="F28" s="149"/>
+      <c r="G28" s="150"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A29" s="116" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="149" t="s">
-        <v>190</v>
-      </c>
-      <c r="C29" s="149"/>
-      <c r="D29" s="149"/>
-      <c r="E29" s="149"/>
-      <c r="F29" s="149"/>
-      <c r="G29" s="149"/>
+      <c r="B29" s="163" t="s">
+        <v>189</v>
+      </c>
+      <c r="C29" s="163"/>
+      <c r="D29" s="163"/>
+      <c r="E29" s="163"/>
+      <c r="F29" s="163"/>
+      <c r="G29" s="163"/>
       <c r="H29" s="106"/>
       <c r="I29" s="106"/>
       <c r="J29" s="106"/>
@@ -4290,14 +4292,14 @@
       <c r="A30" s="117">
         <v>1</v>
       </c>
-      <c r="B30" s="150" t="s">
-        <v>191</v>
-      </c>
-      <c r="C30" s="150"/>
-      <c r="D30" s="150"/>
-      <c r="E30" s="150"/>
-      <c r="F30" s="150"/>
-      <c r="G30" s="150"/>
+      <c r="B30" s="164" t="s">
+        <v>190</v>
+      </c>
+      <c r="C30" s="164"/>
+      <c r="D30" s="164"/>
+      <c r="E30" s="164"/>
+      <c r="F30" s="164"/>
+      <c r="G30" s="164"/>
       <c r="H30" s="113"/>
       <c r="I30" s="113"/>
       <c r="J30" s="113"/>
@@ -4308,12 +4310,12 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A31" s="118"/>
-      <c r="B31" s="151"/>
-      <c r="C31" s="151"/>
-      <c r="D31" s="151"/>
-      <c r="E31" s="151"/>
-      <c r="F31" s="151"/>
-      <c r="G31" s="151"/>
+      <c r="B31" s="165"/>
+      <c r="C31" s="165"/>
+      <c r="D31" s="165"/>
+      <c r="E31" s="165"/>
+      <c r="F31" s="165"/>
+      <c r="G31" s="165"/>
       <c r="H31" s="113"/>
       <c r="I31" s="113"/>
       <c r="J31" s="113"/>
@@ -4324,12 +4326,12 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A32" s="119"/>
-      <c r="B32" s="152"/>
-      <c r="C32" s="152"/>
-      <c r="D32" s="152"/>
-      <c r="E32" s="152"/>
-      <c r="F32" s="152"/>
-      <c r="G32" s="152"/>
+      <c r="B32" s="166"/>
+      <c r="C32" s="166"/>
+      <c r="D32" s="166"/>
+      <c r="E32" s="166"/>
+      <c r="F32" s="166"/>
+      <c r="G32" s="166"/>
       <c r="H32" s="113"/>
       <c r="I32" s="113"/>
       <c r="J32" s="113"/>
@@ -4354,28 +4356,28 @@
       <c r="M33"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A34" s="172" t="s">
-        <v>197</v>
-      </c>
-      <c r="B34" s="173"/>
-      <c r="C34" s="173"/>
-      <c r="D34" s="173"/>
-      <c r="E34" s="173"/>
-      <c r="F34" s="173"/>
-      <c r="G34" s="174"/>
+      <c r="A34" s="148" t="s">
+        <v>196</v>
+      </c>
+      <c r="B34" s="149"/>
+      <c r="C34" s="149"/>
+      <c r="D34" s="149"/>
+      <c r="E34" s="149"/>
+      <c r="F34" s="149"/>
+      <c r="G34" s="150"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A35" s="116" t="s">
         <v>69</v>
       </c>
-      <c r="B35" s="149" t="s">
-        <v>192</v>
-      </c>
-      <c r="C35" s="149"/>
-      <c r="D35" s="149"/>
-      <c r="E35" s="149"/>
-      <c r="F35" s="149"/>
-      <c r="G35" s="149"/>
+      <c r="B35" s="163" t="s">
+        <v>191</v>
+      </c>
+      <c r="C35" s="163"/>
+      <c r="D35" s="163"/>
+      <c r="E35" s="163"/>
+      <c r="F35" s="163"/>
+      <c r="G35" s="163"/>
       <c r="H35" s="106"/>
       <c r="I35" s="106"/>
       <c r="J35" s="106"/>
@@ -4386,12 +4388,12 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A36" s="117"/>
-      <c r="B36" s="153"/>
-      <c r="C36" s="153"/>
-      <c r="D36" s="153"/>
-      <c r="E36" s="153"/>
-      <c r="F36" s="153"/>
-      <c r="G36" s="154"/>
+      <c r="B36" s="157"/>
+      <c r="C36" s="157"/>
+      <c r="D36" s="157"/>
+      <c r="E36" s="157"/>
+      <c r="F36" s="157"/>
+      <c r="G36" s="167"/>
       <c r="H36" s="113"/>
       <c r="I36" s="113"/>
       <c r="J36" s="113"/>
@@ -4402,12 +4404,12 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A37" s="118"/>
-      <c r="B37" s="155"/>
-      <c r="C37" s="155"/>
-      <c r="D37" s="155"/>
-      <c r="E37" s="155"/>
-      <c r="F37" s="155"/>
-      <c r="G37" s="156"/>
+      <c r="B37" s="158"/>
+      <c r="C37" s="158"/>
+      <c r="D37" s="158"/>
+      <c r="E37" s="158"/>
+      <c r="F37" s="158"/>
+      <c r="G37" s="168"/>
       <c r="H37" s="113"/>
       <c r="I37" s="113"/>
       <c r="J37" s="113"/>
@@ -4418,12 +4420,12 @@
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A38" s="119"/>
-      <c r="B38" s="157"/>
-      <c r="C38" s="157"/>
-      <c r="D38" s="157"/>
-      <c r="E38" s="157"/>
-      <c r="F38" s="157"/>
-      <c r="G38" s="158"/>
+      <c r="B38" s="159"/>
+      <c r="C38" s="159"/>
+      <c r="D38" s="159"/>
+      <c r="E38" s="159"/>
+      <c r="F38" s="159"/>
+      <c r="G38" s="169"/>
       <c r="H38" s="113"/>
       <c r="I38" s="113"/>
       <c r="J38" s="113"/>
@@ -4458,250 +4460,262 @@
       <c r="F40" s="5"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A41" s="162" t="s">
+      <c r="A41" s="135" t="s">
         <v>65</v>
       </c>
-      <c r="B41" s="168"/>
-      <c r="C41" s="162" t="s">
+      <c r="B41" s="142"/>
+      <c r="C41" s="135" t="s">
         <v>66</v>
       </c>
-      <c r="D41" s="163"/>
-      <c r="E41" s="164"/>
+      <c r="D41" s="136"/>
+      <c r="E41" s="137"/>
       <c r="F41" s="29" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A42" s="159"/>
-      <c r="B42" s="161"/>
-      <c r="C42" s="159"/>
+      <c r="A42" s="143"/>
+      <c r="B42" s="144"/>
+      <c r="C42" s="143"/>
       <c r="D42" s="160"/>
-      <c r="E42" s="161"/>
+      <c r="E42" s="144"/>
       <c r="F42" s="49"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A43" s="143"/>
-      <c r="B43" s="145"/>
-      <c r="C43" s="143"/>
-      <c r="D43" s="144"/>
-      <c r="E43" s="145"/>
+      <c r="A43" s="133"/>
+      <c r="B43" s="134"/>
+      <c r="C43" s="133"/>
+      <c r="D43" s="161"/>
+      <c r="E43" s="134"/>
       <c r="F43" s="49"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A44" s="143"/>
-      <c r="B44" s="145"/>
-      <c r="C44" s="143"/>
-      <c r="D44" s="144"/>
-      <c r="E44" s="145"/>
+      <c r="A44" s="133"/>
+      <c r="B44" s="134"/>
+      <c r="C44" s="133"/>
+      <c r="D44" s="161"/>
+      <c r="E44" s="134"/>
       <c r="F44" s="49"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A45" s="143"/>
-      <c r="B45" s="145"/>
-      <c r="C45" s="143"/>
-      <c r="D45" s="144"/>
-      <c r="E45" s="145"/>
+      <c r="A45" s="133"/>
+      <c r="B45" s="134"/>
+      <c r="C45" s="133"/>
+      <c r="D45" s="161"/>
+      <c r="E45" s="134"/>
       <c r="F45" s="49"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A46" s="143"/>
-      <c r="B46" s="145"/>
-      <c r="C46" s="143"/>
-      <c r="D46" s="144"/>
-      <c r="E46" s="145"/>
+      <c r="A46" s="133"/>
+      <c r="B46" s="134"/>
+      <c r="C46" s="133"/>
+      <c r="D46" s="161"/>
+      <c r="E46" s="134"/>
       <c r="F46" s="49"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A47" s="143"/>
-      <c r="B47" s="145"/>
-      <c r="C47" s="143"/>
-      <c r="D47" s="144"/>
-      <c r="E47" s="145"/>
+      <c r="A47" s="133"/>
+      <c r="B47" s="134"/>
+      <c r="C47" s="133"/>
+      <c r="D47" s="161"/>
+      <c r="E47" s="134"/>
       <c r="F47" s="49"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A48" s="143"/>
-      <c r="B48" s="145"/>
-      <c r="C48" s="143"/>
-      <c r="D48" s="144"/>
-      <c r="E48" s="145"/>
+      <c r="A48" s="133"/>
+      <c r="B48" s="134"/>
+      <c r="C48" s="133"/>
+      <c r="D48" s="161"/>
+      <c r="E48" s="134"/>
       <c r="F48" s="49"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A49" s="143"/>
-      <c r="B49" s="145"/>
-      <c r="C49" s="143"/>
-      <c r="D49" s="144"/>
-      <c r="E49" s="145"/>
+      <c r="A49" s="133"/>
+      <c r="B49" s="134"/>
+      <c r="C49" s="133"/>
+      <c r="D49" s="161"/>
+      <c r="E49" s="134"/>
       <c r="F49" s="49"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A50" s="143"/>
-      <c r="B50" s="145"/>
-      <c r="C50" s="143"/>
-      <c r="D50" s="144"/>
-      <c r="E50" s="145"/>
+      <c r="A50" s="133"/>
+      <c r="B50" s="134"/>
+      <c r="C50" s="133"/>
+      <c r="D50" s="161"/>
+      <c r="E50" s="134"/>
       <c r="F50" s="49"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A51" s="143"/>
-      <c r="B51" s="145"/>
-      <c r="C51" s="143"/>
-      <c r="D51" s="144"/>
-      <c r="E51" s="145"/>
+      <c r="A51" s="133"/>
+      <c r="B51" s="134"/>
+      <c r="C51" s="133"/>
+      <c r="D51" s="161"/>
+      <c r="E51" s="134"/>
       <c r="F51" s="49"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A52" s="143"/>
-      <c r="B52" s="145"/>
-      <c r="C52" s="143"/>
-      <c r="D52" s="144"/>
-      <c r="E52" s="145"/>
+      <c r="A52" s="133"/>
+      <c r="B52" s="134"/>
+      <c r="C52" s="133"/>
+      <c r="D52" s="161"/>
+      <c r="E52" s="134"/>
       <c r="F52" s="49"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A53" s="143"/>
-      <c r="B53" s="145"/>
-      <c r="C53" s="143"/>
-      <c r="D53" s="144"/>
-      <c r="E53" s="145"/>
+      <c r="A53" s="133"/>
+      <c r="B53" s="134"/>
+      <c r="C53" s="133"/>
+      <c r="D53" s="161"/>
+      <c r="E53" s="134"/>
       <c r="F53" s="49"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A54" s="143"/>
-      <c r="B54" s="145"/>
-      <c r="C54" s="143"/>
-      <c r="D54" s="144"/>
-      <c r="E54" s="145"/>
+      <c r="A54" s="133"/>
+      <c r="B54" s="134"/>
+      <c r="C54" s="133"/>
+      <c r="D54" s="161"/>
+      <c r="E54" s="134"/>
       <c r="F54" s="49"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A55" s="143"/>
-      <c r="B55" s="145"/>
-      <c r="C55" s="143"/>
-      <c r="D55" s="144"/>
-      <c r="E55" s="145"/>
+      <c r="A55" s="133"/>
+      <c r="B55" s="134"/>
+      <c r="C55" s="133"/>
+      <c r="D55" s="161"/>
+      <c r="E55" s="134"/>
       <c r="F55" s="49"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A56" s="143"/>
-      <c r="B56" s="145"/>
-      <c r="C56" s="143"/>
-      <c r="D56" s="144"/>
-      <c r="E56" s="145"/>
+      <c r="A56" s="133"/>
+      <c r="B56" s="134"/>
+      <c r="C56" s="133"/>
+      <c r="D56" s="161"/>
+      <c r="E56" s="134"/>
       <c r="F56" s="49"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A57" s="143"/>
-      <c r="B57" s="145"/>
-      <c r="C57" s="143"/>
-      <c r="D57" s="144"/>
-      <c r="E57" s="145"/>
+      <c r="A57" s="133"/>
+      <c r="B57" s="134"/>
+      <c r="C57" s="133"/>
+      <c r="D57" s="161"/>
+      <c r="E57" s="134"/>
       <c r="F57" s="49"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A58" s="143"/>
-      <c r="B58" s="145"/>
-      <c r="C58" s="143"/>
-      <c r="D58" s="144"/>
-      <c r="E58" s="145"/>
+      <c r="A58" s="133"/>
+      <c r="B58" s="134"/>
+      <c r="C58" s="133"/>
+      <c r="D58" s="161"/>
+      <c r="E58" s="134"/>
       <c r="F58" s="49"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A59" s="143"/>
-      <c r="B59" s="145"/>
-      <c r="C59" s="143"/>
-      <c r="D59" s="144"/>
-      <c r="E59" s="145"/>
+      <c r="A59" s="133"/>
+      <c r="B59" s="134"/>
+      <c r="C59" s="133"/>
+      <c r="D59" s="161"/>
+      <c r="E59" s="134"/>
       <c r="F59" s="49"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A60" s="143"/>
-      <c r="B60" s="145"/>
-      <c r="C60" s="143"/>
-      <c r="D60" s="144"/>
-      <c r="E60" s="145"/>
+      <c r="A60" s="133"/>
+      <c r="B60" s="134"/>
+      <c r="C60" s="133"/>
+      <c r="D60" s="161"/>
+      <c r="E60" s="134"/>
       <c r="F60" s="49"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A61" s="143"/>
-      <c r="B61" s="145"/>
-      <c r="C61" s="143"/>
-      <c r="D61" s="144"/>
-      <c r="E61" s="145"/>
+      <c r="A61" s="133"/>
+      <c r="B61" s="134"/>
+      <c r="C61" s="133"/>
+      <c r="D61" s="161"/>
+      <c r="E61" s="134"/>
       <c r="F61" s="49"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A62" s="143"/>
-      <c r="B62" s="145"/>
-      <c r="C62" s="143"/>
-      <c r="D62" s="144"/>
-      <c r="E62" s="145"/>
+      <c r="A62" s="133"/>
+      <c r="B62" s="134"/>
+      <c r="C62" s="133"/>
+      <c r="D62" s="161"/>
+      <c r="E62" s="134"/>
       <c r="F62" s="49"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A63" s="143"/>
-      <c r="B63" s="145"/>
-      <c r="C63" s="143"/>
-      <c r="D63" s="144"/>
-      <c r="E63" s="145"/>
+      <c r="A63" s="133"/>
+      <c r="B63" s="134"/>
+      <c r="C63" s="133"/>
+      <c r="D63" s="161"/>
+      <c r="E63" s="134"/>
       <c r="F63" s="49"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A64" s="143"/>
-      <c r="B64" s="145"/>
-      <c r="C64" s="143"/>
-      <c r="D64" s="144"/>
-      <c r="E64" s="145"/>
+      <c r="A64" s="133"/>
+      <c r="B64" s="134"/>
+      <c r="C64" s="133"/>
+      <c r="D64" s="161"/>
+      <c r="E64" s="134"/>
       <c r="F64" s="49"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A65" s="143"/>
-      <c r="B65" s="145"/>
-      <c r="C65" s="143"/>
-      <c r="D65" s="144"/>
-      <c r="E65" s="145"/>
+      <c r="A65" s="133"/>
+      <c r="B65" s="134"/>
+      <c r="C65" s="133"/>
+      <c r="D65" s="161"/>
+      <c r="E65" s="134"/>
       <c r="F65" s="49"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A66" s="146"/>
-      <c r="B66" s="148"/>
-      <c r="C66" s="146"/>
-      <c r="D66" s="147"/>
-      <c r="E66" s="148"/>
+      <c r="A66" s="155"/>
+      <c r="B66" s="156"/>
+      <c r="C66" s="155"/>
+      <c r="D66" s="162"/>
+      <c r="E66" s="156"/>
       <c r="F66" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="87">
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="A28:G28"/>
-    <mergeCell ref="A34:G34"/>
-    <mergeCell ref="A22:G22"/>
-    <mergeCell ref="A17:G17"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="C54:E54"/>
     <mergeCell ref="A63:B63"/>
     <mergeCell ref="A64:B64"/>
     <mergeCell ref="A65:B65"/>
@@ -4718,48 +4732,36 @@
     <mergeCell ref="C48:E48"/>
     <mergeCell ref="C49:E49"/>
     <mergeCell ref="A58:B58"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="C51:E51"/>
-    <mergeCell ref="C52:E52"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B36:G36"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="A28:G28"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="A17:G17"/>
     <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="1">
@@ -4794,9 +4796,7 @@
   </sheetPr>
   <dimension ref="A1:T64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I41" sqref="I41:I47"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -4989,24 +4989,24 @@
         <v>180</v>
       </c>
       <c r="B15" s="123"/>
-      <c r="C15" s="135" t="s">
+      <c r="C15" s="175" t="s">
+        <v>204</v>
+      </c>
+      <c r="D15" s="175"/>
+      <c r="E15" s="96" t="s">
         <v>181</v>
-      </c>
-      <c r="D15" s="135"/>
-      <c r="E15" s="96" t="s">
-        <v>182</v>
       </c>
       <c r="G15" s="54"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A16" s="123" t="s">
+        <v>182</v>
+      </c>
+      <c r="B16" s="123"/>
+      <c r="C16" s="175" t="s">
         <v>183</v>
       </c>
-      <c r="B16" s="123"/>
-      <c r="C16" s="135" t="s">
-        <v>184</v>
-      </c>
-      <c r="D16" s="135"/>
+      <c r="D16" s="175"/>
       <c r="E16" s="55"/>
       <c r="F16" s="54"/>
       <c r="G16" s="54"/>
@@ -5015,14 +5015,14 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A17" s="124" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B17" s="125"/>
       <c r="C17" s="101" t="s">
         <v>141</v>
       </c>
       <c r="D17" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F17"/>
       <c r="G17"/>
@@ -5038,28 +5038,28 @@
       <c r="C18" s="28"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A19" s="175" t="s">
-        <v>198</v>
-      </c>
-      <c r="B19" s="175"/>
-      <c r="C19" s="175"/>
-      <c r="D19" s="175"/>
-      <c r="E19" s="175"/>
-      <c r="F19" s="175"/>
-      <c r="G19" s="175"/>
+      <c r="A19" s="151" t="s">
+        <v>197</v>
+      </c>
+      <c r="B19" s="151"/>
+      <c r="C19" s="151"/>
+      <c r="D19" s="151"/>
+      <c r="E19" s="151"/>
+      <c r="F19" s="151"/>
+      <c r="G19" s="151"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A20" s="116" t="s">
         <v>69</v>
       </c>
-      <c r="B20" s="169" t="s">
-        <v>189</v>
-      </c>
-      <c r="C20" s="170"/>
-      <c r="D20" s="170"/>
-      <c r="E20" s="170"/>
-      <c r="F20" s="170"/>
-      <c r="G20" s="171"/>
+      <c r="B20" s="145" t="s">
+        <v>188</v>
+      </c>
+      <c r="C20" s="146"/>
+      <c r="D20" s="146"/>
+      <c r="E20" s="146"/>
+      <c r="F20" s="146"/>
+      <c r="G20" s="147"/>
       <c r="H20" s="106"/>
       <c r="I20" s="106"/>
       <c r="J20" s="106"/>
@@ -5071,12 +5071,12 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A21" s="117"/>
-      <c r="B21" s="153"/>
-      <c r="C21" s="153"/>
-      <c r="D21" s="153"/>
-      <c r="E21" s="153"/>
-      <c r="F21" s="153"/>
-      <c r="G21" s="153"/>
+      <c r="B21" s="157"/>
+      <c r="C21" s="157"/>
+      <c r="D21" s="157"/>
+      <c r="E21" s="157"/>
+      <c r="F21" s="157"/>
+      <c r="G21" s="157"/>
       <c r="H21" s="113"/>
       <c r="I21" s="113"/>
       <c r="J21" s="113"/>
@@ -5088,12 +5088,12 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A22" s="118"/>
-      <c r="B22" s="155"/>
-      <c r="C22" s="155"/>
-      <c r="D22" s="155"/>
-      <c r="E22" s="155"/>
-      <c r="F22" s="155"/>
-      <c r="G22" s="155"/>
+      <c r="B22" s="158"/>
+      <c r="C22" s="158"/>
+      <c r="D22" s="158"/>
+      <c r="E22" s="158"/>
+      <c r="F22" s="158"/>
+      <c r="G22" s="158"/>
       <c r="H22" s="113"/>
       <c r="I22" s="113"/>
       <c r="J22" s="113"/>
@@ -5105,12 +5105,12 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A23" s="119"/>
-      <c r="B23" s="157"/>
-      <c r="C23" s="157"/>
-      <c r="D23" s="157"/>
-      <c r="E23" s="157"/>
-      <c r="F23" s="157"/>
-      <c r="G23" s="157"/>
+      <c r="B23" s="159"/>
+      <c r="C23" s="159"/>
+      <c r="D23" s="159"/>
+      <c r="E23" s="159"/>
+      <c r="F23" s="159"/>
+      <c r="G23" s="159"/>
       <c r="H23" s="113"/>
       <c r="I23" s="113"/>
       <c r="J23" s="113"/>
@@ -5124,28 +5124,28 @@
       <c r="C24"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A25" s="172" t="s">
-        <v>199</v>
-      </c>
-      <c r="B25" s="173"/>
-      <c r="C25" s="173"/>
-      <c r="D25" s="173"/>
-      <c r="E25" s="173"/>
-      <c r="F25" s="173"/>
-      <c r="G25" s="174"/>
+      <c r="A25" s="148" t="s">
+        <v>198</v>
+      </c>
+      <c r="B25" s="149"/>
+      <c r="C25" s="149"/>
+      <c r="D25" s="149"/>
+      <c r="E25" s="149"/>
+      <c r="F25" s="149"/>
+      <c r="G25" s="150"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A26" s="116" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="149" t="s">
-        <v>190</v>
-      </c>
-      <c r="C26" s="149"/>
-      <c r="D26" s="149"/>
-      <c r="E26" s="149"/>
-      <c r="F26" s="149"/>
-      <c r="G26" s="149"/>
+      <c r="B26" s="163" t="s">
+        <v>189</v>
+      </c>
+      <c r="C26" s="163"/>
+      <c r="D26" s="163"/>
+      <c r="E26" s="163"/>
+      <c r="F26" s="163"/>
+      <c r="G26" s="163"/>
       <c r="H26" s="106"/>
       <c r="I26" s="106"/>
       <c r="J26" s="106"/>
@@ -5159,14 +5159,14 @@
       <c r="A27" s="117">
         <v>1</v>
       </c>
-      <c r="B27" s="150" t="s">
-        <v>191</v>
-      </c>
-      <c r="C27" s="150"/>
-      <c r="D27" s="150"/>
-      <c r="E27" s="150"/>
-      <c r="F27" s="150"/>
-      <c r="G27" s="150"/>
+      <c r="B27" s="164" t="s">
+        <v>190</v>
+      </c>
+      <c r="C27" s="164"/>
+      <c r="D27" s="164"/>
+      <c r="E27" s="164"/>
+      <c r="F27" s="164"/>
+      <c r="G27" s="164"/>
       <c r="H27" s="113"/>
       <c r="I27" s="113"/>
       <c r="J27" s="113"/>
@@ -5178,12 +5178,12 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A28" s="118"/>
-      <c r="B28" s="151"/>
-      <c r="C28" s="151"/>
-      <c r="D28" s="151"/>
-      <c r="E28" s="151"/>
-      <c r="F28" s="151"/>
-      <c r="G28" s="151"/>
+      <c r="B28" s="165"/>
+      <c r="C28" s="165"/>
+      <c r="D28" s="165"/>
+      <c r="E28" s="165"/>
+      <c r="F28" s="165"/>
+      <c r="G28" s="165"/>
       <c r="H28" s="113"/>
       <c r="I28" s="113"/>
       <c r="J28" s="113"/>
@@ -5195,12 +5195,12 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A29" s="119"/>
-      <c r="B29" s="152"/>
-      <c r="C29" s="152"/>
-      <c r="D29" s="152"/>
-      <c r="E29" s="152"/>
-      <c r="F29" s="152"/>
-      <c r="G29" s="152"/>
+      <c r="B29" s="166"/>
+      <c r="C29" s="166"/>
+      <c r="D29" s="166"/>
+      <c r="E29" s="166"/>
+      <c r="F29" s="166"/>
+      <c r="G29" s="166"/>
       <c r="H29" s="113"/>
       <c r="I29" s="113"/>
       <c r="J29" s="113"/>
@@ -5227,28 +5227,28 @@
       <c r="N30"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A31" s="172" t="s">
-        <v>200</v>
-      </c>
-      <c r="B31" s="173"/>
-      <c r="C31" s="173"/>
-      <c r="D31" s="173"/>
-      <c r="E31" s="173"/>
-      <c r="F31" s="173"/>
-      <c r="G31" s="174"/>
+      <c r="A31" s="148" t="s">
+        <v>199</v>
+      </c>
+      <c r="B31" s="149"/>
+      <c r="C31" s="149"/>
+      <c r="D31" s="149"/>
+      <c r="E31" s="149"/>
+      <c r="F31" s="149"/>
+      <c r="G31" s="150"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A32" s="116" t="s">
         <v>69</v>
       </c>
-      <c r="B32" s="149" t="s">
-        <v>192</v>
-      </c>
-      <c r="C32" s="149"/>
-      <c r="D32" s="149"/>
-      <c r="E32" s="149"/>
-      <c r="F32" s="149"/>
-      <c r="G32" s="149"/>
+      <c r="B32" s="163" t="s">
+        <v>191</v>
+      </c>
+      <c r="C32" s="163"/>
+      <c r="D32" s="163"/>
+      <c r="E32" s="163"/>
+      <c r="F32" s="163"/>
+      <c r="G32" s="163"/>
       <c r="H32" s="106"/>
       <c r="I32" s="106"/>
       <c r="J32" s="106"/>
@@ -5260,12 +5260,12 @@
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A33" s="117"/>
-      <c r="B33" s="153"/>
-      <c r="C33" s="153"/>
-      <c r="D33" s="153"/>
-      <c r="E33" s="153"/>
-      <c r="F33" s="153"/>
-      <c r="G33" s="154"/>
+      <c r="B33" s="157"/>
+      <c r="C33" s="157"/>
+      <c r="D33" s="157"/>
+      <c r="E33" s="157"/>
+      <c r="F33" s="157"/>
+      <c r="G33" s="167"/>
       <c r="H33" s="113"/>
       <c r="I33" s="113"/>
       <c r="J33" s="113"/>
@@ -5277,12 +5277,12 @@
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A34" s="118"/>
-      <c r="B34" s="155"/>
-      <c r="C34" s="155"/>
-      <c r="D34" s="155"/>
-      <c r="E34" s="155"/>
-      <c r="F34" s="155"/>
-      <c r="G34" s="156"/>
+      <c r="B34" s="158"/>
+      <c r="C34" s="158"/>
+      <c r="D34" s="158"/>
+      <c r="E34" s="158"/>
+      <c r="F34" s="158"/>
+      <c r="G34" s="168"/>
       <c r="H34" s="113"/>
       <c r="I34" s="113"/>
       <c r="J34" s="113"/>
@@ -5294,12 +5294,12 @@
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A35" s="119"/>
-      <c r="B35" s="157"/>
-      <c r="C35" s="157"/>
-      <c r="D35" s="157"/>
-      <c r="E35" s="157"/>
-      <c r="F35" s="157"/>
-      <c r="G35" s="158"/>
+      <c r="B35" s="159"/>
+      <c r="C35" s="159"/>
+      <c r="D35" s="159"/>
+      <c r="E35" s="159"/>
+      <c r="F35" s="159"/>
+      <c r="G35" s="169"/>
       <c r="H35" s="113"/>
       <c r="I35" s="113"/>
       <c r="J35" s="113"/>
@@ -5369,7 +5369,7 @@
         <v>162</v>
       </c>
       <c r="F39" s="184" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G39" s="181" t="s">
         <v>13</v>
@@ -5378,7 +5378,7 @@
         <v>116</v>
       </c>
       <c r="I39" s="181" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J39" s="179" t="s">
         <v>71</v>
@@ -5914,6 +5914,23 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
     <mergeCell ref="J39:K39"/>
     <mergeCell ref="L39:M39"/>
     <mergeCell ref="O39:O40"/>
@@ -5926,23 +5943,6 @@
     <mergeCell ref="E39:E40"/>
     <mergeCell ref="F39:F40"/>
     <mergeCell ref="I39:I40"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="A25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="A31:G31"/>
-    <mergeCell ref="B32:G32"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="3">
@@ -5999,9 +5999,7 @@
   </sheetPr>
   <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I38" sqref="I38:I44"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -6154,12 +6152,12 @@
         <v>180</v>
       </c>
       <c r="B12" s="123"/>
-      <c r="C12" s="135" t="s">
+      <c r="C12" s="175" t="s">
+        <v>204</v>
+      </c>
+      <c r="D12" s="175"/>
+      <c r="E12" s="96" t="s">
         <v>181</v>
-      </c>
-      <c r="D12" s="135"/>
-      <c r="E12" s="96" t="s">
-        <v>182</v>
       </c>
       <c r="F12" s="96"/>
       <c r="H12" s="54"/>
@@ -6167,13 +6165,13 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A13" s="123" t="s">
+        <v>182</v>
+      </c>
+      <c r="B13" s="123"/>
+      <c r="C13" s="175" t="s">
         <v>183</v>
       </c>
-      <c r="B13" s="123"/>
-      <c r="C13" s="135" t="s">
-        <v>184</v>
-      </c>
-      <c r="D13" s="135"/>
+      <c r="D13" s="175"/>
       <c r="E13" s="55"/>
       <c r="F13" s="55"/>
       <c r="G13" s="54"/>
@@ -6182,14 +6180,14 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A14" s="124" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B14" s="125"/>
       <c r="C14" s="101" t="s">
         <v>141</v>
       </c>
       <c r="D14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G14"/>
       <c r="H14"/>
@@ -6205,28 +6203,28 @@
       <c r="F15" s="96"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A16" s="175" t="s">
-        <v>198</v>
-      </c>
-      <c r="B16" s="175"/>
-      <c r="C16" s="175"/>
-      <c r="D16" s="175"/>
-      <c r="E16" s="175"/>
-      <c r="F16" s="175"/>
-      <c r="G16" s="175"/>
+      <c r="A16" s="151" t="s">
+        <v>197</v>
+      </c>
+      <c r="B16" s="151"/>
+      <c r="C16" s="151"/>
+      <c r="D16" s="151"/>
+      <c r="E16" s="151"/>
+      <c r="F16" s="151"/>
+      <c r="G16" s="151"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A17" s="116" t="s">
         <v>69</v>
       </c>
-      <c r="B17" s="169" t="s">
-        <v>189</v>
-      </c>
-      <c r="C17" s="170"/>
-      <c r="D17" s="170"/>
-      <c r="E17" s="170"/>
-      <c r="F17" s="170"/>
-      <c r="G17" s="171"/>
+      <c r="B17" s="145" t="s">
+        <v>188</v>
+      </c>
+      <c r="C17" s="146"/>
+      <c r="D17" s="146"/>
+      <c r="E17" s="146"/>
+      <c r="F17" s="146"/>
+      <c r="G17" s="147"/>
       <c r="H17" s="106"/>
       <c r="J17" s="106"/>
       <c r="K17" s="106"/>
@@ -6237,12 +6235,12 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A18" s="117"/>
-      <c r="B18" s="153"/>
-      <c r="C18" s="153"/>
-      <c r="D18" s="153"/>
-      <c r="E18" s="153"/>
-      <c r="F18" s="153"/>
-      <c r="G18" s="153"/>
+      <c r="B18" s="157"/>
+      <c r="C18" s="157"/>
+      <c r="D18" s="157"/>
+      <c r="E18" s="157"/>
+      <c r="F18" s="157"/>
+      <c r="G18" s="157"/>
       <c r="H18" s="113"/>
       <c r="J18" s="113"/>
       <c r="K18" s="113"/>
@@ -6253,12 +6251,12 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A19" s="118"/>
-      <c r="B19" s="155"/>
-      <c r="C19" s="155"/>
-      <c r="D19" s="155"/>
-      <c r="E19" s="155"/>
-      <c r="F19" s="155"/>
-      <c r="G19" s="155"/>
+      <c r="B19" s="158"/>
+      <c r="C19" s="158"/>
+      <c r="D19" s="158"/>
+      <c r="E19" s="158"/>
+      <c r="F19" s="158"/>
+      <c r="G19" s="158"/>
       <c r="H19" s="113"/>
       <c r="J19" s="113"/>
       <c r="K19" s="113"/>
@@ -6269,12 +6267,12 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A20" s="119"/>
-      <c r="B20" s="157"/>
-      <c r="C20" s="157"/>
-      <c r="D20" s="157"/>
-      <c r="E20" s="157"/>
-      <c r="F20" s="157"/>
-      <c r="G20" s="157"/>
+      <c r="B20" s="159"/>
+      <c r="C20" s="159"/>
+      <c r="D20" s="159"/>
+      <c r="E20" s="159"/>
+      <c r="F20" s="159"/>
+      <c r="G20" s="159"/>
       <c r="H20" s="113"/>
       <c r="I20" s="106"/>
       <c r="J20" s="113"/>
@@ -6289,29 +6287,29 @@
       <c r="I21" s="113"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A22" s="172" t="s">
-        <v>199</v>
-      </c>
-      <c r="B22" s="173"/>
-      <c r="C22" s="173"/>
-      <c r="D22" s="173"/>
-      <c r="E22" s="173"/>
-      <c r="F22" s="173"/>
-      <c r="G22" s="174"/>
+      <c r="A22" s="148" t="s">
+        <v>198</v>
+      </c>
+      <c r="B22" s="149"/>
+      <c r="C22" s="149"/>
+      <c r="D22" s="149"/>
+      <c r="E22" s="149"/>
+      <c r="F22" s="149"/>
+      <c r="G22" s="150"/>
       <c r="I22" s="113"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A23" s="116" t="s">
         <v>69</v>
       </c>
-      <c r="B23" s="149" t="s">
-        <v>190</v>
-      </c>
-      <c r="C23" s="149"/>
-      <c r="D23" s="149"/>
-      <c r="E23" s="149"/>
-      <c r="F23" s="149"/>
-      <c r="G23" s="149"/>
+      <c r="B23" s="163" t="s">
+        <v>189</v>
+      </c>
+      <c r="C23" s="163"/>
+      <c r="D23" s="163"/>
+      <c r="E23" s="163"/>
+      <c r="F23" s="163"/>
+      <c r="G23" s="163"/>
       <c r="H23" s="106"/>
       <c r="I23" s="113"/>
       <c r="J23" s="106"/>
@@ -6325,14 +6323,14 @@
       <c r="A24" s="117">
         <v>1</v>
       </c>
-      <c r="B24" s="150" t="s">
-        <v>191</v>
-      </c>
-      <c r="C24" s="150"/>
-      <c r="D24" s="150"/>
-      <c r="E24" s="150"/>
-      <c r="F24" s="150"/>
-      <c r="G24" s="150"/>
+      <c r="B24" s="164" t="s">
+        <v>190</v>
+      </c>
+      <c r="C24" s="164"/>
+      <c r="D24" s="164"/>
+      <c r="E24" s="164"/>
+      <c r="F24" s="164"/>
+      <c r="G24" s="164"/>
       <c r="H24" s="113"/>
       <c r="J24" s="113"/>
       <c r="K24" s="113"/>
@@ -6343,12 +6341,12 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A25" s="118"/>
-      <c r="B25" s="151"/>
-      <c r="C25" s="151"/>
-      <c r="D25" s="151"/>
-      <c r="E25" s="151"/>
-      <c r="F25" s="151"/>
-      <c r="G25" s="151"/>
+      <c r="B25" s="165"/>
+      <c r="C25" s="165"/>
+      <c r="D25" s="165"/>
+      <c r="E25" s="165"/>
+      <c r="F25" s="165"/>
+      <c r="G25" s="165"/>
       <c r="H25" s="113"/>
       <c r="J25" s="113"/>
       <c r="K25" s="113"/>
@@ -6359,12 +6357,12 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A26" s="119"/>
-      <c r="B26" s="152"/>
-      <c r="C26" s="152"/>
-      <c r="D26" s="152"/>
-      <c r="E26" s="152"/>
-      <c r="F26" s="152"/>
-      <c r="G26" s="152"/>
+      <c r="B26" s="166"/>
+      <c r="C26" s="166"/>
+      <c r="D26" s="166"/>
+      <c r="E26" s="166"/>
+      <c r="F26" s="166"/>
+      <c r="G26" s="166"/>
       <c r="H26" s="113"/>
       <c r="I26" s="106"/>
       <c r="J26" s="113"/>
@@ -6391,29 +6389,29 @@
       <c r="N27"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A28" s="172" t="s">
-        <v>200</v>
-      </c>
-      <c r="B28" s="173"/>
-      <c r="C28" s="173"/>
-      <c r="D28" s="173"/>
-      <c r="E28" s="173"/>
-      <c r="F28" s="173"/>
-      <c r="G28" s="174"/>
+      <c r="A28" s="148" t="s">
+        <v>199</v>
+      </c>
+      <c r="B28" s="149"/>
+      <c r="C28" s="149"/>
+      <c r="D28" s="149"/>
+      <c r="E28" s="149"/>
+      <c r="F28" s="149"/>
+      <c r="G28" s="150"/>
       <c r="I28" s="113"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A29" s="116" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="149" t="s">
-        <v>192</v>
-      </c>
-      <c r="C29" s="149"/>
-      <c r="D29" s="149"/>
-      <c r="E29" s="149"/>
-      <c r="F29" s="149"/>
-      <c r="G29" s="149"/>
+      <c r="B29" s="163" t="s">
+        <v>191</v>
+      </c>
+      <c r="C29" s="163"/>
+      <c r="D29" s="163"/>
+      <c r="E29" s="163"/>
+      <c r="F29" s="163"/>
+      <c r="G29" s="163"/>
       <c r="H29" s="106"/>
       <c r="I29" s="113"/>
       <c r="J29" s="106"/>
@@ -6425,12 +6423,12 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A30" s="117"/>
-      <c r="B30" s="153"/>
-      <c r="C30" s="153"/>
-      <c r="D30" s="153"/>
-      <c r="E30" s="153"/>
-      <c r="F30" s="153"/>
-      <c r="G30" s="154"/>
+      <c r="B30" s="157"/>
+      <c r="C30" s="157"/>
+      <c r="D30" s="157"/>
+      <c r="E30" s="157"/>
+      <c r="F30" s="157"/>
+      <c r="G30" s="167"/>
       <c r="H30" s="113"/>
       <c r="I30"/>
       <c r="J30" s="113"/>
@@ -6442,12 +6440,12 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A31" s="118"/>
-      <c r="B31" s="155"/>
-      <c r="C31" s="155"/>
-      <c r="D31" s="155"/>
-      <c r="E31" s="155"/>
-      <c r="F31" s="155"/>
-      <c r="G31" s="156"/>
+      <c r="B31" s="158"/>
+      <c r="C31" s="158"/>
+      <c r="D31" s="158"/>
+      <c r="E31" s="158"/>
+      <c r="F31" s="158"/>
+      <c r="G31" s="168"/>
       <c r="H31" s="113"/>
       <c r="J31" s="113"/>
       <c r="K31" s="113"/>
@@ -6458,12 +6456,12 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A32" s="119"/>
-      <c r="B32" s="157"/>
-      <c r="C32" s="157"/>
-      <c r="D32" s="157"/>
-      <c r="E32" s="157"/>
-      <c r="F32" s="157"/>
-      <c r="G32" s="158"/>
+      <c r="B32" s="159"/>
+      <c r="C32" s="159"/>
+      <c r="D32" s="159"/>
+      <c r="E32" s="159"/>
+      <c r="F32" s="159"/>
+      <c r="G32" s="169"/>
       <c r="H32" s="113"/>
       <c r="I32" s="106"/>
       <c r="J32" s="113"/>
@@ -6529,7 +6527,7 @@
         <v>162</v>
       </c>
       <c r="F36" s="184" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G36" s="184" t="s">
         <v>140</v>
@@ -6538,7 +6536,7 @@
         <v>139</v>
       </c>
       <c r="I36" s="181" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J36" s="191" t="s">
         <v>122</v>
@@ -7058,6 +7056,23 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="A28:G28"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B18:G18"/>
     <mergeCell ref="L36:M36"/>
     <mergeCell ref="O36:O37"/>
     <mergeCell ref="A36:A37"/>
@@ -7069,23 +7084,6 @@
     <mergeCell ref="E36:E37"/>
     <mergeCell ref="F36:F37"/>
     <mergeCell ref="I36:I37"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="A22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="A28:G28"/>
-    <mergeCell ref="B29:G29"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="3">
@@ -7133,9 +7131,7 @@
   </sheetPr>
   <dimension ref="A1:T64"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41:I47"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -7328,24 +7324,24 @@
         <v>180</v>
       </c>
       <c r="B15" s="123"/>
-      <c r="C15" s="135" t="s">
+      <c r="C15" s="175" t="s">
+        <v>204</v>
+      </c>
+      <c r="D15" s="175"/>
+      <c r="E15" s="96" t="s">
         <v>181</v>
-      </c>
-      <c r="D15" s="135"/>
-      <c r="E15" s="96" t="s">
-        <v>182</v>
       </c>
       <c r="G15" s="54"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A16" s="123" t="s">
+        <v>182</v>
+      </c>
+      <c r="B16" s="123"/>
+      <c r="C16" s="175" t="s">
         <v>183</v>
       </c>
-      <c r="B16" s="123"/>
-      <c r="C16" s="135" t="s">
-        <v>184</v>
-      </c>
-      <c r="D16" s="135"/>
+      <c r="D16" s="175"/>
       <c r="E16" s="55"/>
       <c r="F16" s="54"/>
       <c r="G16" s="54"/>
@@ -7354,14 +7350,14 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A17" s="124" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B17" s="125"/>
       <c r="C17" s="101" t="s">
         <v>141</v>
       </c>
       <c r="D17" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F17"/>
       <c r="G17"/>
@@ -7377,28 +7373,28 @@
       <c r="C18" s="28"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A19" s="175" t="s">
-        <v>198</v>
-      </c>
-      <c r="B19" s="175"/>
-      <c r="C19" s="175"/>
-      <c r="D19" s="175"/>
-      <c r="E19" s="175"/>
-      <c r="F19" s="175"/>
-      <c r="G19" s="175"/>
+      <c r="A19" s="151" t="s">
+        <v>197</v>
+      </c>
+      <c r="B19" s="151"/>
+      <c r="C19" s="151"/>
+      <c r="D19" s="151"/>
+      <c r="E19" s="151"/>
+      <c r="F19" s="151"/>
+      <c r="G19" s="151"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A20" s="116" t="s">
         <v>69</v>
       </c>
-      <c r="B20" s="169" t="s">
-        <v>189</v>
-      </c>
-      <c r="C20" s="170"/>
-      <c r="D20" s="170"/>
-      <c r="E20" s="170"/>
-      <c r="F20" s="170"/>
-      <c r="G20" s="171"/>
+      <c r="B20" s="145" t="s">
+        <v>188</v>
+      </c>
+      <c r="C20" s="146"/>
+      <c r="D20" s="146"/>
+      <c r="E20" s="146"/>
+      <c r="F20" s="146"/>
+      <c r="G20" s="147"/>
       <c r="H20" s="106"/>
       <c r="I20" s="106"/>
       <c r="J20" s="106"/>
@@ -7410,12 +7406,12 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A21" s="117"/>
-      <c r="B21" s="153"/>
-      <c r="C21" s="153"/>
-      <c r="D21" s="153"/>
-      <c r="E21" s="153"/>
-      <c r="F21" s="153"/>
-      <c r="G21" s="153"/>
+      <c r="B21" s="157"/>
+      <c r="C21" s="157"/>
+      <c r="D21" s="157"/>
+      <c r="E21" s="157"/>
+      <c r="F21" s="157"/>
+      <c r="G21" s="157"/>
       <c r="H21" s="113"/>
       <c r="I21" s="113"/>
       <c r="J21" s="113"/>
@@ -7427,12 +7423,12 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A22" s="118"/>
-      <c r="B22" s="155"/>
-      <c r="C22" s="155"/>
-      <c r="D22" s="155"/>
-      <c r="E22" s="155"/>
-      <c r="F22" s="155"/>
-      <c r="G22" s="155"/>
+      <c r="B22" s="158"/>
+      <c r="C22" s="158"/>
+      <c r="D22" s="158"/>
+      <c r="E22" s="158"/>
+      <c r="F22" s="158"/>
+      <c r="G22" s="158"/>
       <c r="H22" s="113"/>
       <c r="I22" s="113"/>
       <c r="J22" s="113"/>
@@ -7444,12 +7440,12 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A23" s="119"/>
-      <c r="B23" s="157"/>
-      <c r="C23" s="157"/>
-      <c r="D23" s="157"/>
-      <c r="E23" s="157"/>
-      <c r="F23" s="157"/>
-      <c r="G23" s="157"/>
+      <c r="B23" s="159"/>
+      <c r="C23" s="159"/>
+      <c r="D23" s="159"/>
+      <c r="E23" s="159"/>
+      <c r="F23" s="159"/>
+      <c r="G23" s="159"/>
       <c r="H23" s="113"/>
       <c r="I23" s="113"/>
       <c r="J23" s="113"/>
@@ -7463,28 +7459,28 @@
       <c r="C24"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A25" s="172" t="s">
-        <v>199</v>
-      </c>
-      <c r="B25" s="173"/>
-      <c r="C25" s="173"/>
-      <c r="D25" s="173"/>
-      <c r="E25" s="173"/>
-      <c r="F25" s="173"/>
-      <c r="G25" s="174"/>
+      <c r="A25" s="148" t="s">
+        <v>198</v>
+      </c>
+      <c r="B25" s="149"/>
+      <c r="C25" s="149"/>
+      <c r="D25" s="149"/>
+      <c r="E25" s="149"/>
+      <c r="F25" s="149"/>
+      <c r="G25" s="150"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A26" s="116" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="149" t="s">
-        <v>190</v>
-      </c>
-      <c r="C26" s="149"/>
-      <c r="D26" s="149"/>
-      <c r="E26" s="149"/>
-      <c r="F26" s="149"/>
-      <c r="G26" s="149"/>
+      <c r="B26" s="163" t="s">
+        <v>189</v>
+      </c>
+      <c r="C26" s="163"/>
+      <c r="D26" s="163"/>
+      <c r="E26" s="163"/>
+      <c r="F26" s="163"/>
+      <c r="G26" s="163"/>
       <c r="H26" s="106"/>
       <c r="I26" s="106"/>
       <c r="J26" s="106"/>
@@ -7498,14 +7494,14 @@
       <c r="A27" s="117">
         <v>1</v>
       </c>
-      <c r="B27" s="150" t="s">
-        <v>191</v>
-      </c>
-      <c r="C27" s="150"/>
-      <c r="D27" s="150"/>
-      <c r="E27" s="150"/>
-      <c r="F27" s="150"/>
-      <c r="G27" s="150"/>
+      <c r="B27" s="164" t="s">
+        <v>190</v>
+      </c>
+      <c r="C27" s="164"/>
+      <c r="D27" s="164"/>
+      <c r="E27" s="164"/>
+      <c r="F27" s="164"/>
+      <c r="G27" s="164"/>
       <c r="H27" s="113"/>
       <c r="I27" s="113"/>
       <c r="J27" s="113"/>
@@ -7517,12 +7513,12 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A28" s="118"/>
-      <c r="B28" s="151"/>
-      <c r="C28" s="151"/>
-      <c r="D28" s="151"/>
-      <c r="E28" s="151"/>
-      <c r="F28" s="151"/>
-      <c r="G28" s="151"/>
+      <c r="B28" s="165"/>
+      <c r="C28" s="165"/>
+      <c r="D28" s="165"/>
+      <c r="E28" s="165"/>
+      <c r="F28" s="165"/>
+      <c r="G28" s="165"/>
       <c r="H28" s="113"/>
       <c r="I28" s="113"/>
       <c r="J28" s="113"/>
@@ -7534,12 +7530,12 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A29" s="119"/>
-      <c r="B29" s="152"/>
-      <c r="C29" s="152"/>
-      <c r="D29" s="152"/>
-      <c r="E29" s="152"/>
-      <c r="F29" s="152"/>
-      <c r="G29" s="152"/>
+      <c r="B29" s="166"/>
+      <c r="C29" s="166"/>
+      <c r="D29" s="166"/>
+      <c r="E29" s="166"/>
+      <c r="F29" s="166"/>
+      <c r="G29" s="166"/>
       <c r="H29" s="113"/>
       <c r="I29" s="113"/>
       <c r="J29" s="113"/>
@@ -7566,28 +7562,28 @@
       <c r="N30"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A31" s="172" t="s">
-        <v>200</v>
-      </c>
-      <c r="B31" s="173"/>
-      <c r="C31" s="173"/>
-      <c r="D31" s="173"/>
-      <c r="E31" s="173"/>
-      <c r="F31" s="173"/>
-      <c r="G31" s="174"/>
+      <c r="A31" s="148" t="s">
+        <v>199</v>
+      </c>
+      <c r="B31" s="149"/>
+      <c r="C31" s="149"/>
+      <c r="D31" s="149"/>
+      <c r="E31" s="149"/>
+      <c r="F31" s="149"/>
+      <c r="G31" s="150"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A32" s="116" t="s">
         <v>69</v>
       </c>
-      <c r="B32" s="149" t="s">
-        <v>192</v>
-      </c>
-      <c r="C32" s="149"/>
-      <c r="D32" s="149"/>
-      <c r="E32" s="149"/>
-      <c r="F32" s="149"/>
-      <c r="G32" s="149"/>
+      <c r="B32" s="163" t="s">
+        <v>191</v>
+      </c>
+      <c r="C32" s="163"/>
+      <c r="D32" s="163"/>
+      <c r="E32" s="163"/>
+      <c r="F32" s="163"/>
+      <c r="G32" s="163"/>
       <c r="H32" s="106"/>
       <c r="I32" s="106"/>
       <c r="J32" s="106"/>
@@ -7599,12 +7595,12 @@
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A33" s="117"/>
-      <c r="B33" s="153"/>
-      <c r="C33" s="153"/>
-      <c r="D33" s="153"/>
-      <c r="E33" s="153"/>
-      <c r="F33" s="153"/>
-      <c r="G33" s="154"/>
+      <c r="B33" s="157"/>
+      <c r="C33" s="157"/>
+      <c r="D33" s="157"/>
+      <c r="E33" s="157"/>
+      <c r="F33" s="157"/>
+      <c r="G33" s="167"/>
       <c r="H33" s="113"/>
       <c r="I33" s="113"/>
       <c r="J33" s="113"/>
@@ -7616,12 +7612,12 @@
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A34" s="118"/>
-      <c r="B34" s="155"/>
-      <c r="C34" s="155"/>
-      <c r="D34" s="155"/>
-      <c r="E34" s="155"/>
-      <c r="F34" s="155"/>
-      <c r="G34" s="156"/>
+      <c r="B34" s="158"/>
+      <c r="C34" s="158"/>
+      <c r="D34" s="158"/>
+      <c r="E34" s="158"/>
+      <c r="F34" s="158"/>
+      <c r="G34" s="168"/>
       <c r="H34" s="113"/>
       <c r="I34" s="113"/>
       <c r="J34" s="113"/>
@@ -7633,12 +7629,12 @@
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A35" s="119"/>
-      <c r="B35" s="157"/>
-      <c r="C35" s="157"/>
-      <c r="D35" s="157"/>
-      <c r="E35" s="157"/>
-      <c r="F35" s="157"/>
-      <c r="G35" s="158"/>
+      <c r="B35" s="159"/>
+      <c r="C35" s="159"/>
+      <c r="D35" s="159"/>
+      <c r="E35" s="159"/>
+      <c r="F35" s="159"/>
+      <c r="G35" s="169"/>
       <c r="H35" s="113"/>
       <c r="I35" s="113"/>
       <c r="J35" s="113"/>
@@ -7708,7 +7704,7 @@
         <v>162</v>
       </c>
       <c r="F39" s="184" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G39" s="181" t="s">
         <v>13</v>
@@ -7717,7 +7713,7 @@
         <v>116</v>
       </c>
       <c r="I39" s="181" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J39" s="179" t="s">
         <v>71</v>
@@ -8253,6 +8249,23 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
     <mergeCell ref="J39:K39"/>
     <mergeCell ref="L39:M39"/>
     <mergeCell ref="O39:O40"/>
@@ -8265,23 +8278,6 @@
     <mergeCell ref="E39:E40"/>
     <mergeCell ref="F39:F40"/>
     <mergeCell ref="I39:I40"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="A25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="A31:G31"/>
-    <mergeCell ref="B32:G32"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="3">
@@ -8338,8 +8334,8 @@
   </sheetPr>
   <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38:I44"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -8493,12 +8489,12 @@
         <v>180</v>
       </c>
       <c r="B12" s="123"/>
-      <c r="C12" s="135" t="s">
+      <c r="C12" s="175" t="s">
+        <v>205</v>
+      </c>
+      <c r="D12" s="175"/>
+      <c r="E12" s="96" t="s">
         <v>181</v>
-      </c>
-      <c r="D12" s="135"/>
-      <c r="E12" s="96" t="s">
-        <v>182</v>
       </c>
       <c r="F12" s="96"/>
       <c r="H12" s="54"/>
@@ -8506,13 +8502,13 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A13" s="123" t="s">
+        <v>182</v>
+      </c>
+      <c r="B13" s="123"/>
+      <c r="C13" s="175" t="s">
         <v>183</v>
       </c>
-      <c r="B13" s="123"/>
-      <c r="C13" s="135" t="s">
-        <v>184</v>
-      </c>
-      <c r="D13" s="135"/>
+      <c r="D13" s="175"/>
       <c r="E13" s="55"/>
       <c r="F13" s="55"/>
       <c r="G13" s="54"/>
@@ -8521,14 +8517,14 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A14" s="124" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B14" s="125"/>
       <c r="C14" s="101" t="s">
         <v>141</v>
       </c>
       <c r="D14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G14"/>
       <c r="H14"/>
@@ -8544,28 +8540,28 @@
       <c r="F15" s="96"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A16" s="175" t="s">
-        <v>198</v>
-      </c>
-      <c r="B16" s="175"/>
-      <c r="C16" s="175"/>
-      <c r="D16" s="175"/>
-      <c r="E16" s="175"/>
-      <c r="F16" s="175"/>
-      <c r="G16" s="175"/>
+      <c r="A16" s="151" t="s">
+        <v>197</v>
+      </c>
+      <c r="B16" s="151"/>
+      <c r="C16" s="151"/>
+      <c r="D16" s="151"/>
+      <c r="E16" s="151"/>
+      <c r="F16" s="151"/>
+      <c r="G16" s="151"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A17" s="116" t="s">
         <v>69</v>
       </c>
-      <c r="B17" s="169" t="s">
-        <v>189</v>
-      </c>
-      <c r="C17" s="170"/>
-      <c r="D17" s="170"/>
-      <c r="E17" s="170"/>
-      <c r="F17" s="170"/>
-      <c r="G17" s="171"/>
+      <c r="B17" s="145" t="s">
+        <v>188</v>
+      </c>
+      <c r="C17" s="146"/>
+      <c r="D17" s="146"/>
+      <c r="E17" s="146"/>
+      <c r="F17" s="146"/>
+      <c r="G17" s="147"/>
       <c r="H17" s="106"/>
       <c r="J17" s="106"/>
       <c r="K17" s="106"/>
@@ -8576,12 +8572,12 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A18" s="117"/>
-      <c r="B18" s="153"/>
-      <c r="C18" s="153"/>
-      <c r="D18" s="153"/>
-      <c r="E18" s="153"/>
-      <c r="F18" s="153"/>
-      <c r="G18" s="153"/>
+      <c r="B18" s="157"/>
+      <c r="C18" s="157"/>
+      <c r="D18" s="157"/>
+      <c r="E18" s="157"/>
+      <c r="F18" s="157"/>
+      <c r="G18" s="157"/>
       <c r="H18" s="113"/>
       <c r="J18" s="113"/>
       <c r="K18" s="113"/>
@@ -8592,12 +8588,12 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A19" s="118"/>
-      <c r="B19" s="155"/>
-      <c r="C19" s="155"/>
-      <c r="D19" s="155"/>
-      <c r="E19" s="155"/>
-      <c r="F19" s="155"/>
-      <c r="G19" s="155"/>
+      <c r="B19" s="158"/>
+      <c r="C19" s="158"/>
+      <c r="D19" s="158"/>
+      <c r="E19" s="158"/>
+      <c r="F19" s="158"/>
+      <c r="G19" s="158"/>
       <c r="H19" s="113"/>
       <c r="J19" s="113"/>
       <c r="K19" s="113"/>
@@ -8608,12 +8604,12 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A20" s="119"/>
-      <c r="B20" s="157"/>
-      <c r="C20" s="157"/>
-      <c r="D20" s="157"/>
-      <c r="E20" s="157"/>
-      <c r="F20" s="157"/>
-      <c r="G20" s="157"/>
+      <c r="B20" s="159"/>
+      <c r="C20" s="159"/>
+      <c r="D20" s="159"/>
+      <c r="E20" s="159"/>
+      <c r="F20" s="159"/>
+      <c r="G20" s="159"/>
       <c r="H20" s="113"/>
       <c r="I20" s="106"/>
       <c r="J20" s="113"/>
@@ -8628,29 +8624,29 @@
       <c r="I21" s="113"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A22" s="172" t="s">
-        <v>199</v>
-      </c>
-      <c r="B22" s="173"/>
-      <c r="C22" s="173"/>
-      <c r="D22" s="173"/>
-      <c r="E22" s="173"/>
-      <c r="F22" s="173"/>
-      <c r="G22" s="174"/>
+      <c r="A22" s="148" t="s">
+        <v>198</v>
+      </c>
+      <c r="B22" s="149"/>
+      <c r="C22" s="149"/>
+      <c r="D22" s="149"/>
+      <c r="E22" s="149"/>
+      <c r="F22" s="149"/>
+      <c r="G22" s="150"/>
       <c r="I22" s="113"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A23" s="116" t="s">
         <v>69</v>
       </c>
-      <c r="B23" s="149" t="s">
-        <v>190</v>
-      </c>
-      <c r="C23" s="149"/>
-      <c r="D23" s="149"/>
-      <c r="E23" s="149"/>
-      <c r="F23" s="149"/>
-      <c r="G23" s="149"/>
+      <c r="B23" s="163" t="s">
+        <v>189</v>
+      </c>
+      <c r="C23" s="163"/>
+      <c r="D23" s="163"/>
+      <c r="E23" s="163"/>
+      <c r="F23" s="163"/>
+      <c r="G23" s="163"/>
       <c r="H23" s="106"/>
       <c r="I23" s="113"/>
       <c r="J23" s="106"/>
@@ -8664,14 +8660,14 @@
       <c r="A24" s="117">
         <v>1</v>
       </c>
-      <c r="B24" s="150" t="s">
-        <v>191</v>
-      </c>
-      <c r="C24" s="150"/>
-      <c r="D24" s="150"/>
-      <c r="E24" s="150"/>
-      <c r="F24" s="150"/>
-      <c r="G24" s="150"/>
+      <c r="B24" s="164" t="s">
+        <v>190</v>
+      </c>
+      <c r="C24" s="164"/>
+      <c r="D24" s="164"/>
+      <c r="E24" s="164"/>
+      <c r="F24" s="164"/>
+      <c r="G24" s="164"/>
       <c r="H24" s="113"/>
       <c r="J24" s="113"/>
       <c r="K24" s="113"/>
@@ -8682,12 +8678,12 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A25" s="118"/>
-      <c r="B25" s="151"/>
-      <c r="C25" s="151"/>
-      <c r="D25" s="151"/>
-      <c r="E25" s="151"/>
-      <c r="F25" s="151"/>
-      <c r="G25" s="151"/>
+      <c r="B25" s="165"/>
+      <c r="C25" s="165"/>
+      <c r="D25" s="165"/>
+      <c r="E25" s="165"/>
+      <c r="F25" s="165"/>
+      <c r="G25" s="165"/>
       <c r="H25" s="113"/>
       <c r="J25" s="113"/>
       <c r="K25" s="113"/>
@@ -8698,12 +8694,12 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A26" s="119"/>
-      <c r="B26" s="152"/>
-      <c r="C26" s="152"/>
-      <c r="D26" s="152"/>
-      <c r="E26" s="152"/>
-      <c r="F26" s="152"/>
-      <c r="G26" s="152"/>
+      <c r="B26" s="166"/>
+      <c r="C26" s="166"/>
+      <c r="D26" s="166"/>
+      <c r="E26" s="166"/>
+      <c r="F26" s="166"/>
+      <c r="G26" s="166"/>
       <c r="H26" s="113"/>
       <c r="I26" s="106"/>
       <c r="J26" s="113"/>
@@ -8730,29 +8726,29 @@
       <c r="N27"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A28" s="172" t="s">
-        <v>200</v>
-      </c>
-      <c r="B28" s="173"/>
-      <c r="C28" s="173"/>
-      <c r="D28" s="173"/>
-      <c r="E28" s="173"/>
-      <c r="F28" s="173"/>
-      <c r="G28" s="174"/>
+      <c r="A28" s="148" t="s">
+        <v>199</v>
+      </c>
+      <c r="B28" s="149"/>
+      <c r="C28" s="149"/>
+      <c r="D28" s="149"/>
+      <c r="E28" s="149"/>
+      <c r="F28" s="149"/>
+      <c r="G28" s="150"/>
       <c r="I28" s="113"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A29" s="116" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="149" t="s">
-        <v>192</v>
-      </c>
-      <c r="C29" s="149"/>
-      <c r="D29" s="149"/>
-      <c r="E29" s="149"/>
-      <c r="F29" s="149"/>
-      <c r="G29" s="149"/>
+      <c r="B29" s="163" t="s">
+        <v>191</v>
+      </c>
+      <c r="C29" s="163"/>
+      <c r="D29" s="163"/>
+      <c r="E29" s="163"/>
+      <c r="F29" s="163"/>
+      <c r="G29" s="163"/>
       <c r="H29" s="106"/>
       <c r="I29" s="113"/>
       <c r="J29" s="106"/>
@@ -8764,12 +8760,12 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A30" s="117"/>
-      <c r="B30" s="153"/>
-      <c r="C30" s="153"/>
-      <c r="D30" s="153"/>
-      <c r="E30" s="153"/>
-      <c r="F30" s="153"/>
-      <c r="G30" s="154"/>
+      <c r="B30" s="157"/>
+      <c r="C30" s="157"/>
+      <c r="D30" s="157"/>
+      <c r="E30" s="157"/>
+      <c r="F30" s="157"/>
+      <c r="G30" s="167"/>
       <c r="H30" s="113"/>
       <c r="I30"/>
       <c r="J30" s="113"/>
@@ -8781,12 +8777,12 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A31" s="118"/>
-      <c r="B31" s="155"/>
-      <c r="C31" s="155"/>
-      <c r="D31" s="155"/>
-      <c r="E31" s="155"/>
-      <c r="F31" s="155"/>
-      <c r="G31" s="156"/>
+      <c r="B31" s="158"/>
+      <c r="C31" s="158"/>
+      <c r="D31" s="158"/>
+      <c r="E31" s="158"/>
+      <c r="F31" s="158"/>
+      <c r="G31" s="168"/>
       <c r="H31" s="113"/>
       <c r="J31" s="113"/>
       <c r="K31" s="113"/>
@@ -8797,12 +8793,12 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A32" s="119"/>
-      <c r="B32" s="157"/>
-      <c r="C32" s="157"/>
-      <c r="D32" s="157"/>
-      <c r="E32" s="157"/>
-      <c r="F32" s="157"/>
-      <c r="G32" s="158"/>
+      <c r="B32" s="159"/>
+      <c r="C32" s="159"/>
+      <c r="D32" s="159"/>
+      <c r="E32" s="159"/>
+      <c r="F32" s="159"/>
+      <c r="G32" s="169"/>
       <c r="H32" s="113"/>
       <c r="I32" s="106"/>
       <c r="J32" s="113"/>
@@ -8868,7 +8864,7 @@
         <v>162</v>
       </c>
       <c r="F36" s="184" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G36" s="184" t="s">
         <v>140</v>
@@ -8877,7 +8873,7 @@
         <v>139</v>
       </c>
       <c r="I36" s="181" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J36" s="191" t="s">
         <v>122</v>
@@ -9397,6 +9393,23 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="A28:G28"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B18:G18"/>
     <mergeCell ref="L36:M36"/>
     <mergeCell ref="O36:O37"/>
     <mergeCell ref="A36:A37"/>
@@ -9408,23 +9421,6 @@
     <mergeCell ref="E36:E37"/>
     <mergeCell ref="F36:F37"/>
     <mergeCell ref="I36:I37"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="A22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="A28:G28"/>
-    <mergeCell ref="B29:G29"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="3">
@@ -9472,9 +9468,7 @@
   </sheetPr>
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -9851,10 +9845,10 @@
         <v>152</v>
       </c>
       <c r="E4" s="43" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F4" s="43" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
0.0.1: first release of blancoRestGeneratorKt! It's for micronaut framework only.
</commit_message>
<xml_diff>
--- a/meta/api/BlancoApiPostSample.xlsx
+++ b/meta/api/BlancoApiPostSample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorKt/meta/api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78017DD8-DF99-F342-AB03-4F796A4B6A47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5767E96-1D66-E04B-9E2E-EF918699AA93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="2240" windowWidth="21420" windowHeight="17540" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="180" yWindow="680" windowWidth="21420" windowHeight="17540" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="process" sheetId="19" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="222">
   <si>
     <t>項目名</t>
     <rPh sb="0" eb="3">
@@ -2291,6 +2291,72 @@
   </si>
   <si>
     <t>メタIDリスト</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>blanco.restgenerator.valueobject.BusinessApiRequestHeader</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>レスポンスヘッダ情報実装クラス(Kt)</t>
+    <rPh sb="8" eb="10">
+      <t xml:space="preserve">ジョウホウ </t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t xml:space="preserve">ジッソウ </t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>リクエストヘッダ情報実装クラス(Kt)</t>
+    <rPh sb="8" eb="10">
+      <t xml:space="preserve">ジョウホウ </t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t xml:space="preserve">ジッソウ </t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>blanco.restgenerator.valueobject.*</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>※ CommonResponse#info の実装クラスを指定します。infoフィールドが存在しない場合は無視されます。</t>
+    <rPh sb="23" eb="25">
+      <t xml:space="preserve">ジッソウクラス </t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t xml:space="preserve">シテイ </t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t xml:space="preserve">ソンザイ </t>
+    </rPh>
+    <rPh sb="50" eb="52">
+      <t xml:space="preserve">バアイハ </t>
+    </rPh>
+    <rPh sb="53" eb="55">
+      <t xml:space="preserve">ムシサレマス。 </t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>※ CommonRequest#info の実装クラスを指定します。infoフィールドが存在しない場合は無視されます。</t>
+    <rPh sb="22" eb="24">
+      <t xml:space="preserve">ジッソウクラス </t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t xml:space="preserve">シテイ </t>
+    </rPh>
+    <rPh sb="44" eb="46">
+      <t xml:space="preserve">ソンザイ </t>
+    </rPh>
+    <rPh sb="49" eb="51">
+      <t xml:space="preserve">バアイハ </t>
+    </rPh>
+    <rPh sb="52" eb="54">
+      <t xml:space="preserve">ムシサレマス。 </t>
+    </rPh>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -3672,12 +3738,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3704,6 +3764,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4277,10 +4343,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O68"/>
+  <dimension ref="A1:O70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D15" sqref="D15:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -4462,173 +4528,171 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="145" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B15" s="145"/>
       <c r="C15" s="145"/>
-      <c r="D15" s="141"/>
+      <c r="D15" s="141" t="s">
+        <v>216</v>
+      </c>
       <c r="E15" s="140"/>
       <c r="F15" s="54" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="G15" s="54"/>
       <c r="H15" s="95"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="182" t="s">
+      <c r="A16" s="145" t="s">
+        <v>217</v>
+      </c>
+      <c r="B16" s="145"/>
+      <c r="C16" s="145"/>
+      <c r="D16" s="141"/>
+      <c r="E16" s="140"/>
+      <c r="F16" s="54" t="s">
+        <v>220</v>
+      </c>
+      <c r="G16" s="54"/>
+      <c r="H16" s="95"/>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" s="145" t="s">
+        <v>215</v>
+      </c>
+      <c r="B17" s="145"/>
+      <c r="C17" s="145"/>
+      <c r="D17" s="141"/>
+      <c r="E17" s="140"/>
+      <c r="F17" s="54" t="s">
+        <v>214</v>
+      </c>
+      <c r="G17" s="54"/>
+      <c r="H17" s="95"/>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" s="182" t="s">
         <v>143</v>
       </c>
-      <c r="B16" s="183"/>
-      <c r="C16" s="184"/>
-      <c r="D16" s="114"/>
-    </row>
-    <row r="17" spans="1:15">
-      <c r="A17" s="168" t="s">
+      <c r="B18" s="183"/>
+      <c r="C18" s="184"/>
+      <c r="D18" s="114"/>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" s="168" t="s">
         <v>179</v>
       </c>
-      <c r="B17" s="169"/>
-      <c r="C17" s="170"/>
-      <c r="D17" s="100" t="s">
+      <c r="B19" s="169"/>
+      <c r="C19" s="170"/>
+      <c r="D19" s="100" t="s">
         <v>141</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E19" t="s">
         <v>180</v>
       </c>
-      <c r="F17"/>
-      <c r="G17"/>
-      <c r="H17"/>
-      <c r="I17"/>
-      <c r="J17"/>
-      <c r="K17"/>
-      <c r="L17"/>
-    </row>
-    <row r="18" spans="1:15">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-    </row>
-    <row r="19" spans="1:15">
-      <c r="A19" s="179" t="s">
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19"/>
+      <c r="K19"/>
+      <c r="L19"/>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" s="179" t="s">
         <v>188</v>
       </c>
-      <c r="B19" s="180"/>
-      <c r="C19" s="180"/>
-      <c r="D19" s="180"/>
-      <c r="E19" s="180"/>
-      <c r="F19" s="180"/>
-      <c r="G19" s="181"/>
-    </row>
-    <row r="20" spans="1:15">
-      <c r="A20" s="101" t="s">
+      <c r="B21" s="180"/>
+      <c r="C21" s="180"/>
+      <c r="D21" s="180"/>
+      <c r="E21" s="180"/>
+      <c r="F21" s="180"/>
+      <c r="G21" s="181"/>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" s="101" t="s">
         <v>181</v>
       </c>
-      <c r="B20" s="110"/>
-      <c r="C20" s="102"/>
-      <c r="D20" s="103"/>
-      <c r="E20" s="103"/>
-      <c r="F20" s="103"/>
-      <c r="G20" s="104"/>
-      <c r="H20" s="105"/>
-      <c r="I20" s="105"/>
-      <c r="J20" s="105"/>
-      <c r="K20" s="105"/>
-      <c r="L20" s="105"/>
-    </row>
-    <row r="21" spans="1:15">
-      <c r="A21" s="98" t="s">
+      <c r="B22" s="110"/>
+      <c r="C22" s="102"/>
+      <c r="D22" s="103"/>
+      <c r="E22" s="103"/>
+      <c r="F22" s="103"/>
+      <c r="G22" s="104"/>
+      <c r="H22" s="105"/>
+      <c r="I22" s="105"/>
+      <c r="J22" s="105"/>
+      <c r="K22" s="105"/>
+      <c r="L22" s="105"/>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" s="98" t="s">
         <v>99</v>
       </c>
-      <c r="B21" s="113"/>
-      <c r="C21" s="99"/>
-      <c r="D21" s="96"/>
-      <c r="E21" s="97"/>
-      <c r="F21" s="97"/>
-      <c r="G21" s="106"/>
-    </row>
-    <row r="22" spans="1:15">
-      <c r="A22" s="98" t="s">
+      <c r="B23" s="113"/>
+      <c r="C23" s="99"/>
+      <c r="D23" s="96"/>
+      <c r="E23" s="97"/>
+      <c r="F23" s="97"/>
+      <c r="G23" s="106"/>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" s="98" t="s">
         <v>182</v>
       </c>
-      <c r="B22" s="113"/>
-      <c r="C22" s="99"/>
-      <c r="D22" s="107"/>
-      <c r="E22" s="108"/>
-      <c r="F22" s="108"/>
-      <c r="G22" s="109"/>
-    </row>
-    <row r="23" spans="1:15">
-      <c r="C23"/>
-    </row>
-    <row r="24" spans="1:15">
-      <c r="A24" s="178" t="s">
+      <c r="B24" s="113"/>
+      <c r="C24" s="99"/>
+      <c r="D24" s="107"/>
+      <c r="E24" s="108"/>
+      <c r="F24" s="108"/>
+      <c r="G24" s="109"/>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="C25"/>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26" s="178" t="s">
         <v>189</v>
       </c>
-      <c r="B24" s="178"/>
-      <c r="C24" s="178"/>
-      <c r="D24" s="178"/>
-      <c r="E24" s="178"/>
-      <c r="F24" s="178"/>
-      <c r="G24" s="178"/>
-    </row>
-    <row r="25" spans="1:15">
-      <c r="A25" s="115" t="s">
+      <c r="B26" s="178"/>
+      <c r="C26" s="178"/>
+      <c r="D26" s="178"/>
+      <c r="E26" s="178"/>
+      <c r="F26" s="178"/>
+      <c r="G26" s="178"/>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B25" s="172" t="s">
+      <c r="B27" s="172" t="s">
         <v>183</v>
       </c>
-      <c r="C25" s="173"/>
-      <c r="D25" s="173"/>
-      <c r="E25" s="173"/>
-      <c r="F25" s="173"/>
-      <c r="G25" s="174"/>
-      <c r="H25" s="105"/>
-      <c r="I25" s="105"/>
-      <c r="J25" s="105"/>
-      <c r="K25" s="105"/>
-      <c r="L25" s="105"/>
-      <c r="N25" s="111"/>
-      <c r="O25" s="111"/>
-    </row>
-    <row r="26" spans="1:15">
-      <c r="A26" s="116"/>
-      <c r="B26" s="156"/>
-      <c r="C26" s="156"/>
-      <c r="D26" s="156"/>
-      <c r="E26" s="156"/>
-      <c r="F26" s="156"/>
-      <c r="G26" s="156"/>
-      <c r="H26" s="112"/>
-      <c r="I26" s="112"/>
-      <c r="J26" s="112"/>
-      <c r="K26" s="112"/>
-      <c r="M26"/>
-      <c r="N26"/>
-      <c r="O26"/>
-    </row>
-    <row r="27" spans="1:15">
-      <c r="A27" s="117"/>
-      <c r="B27" s="158"/>
-      <c r="C27" s="158"/>
-      <c r="D27" s="158"/>
-      <c r="E27" s="158"/>
-      <c r="F27" s="158"/>
-      <c r="G27" s="158"/>
-      <c r="H27" s="112"/>
-      <c r="I27" s="112"/>
-      <c r="J27" s="112"/>
-      <c r="K27" s="112"/>
-      <c r="M27"/>
-      <c r="N27"/>
-      <c r="O27"/>
+      <c r="C27" s="173"/>
+      <c r="D27" s="173"/>
+      <c r="E27" s="173"/>
+      <c r="F27" s="173"/>
+      <c r="G27" s="174"/>
+      <c r="H27" s="105"/>
+      <c r="I27" s="105"/>
+      <c r="J27" s="105"/>
+      <c r="K27" s="105"/>
+      <c r="L27" s="105"/>
+      <c r="N27" s="111"/>
+      <c r="O27" s="111"/>
     </row>
     <row r="28" spans="1:15">
-      <c r="A28" s="118"/>
-      <c r="B28" s="160"/>
-      <c r="C28" s="160"/>
-      <c r="D28" s="160"/>
-      <c r="E28" s="160"/>
-      <c r="F28" s="160"/>
-      <c r="G28" s="160"/>
+      <c r="A28" s="116"/>
+      <c r="B28" s="156"/>
+      <c r="C28" s="156"/>
+      <c r="D28" s="156"/>
+      <c r="E28" s="156"/>
+      <c r="F28" s="156"/>
+      <c r="G28" s="156"/>
       <c r="H28" s="112"/>
       <c r="I28" s="112"/>
       <c r="J28" s="112"/>
@@ -4638,83 +4702,83 @@
       <c r="O28"/>
     </row>
     <row r="29" spans="1:15">
-      <c r="C29"/>
+      <c r="A29" s="117"/>
+      <c r="B29" s="158"/>
+      <c r="C29" s="158"/>
+      <c r="D29" s="158"/>
+      <c r="E29" s="158"/>
+      <c r="F29" s="158"/>
+      <c r="G29" s="158"/>
+      <c r="H29" s="112"/>
+      <c r="I29" s="112"/>
+      <c r="J29" s="112"/>
+      <c r="K29" s="112"/>
+      <c r="M29"/>
+      <c r="N29"/>
+      <c r="O29"/>
     </row>
     <row r="30" spans="1:15">
-      <c r="A30" s="175" t="s">
+      <c r="A30" s="118"/>
+      <c r="B30" s="160"/>
+      <c r="C30" s="160"/>
+      <c r="D30" s="160"/>
+      <c r="E30" s="160"/>
+      <c r="F30" s="160"/>
+      <c r="G30" s="160"/>
+      <c r="H30" s="112"/>
+      <c r="I30" s="112"/>
+      <c r="J30" s="112"/>
+      <c r="K30" s="112"/>
+      <c r="M30"/>
+      <c r="N30"/>
+      <c r="O30"/>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="C31"/>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="A32" s="175" t="s">
         <v>190</v>
       </c>
-      <c r="B30" s="176"/>
-      <c r="C30" s="176"/>
-      <c r="D30" s="176"/>
-      <c r="E30" s="176"/>
-      <c r="F30" s="176"/>
-      <c r="G30" s="177"/>
-    </row>
-    <row r="31" spans="1:15">
-      <c r="A31" s="115" t="s">
+      <c r="B32" s="176"/>
+      <c r="C32" s="176"/>
+      <c r="D32" s="176"/>
+      <c r="E32" s="176"/>
+      <c r="F32" s="176"/>
+      <c r="G32" s="177"/>
+    </row>
+    <row r="33" spans="1:15">
+      <c r="A33" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B31" s="152" t="s">
+      <c r="B33" s="152" t="s">
         <v>184</v>
       </c>
-      <c r="C31" s="152"/>
-      <c r="D31" s="152"/>
-      <c r="E31" s="152"/>
-      <c r="F31" s="152"/>
-      <c r="G31" s="152"/>
-      <c r="H31" s="105"/>
-      <c r="I31" s="105"/>
-      <c r="J31" s="105"/>
-      <c r="K31" s="105"/>
-      <c r="L31" s="105"/>
-      <c r="N31" s="111"/>
-      <c r="O31" s="111"/>
-    </row>
-    <row r="32" spans="1:15">
-      <c r="A32" s="116">
+      <c r="C33" s="152"/>
+      <c r="D33" s="152"/>
+      <c r="E33" s="152"/>
+      <c r="F33" s="152"/>
+      <c r="G33" s="152"/>
+      <c r="H33" s="105"/>
+      <c r="I33" s="105"/>
+      <c r="J33" s="105"/>
+      <c r="K33" s="105"/>
+      <c r="L33" s="105"/>
+      <c r="N33" s="111"/>
+      <c r="O33" s="111"/>
+    </row>
+    <row r="34" spans="1:15">
+      <c r="A34" s="116">
         <v>1</v>
       </c>
-      <c r="B32" s="153" t="s">
-        <v>185</v>
-      </c>
-      <c r="C32" s="153"/>
-      <c r="D32" s="153"/>
-      <c r="E32" s="153"/>
-      <c r="F32" s="153"/>
-      <c r="G32" s="153"/>
-      <c r="H32" s="112"/>
-      <c r="I32" s="112"/>
-      <c r="J32" s="112"/>
-      <c r="K32" s="112"/>
-      <c r="M32"/>
-      <c r="N32"/>
-      <c r="O32"/>
-    </row>
-    <row r="33" spans="1:15">
-      <c r="A33" s="117"/>
-      <c r="B33" s="154"/>
-      <c r="C33" s="154"/>
-      <c r="D33" s="154"/>
-      <c r="E33" s="154"/>
-      <c r="F33" s="154"/>
-      <c r="G33" s="154"/>
-      <c r="H33" s="112"/>
-      <c r="I33" s="112"/>
-      <c r="J33" s="112"/>
-      <c r="K33" s="112"/>
-      <c r="M33"/>
-      <c r="N33"/>
-      <c r="O33"/>
-    </row>
-    <row r="34" spans="1:15">
-      <c r="A34" s="118"/>
-      <c r="B34" s="155"/>
-      <c r="C34" s="155"/>
-      <c r="D34" s="155"/>
-      <c r="E34" s="155"/>
-      <c r="F34" s="155"/>
-      <c r="G34" s="155"/>
+      <c r="B34" s="153" t="s">
+        <v>219</v>
+      </c>
+      <c r="C34" s="153"/>
+      <c r="D34" s="153"/>
+      <c r="E34" s="153"/>
+      <c r="F34" s="153"/>
+      <c r="G34" s="153"/>
       <c r="H34" s="112"/>
       <c r="I34" s="112"/>
       <c r="J34" s="112"/>
@@ -4724,91 +4788,91 @@
       <c r="O34"/>
     </row>
     <row r="35" spans="1:15">
-      <c r="A35"/>
-      <c r="B35"/>
-      <c r="C35"/>
-      <c r="D35"/>
-      <c r="E35"/>
-      <c r="F35"/>
-      <c r="G35"/>
-      <c r="H35"/>
-      <c r="I35"/>
-      <c r="J35"/>
-      <c r="K35"/>
-      <c r="L35"/>
+      <c r="A35" s="117"/>
+      <c r="B35" s="154"/>
+      <c r="C35" s="154"/>
+      <c r="D35" s="154"/>
+      <c r="E35" s="154"/>
+      <c r="F35" s="154"/>
+      <c r="G35" s="154"/>
+      <c r="H35" s="112"/>
+      <c r="I35" s="112"/>
+      <c r="J35" s="112"/>
+      <c r="K35" s="112"/>
       <c r="M35"/>
+      <c r="N35"/>
+      <c r="O35"/>
     </row>
     <row r="36" spans="1:15">
-      <c r="A36" s="175" t="s">
+      <c r="A36" s="118"/>
+      <c r="B36" s="155"/>
+      <c r="C36" s="155"/>
+      <c r="D36" s="155"/>
+      <c r="E36" s="155"/>
+      <c r="F36" s="155"/>
+      <c r="G36" s="155"/>
+      <c r="H36" s="112"/>
+      <c r="I36" s="112"/>
+      <c r="J36" s="112"/>
+      <c r="K36" s="112"/>
+      <c r="M36"/>
+      <c r="N36"/>
+      <c r="O36"/>
+    </row>
+    <row r="37" spans="1:15">
+      <c r="A37"/>
+      <c r="B37"/>
+      <c r="C37"/>
+      <c r="D37"/>
+      <c r="E37"/>
+      <c r="F37"/>
+      <c r="G37"/>
+      <c r="H37"/>
+      <c r="I37"/>
+      <c r="J37"/>
+      <c r="K37"/>
+      <c r="L37"/>
+      <c r="M37"/>
+    </row>
+    <row r="38" spans="1:15">
+      <c r="A38" s="175" t="s">
         <v>191</v>
       </c>
-      <c r="B36" s="176"/>
-      <c r="C36" s="176"/>
-      <c r="D36" s="176"/>
-      <c r="E36" s="176"/>
-      <c r="F36" s="176"/>
-      <c r="G36" s="177"/>
-    </row>
-    <row r="37" spans="1:15">
-      <c r="A37" s="115" t="s">
+      <c r="B38" s="176"/>
+      <c r="C38" s="176"/>
+      <c r="D38" s="176"/>
+      <c r="E38" s="176"/>
+      <c r="F38" s="176"/>
+      <c r="G38" s="177"/>
+    </row>
+    <row r="39" spans="1:15">
+      <c r="A39" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B37" s="152" t="s">
+      <c r="B39" s="152" t="s">
         <v>186</v>
       </c>
-      <c r="C37" s="152"/>
-      <c r="D37" s="152"/>
-      <c r="E37" s="152"/>
-      <c r="F37" s="152"/>
-      <c r="G37" s="152"/>
-      <c r="H37" s="105"/>
-      <c r="I37" s="105"/>
-      <c r="J37" s="105"/>
-      <c r="K37" s="105"/>
-      <c r="L37" s="105"/>
-      <c r="N37" s="111"/>
-      <c r="O37" s="111"/>
-    </row>
-    <row r="38" spans="1:15">
-      <c r="A38" s="116"/>
-      <c r="B38" s="156"/>
-      <c r="C38" s="156"/>
-      <c r="D38" s="156"/>
-      <c r="E38" s="156"/>
-      <c r="F38" s="156"/>
-      <c r="G38" s="157"/>
-      <c r="H38" s="112"/>
-      <c r="I38" s="112"/>
-      <c r="J38" s="112"/>
-      <c r="K38" s="112"/>
-      <c r="M38"/>
-      <c r="N38"/>
-      <c r="O38"/>
-    </row>
-    <row r="39" spans="1:15">
-      <c r="A39" s="117"/>
-      <c r="B39" s="158"/>
-      <c r="C39" s="158"/>
-      <c r="D39" s="158"/>
-      <c r="E39" s="158"/>
-      <c r="F39" s="158"/>
-      <c r="G39" s="159"/>
-      <c r="H39" s="112"/>
-      <c r="I39" s="112"/>
-      <c r="J39" s="112"/>
-      <c r="K39" s="112"/>
-      <c r="M39"/>
-      <c r="N39"/>
-      <c r="O39"/>
+      <c r="C39" s="152"/>
+      <c r="D39" s="152"/>
+      <c r="E39" s="152"/>
+      <c r="F39" s="152"/>
+      <c r="G39" s="152"/>
+      <c r="H39" s="105"/>
+      <c r="I39" s="105"/>
+      <c r="J39" s="105"/>
+      <c r="K39" s="105"/>
+      <c r="L39" s="105"/>
+      <c r="N39" s="111"/>
+      <c r="O39" s="111"/>
     </row>
     <row r="40" spans="1:15">
-      <c r="A40" s="118"/>
-      <c r="B40" s="160"/>
-      <c r="C40" s="160"/>
-      <c r="D40" s="160"/>
-      <c r="E40" s="160"/>
-      <c r="F40" s="160"/>
-      <c r="G40" s="161"/>
+      <c r="A40" s="116"/>
+      <c r="B40" s="156"/>
+      <c r="C40" s="156"/>
+      <c r="D40" s="156"/>
+      <c r="E40" s="156"/>
+      <c r="F40" s="156"/>
+      <c r="G40" s="157"/>
       <c r="H40" s="112"/>
       <c r="I40" s="112"/>
       <c r="J40" s="112"/>
@@ -4818,66 +4882,82 @@
       <c r="O40"/>
     </row>
     <row r="41" spans="1:15">
-      <c r="A41"/>
-      <c r="B41"/>
-      <c r="C41"/>
-      <c r="D41"/>
-      <c r="E41"/>
-      <c r="F41"/>
-      <c r="G41"/>
-      <c r="H41"/>
-      <c r="I41"/>
-      <c r="J41"/>
-      <c r="K41"/>
-      <c r="L41"/>
+      <c r="A41" s="117"/>
+      <c r="B41" s="158"/>
+      <c r="C41" s="158"/>
+      <c r="D41" s="158"/>
+      <c r="E41" s="158"/>
+      <c r="F41" s="158"/>
+      <c r="G41" s="159"/>
+      <c r="H41" s="112"/>
+      <c r="I41" s="112"/>
+      <c r="J41" s="112"/>
+      <c r="K41" s="112"/>
       <c r="M41"/>
+      <c r="N41"/>
+      <c r="O41"/>
     </row>
     <row r="42" spans="1:15">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="118"/>
+      <c r="B42" s="160"/>
+      <c r="C42" s="160"/>
+      <c r="D42" s="160"/>
+      <c r="E42" s="160"/>
+      <c r="F42" s="160"/>
+      <c r="G42" s="161"/>
+      <c r="H42" s="112"/>
+      <c r="I42" s="112"/>
+      <c r="J42" s="112"/>
+      <c r="K42" s="112"/>
+      <c r="M42"/>
+      <c r="N42"/>
+      <c r="O42"/>
+    </row>
+    <row r="43" spans="1:15">
+      <c r="A43"/>
+      <c r="B43"/>
+      <c r="C43"/>
+      <c r="D43"/>
+      <c r="E43"/>
+      <c r="F43"/>
+      <c r="G43"/>
+      <c r="H43"/>
+      <c r="I43"/>
+      <c r="J43"/>
+      <c r="K43"/>
+      <c r="L43"/>
+      <c r="M43"/>
+    </row>
+    <row r="44" spans="1:15">
+      <c r="A44" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="5"/>
-    </row>
-    <row r="43" spans="1:15">
-      <c r="A43" s="165" t="s">
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="5"/>
+    </row>
+    <row r="45" spans="1:15">
+      <c r="A45" s="165" t="s">
         <v>65</v>
       </c>
-      <c r="B43" s="171"/>
-      <c r="C43" s="165" t="s">
+      <c r="B45" s="171"/>
+      <c r="C45" s="165" t="s">
         <v>66</v>
       </c>
-      <c r="D43" s="166"/>
-      <c r="E43" s="167"/>
-      <c r="F43" s="29" t="s">
+      <c r="D45" s="166"/>
+      <c r="E45" s="167"/>
+      <c r="F45" s="29" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="44" spans="1:15">
-      <c r="A44" s="162"/>
-      <c r="B44" s="164"/>
-      <c r="C44" s="162"/>
-      <c r="D44" s="163"/>
-      <c r="E44" s="164"/>
-      <c r="F44" s="49"/>
-    </row>
-    <row r="45" spans="1:15">
-      <c r="A45" s="146"/>
-      <c r="B45" s="148"/>
-      <c r="C45" s="146"/>
-      <c r="D45" s="147"/>
-      <c r="E45" s="148"/>
-      <c r="F45" s="49"/>
-    </row>
     <row r="46" spans="1:15">
-      <c r="A46" s="146"/>
-      <c r="B46" s="148"/>
-      <c r="C46" s="146"/>
-      <c r="D46" s="147"/>
-      <c r="E46" s="148"/>
+      <c r="A46" s="162"/>
+      <c r="B46" s="164"/>
+      <c r="C46" s="162"/>
+      <c r="D46" s="163"/>
+      <c r="E46" s="164"/>
       <c r="F46" s="49"/>
     </row>
     <row r="47" spans="1:15">
@@ -5049,101 +5129,121 @@
       <c r="F67" s="49"/>
     </row>
     <row r="68" spans="1:6">
-      <c r="A68" s="149"/>
-      <c r="B68" s="151"/>
-      <c r="C68" s="149"/>
-      <c r="D68" s="150"/>
-      <c r="E68" s="151"/>
-      <c r="F68" s="50"/>
+      <c r="A68" s="146"/>
+      <c r="B68" s="148"/>
+      <c r="C68" s="146"/>
+      <c r="D68" s="147"/>
+      <c r="E68" s="148"/>
+      <c r="F68" s="49"/>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" s="146"/>
+      <c r="B69" s="148"/>
+      <c r="C69" s="146"/>
+      <c r="D69" s="147"/>
+      <c r="E69" s="148"/>
+      <c r="F69" s="49"/>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" s="149"/>
+      <c r="B70" s="151"/>
+      <c r="C70" s="149"/>
+      <c r="D70" s="150"/>
+      <c r="E70" s="151"/>
+      <c r="F70" s="50"/>
     </row>
   </sheetData>
-  <mergeCells count="91">
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
+  <mergeCells count="95">
     <mergeCell ref="A52:B52"/>
     <mergeCell ref="A53:B53"/>
     <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="A48:B48"/>
     <mergeCell ref="A49:B49"/>
-    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="C45:E45"/>
     <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="A30:G30"/>
-    <mergeCell ref="A36:G36"/>
-    <mergeCell ref="A24:G24"/>
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="A38:G38"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="A18:C18"/>
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="D14:E14"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A15:C15"/>
     <mergeCell ref="A63:B63"/>
     <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
     <mergeCell ref="A57:B57"/>
     <mergeCell ref="A58:B58"/>
     <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
     <mergeCell ref="A67:B67"/>
     <mergeCell ref="A68:B68"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
     <mergeCell ref="B28:G28"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B30:G30"/>
     <mergeCell ref="C46:E46"/>
     <mergeCell ref="C47:E47"/>
     <mergeCell ref="C48:E48"/>
     <mergeCell ref="C49:E49"/>
     <mergeCell ref="C50:E50"/>
     <mergeCell ref="C51:E51"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="A62:B62"/>
     <mergeCell ref="C60:E60"/>
     <mergeCell ref="C61:E61"/>
-    <mergeCell ref="C52:E52"/>
-    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C63:E63"/>
     <mergeCell ref="C54:E54"/>
     <mergeCell ref="C55:E55"/>
     <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C70:E70"/>
     <mergeCell ref="B33:G33"/>
     <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B36:G36"/>
     <mergeCell ref="B39:G39"/>
     <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="B41:G41"/>
+    <mergeCell ref="B42:G42"/>
     <mergeCell ref="C64:E64"/>
     <mergeCell ref="C65:E65"/>
     <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="C59:E59"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D17:E17"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A17:C17"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:E16"/>
     <mergeCell ref="A5:E5"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D7:E7"/>
@@ -5152,7 +5252,7 @@
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D17" xr:uid="{AA005DBF-E840-AD43-AC91-CD6CE016CB50}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D19" xr:uid="{AA005DBF-E840-AD43-AC91-CD6CE016CB50}">
       <formula1>isImport</formula1>
     </dataValidation>
   </dataValidations>
@@ -5168,7 +5268,7 @@
           <x14:formula1>
             <xm:f>config!$B$5:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>D16</xm:sqref>
+          <xm:sqref>D18</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5184,7 +5284,7 @@
   <dimension ref="A1:Z64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:G25"/>
+      <selection activeCell="C39" sqref="C39:C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -5872,82 +5972,82 @@
       <c r="Z38" s="39"/>
     </row>
     <row r="39" spans="1:26">
-      <c r="A39" s="187" t="s">
+      <c r="A39" s="185" t="s">
         <v>69</v>
       </c>
-      <c r="B39" s="187" t="s">
+      <c r="B39" s="185" t="s">
         <v>0</v>
       </c>
-      <c r="C39" s="189" t="s">
+      <c r="C39" s="187" t="s">
         <v>1</v>
       </c>
-      <c r="D39" s="187" t="s">
+      <c r="D39" s="185" t="s">
         <v>2</v>
       </c>
-      <c r="E39" s="190" t="s">
+      <c r="E39" s="188" t="s">
         <v>161</v>
       </c>
-      <c r="F39" s="190" t="s">
+      <c r="F39" s="188" t="s">
         <v>177</v>
       </c>
-      <c r="G39" s="187" t="s">
+      <c r="G39" s="185" t="s">
         <v>13</v>
       </c>
-      <c r="H39" s="187" t="s">
+      <c r="H39" s="185" t="s">
         <v>116</v>
       </c>
-      <c r="I39" s="194" t="s">
+      <c r="I39" s="192" t="s">
         <v>201</v>
       </c>
-      <c r="J39" s="194" t="s">
+      <c r="J39" s="192" t="s">
         <v>202</v>
       </c>
-      <c r="K39" s="194" t="s">
+      <c r="K39" s="192" t="s">
         <v>203</v>
       </c>
-      <c r="L39" s="195" t="s">
+      <c r="L39" s="193" t="s">
         <v>204</v>
       </c>
-      <c r="M39" s="187" t="s">
+      <c r="M39" s="185" t="s">
         <v>195</v>
       </c>
-      <c r="N39" s="187" t="s">
+      <c r="N39" s="185" t="s">
         <v>210</v>
       </c>
-      <c r="O39" s="189" t="s">
+      <c r="O39" s="187" t="s">
         <v>209</v>
       </c>
-      <c r="P39" s="185" t="s">
+      <c r="P39" s="195" t="s">
         <v>71</v>
       </c>
-      <c r="Q39" s="186"/>
-      <c r="R39" s="185" t="s">
+      <c r="Q39" s="196"/>
+      <c r="R39" s="195" t="s">
         <v>17</v>
       </c>
-      <c r="S39" s="186"/>
+      <c r="S39" s="196"/>
       <c r="T39" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="U39" s="187" t="s">
+      <c r="U39" s="185" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:26">
-      <c r="A40" s="188"/>
-      <c r="B40" s="188"/>
-      <c r="C40" s="188"/>
-      <c r="D40" s="188"/>
-      <c r="E40" s="191"/>
-      <c r="F40" s="192"/>
-      <c r="G40" s="188"/>
-      <c r="H40" s="188"/>
-      <c r="I40" s="194"/>
-      <c r="J40" s="194"/>
-      <c r="K40" s="194"/>
-      <c r="L40" s="196"/>
-      <c r="M40" s="193"/>
-      <c r="N40" s="193"/>
-      <c r="O40" s="193"/>
+      <c r="A40" s="186"/>
+      <c r="B40" s="186"/>
+      <c r="C40" s="186"/>
+      <c r="D40" s="186"/>
+      <c r="E40" s="189"/>
+      <c r="F40" s="190"/>
+      <c r="G40" s="186"/>
+      <c r="H40" s="186"/>
+      <c r="I40" s="192"/>
+      <c r="J40" s="192"/>
+      <c r="K40" s="192"/>
+      <c r="L40" s="194"/>
+      <c r="M40" s="191"/>
+      <c r="N40" s="191"/>
+      <c r="O40" s="191"/>
       <c r="P40" s="29" t="s">
         <v>75</v>
       </c>
@@ -5963,7 +6063,7 @@
       <c r="T40" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="U40" s="188"/>
+      <c r="U40" s="186"/>
     </row>
     <row r="41" spans="1:26">
       <c r="A41" s="7">
@@ -6637,11 +6737,20 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="N39:N40"/>
-    <mergeCell ref="M39:M40"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="P39:Q39"/>
     <mergeCell ref="R39:S39"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B35:G35"/>
     <mergeCell ref="U39:U40"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="B39:B40"/>
@@ -6656,17 +6765,8 @@
     <mergeCell ref="J39:J40"/>
     <mergeCell ref="K39:K40"/>
     <mergeCell ref="L39:L40"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="A25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="N39:N40"/>
+    <mergeCell ref="M39:M40"/>
     <mergeCell ref="B27:G27"/>
     <mergeCell ref="B28:G28"/>
     <mergeCell ref="B29:G29"/>
@@ -6674,7 +6774,7 @@
     <mergeCell ref="B32:G32"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
-  <dataValidations count="3">
+  <dataValidations disablePrompts="1" count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>Validate実装パターン</formula1>
     </dataValidation>
@@ -6696,7 +6796,7 @@
   </headerFooter>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="3">
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000001000000}">
           <x14:formula1>
             <xm:f>config!$D$5:$D$8</xm:f>
@@ -6728,7 +6828,7 @@
   </sheetPr>
   <dimension ref="A1:V61"/>
   <sheetViews>
-    <sheetView topLeftCell="F26" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="N38" sqref="N38"/>
     </sheetView>
   </sheetViews>
@@ -7369,28 +7469,28 @@
       <c r="U35" s="58"/>
     </row>
     <row r="36" spans="1:21" ht="30" customHeight="1">
-      <c r="A36" s="190" t="s">
+      <c r="A36" s="188" t="s">
         <v>118</v>
       </c>
-      <c r="B36" s="190" t="s">
+      <c r="B36" s="188" t="s">
         <v>119</v>
       </c>
       <c r="C36" s="60" t="s">
         <v>120</v>
       </c>
-      <c r="D36" s="190" t="s">
+      <c r="D36" s="188" t="s">
         <v>101</v>
       </c>
-      <c r="E36" s="190" t="s">
+      <c r="E36" s="188" t="s">
         <v>161</v>
       </c>
-      <c r="F36" s="190" t="s">
+      <c r="F36" s="188" t="s">
         <v>177</v>
       </c>
-      <c r="G36" s="190" t="s">
+      <c r="G36" s="188" t="s">
         <v>140</v>
       </c>
-      <c r="H36" s="190" t="s">
+      <c r="H36" s="188" t="s">
         <v>139</v>
       </c>
       <c r="I36" s="202" t="s">
@@ -7402,16 +7502,16 @@
       <c r="K36" s="204" t="s">
         <v>203</v>
       </c>
-      <c r="L36" s="195" t="s">
+      <c r="L36" s="193" t="s">
         <v>204</v>
       </c>
-      <c r="M36" s="187" t="s">
+      <c r="M36" s="185" t="s">
         <v>195</v>
       </c>
-      <c r="N36" s="187" t="s">
+      <c r="N36" s="185" t="s">
         <v>210</v>
       </c>
-      <c r="O36" s="189" t="s">
+      <c r="O36" s="187" t="s">
         <v>209</v>
       </c>
       <c r="P36" s="201" t="s">
@@ -7425,7 +7525,7 @@
       <c r="T36" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="U36" s="190" t="s">
+      <c r="U36" s="188" t="s">
         <v>125</v>
       </c>
     </row>
@@ -7436,16 +7536,16 @@
         <v>121</v>
       </c>
       <c r="D37" s="200"/>
-      <c r="E37" s="192"/>
-      <c r="F37" s="192"/>
+      <c r="E37" s="190"/>
+      <c r="F37" s="190"/>
       <c r="G37" s="200"/>
       <c r="H37" s="200"/>
       <c r="I37" s="203"/>
       <c r="J37" s="205"/>
       <c r="K37" s="205"/>
-      <c r="L37" s="196"/>
-      <c r="M37" s="193"/>
-      <c r="N37" s="193"/>
+      <c r="L37" s="194"/>
+      <c r="M37" s="191"/>
+      <c r="N37" s="191"/>
       <c r="O37" s="197"/>
       <c r="P37" s="62" t="s">
         <v>126</v>
@@ -8131,14 +8231,14 @@
     <mergeCell ref="I36:I37"/>
     <mergeCell ref="J36:J37"/>
     <mergeCell ref="K36:K37"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
     <mergeCell ref="O36:O37"/>
     <mergeCell ref="M36:M37"/>
     <mergeCell ref="R36:S36"/>
     <mergeCell ref="A28:G28"/>
     <mergeCell ref="B29:G29"/>
     <mergeCell ref="L36:L37"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="B32:G32"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="A16:G16"/>
@@ -8149,9 +8249,9 @@
     <mergeCell ref="A22:G22"/>
     <mergeCell ref="B23:G23"/>
     <mergeCell ref="B30:G30"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="B32:G32"/>
     <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="3">

</xml_diff>

<commit_message>
0.0.11: Extends of telegramProcess is ignored on micronaut serverType.
</commit_message>
<xml_diff>
--- a/meta/api/BlancoApiPostSample.xlsx
+++ b/meta/api/BlancoApiPostSample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorKt/meta/api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5767E96-1D66-E04B-9E2E-EF918699AA93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{989AA31C-E664-744D-A6AA-D40E97D888E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="180" yWindow="680" windowWidth="21420" windowHeight="17540" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="225">
   <si>
     <t>項目名</t>
     <rPh sb="0" eb="3">
@@ -2356,6 +2356,24 @@
     </rPh>
     <rPh sb="52" eb="54">
       <t xml:space="preserve">ムシサレマス。 </t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ApiBase</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>blanco.sample.util</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>※ serverTypeがmicronautの場合は無視します。</t>
+    <rPh sb="23" eb="25">
+      <t xml:space="preserve">バアイハ </t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t xml:space="preserve">ムシ </t>
     </rPh>
     <phoneticPr fontId="2"/>
   </si>
@@ -3597,146 +3615,152 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3766,37 +3790,31 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="62" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="63" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="65" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="62" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="63" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="65" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4346,7 +4364,7 @@
   <dimension ref="A1:O70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15:E15"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -4389,137 +4407,137 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="138" t="s">
+      <c r="A5" s="184" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="138"/>
-      <c r="C5" s="138"/>
-      <c r="D5" s="138"/>
-      <c r="E5" s="138"/>
+      <c r="B5" s="184"/>
+      <c r="C5" s="184"/>
+      <c r="D5" s="184"/>
+      <c r="E5" s="184"/>
       <c r="F5" s="55"/>
       <c r="G5" s="55"/>
       <c r="H5" s="95"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="142" t="s">
+      <c r="A6" s="181" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="143"/>
-      <c r="C6" s="144"/>
-      <c r="D6" s="139" t="s">
+      <c r="B6" s="182"/>
+      <c r="C6" s="183"/>
+      <c r="D6" s="180" t="s">
         <v>197</v>
       </c>
-      <c r="E6" s="139"/>
+      <c r="E6" s="180"/>
       <c r="F6" s="55"/>
       <c r="G6" s="55"/>
       <c r="H6" s="95"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="138" t="s">
+      <c r="A7" s="184" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="138"/>
-      <c r="C7" s="138"/>
-      <c r="D7" s="139" t="s">
+      <c r="B7" s="184"/>
+      <c r="C7" s="184"/>
+      <c r="D7" s="180" t="s">
         <v>166</v>
       </c>
-      <c r="E7" s="139"/>
+      <c r="E7" s="180"/>
       <c r="F7" s="55"/>
       <c r="G7" s="55"/>
       <c r="H7" s="95"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="138" t="s">
+      <c r="A8" s="184" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="138"/>
-      <c r="C8" s="138"/>
-      <c r="D8" s="139" t="s">
+      <c r="B8" s="184"/>
+      <c r="C8" s="184"/>
+      <c r="D8" s="180" t="s">
         <v>162</v>
       </c>
-      <c r="E8" s="139"/>
+      <c r="E8" s="180"/>
       <c r="F8" s="95"/>
       <c r="G8" s="95"/>
       <c r="H8" s="95"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="138" t="s">
+      <c r="A9" s="184" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="138"/>
-      <c r="C9" s="138"/>
-      <c r="D9" s="139" t="s">
+      <c r="B9" s="184"/>
+      <c r="C9" s="184"/>
+      <c r="D9" s="180" t="s">
         <v>100</v>
       </c>
-      <c r="E9" s="139"/>
+      <c r="E9" s="180"/>
       <c r="F9" s="95"/>
       <c r="G9" s="95"/>
       <c r="H9" s="95"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="138" t="s">
+      <c r="A10" s="184" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="138"/>
-      <c r="C10" s="138"/>
-      <c r="D10" s="139"/>
-      <c r="E10" s="139"/>
+      <c r="B10" s="184"/>
+      <c r="C10" s="184"/>
+      <c r="D10" s="180"/>
+      <c r="E10" s="180"/>
       <c r="F10" s="95"/>
       <c r="G10" s="95"/>
       <c r="H10" s="95"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="138" t="s">
+      <c r="A11" s="184" t="s">
         <v>99</v>
       </c>
-      <c r="B11" s="138"/>
-      <c r="C11" s="138"/>
-      <c r="D11" s="139" t="s">
+      <c r="B11" s="184"/>
+      <c r="C11" s="184"/>
+      <c r="D11" s="180" t="s">
         <v>163</v>
       </c>
-      <c r="E11" s="139"/>
+      <c r="E11" s="180"/>
       <c r="F11" s="95"/>
       <c r="G11" s="95"/>
       <c r="H11" s="95"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="145" t="s">
+      <c r="A12" s="143" t="s">
         <v>174</v>
       </c>
-      <c r="B12" s="145"/>
-      <c r="C12" s="145"/>
-      <c r="D12" s="140" t="s">
+      <c r="B12" s="143"/>
+      <c r="C12" s="143"/>
+      <c r="D12" s="164" t="s">
         <v>175</v>
       </c>
-      <c r="E12" s="140"/>
+      <c r="E12" s="164"/>
       <c r="F12" s="95" t="s">
         <v>176</v>
       </c>
       <c r="G12" s="54"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="145" t="s">
+      <c r="A13" s="143" t="s">
         <v>213</v>
       </c>
-      <c r="B13" s="145"/>
-      <c r="C13" s="145"/>
-      <c r="D13" s="140" t="s">
+      <c r="B13" s="143"/>
+      <c r="C13" s="143"/>
+      <c r="D13" s="164" t="s">
         <v>211</v>
       </c>
-      <c r="E13" s="140"/>
+      <c r="E13" s="164"/>
       <c r="F13" s="95" t="s">
         <v>212</v>
       </c>
       <c r="G13" s="54"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="145" t="s">
+      <c r="A14" s="143" t="s">
         <v>177</v>
       </c>
-      <c r="B14" s="145"/>
-      <c r="C14" s="145"/>
-      <c r="D14" s="141"/>
-      <c r="E14" s="140"/>
+      <c r="B14" s="143"/>
+      <c r="C14" s="143"/>
+      <c r="D14" s="163"/>
+      <c r="E14" s="164"/>
       <c r="F14" s="54" t="s">
         <v>198</v>
       </c>
@@ -4527,15 +4545,15 @@
       <c r="H14" s="95"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="145" t="s">
+      <c r="A15" s="143" t="s">
         <v>218</v>
       </c>
-      <c r="B15" s="145"/>
-      <c r="C15" s="145"/>
-      <c r="D15" s="141" t="s">
+      <c r="B15" s="143"/>
+      <c r="C15" s="143"/>
+      <c r="D15" s="163" t="s">
         <v>216</v>
       </c>
-      <c r="E15" s="140"/>
+      <c r="E15" s="164"/>
       <c r="F15" s="54" t="s">
         <v>221</v>
       </c>
@@ -4543,13 +4561,13 @@
       <c r="H15" s="95"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="145" t="s">
+      <c r="A16" s="143" t="s">
         <v>217</v>
       </c>
-      <c r="B16" s="145"/>
-      <c r="C16" s="145"/>
-      <c r="D16" s="141"/>
-      <c r="E16" s="140"/>
+      <c r="B16" s="143"/>
+      <c r="C16" s="143"/>
+      <c r="D16" s="163"/>
+      <c r="E16" s="164"/>
       <c r="F16" s="54" t="s">
         <v>220</v>
       </c>
@@ -4557,13 +4575,13 @@
       <c r="H16" s="95"/>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="145" t="s">
+      <c r="A17" s="143" t="s">
         <v>215</v>
       </c>
-      <c r="B17" s="145"/>
-      <c r="C17" s="145"/>
-      <c r="D17" s="141"/>
-      <c r="E17" s="140"/>
+      <c r="B17" s="143"/>
+      <c r="C17" s="143"/>
+      <c r="D17" s="163"/>
+      <c r="E17" s="164"/>
       <c r="F17" s="54" t="s">
         <v>214</v>
       </c>
@@ -4571,19 +4589,19 @@
       <c r="H17" s="95"/>
     </row>
     <row r="18" spans="1:15">
-      <c r="A18" s="182" t="s">
+      <c r="A18" s="160" t="s">
         <v>143</v>
       </c>
-      <c r="B18" s="183"/>
-      <c r="C18" s="184"/>
+      <c r="B18" s="161"/>
+      <c r="C18" s="162"/>
       <c r="D18" s="114"/>
     </row>
     <row r="19" spans="1:15">
-      <c r="A19" s="168" t="s">
+      <c r="A19" s="144" t="s">
         <v>179</v>
       </c>
-      <c r="B19" s="169"/>
-      <c r="C19" s="170"/>
+      <c r="B19" s="145"/>
+      <c r="C19" s="146"/>
       <c r="D19" s="100" t="s">
         <v>141</v>
       </c>
@@ -4603,15 +4621,18 @@
       <c r="B20" s="6"/>
     </row>
     <row r="21" spans="1:15">
-      <c r="A21" s="179" t="s">
+      <c r="A21" s="157" t="s">
         <v>188</v>
       </c>
-      <c r="B21" s="180"/>
-      <c r="C21" s="180"/>
-      <c r="D21" s="180"/>
-      <c r="E21" s="180"/>
-      <c r="F21" s="180"/>
-      <c r="G21" s="181"/>
+      <c r="B21" s="158"/>
+      <c r="C21" s="158"/>
+      <c r="D21" s="158"/>
+      <c r="E21" s="158"/>
+      <c r="F21" s="158"/>
+      <c r="G21" s="159"/>
+      <c r="H21" s="1" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="22" spans="1:15">
       <c r="A22" s="101" t="s">
@@ -4619,7 +4640,9 @@
       </c>
       <c r="B22" s="110"/>
       <c r="C22" s="102"/>
-      <c r="D22" s="103"/>
+      <c r="D22" s="103" t="s">
+        <v>222</v>
+      </c>
       <c r="E22" s="103"/>
       <c r="F22" s="103"/>
       <c r="G22" s="104"/>
@@ -4635,7 +4658,9 @@
       </c>
       <c r="B23" s="113"/>
       <c r="C23" s="99"/>
-      <c r="D23" s="96"/>
+      <c r="D23" s="96" t="s">
+        <v>223</v>
+      </c>
       <c r="E23" s="97"/>
       <c r="F23" s="97"/>
       <c r="G23" s="106"/>
@@ -4655,28 +4680,28 @@
       <c r="C25"/>
     </row>
     <row r="26" spans="1:15">
-      <c r="A26" s="178" t="s">
+      <c r="A26" s="156" t="s">
         <v>189</v>
       </c>
-      <c r="B26" s="178"/>
-      <c r="C26" s="178"/>
-      <c r="D26" s="178"/>
-      <c r="E26" s="178"/>
-      <c r="F26" s="178"/>
-      <c r="G26" s="178"/>
+      <c r="B26" s="156"/>
+      <c r="C26" s="156"/>
+      <c r="D26" s="156"/>
+      <c r="E26" s="156"/>
+      <c r="F26" s="156"/>
+      <c r="G26" s="156"/>
     </row>
     <row r="27" spans="1:15">
       <c r="A27" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B27" s="172" t="s">
+      <c r="B27" s="150" t="s">
         <v>183</v>
       </c>
-      <c r="C27" s="173"/>
-      <c r="D27" s="173"/>
-      <c r="E27" s="173"/>
-      <c r="F27" s="173"/>
-      <c r="G27" s="174"/>
+      <c r="C27" s="151"/>
+      <c r="D27" s="151"/>
+      <c r="E27" s="151"/>
+      <c r="F27" s="151"/>
+      <c r="G27" s="152"/>
       <c r="H27" s="105"/>
       <c r="I27" s="105"/>
       <c r="J27" s="105"/>
@@ -4687,12 +4712,12 @@
     </row>
     <row r="28" spans="1:15">
       <c r="A28" s="116"/>
-      <c r="B28" s="156"/>
-      <c r="C28" s="156"/>
-      <c r="D28" s="156"/>
-      <c r="E28" s="156"/>
-      <c r="F28" s="156"/>
-      <c r="G28" s="156"/>
+      <c r="B28" s="167"/>
+      <c r="C28" s="167"/>
+      <c r="D28" s="167"/>
+      <c r="E28" s="167"/>
+      <c r="F28" s="167"/>
+      <c r="G28" s="167"/>
       <c r="H28" s="112"/>
       <c r="I28" s="112"/>
       <c r="J28" s="112"/>
@@ -4703,12 +4728,12 @@
     </row>
     <row r="29" spans="1:15">
       <c r="A29" s="117"/>
-      <c r="B29" s="158"/>
-      <c r="C29" s="158"/>
-      <c r="D29" s="158"/>
-      <c r="E29" s="158"/>
-      <c r="F29" s="158"/>
-      <c r="G29" s="158"/>
+      <c r="B29" s="168"/>
+      <c r="C29" s="168"/>
+      <c r="D29" s="168"/>
+      <c r="E29" s="168"/>
+      <c r="F29" s="168"/>
+      <c r="G29" s="168"/>
       <c r="H29" s="112"/>
       <c r="I29" s="112"/>
       <c r="J29" s="112"/>
@@ -4719,12 +4744,12 @@
     </row>
     <row r="30" spans="1:15">
       <c r="A30" s="118"/>
-      <c r="B30" s="160"/>
-      <c r="C30" s="160"/>
-      <c r="D30" s="160"/>
-      <c r="E30" s="160"/>
-      <c r="F30" s="160"/>
-      <c r="G30" s="160"/>
+      <c r="B30" s="169"/>
+      <c r="C30" s="169"/>
+      <c r="D30" s="169"/>
+      <c r="E30" s="169"/>
+      <c r="F30" s="169"/>
+      <c r="G30" s="169"/>
       <c r="H30" s="112"/>
       <c r="I30" s="112"/>
       <c r="J30" s="112"/>
@@ -4737,28 +4762,28 @@
       <c r="C31"/>
     </row>
     <row r="32" spans="1:15">
-      <c r="A32" s="175" t="s">
+      <c r="A32" s="153" t="s">
         <v>190</v>
       </c>
-      <c r="B32" s="176"/>
-      <c r="C32" s="176"/>
-      <c r="D32" s="176"/>
-      <c r="E32" s="176"/>
-      <c r="F32" s="176"/>
-      <c r="G32" s="177"/>
+      <c r="B32" s="154"/>
+      <c r="C32" s="154"/>
+      <c r="D32" s="154"/>
+      <c r="E32" s="154"/>
+      <c r="F32" s="154"/>
+      <c r="G32" s="155"/>
     </row>
     <row r="33" spans="1:15">
       <c r="A33" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B33" s="152" t="s">
+      <c r="B33" s="173" t="s">
         <v>184</v>
       </c>
-      <c r="C33" s="152"/>
-      <c r="D33" s="152"/>
-      <c r="E33" s="152"/>
-      <c r="F33" s="152"/>
-      <c r="G33" s="152"/>
+      <c r="C33" s="173"/>
+      <c r="D33" s="173"/>
+      <c r="E33" s="173"/>
+      <c r="F33" s="173"/>
+      <c r="G33" s="173"/>
       <c r="H33" s="105"/>
       <c r="I33" s="105"/>
       <c r="J33" s="105"/>
@@ -4771,14 +4796,14 @@
       <c r="A34" s="116">
         <v>1</v>
       </c>
-      <c r="B34" s="153" t="s">
+      <c r="B34" s="174" t="s">
         <v>219</v>
       </c>
-      <c r="C34" s="153"/>
-      <c r="D34" s="153"/>
-      <c r="E34" s="153"/>
-      <c r="F34" s="153"/>
-      <c r="G34" s="153"/>
+      <c r="C34" s="174"/>
+      <c r="D34" s="174"/>
+      <c r="E34" s="174"/>
+      <c r="F34" s="174"/>
+      <c r="G34" s="174"/>
       <c r="H34" s="112"/>
       <c r="I34" s="112"/>
       <c r="J34" s="112"/>
@@ -4789,12 +4814,12 @@
     </row>
     <row r="35" spans="1:15">
       <c r="A35" s="117"/>
-      <c r="B35" s="154"/>
-      <c r="C35" s="154"/>
-      <c r="D35" s="154"/>
-      <c r="E35" s="154"/>
-      <c r="F35" s="154"/>
-      <c r="G35" s="154"/>
+      <c r="B35" s="175"/>
+      <c r="C35" s="175"/>
+      <c r="D35" s="175"/>
+      <c r="E35" s="175"/>
+      <c r="F35" s="175"/>
+      <c r="G35" s="175"/>
       <c r="H35" s="112"/>
       <c r="I35" s="112"/>
       <c r="J35" s="112"/>
@@ -4805,12 +4830,12 @@
     </row>
     <row r="36" spans="1:15">
       <c r="A36" s="118"/>
-      <c r="B36" s="155"/>
-      <c r="C36" s="155"/>
-      <c r="D36" s="155"/>
-      <c r="E36" s="155"/>
-      <c r="F36" s="155"/>
-      <c r="G36" s="155"/>
+      <c r="B36" s="176"/>
+      <c r="C36" s="176"/>
+      <c r="D36" s="176"/>
+      <c r="E36" s="176"/>
+      <c r="F36" s="176"/>
+      <c r="G36" s="176"/>
       <c r="H36" s="112"/>
       <c r="I36" s="112"/>
       <c r="J36" s="112"/>
@@ -4835,28 +4860,28 @@
       <c r="M37"/>
     </row>
     <row r="38" spans="1:15">
-      <c r="A38" s="175" t="s">
+      <c r="A38" s="153" t="s">
         <v>191</v>
       </c>
-      <c r="B38" s="176"/>
-      <c r="C38" s="176"/>
-      <c r="D38" s="176"/>
-      <c r="E38" s="176"/>
-      <c r="F38" s="176"/>
-      <c r="G38" s="177"/>
+      <c r="B38" s="154"/>
+      <c r="C38" s="154"/>
+      <c r="D38" s="154"/>
+      <c r="E38" s="154"/>
+      <c r="F38" s="154"/>
+      <c r="G38" s="155"/>
     </row>
     <row r="39" spans="1:15">
       <c r="A39" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B39" s="152" t="s">
+      <c r="B39" s="173" t="s">
         <v>186</v>
       </c>
-      <c r="C39" s="152"/>
-      <c r="D39" s="152"/>
-      <c r="E39" s="152"/>
-      <c r="F39" s="152"/>
-      <c r="G39" s="152"/>
+      <c r="C39" s="173"/>
+      <c r="D39" s="173"/>
+      <c r="E39" s="173"/>
+      <c r="F39" s="173"/>
+      <c r="G39" s="173"/>
       <c r="H39" s="105"/>
       <c r="I39" s="105"/>
       <c r="J39" s="105"/>
@@ -4867,12 +4892,12 @@
     </row>
     <row r="40" spans="1:15">
       <c r="A40" s="116"/>
-      <c r="B40" s="156"/>
-      <c r="C40" s="156"/>
-      <c r="D40" s="156"/>
-      <c r="E40" s="156"/>
-      <c r="F40" s="156"/>
-      <c r="G40" s="157"/>
+      <c r="B40" s="167"/>
+      <c r="C40" s="167"/>
+      <c r="D40" s="167"/>
+      <c r="E40" s="167"/>
+      <c r="F40" s="167"/>
+      <c r="G40" s="177"/>
       <c r="H40" s="112"/>
       <c r="I40" s="112"/>
       <c r="J40" s="112"/>
@@ -4883,12 +4908,12 @@
     </row>
     <row r="41" spans="1:15">
       <c r="A41" s="117"/>
-      <c r="B41" s="158"/>
-      <c r="C41" s="158"/>
-      <c r="D41" s="158"/>
-      <c r="E41" s="158"/>
-      <c r="F41" s="158"/>
-      <c r="G41" s="159"/>
+      <c r="B41" s="168"/>
+      <c r="C41" s="168"/>
+      <c r="D41" s="168"/>
+      <c r="E41" s="168"/>
+      <c r="F41" s="168"/>
+      <c r="G41" s="178"/>
       <c r="H41" s="112"/>
       <c r="I41" s="112"/>
       <c r="J41" s="112"/>
@@ -4899,12 +4924,12 @@
     </row>
     <row r="42" spans="1:15">
       <c r="A42" s="118"/>
-      <c r="B42" s="160"/>
-      <c r="C42" s="160"/>
-      <c r="D42" s="160"/>
-      <c r="E42" s="160"/>
-      <c r="F42" s="160"/>
-      <c r="G42" s="161"/>
+      <c r="B42" s="169"/>
+      <c r="C42" s="169"/>
+      <c r="D42" s="169"/>
+      <c r="E42" s="169"/>
+      <c r="F42" s="169"/>
+      <c r="G42" s="179"/>
       <c r="H42" s="112"/>
       <c r="I42" s="112"/>
       <c r="J42" s="112"/>
@@ -4939,254 +4964,267 @@
       <c r="F44" s="5"/>
     </row>
     <row r="45" spans="1:15">
-      <c r="A45" s="165" t="s">
+      <c r="A45" s="140" t="s">
         <v>65</v>
       </c>
-      <c r="B45" s="171"/>
-      <c r="C45" s="165" t="s">
+      <c r="B45" s="147"/>
+      <c r="C45" s="140" t="s">
         <v>66</v>
       </c>
-      <c r="D45" s="166"/>
-      <c r="E45" s="167"/>
+      <c r="D45" s="141"/>
+      <c r="E45" s="142"/>
       <c r="F45" s="29" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:15">
-      <c r="A46" s="162"/>
-      <c r="B46" s="164"/>
-      <c r="C46" s="162"/>
-      <c r="D46" s="163"/>
-      <c r="E46" s="164"/>
+      <c r="A46" s="148"/>
+      <c r="B46" s="149"/>
+      <c r="C46" s="148"/>
+      <c r="D46" s="170"/>
+      <c r="E46" s="149"/>
       <c r="F46" s="49"/>
     </row>
     <row r="47" spans="1:15">
-      <c r="A47" s="146"/>
-      <c r="B47" s="148"/>
-      <c r="C47" s="146"/>
-      <c r="D47" s="147"/>
-      <c r="E47" s="148"/>
+      <c r="A47" s="138"/>
+      <c r="B47" s="139"/>
+      <c r="C47" s="138"/>
+      <c r="D47" s="171"/>
+      <c r="E47" s="139"/>
       <c r="F47" s="49"/>
     </row>
     <row r="48" spans="1:15">
-      <c r="A48" s="146"/>
-      <c r="B48" s="148"/>
-      <c r="C48" s="146"/>
-      <c r="D48" s="147"/>
-      <c r="E48" s="148"/>
+      <c r="A48" s="138"/>
+      <c r="B48" s="139"/>
+      <c r="C48" s="138"/>
+      <c r="D48" s="171"/>
+      <c r="E48" s="139"/>
       <c r="F48" s="49"/>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="146"/>
-      <c r="B49" s="148"/>
-      <c r="C49" s="146"/>
-      <c r="D49" s="147"/>
-      <c r="E49" s="148"/>
+      <c r="A49" s="138"/>
+      <c r="B49" s="139"/>
+      <c r="C49" s="138"/>
+      <c r="D49" s="171"/>
+      <c r="E49" s="139"/>
       <c r="F49" s="49"/>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="146"/>
-      <c r="B50" s="148"/>
-      <c r="C50" s="146"/>
-      <c r="D50" s="147"/>
-      <c r="E50" s="148"/>
+      <c r="A50" s="138"/>
+      <c r="B50" s="139"/>
+      <c r="C50" s="138"/>
+      <c r="D50" s="171"/>
+      <c r="E50" s="139"/>
       <c r="F50" s="49"/>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="146"/>
-      <c r="B51" s="148"/>
-      <c r="C51" s="146"/>
-      <c r="D51" s="147"/>
-      <c r="E51" s="148"/>
+      <c r="A51" s="138"/>
+      <c r="B51" s="139"/>
+      <c r="C51" s="138"/>
+      <c r="D51" s="171"/>
+      <c r="E51" s="139"/>
       <c r="F51" s="49"/>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="146"/>
-      <c r="B52" s="148"/>
-      <c r="C52" s="146"/>
-      <c r="D52" s="147"/>
-      <c r="E52" s="148"/>
+      <c r="A52" s="138"/>
+      <c r="B52" s="139"/>
+      <c r="C52" s="138"/>
+      <c r="D52" s="171"/>
+      <c r="E52" s="139"/>
       <c r="F52" s="49"/>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="146"/>
-      <c r="B53" s="148"/>
-      <c r="C53" s="146"/>
-      <c r="D53" s="147"/>
-      <c r="E53" s="148"/>
+      <c r="A53" s="138"/>
+      <c r="B53" s="139"/>
+      <c r="C53" s="138"/>
+      <c r="D53" s="171"/>
+      <c r="E53" s="139"/>
       <c r="F53" s="49"/>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="146"/>
-      <c r="B54" s="148"/>
-      <c r="C54" s="146"/>
-      <c r="D54" s="147"/>
-      <c r="E54" s="148"/>
+      <c r="A54" s="138"/>
+      <c r="B54" s="139"/>
+      <c r="C54" s="138"/>
+      <c r="D54" s="171"/>
+      <c r="E54" s="139"/>
       <c r="F54" s="49"/>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="146"/>
-      <c r="B55" s="148"/>
-      <c r="C55" s="146"/>
-      <c r="D55" s="147"/>
-      <c r="E55" s="148"/>
+      <c r="A55" s="138"/>
+      <c r="B55" s="139"/>
+      <c r="C55" s="138"/>
+      <c r="D55" s="171"/>
+      <c r="E55" s="139"/>
       <c r="F55" s="49"/>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="146"/>
-      <c r="B56" s="148"/>
-      <c r="C56" s="146"/>
-      <c r="D56" s="147"/>
-      <c r="E56" s="148"/>
+      <c r="A56" s="138"/>
+      <c r="B56" s="139"/>
+      <c r="C56" s="138"/>
+      <c r="D56" s="171"/>
+      <c r="E56" s="139"/>
       <c r="F56" s="49"/>
     </row>
     <row r="57" spans="1:6">
-      <c r="A57" s="146"/>
-      <c r="B57" s="148"/>
-      <c r="C57" s="146"/>
-      <c r="D57" s="147"/>
-      <c r="E57" s="148"/>
+      <c r="A57" s="138"/>
+      <c r="B57" s="139"/>
+      <c r="C57" s="138"/>
+      <c r="D57" s="171"/>
+      <c r="E57" s="139"/>
       <c r="F57" s="49"/>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="146"/>
-      <c r="B58" s="148"/>
-      <c r="C58" s="146"/>
-      <c r="D58" s="147"/>
-      <c r="E58" s="148"/>
+      <c r="A58" s="138"/>
+      <c r="B58" s="139"/>
+      <c r="C58" s="138"/>
+      <c r="D58" s="171"/>
+      <c r="E58" s="139"/>
       <c r="F58" s="49"/>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="146"/>
-      <c r="B59" s="148"/>
-      <c r="C59" s="146"/>
-      <c r="D59" s="147"/>
-      <c r="E59" s="148"/>
+      <c r="A59" s="138"/>
+      <c r="B59" s="139"/>
+      <c r="C59" s="138"/>
+      <c r="D59" s="171"/>
+      <c r="E59" s="139"/>
       <c r="F59" s="49"/>
     </row>
     <row r="60" spans="1:6">
-      <c r="A60" s="146"/>
-      <c r="B60" s="148"/>
-      <c r="C60" s="146"/>
-      <c r="D60" s="147"/>
-      <c r="E60" s="148"/>
+      <c r="A60" s="138"/>
+      <c r="B60" s="139"/>
+      <c r="C60" s="138"/>
+      <c r="D60" s="171"/>
+      <c r="E60" s="139"/>
       <c r="F60" s="49"/>
     </row>
     <row r="61" spans="1:6">
-      <c r="A61" s="146"/>
-      <c r="B61" s="148"/>
-      <c r="C61" s="146"/>
-      <c r="D61" s="147"/>
-      <c r="E61" s="148"/>
+      <c r="A61" s="138"/>
+      <c r="B61" s="139"/>
+      <c r="C61" s="138"/>
+      <c r="D61" s="171"/>
+      <c r="E61" s="139"/>
       <c r="F61" s="49"/>
     </row>
     <row r="62" spans="1:6">
-      <c r="A62" s="146"/>
-      <c r="B62" s="148"/>
-      <c r="C62" s="146"/>
-      <c r="D62" s="147"/>
-      <c r="E62" s="148"/>
+      <c r="A62" s="138"/>
+      <c r="B62" s="139"/>
+      <c r="C62" s="138"/>
+      <c r="D62" s="171"/>
+      <c r="E62" s="139"/>
       <c r="F62" s="49"/>
     </row>
     <row r="63" spans="1:6">
-      <c r="A63" s="146"/>
-      <c r="B63" s="148"/>
-      <c r="C63" s="146"/>
-      <c r="D63" s="147"/>
-      <c r="E63" s="148"/>
+      <c r="A63" s="138"/>
+      <c r="B63" s="139"/>
+      <c r="C63" s="138"/>
+      <c r="D63" s="171"/>
+      <c r="E63" s="139"/>
       <c r="F63" s="49"/>
     </row>
     <row r="64" spans="1:6">
-      <c r="A64" s="146"/>
-      <c r="B64" s="148"/>
-      <c r="C64" s="146"/>
-      <c r="D64" s="147"/>
-      <c r="E64" s="148"/>
+      <c r="A64" s="138"/>
+      <c r="B64" s="139"/>
+      <c r="C64" s="138"/>
+      <c r="D64" s="171"/>
+      <c r="E64" s="139"/>
       <c r="F64" s="49"/>
     </row>
     <row r="65" spans="1:6">
-      <c r="A65" s="146"/>
-      <c r="B65" s="148"/>
-      <c r="C65" s="146"/>
-      <c r="D65" s="147"/>
-      <c r="E65" s="148"/>
+      <c r="A65" s="138"/>
+      <c r="B65" s="139"/>
+      <c r="C65" s="138"/>
+      <c r="D65" s="171"/>
+      <c r="E65" s="139"/>
       <c r="F65" s="49"/>
     </row>
     <row r="66" spans="1:6">
-      <c r="A66" s="146"/>
-      <c r="B66" s="148"/>
-      <c r="C66" s="146"/>
-      <c r="D66" s="147"/>
-      <c r="E66" s="148"/>
+      <c r="A66" s="138"/>
+      <c r="B66" s="139"/>
+      <c r="C66" s="138"/>
+      <c r="D66" s="171"/>
+      <c r="E66" s="139"/>
       <c r="F66" s="49"/>
     </row>
     <row r="67" spans="1:6">
-      <c r="A67" s="146"/>
-      <c r="B67" s="148"/>
-      <c r="C67" s="146"/>
-      <c r="D67" s="147"/>
-      <c r="E67" s="148"/>
+      <c r="A67" s="138"/>
+      <c r="B67" s="139"/>
+      <c r="C67" s="138"/>
+      <c r="D67" s="171"/>
+      <c r="E67" s="139"/>
       <c r="F67" s="49"/>
     </row>
     <row r="68" spans="1:6">
-      <c r="A68" s="146"/>
-      <c r="B68" s="148"/>
-      <c r="C68" s="146"/>
-      <c r="D68" s="147"/>
-      <c r="E68" s="148"/>
+      <c r="A68" s="138"/>
+      <c r="B68" s="139"/>
+      <c r="C68" s="138"/>
+      <c r="D68" s="171"/>
+      <c r="E68" s="139"/>
       <c r="F68" s="49"/>
     </row>
     <row r="69" spans="1:6">
-      <c r="A69" s="146"/>
-      <c r="B69" s="148"/>
-      <c r="C69" s="146"/>
-      <c r="D69" s="147"/>
-      <c r="E69" s="148"/>
+      <c r="A69" s="138"/>
+      <c r="B69" s="139"/>
+      <c r="C69" s="138"/>
+      <c r="D69" s="171"/>
+      <c r="E69" s="139"/>
       <c r="F69" s="49"/>
     </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="149"/>
-      <c r="B70" s="151"/>
-      <c r="C70" s="149"/>
-      <c r="D70" s="150"/>
-      <c r="E70" s="151"/>
+      <c r="A70" s="165"/>
+      <c r="B70" s="166"/>
+      <c r="C70" s="165"/>
+      <c r="D70" s="172"/>
+      <c r="E70" s="166"/>
       <c r="F70" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="95">
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="A38:G38"/>
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C70:E70"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="B41:G41"/>
+    <mergeCell ref="B42:G42"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C58:E58"/>
     <mergeCell ref="A67:B67"/>
     <mergeCell ref="A68:B68"/>
     <mergeCell ref="A69:B69"/>
@@ -5203,52 +5241,39 @@
     <mergeCell ref="C52:E52"/>
     <mergeCell ref="C53:E53"/>
     <mergeCell ref="A62:B62"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="C70:E70"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B36:G36"/>
-    <mergeCell ref="B39:G39"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="B41:G41"/>
-    <mergeCell ref="B42:G42"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="A38:G38"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="1">
@@ -5506,10 +5531,10 @@
         <v>174</v>
       </c>
       <c r="B15" s="122"/>
-      <c r="C15" s="140" t="s">
+      <c r="C15" s="164" t="s">
         <v>175</v>
       </c>
-      <c r="D15" s="140"/>
+      <c r="D15" s="164"/>
       <c r="E15" s="95" t="s">
         <v>176</v>
       </c>
@@ -5524,8 +5549,8 @@
         <v>177</v>
       </c>
       <c r="B16" s="122"/>
-      <c r="C16" s="141"/>
-      <c r="D16" s="140"/>
+      <c r="C16" s="163"/>
+      <c r="D16" s="164"/>
       <c r="E16" s="55" t="s">
         <v>199</v>
       </c>
@@ -5575,15 +5600,15 @@
       <c r="L18"/>
     </row>
     <row r="19" spans="1:22">
-      <c r="A19" s="178" t="s">
+      <c r="A19" s="156" t="s">
         <v>192</v>
       </c>
-      <c r="B19" s="178"/>
-      <c r="C19" s="178"/>
-      <c r="D19" s="178"/>
-      <c r="E19" s="178"/>
-      <c r="F19" s="178"/>
-      <c r="G19" s="178"/>
+      <c r="B19" s="156"/>
+      <c r="C19" s="156"/>
+      <c r="D19" s="156"/>
+      <c r="E19" s="156"/>
+      <c r="F19" s="156"/>
+      <c r="G19" s="156"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -5593,14 +5618,14 @@
       <c r="A20" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B20" s="172" t="s">
+      <c r="B20" s="150" t="s">
         <v>183</v>
       </c>
-      <c r="C20" s="173"/>
-      <c r="D20" s="173"/>
-      <c r="E20" s="173"/>
-      <c r="F20" s="173"/>
-      <c r="G20" s="174"/>
+      <c r="C20" s="151"/>
+      <c r="D20" s="151"/>
+      <c r="E20" s="151"/>
+      <c r="F20" s="151"/>
+      <c r="G20" s="152"/>
       <c r="H20" s="105"/>
       <c r="I20"/>
       <c r="J20"/>
@@ -5618,12 +5643,12 @@
     </row>
     <row r="21" spans="1:22">
       <c r="A21" s="116"/>
-      <c r="B21" s="156"/>
-      <c r="C21" s="156"/>
-      <c r="D21" s="156"/>
-      <c r="E21" s="156"/>
-      <c r="F21" s="156"/>
-      <c r="G21" s="156"/>
+      <c r="B21" s="167"/>
+      <c r="C21" s="167"/>
+      <c r="D21" s="167"/>
+      <c r="E21" s="167"/>
+      <c r="F21" s="167"/>
+      <c r="G21" s="167"/>
       <c r="H21" s="112"/>
       <c r="I21"/>
       <c r="J21"/>
@@ -5641,12 +5666,12 @@
     </row>
     <row r="22" spans="1:22">
       <c r="A22" s="117"/>
-      <c r="B22" s="158"/>
-      <c r="C22" s="158"/>
-      <c r="D22" s="158"/>
-      <c r="E22" s="158"/>
-      <c r="F22" s="158"/>
-      <c r="G22" s="158"/>
+      <c r="B22" s="168"/>
+      <c r="C22" s="168"/>
+      <c r="D22" s="168"/>
+      <c r="E22" s="168"/>
+      <c r="F22" s="168"/>
+      <c r="G22" s="168"/>
       <c r="H22" s="112"/>
       <c r="I22"/>
       <c r="J22"/>
@@ -5664,12 +5689,12 @@
     </row>
     <row r="23" spans="1:22">
       <c r="A23" s="118"/>
-      <c r="B23" s="160"/>
-      <c r="C23" s="160"/>
-      <c r="D23" s="160"/>
-      <c r="E23" s="160"/>
-      <c r="F23" s="160"/>
-      <c r="G23" s="160"/>
+      <c r="B23" s="169"/>
+      <c r="C23" s="169"/>
+      <c r="D23" s="169"/>
+      <c r="E23" s="169"/>
+      <c r="F23" s="169"/>
+      <c r="G23" s="169"/>
       <c r="H23" s="112"/>
       <c r="M23" s="112"/>
       <c r="N23" s="112"/>
@@ -5689,15 +5714,15 @@
       <c r="L24" s="105"/>
     </row>
     <row r="25" spans="1:22">
-      <c r="A25" s="175" t="s">
+      <c r="A25" s="153" t="s">
         <v>193</v>
       </c>
-      <c r="B25" s="176"/>
-      <c r="C25" s="176"/>
-      <c r="D25" s="176"/>
-      <c r="E25" s="176"/>
-      <c r="F25" s="176"/>
-      <c r="G25" s="177"/>
+      <c r="B25" s="154"/>
+      <c r="C25" s="154"/>
+      <c r="D25" s="154"/>
+      <c r="E25" s="154"/>
+      <c r="F25" s="154"/>
+      <c r="G25" s="155"/>
       <c r="I25" s="105"/>
       <c r="J25" s="105"/>
       <c r="K25" s="105"/>
@@ -5707,14 +5732,14 @@
       <c r="A26" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="152" t="s">
+      <c r="B26" s="173" t="s">
         <v>184</v>
       </c>
-      <c r="C26" s="152"/>
-      <c r="D26" s="152"/>
-      <c r="E26" s="152"/>
-      <c r="F26" s="152"/>
-      <c r="G26" s="152"/>
+      <c r="C26" s="173"/>
+      <c r="D26" s="173"/>
+      <c r="E26" s="173"/>
+      <c r="F26" s="173"/>
+      <c r="G26" s="173"/>
       <c r="H26" s="105"/>
       <c r="I26" s="105"/>
       <c r="J26" s="105"/>
@@ -5732,12 +5757,12 @@
     </row>
     <row r="27" spans="1:22">
       <c r="A27" s="116"/>
-      <c r="B27" s="153"/>
-      <c r="C27" s="153"/>
-      <c r="D27" s="153"/>
-      <c r="E27" s="153"/>
-      <c r="F27" s="153"/>
-      <c r="G27" s="153"/>
+      <c r="B27" s="174"/>
+      <c r="C27" s="174"/>
+      <c r="D27" s="174"/>
+      <c r="E27" s="174"/>
+      <c r="F27" s="174"/>
+      <c r="G27" s="174"/>
       <c r="H27" s="112"/>
       <c r="I27"/>
       <c r="J27"/>
@@ -5755,12 +5780,12 @@
     </row>
     <row r="28" spans="1:22">
       <c r="A28" s="117"/>
-      <c r="B28" s="154"/>
-      <c r="C28" s="154"/>
-      <c r="D28" s="154"/>
-      <c r="E28" s="154"/>
-      <c r="F28" s="154"/>
-      <c r="G28" s="154"/>
+      <c r="B28" s="175"/>
+      <c r="C28" s="175"/>
+      <c r="D28" s="175"/>
+      <c r="E28" s="175"/>
+      <c r="F28" s="175"/>
+      <c r="G28" s="175"/>
       <c r="H28" s="112"/>
       <c r="M28" s="112"/>
       <c r="N28" s="112"/>
@@ -5774,12 +5799,12 @@
     </row>
     <row r="29" spans="1:22">
       <c r="A29" s="118"/>
-      <c r="B29" s="155"/>
-      <c r="C29" s="155"/>
-      <c r="D29" s="155"/>
-      <c r="E29" s="155"/>
-      <c r="F29" s="155"/>
-      <c r="G29" s="155"/>
+      <c r="B29" s="176"/>
+      <c r="C29" s="176"/>
+      <c r="D29" s="176"/>
+      <c r="E29" s="176"/>
+      <c r="F29" s="176"/>
+      <c r="G29" s="176"/>
       <c r="H29" s="112"/>
       <c r="I29" s="105"/>
       <c r="J29" s="105"/>
@@ -5818,15 +5843,15 @@
       <c r="T30"/>
     </row>
     <row r="31" spans="1:22">
-      <c r="A31" s="175" t="s">
+      <c r="A31" s="153" t="s">
         <v>194</v>
       </c>
-      <c r="B31" s="176"/>
-      <c r="C31" s="176"/>
-      <c r="D31" s="176"/>
-      <c r="E31" s="176"/>
-      <c r="F31" s="176"/>
-      <c r="G31" s="177"/>
+      <c r="B31" s="154"/>
+      <c r="C31" s="154"/>
+      <c r="D31" s="154"/>
+      <c r="E31" s="154"/>
+      <c r="F31" s="154"/>
+      <c r="G31" s="155"/>
       <c r="I31" s="112"/>
       <c r="J31" s="112"/>
       <c r="K31" s="112"/>
@@ -5836,14 +5861,14 @@
       <c r="A32" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B32" s="152" t="s">
+      <c r="B32" s="173" t="s">
         <v>186</v>
       </c>
-      <c r="C32" s="152"/>
-      <c r="D32" s="152"/>
-      <c r="E32" s="152"/>
-      <c r="F32" s="152"/>
-      <c r="G32" s="152"/>
+      <c r="C32" s="173"/>
+      <c r="D32" s="173"/>
+      <c r="E32" s="173"/>
+      <c r="F32" s="173"/>
+      <c r="G32" s="173"/>
       <c r="H32" s="105"/>
       <c r="I32" s="112"/>
       <c r="J32" s="112"/>
@@ -5861,12 +5886,12 @@
     </row>
     <row r="33" spans="1:26">
       <c r="A33" s="116"/>
-      <c r="B33" s="156"/>
-      <c r="C33" s="156"/>
-      <c r="D33" s="156"/>
-      <c r="E33" s="156"/>
-      <c r="F33" s="156"/>
-      <c r="G33" s="157"/>
+      <c r="B33" s="167"/>
+      <c r="C33" s="167"/>
+      <c r="D33" s="167"/>
+      <c r="E33" s="167"/>
+      <c r="F33" s="167"/>
+      <c r="G33" s="177"/>
       <c r="H33" s="112"/>
       <c r="I33"/>
       <c r="J33"/>
@@ -5884,12 +5909,12 @@
     </row>
     <row r="34" spans="1:26">
       <c r="A34" s="117"/>
-      <c r="B34" s="158"/>
-      <c r="C34" s="158"/>
-      <c r="D34" s="158"/>
-      <c r="E34" s="158"/>
-      <c r="F34" s="158"/>
-      <c r="G34" s="159"/>
+      <c r="B34" s="168"/>
+      <c r="C34" s="168"/>
+      <c r="D34" s="168"/>
+      <c r="E34" s="168"/>
+      <c r="F34" s="168"/>
+      <c r="G34" s="178"/>
       <c r="H34" s="112"/>
       <c r="M34" s="112"/>
       <c r="N34" s="112"/>
@@ -5903,12 +5928,12 @@
     </row>
     <row r="35" spans="1:26">
       <c r="A35" s="118"/>
-      <c r="B35" s="160"/>
-      <c r="C35" s="160"/>
-      <c r="D35" s="160"/>
-      <c r="E35" s="160"/>
-      <c r="F35" s="160"/>
-      <c r="G35" s="161"/>
+      <c r="B35" s="169"/>
+      <c r="C35" s="169"/>
+      <c r="D35" s="169"/>
+      <c r="E35" s="169"/>
+      <c r="F35" s="169"/>
+      <c r="G35" s="179"/>
       <c r="H35" s="112"/>
       <c r="M35" s="112"/>
       <c r="N35" s="112"/>
@@ -5972,82 +5997,82 @@
       <c r="Z38" s="39"/>
     </row>
     <row r="39" spans="1:26">
-      <c r="A39" s="185" t="s">
+      <c r="A39" s="187" t="s">
         <v>69</v>
       </c>
-      <c r="B39" s="185" t="s">
+      <c r="B39" s="187" t="s">
         <v>0</v>
       </c>
-      <c r="C39" s="187" t="s">
+      <c r="C39" s="189" t="s">
         <v>1</v>
       </c>
-      <c r="D39" s="185" t="s">
+      <c r="D39" s="187" t="s">
         <v>2</v>
       </c>
-      <c r="E39" s="188" t="s">
+      <c r="E39" s="190" t="s">
         <v>161</v>
       </c>
-      <c r="F39" s="188" t="s">
+      <c r="F39" s="190" t="s">
         <v>177</v>
       </c>
-      <c r="G39" s="185" t="s">
+      <c r="G39" s="187" t="s">
         <v>13</v>
       </c>
-      <c r="H39" s="185" t="s">
+      <c r="H39" s="187" t="s">
         <v>116</v>
       </c>
-      <c r="I39" s="192" t="s">
+      <c r="I39" s="194" t="s">
         <v>201</v>
       </c>
-      <c r="J39" s="192" t="s">
+      <c r="J39" s="194" t="s">
         <v>202</v>
       </c>
-      <c r="K39" s="192" t="s">
+      <c r="K39" s="194" t="s">
         <v>203</v>
       </c>
-      <c r="L39" s="193" t="s">
+      <c r="L39" s="195" t="s">
         <v>204</v>
       </c>
-      <c r="M39" s="185" t="s">
+      <c r="M39" s="187" t="s">
         <v>195</v>
       </c>
-      <c r="N39" s="185" t="s">
+      <c r="N39" s="187" t="s">
         <v>210</v>
       </c>
-      <c r="O39" s="187" t="s">
+      <c r="O39" s="189" t="s">
         <v>209</v>
       </c>
-      <c r="P39" s="195" t="s">
+      <c r="P39" s="185" t="s">
         <v>71</v>
       </c>
-      <c r="Q39" s="196"/>
-      <c r="R39" s="195" t="s">
+      <c r="Q39" s="186"/>
+      <c r="R39" s="185" t="s">
         <v>17</v>
       </c>
-      <c r="S39" s="196"/>
+      <c r="S39" s="186"/>
       <c r="T39" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="U39" s="185" t="s">
+      <c r="U39" s="187" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:26">
-      <c r="A40" s="186"/>
-      <c r="B40" s="186"/>
-      <c r="C40" s="186"/>
-      <c r="D40" s="186"/>
-      <c r="E40" s="189"/>
-      <c r="F40" s="190"/>
-      <c r="G40" s="186"/>
-      <c r="H40" s="186"/>
-      <c r="I40" s="192"/>
-      <c r="J40" s="192"/>
-      <c r="K40" s="192"/>
-      <c r="L40" s="194"/>
-      <c r="M40" s="191"/>
-      <c r="N40" s="191"/>
-      <c r="O40" s="191"/>
+      <c r="A40" s="188"/>
+      <c r="B40" s="188"/>
+      <c r="C40" s="188"/>
+      <c r="D40" s="188"/>
+      <c r="E40" s="191"/>
+      <c r="F40" s="192"/>
+      <c r="G40" s="188"/>
+      <c r="H40" s="188"/>
+      <c r="I40" s="194"/>
+      <c r="J40" s="194"/>
+      <c r="K40" s="194"/>
+      <c r="L40" s="196"/>
+      <c r="M40" s="193"/>
+      <c r="N40" s="193"/>
+      <c r="O40" s="193"/>
       <c r="P40" s="29" t="s">
         <v>75</v>
       </c>
@@ -6063,7 +6088,7 @@
       <c r="T40" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="U40" s="186"/>
+      <c r="U40" s="188"/>
     </row>
     <row r="41" spans="1:26">
       <c r="A41" s="7">
@@ -6737,20 +6762,9 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="P39:Q39"/>
-    <mergeCell ref="R39:S39"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="A25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="B32:G32"/>
     <mergeCell ref="U39:U40"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="B39:B40"/>
@@ -6767,11 +6781,22 @@
     <mergeCell ref="L39:L40"/>
     <mergeCell ref="N39:N40"/>
     <mergeCell ref="M39:M40"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="P39:Q39"/>
+    <mergeCell ref="R39:S39"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B35:G35"/>
     <mergeCell ref="B27:G27"/>
     <mergeCell ref="B28:G28"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="A31:G31"/>
-    <mergeCell ref="B32:G32"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations disablePrompts="1" count="3">
@@ -7004,10 +7029,10 @@
         <v>174</v>
       </c>
       <c r="B12" s="122"/>
-      <c r="C12" s="140" t="s">
+      <c r="C12" s="164" t="s">
         <v>175</v>
       </c>
-      <c r="D12" s="140"/>
+      <c r="D12" s="164"/>
       <c r="E12" s="95" t="s">
         <v>176</v>
       </c>
@@ -7022,10 +7047,10 @@
         <v>177</v>
       </c>
       <c r="B13" s="122"/>
-      <c r="C13" s="140" t="s">
+      <c r="C13" s="164" t="s">
         <v>178</v>
       </c>
-      <c r="D13" s="140"/>
+      <c r="D13" s="164"/>
       <c r="E13" s="55"/>
       <c r="F13" s="55"/>
       <c r="G13" s="54"/>
@@ -7065,15 +7090,15 @@
       <c r="L15"/>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="178" t="s">
+      <c r="A16" s="156" t="s">
         <v>192</v>
       </c>
-      <c r="B16" s="178"/>
-      <c r="C16" s="178"/>
-      <c r="D16" s="178"/>
-      <c r="E16" s="178"/>
-      <c r="F16" s="178"/>
-      <c r="G16" s="178"/>
+      <c r="B16" s="156"/>
+      <c r="C16" s="156"/>
+      <c r="D16" s="156"/>
+      <c r="E16" s="156"/>
+      <c r="F16" s="156"/>
+      <c r="G16" s="156"/>
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16"/>
@@ -7084,14 +7109,14 @@
       <c r="A17" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B17" s="172" t="s">
+      <c r="B17" s="150" t="s">
         <v>183</v>
       </c>
-      <c r="C17" s="173"/>
-      <c r="D17" s="173"/>
-      <c r="E17" s="173"/>
-      <c r="F17" s="173"/>
-      <c r="G17" s="174"/>
+      <c r="C17" s="151"/>
+      <c r="D17" s="151"/>
+      <c r="E17" s="151"/>
+      <c r="F17" s="151"/>
+      <c r="G17" s="152"/>
       <c r="H17" s="105"/>
       <c r="I17"/>
       <c r="J17"/>
@@ -7107,12 +7132,12 @@
     </row>
     <row r="18" spans="1:22">
       <c r="A18" s="116"/>
-      <c r="B18" s="156"/>
-      <c r="C18" s="156"/>
-      <c r="D18" s="156"/>
-      <c r="E18" s="156"/>
-      <c r="F18" s="156"/>
-      <c r="G18" s="156"/>
+      <c r="B18" s="167"/>
+      <c r="C18" s="167"/>
+      <c r="D18" s="167"/>
+      <c r="E18" s="167"/>
+      <c r="F18" s="167"/>
+      <c r="G18" s="167"/>
       <c r="H18" s="112"/>
       <c r="I18"/>
       <c r="J18"/>
@@ -7127,12 +7152,12 @@
     </row>
     <row r="19" spans="1:22">
       <c r="A19" s="117"/>
-      <c r="B19" s="158"/>
-      <c r="C19" s="158"/>
-      <c r="D19" s="158"/>
-      <c r="E19" s="158"/>
-      <c r="F19" s="158"/>
-      <c r="G19" s="158"/>
+      <c r="B19" s="168"/>
+      <c r="C19" s="168"/>
+      <c r="D19" s="168"/>
+      <c r="E19" s="168"/>
+      <c r="F19" s="168"/>
+      <c r="G19" s="168"/>
       <c r="H19" s="112"/>
       <c r="I19"/>
       <c r="J19"/>
@@ -7147,12 +7172,12 @@
     </row>
     <row r="20" spans="1:22">
       <c r="A20" s="118"/>
-      <c r="B20" s="160"/>
-      <c r="C20" s="160"/>
-      <c r="D20" s="160"/>
-      <c r="E20" s="160"/>
-      <c r="F20" s="160"/>
-      <c r="G20" s="160"/>
+      <c r="B20" s="169"/>
+      <c r="C20" s="169"/>
+      <c r="D20" s="169"/>
+      <c r="E20" s="169"/>
+      <c r="F20" s="169"/>
+      <c r="G20" s="169"/>
       <c r="H20" s="112"/>
       <c r="I20"/>
       <c r="J20"/>
@@ -7179,15 +7204,15 @@
       <c r="O21" s="112"/>
     </row>
     <row r="22" spans="1:22">
-      <c r="A22" s="175" t="s">
+      <c r="A22" s="153" t="s">
         <v>193</v>
       </c>
-      <c r="B22" s="176"/>
-      <c r="C22" s="176"/>
-      <c r="D22" s="176"/>
-      <c r="E22" s="176"/>
-      <c r="F22" s="176"/>
-      <c r="G22" s="177"/>
+      <c r="B22" s="154"/>
+      <c r="C22" s="154"/>
+      <c r="D22" s="154"/>
+      <c r="E22" s="154"/>
+      <c r="F22" s="154"/>
+      <c r="G22" s="155"/>
       <c r="I22"/>
       <c r="J22"/>
       <c r="K22"/>
@@ -7200,14 +7225,14 @@
       <c r="A23" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B23" s="152" t="s">
+      <c r="B23" s="173" t="s">
         <v>184</v>
       </c>
-      <c r="C23" s="152"/>
-      <c r="D23" s="152"/>
-      <c r="E23" s="152"/>
-      <c r="F23" s="152"/>
-      <c r="G23" s="152"/>
+      <c r="C23" s="173"/>
+      <c r="D23" s="173"/>
+      <c r="E23" s="173"/>
+      <c r="F23" s="173"/>
+      <c r="G23" s="173"/>
       <c r="H23" s="105"/>
       <c r="M23" s="112"/>
       <c r="N23" s="112"/>
@@ -7223,14 +7248,14 @@
       <c r="A24" s="116">
         <v>1</v>
       </c>
-      <c r="B24" s="153" t="s">
+      <c r="B24" s="174" t="s">
         <v>185</v>
       </c>
-      <c r="C24" s="153"/>
-      <c r="D24" s="153"/>
-      <c r="E24" s="153"/>
-      <c r="F24" s="153"/>
-      <c r="G24" s="153"/>
+      <c r="C24" s="174"/>
+      <c r="D24" s="174"/>
+      <c r="E24" s="174"/>
+      <c r="F24" s="174"/>
+      <c r="G24" s="174"/>
       <c r="H24" s="112"/>
       <c r="I24" s="105"/>
       <c r="J24" s="105"/>
@@ -7245,12 +7270,12 @@
     </row>
     <row r="25" spans="1:22">
       <c r="A25" s="117"/>
-      <c r="B25" s="154"/>
-      <c r="C25" s="154"/>
-      <c r="D25" s="154"/>
-      <c r="E25" s="154"/>
-      <c r="F25" s="154"/>
-      <c r="G25" s="154"/>
+      <c r="B25" s="175"/>
+      <c r="C25" s="175"/>
+      <c r="D25" s="175"/>
+      <c r="E25" s="175"/>
+      <c r="F25" s="175"/>
+      <c r="G25" s="175"/>
       <c r="H25" s="112"/>
       <c r="I25" s="105"/>
       <c r="J25" s="105"/>
@@ -7265,12 +7290,12 @@
     </row>
     <row r="26" spans="1:22">
       <c r="A26" s="118"/>
-      <c r="B26" s="155"/>
-      <c r="C26" s="155"/>
-      <c r="D26" s="155"/>
-      <c r="E26" s="155"/>
-      <c r="F26" s="155"/>
-      <c r="G26" s="155"/>
+      <c r="B26" s="176"/>
+      <c r="C26" s="176"/>
+      <c r="D26" s="176"/>
+      <c r="E26" s="176"/>
+      <c r="F26" s="176"/>
+      <c r="G26" s="176"/>
       <c r="H26" s="112"/>
       <c r="I26" s="105"/>
       <c r="J26" s="105"/>
@@ -7309,15 +7334,15 @@
       <c r="T27"/>
     </row>
     <row r="28" spans="1:22">
-      <c r="A28" s="175" t="s">
+      <c r="A28" s="153" t="s">
         <v>194</v>
       </c>
-      <c r="B28" s="176"/>
-      <c r="C28" s="176"/>
-      <c r="D28" s="176"/>
-      <c r="E28" s="176"/>
-      <c r="F28" s="176"/>
-      <c r="G28" s="177"/>
+      <c r="B28" s="154"/>
+      <c r="C28" s="154"/>
+      <c r="D28" s="154"/>
+      <c r="E28" s="154"/>
+      <c r="F28" s="154"/>
+      <c r="G28" s="155"/>
       <c r="M28" s="112"/>
       <c r="N28" s="112"/>
       <c r="O28" s="112"/>
@@ -7326,14 +7351,14 @@
       <c r="A29" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="152" t="s">
+      <c r="B29" s="173" t="s">
         <v>186</v>
       </c>
-      <c r="C29" s="152"/>
-      <c r="D29" s="152"/>
-      <c r="E29" s="152"/>
-      <c r="F29" s="152"/>
-      <c r="G29" s="152"/>
+      <c r="C29" s="173"/>
+      <c r="D29" s="173"/>
+      <c r="E29" s="173"/>
+      <c r="F29" s="173"/>
+      <c r="G29" s="173"/>
       <c r="H29" s="105"/>
       <c r="I29" s="105"/>
       <c r="J29" s="105"/>
@@ -7351,12 +7376,12 @@
     </row>
     <row r="30" spans="1:22">
       <c r="A30" s="116"/>
-      <c r="B30" s="156"/>
-      <c r="C30" s="156"/>
-      <c r="D30" s="156"/>
-      <c r="E30" s="156"/>
-      <c r="F30" s="156"/>
-      <c r="G30" s="157"/>
+      <c r="B30" s="167"/>
+      <c r="C30" s="167"/>
+      <c r="D30" s="167"/>
+      <c r="E30" s="167"/>
+      <c r="F30" s="167"/>
+      <c r="G30" s="177"/>
       <c r="H30" s="112"/>
       <c r="I30" s="112"/>
       <c r="J30" s="112"/>
@@ -7374,12 +7399,12 @@
     </row>
     <row r="31" spans="1:22">
       <c r="A31" s="117"/>
-      <c r="B31" s="158"/>
-      <c r="C31" s="158"/>
-      <c r="D31" s="158"/>
-      <c r="E31" s="158"/>
-      <c r="F31" s="158"/>
-      <c r="G31" s="159"/>
+      <c r="B31" s="168"/>
+      <c r="C31" s="168"/>
+      <c r="D31" s="168"/>
+      <c r="E31" s="168"/>
+      <c r="F31" s="168"/>
+      <c r="G31" s="178"/>
       <c r="H31" s="112"/>
       <c r="I31" s="112"/>
       <c r="J31" s="112"/>
@@ -7394,12 +7419,12 @@
     </row>
     <row r="32" spans="1:22">
       <c r="A32" s="118"/>
-      <c r="B32" s="160"/>
-      <c r="C32" s="160"/>
-      <c r="D32" s="160"/>
-      <c r="E32" s="160"/>
-      <c r="F32" s="160"/>
-      <c r="G32" s="161"/>
+      <c r="B32" s="169"/>
+      <c r="C32" s="169"/>
+      <c r="D32" s="169"/>
+      <c r="E32" s="169"/>
+      <c r="F32" s="169"/>
+      <c r="G32" s="179"/>
       <c r="H32" s="112"/>
       <c r="I32" s="112"/>
       <c r="J32" s="112"/>
@@ -7469,84 +7494,84 @@
       <c r="U35" s="58"/>
     </row>
     <row r="36" spans="1:21" ht="30" customHeight="1">
-      <c r="A36" s="188" t="s">
+      <c r="A36" s="190" t="s">
         <v>118</v>
       </c>
-      <c r="B36" s="188" t="s">
+      <c r="B36" s="190" t="s">
         <v>119</v>
       </c>
       <c r="C36" s="60" t="s">
         <v>120</v>
       </c>
-      <c r="D36" s="188" t="s">
+      <c r="D36" s="190" t="s">
         <v>101</v>
       </c>
-      <c r="E36" s="188" t="s">
+      <c r="E36" s="190" t="s">
         <v>161</v>
       </c>
-      <c r="F36" s="188" t="s">
+      <c r="F36" s="190" t="s">
         <v>177</v>
       </c>
-      <c r="G36" s="188" t="s">
+      <c r="G36" s="190" t="s">
         <v>140</v>
       </c>
-      <c r="H36" s="188" t="s">
+      <c r="H36" s="190" t="s">
         <v>139</v>
       </c>
-      <c r="I36" s="202" t="s">
+      <c r="I36" s="200" t="s">
         <v>201</v>
       </c>
-      <c r="J36" s="204" t="s">
+      <c r="J36" s="202" t="s">
         <v>202</v>
       </c>
-      <c r="K36" s="204" t="s">
+      <c r="K36" s="202" t="s">
         <v>203</v>
       </c>
-      <c r="L36" s="193" t="s">
+      <c r="L36" s="195" t="s">
         <v>204</v>
       </c>
-      <c r="M36" s="185" t="s">
+      <c r="M36" s="187" t="s">
         <v>195</v>
       </c>
-      <c r="N36" s="185" t="s">
+      <c r="N36" s="187" t="s">
         <v>210</v>
       </c>
-      <c r="O36" s="187" t="s">
+      <c r="O36" s="189" t="s">
         <v>209</v>
       </c>
-      <c r="P36" s="201" t="s">
+      <c r="P36" s="198" t="s">
         <v>122</v>
       </c>
       <c r="Q36" s="199"/>
-      <c r="R36" s="198" t="s">
+      <c r="R36" s="205" t="s">
         <v>123</v>
       </c>
       <c r="S36" s="199"/>
       <c r="T36" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="U36" s="188" t="s">
+      <c r="U36" s="190" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="37" spans="1:21" ht="15">
-      <c r="A37" s="200"/>
-      <c r="B37" s="200"/>
+      <c r="A37" s="197"/>
+      <c r="B37" s="197"/>
       <c r="C37" s="61" t="s">
         <v>121</v>
       </c>
-      <c r="D37" s="200"/>
-      <c r="E37" s="190"/>
-      <c r="F37" s="190"/>
-      <c r="G37" s="200"/>
-      <c r="H37" s="200"/>
-      <c r="I37" s="203"/>
-      <c r="J37" s="205"/>
-      <c r="K37" s="205"/>
-      <c r="L37" s="194"/>
-      <c r="M37" s="191"/>
-      <c r="N37" s="191"/>
-      <c r="O37" s="197"/>
+      <c r="D37" s="197"/>
+      <c r="E37" s="192"/>
+      <c r="F37" s="192"/>
+      <c r="G37" s="197"/>
+      <c r="H37" s="197"/>
+      <c r="I37" s="201"/>
+      <c r="J37" s="203"/>
+      <c r="K37" s="203"/>
+      <c r="L37" s="196"/>
+      <c r="M37" s="193"/>
+      <c r="N37" s="193"/>
+      <c r="O37" s="204"/>
       <c r="P37" s="62" t="s">
         <v>126</v>
       </c>
@@ -7562,7 +7587,7 @@
       <c r="T37" s="63" t="s">
         <v>130</v>
       </c>
-      <c r="U37" s="200"/>
+      <c r="U37" s="197"/>
     </row>
     <row r="38" spans="1:21">
       <c r="A38" s="64">
@@ -8218,6 +8243,24 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="A28:G28"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="L36:L37"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="B32:G32"/>
     <mergeCell ref="U36:U37"/>
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="B36:B37"/>
@@ -8234,24 +8277,6 @@
     <mergeCell ref="O36:O37"/>
     <mergeCell ref="M36:M37"/>
     <mergeCell ref="R36:S36"/>
-    <mergeCell ref="A28:G28"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="L36:L37"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="A22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="3">

</xml_diff>

<commit_message>
0.0.13: bufix: specific import statement is now available
</commit_message>
<xml_diff>
--- a/meta/api/BlancoApiPostSample.xlsx
+++ b/meta/api/BlancoApiPostSample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorKt/meta/api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{989AA31C-E664-744D-A6AA-D40E97D888E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC9C4D5-7EA9-0D40-9F87-47BF66A71240}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="680" windowWidth="21420" windowHeight="17540" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="180" yWindow="680" windowWidth="21420" windowHeight="17540" tabRatio="860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="process" sheetId="19" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="227">
   <si>
     <t>項目名</t>
     <rPh sb="0" eb="3">
@@ -2375,6 +2375,15 @@
     <rPh sb="26" eb="28">
       <t xml:space="preserve">ムシ </t>
     </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>@NotNull(message = "{E005}")
+@field:Valid</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>javax.validation.Valid</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -3360,7 +3369,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="206">
+  <cellXfs count="207">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -3615,12 +3624,87 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3630,9 +3714,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3645,12 +3726,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3689,78 +3764,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3790,6 +3793,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3816,6 +3825,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="60" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -4363,7 +4375,7 @@
   </sheetPr>
   <dimension ref="A1:O70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A30" workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
@@ -4407,137 +4419,137 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="184" t="s">
+      <c r="A5" s="138" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="184"/>
-      <c r="C5" s="184"/>
-      <c r="D5" s="184"/>
-      <c r="E5" s="184"/>
+      <c r="B5" s="138"/>
+      <c r="C5" s="138"/>
+      <c r="D5" s="138"/>
+      <c r="E5" s="138"/>
       <c r="F5" s="55"/>
       <c r="G5" s="55"/>
       <c r="H5" s="95"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="181" t="s">
+      <c r="A6" s="142" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="182"/>
-      <c r="C6" s="183"/>
-      <c r="D6" s="180" t="s">
+      <c r="B6" s="143"/>
+      <c r="C6" s="144"/>
+      <c r="D6" s="139" t="s">
         <v>197</v>
       </c>
-      <c r="E6" s="180"/>
+      <c r="E6" s="139"/>
       <c r="F6" s="55"/>
       <c r="G6" s="55"/>
       <c r="H6" s="95"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="184" t="s">
+      <c r="A7" s="138" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="184"/>
-      <c r="C7" s="184"/>
-      <c r="D7" s="180" t="s">
+      <c r="B7" s="138"/>
+      <c r="C7" s="138"/>
+      <c r="D7" s="139" t="s">
         <v>166</v>
       </c>
-      <c r="E7" s="180"/>
+      <c r="E7" s="139"/>
       <c r="F7" s="55"/>
       <c r="G7" s="55"/>
       <c r="H7" s="95"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="184" t="s">
+      <c r="A8" s="138" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="184"/>
-      <c r="C8" s="184"/>
-      <c r="D8" s="180" t="s">
+      <c r="B8" s="138"/>
+      <c r="C8" s="138"/>
+      <c r="D8" s="139" t="s">
         <v>162</v>
       </c>
-      <c r="E8" s="180"/>
+      <c r="E8" s="139"/>
       <c r="F8" s="95"/>
       <c r="G8" s="95"/>
       <c r="H8" s="95"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="184" t="s">
+      <c r="A9" s="138" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="184"/>
-      <c r="C9" s="184"/>
-      <c r="D9" s="180" t="s">
+      <c r="B9" s="138"/>
+      <c r="C9" s="138"/>
+      <c r="D9" s="139" t="s">
         <v>100</v>
       </c>
-      <c r="E9" s="180"/>
+      <c r="E9" s="139"/>
       <c r="F9" s="95"/>
       <c r="G9" s="95"/>
       <c r="H9" s="95"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="184" t="s">
+      <c r="A10" s="138" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="184"/>
-      <c r="C10" s="184"/>
-      <c r="D10" s="180"/>
-      <c r="E10" s="180"/>
+      <c r="B10" s="138"/>
+      <c r="C10" s="138"/>
+      <c r="D10" s="139"/>
+      <c r="E10" s="139"/>
       <c r="F10" s="95"/>
       <c r="G10" s="95"/>
       <c r="H10" s="95"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="184" t="s">
+      <c r="A11" s="138" t="s">
         <v>99</v>
       </c>
-      <c r="B11" s="184"/>
-      <c r="C11" s="184"/>
-      <c r="D11" s="180" t="s">
+      <c r="B11" s="138"/>
+      <c r="C11" s="138"/>
+      <c r="D11" s="139" t="s">
         <v>163</v>
       </c>
-      <c r="E11" s="180"/>
+      <c r="E11" s="139"/>
       <c r="F11" s="95"/>
       <c r="G11" s="95"/>
       <c r="H11" s="95"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="143" t="s">
+      <c r="A12" s="145" t="s">
         <v>174</v>
       </c>
-      <c r="B12" s="143"/>
-      <c r="C12" s="143"/>
-      <c r="D12" s="164" t="s">
+      <c r="B12" s="145"/>
+      <c r="C12" s="145"/>
+      <c r="D12" s="140" t="s">
         <v>175</v>
       </c>
-      <c r="E12" s="164"/>
+      <c r="E12" s="140"/>
       <c r="F12" s="95" t="s">
         <v>176</v>
       </c>
       <c r="G12" s="54"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="143" t="s">
+      <c r="A13" s="145" t="s">
         <v>213</v>
       </c>
-      <c r="B13" s="143"/>
-      <c r="C13" s="143"/>
-      <c r="D13" s="164" t="s">
+      <c r="B13" s="145"/>
+      <c r="C13" s="145"/>
+      <c r="D13" s="140" t="s">
         <v>211</v>
       </c>
-      <c r="E13" s="164"/>
+      <c r="E13" s="140"/>
       <c r="F13" s="95" t="s">
         <v>212</v>
       </c>
       <c r="G13" s="54"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="143" t="s">
+      <c r="A14" s="145" t="s">
         <v>177</v>
       </c>
-      <c r="B14" s="143"/>
-      <c r="C14" s="143"/>
-      <c r="D14" s="163"/>
-      <c r="E14" s="164"/>
+      <c r="B14" s="145"/>
+      <c r="C14" s="145"/>
+      <c r="D14" s="141"/>
+      <c r="E14" s="140"/>
       <c r="F14" s="54" t="s">
         <v>198</v>
       </c>
@@ -4545,15 +4557,15 @@
       <c r="H14" s="95"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="143" t="s">
+      <c r="A15" s="145" t="s">
         <v>218</v>
       </c>
-      <c r="B15" s="143"/>
-      <c r="C15" s="143"/>
-      <c r="D15" s="163" t="s">
+      <c r="B15" s="145"/>
+      <c r="C15" s="145"/>
+      <c r="D15" s="141" t="s">
         <v>216</v>
       </c>
-      <c r="E15" s="164"/>
+      <c r="E15" s="140"/>
       <c r="F15" s="54" t="s">
         <v>221</v>
       </c>
@@ -4561,13 +4573,13 @@
       <c r="H15" s="95"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="143" t="s">
+      <c r="A16" s="145" t="s">
         <v>217</v>
       </c>
-      <c r="B16" s="143"/>
-      <c r="C16" s="143"/>
-      <c r="D16" s="163"/>
-      <c r="E16" s="164"/>
+      <c r="B16" s="145"/>
+      <c r="C16" s="145"/>
+      <c r="D16" s="141"/>
+      <c r="E16" s="140"/>
       <c r="F16" s="54" t="s">
         <v>220</v>
       </c>
@@ -4575,13 +4587,13 @@
       <c r="H16" s="95"/>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="143" t="s">
+      <c r="A17" s="145" t="s">
         <v>215</v>
       </c>
-      <c r="B17" s="143"/>
-      <c r="C17" s="143"/>
-      <c r="D17" s="163"/>
-      <c r="E17" s="164"/>
+      <c r="B17" s="145"/>
+      <c r="C17" s="145"/>
+      <c r="D17" s="141"/>
+      <c r="E17" s="140"/>
       <c r="F17" s="54" t="s">
         <v>214</v>
       </c>
@@ -4589,19 +4601,19 @@
       <c r="H17" s="95"/>
     </row>
     <row r="18" spans="1:15">
-      <c r="A18" s="160" t="s">
+      <c r="A18" s="182" t="s">
         <v>143</v>
       </c>
-      <c r="B18" s="161"/>
-      <c r="C18" s="162"/>
+      <c r="B18" s="183"/>
+      <c r="C18" s="184"/>
       <c r="D18" s="114"/>
     </row>
     <row r="19" spans="1:15">
-      <c r="A19" s="144" t="s">
+      <c r="A19" s="168" t="s">
         <v>179</v>
       </c>
-      <c r="B19" s="145"/>
-      <c r="C19" s="146"/>
+      <c r="B19" s="169"/>
+      <c r="C19" s="170"/>
       <c r="D19" s="100" t="s">
         <v>141</v>
       </c>
@@ -4621,15 +4633,15 @@
       <c r="B20" s="6"/>
     </row>
     <row r="21" spans="1:15">
-      <c r="A21" s="157" t="s">
+      <c r="A21" s="179" t="s">
         <v>188</v>
       </c>
-      <c r="B21" s="158"/>
-      <c r="C21" s="158"/>
-      <c r="D21" s="158"/>
-      <c r="E21" s="158"/>
-      <c r="F21" s="158"/>
-      <c r="G21" s="159"/>
+      <c r="B21" s="180"/>
+      <c r="C21" s="180"/>
+      <c r="D21" s="180"/>
+      <c r="E21" s="180"/>
+      <c r="F21" s="180"/>
+      <c r="G21" s="181"/>
       <c r="H21" s="1" t="s">
         <v>224</v>
       </c>
@@ -4680,28 +4692,28 @@
       <c r="C25"/>
     </row>
     <row r="26" spans="1:15">
-      <c r="A26" s="156" t="s">
+      <c r="A26" s="178" t="s">
         <v>189</v>
       </c>
-      <c r="B26" s="156"/>
-      <c r="C26" s="156"/>
-      <c r="D26" s="156"/>
-      <c r="E26" s="156"/>
-      <c r="F26" s="156"/>
-      <c r="G26" s="156"/>
+      <c r="B26" s="178"/>
+      <c r="C26" s="178"/>
+      <c r="D26" s="178"/>
+      <c r="E26" s="178"/>
+      <c r="F26" s="178"/>
+      <c r="G26" s="178"/>
     </row>
     <row r="27" spans="1:15">
       <c r="A27" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B27" s="150" t="s">
+      <c r="B27" s="172" t="s">
         <v>183</v>
       </c>
-      <c r="C27" s="151"/>
-      <c r="D27" s="151"/>
-      <c r="E27" s="151"/>
-      <c r="F27" s="151"/>
-      <c r="G27" s="152"/>
+      <c r="C27" s="173"/>
+      <c r="D27" s="173"/>
+      <c r="E27" s="173"/>
+      <c r="F27" s="173"/>
+      <c r="G27" s="174"/>
       <c r="H27" s="105"/>
       <c r="I27" s="105"/>
       <c r="J27" s="105"/>
@@ -4712,12 +4724,12 @@
     </row>
     <row r="28" spans="1:15">
       <c r="A28" s="116"/>
-      <c r="B28" s="167"/>
-      <c r="C28" s="167"/>
-      <c r="D28" s="167"/>
-      <c r="E28" s="167"/>
-      <c r="F28" s="167"/>
-      <c r="G28" s="167"/>
+      <c r="B28" s="156"/>
+      <c r="C28" s="156"/>
+      <c r="D28" s="156"/>
+      <c r="E28" s="156"/>
+      <c r="F28" s="156"/>
+      <c r="G28" s="156"/>
       <c r="H28" s="112"/>
       <c r="I28" s="112"/>
       <c r="J28" s="112"/>
@@ -4728,12 +4740,12 @@
     </row>
     <row r="29" spans="1:15">
       <c r="A29" s="117"/>
-      <c r="B29" s="168"/>
-      <c r="C29" s="168"/>
-      <c r="D29" s="168"/>
-      <c r="E29" s="168"/>
-      <c r="F29" s="168"/>
-      <c r="G29" s="168"/>
+      <c r="B29" s="158"/>
+      <c r="C29" s="158"/>
+      <c r="D29" s="158"/>
+      <c r="E29" s="158"/>
+      <c r="F29" s="158"/>
+      <c r="G29" s="158"/>
       <c r="H29" s="112"/>
       <c r="I29" s="112"/>
       <c r="J29" s="112"/>
@@ -4744,12 +4756,12 @@
     </row>
     <row r="30" spans="1:15">
       <c r="A30" s="118"/>
-      <c r="B30" s="169"/>
-      <c r="C30" s="169"/>
-      <c r="D30" s="169"/>
-      <c r="E30" s="169"/>
-      <c r="F30" s="169"/>
-      <c r="G30" s="169"/>
+      <c r="B30" s="160"/>
+      <c r="C30" s="160"/>
+      <c r="D30" s="160"/>
+      <c r="E30" s="160"/>
+      <c r="F30" s="160"/>
+      <c r="G30" s="160"/>
       <c r="H30" s="112"/>
       <c r="I30" s="112"/>
       <c r="J30" s="112"/>
@@ -4762,28 +4774,28 @@
       <c r="C31"/>
     </row>
     <row r="32" spans="1:15">
-      <c r="A32" s="153" t="s">
+      <c r="A32" s="175" t="s">
         <v>190</v>
       </c>
-      <c r="B32" s="154"/>
-      <c r="C32" s="154"/>
-      <c r="D32" s="154"/>
-      <c r="E32" s="154"/>
-      <c r="F32" s="154"/>
-      <c r="G32" s="155"/>
+      <c r="B32" s="176"/>
+      <c r="C32" s="176"/>
+      <c r="D32" s="176"/>
+      <c r="E32" s="176"/>
+      <c r="F32" s="176"/>
+      <c r="G32" s="177"/>
     </row>
     <row r="33" spans="1:15">
       <c r="A33" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B33" s="173" t="s">
+      <c r="B33" s="152" t="s">
         <v>184</v>
       </c>
-      <c r="C33" s="173"/>
-      <c r="D33" s="173"/>
-      <c r="E33" s="173"/>
-      <c r="F33" s="173"/>
-      <c r="G33" s="173"/>
+      <c r="C33" s="152"/>
+      <c r="D33" s="152"/>
+      <c r="E33" s="152"/>
+      <c r="F33" s="152"/>
+      <c r="G33" s="152"/>
       <c r="H33" s="105"/>
       <c r="I33" s="105"/>
       <c r="J33" s="105"/>
@@ -4796,14 +4808,14 @@
       <c r="A34" s="116">
         <v>1</v>
       </c>
-      <c r="B34" s="174" t="s">
+      <c r="B34" s="153" t="s">
         <v>219</v>
       </c>
-      <c r="C34" s="174"/>
-      <c r="D34" s="174"/>
-      <c r="E34" s="174"/>
-      <c r="F34" s="174"/>
-      <c r="G34" s="174"/>
+      <c r="C34" s="153"/>
+      <c r="D34" s="153"/>
+      <c r="E34" s="153"/>
+      <c r="F34" s="153"/>
+      <c r="G34" s="153"/>
       <c r="H34" s="112"/>
       <c r="I34" s="112"/>
       <c r="J34" s="112"/>
@@ -4814,12 +4826,12 @@
     </row>
     <row r="35" spans="1:15">
       <c r="A35" s="117"/>
-      <c r="B35" s="175"/>
-      <c r="C35" s="175"/>
-      <c r="D35" s="175"/>
-      <c r="E35" s="175"/>
-      <c r="F35" s="175"/>
-      <c r="G35" s="175"/>
+      <c r="B35" s="154"/>
+      <c r="C35" s="154"/>
+      <c r="D35" s="154"/>
+      <c r="E35" s="154"/>
+      <c r="F35" s="154"/>
+      <c r="G35" s="154"/>
       <c r="H35" s="112"/>
       <c r="I35" s="112"/>
       <c r="J35" s="112"/>
@@ -4830,12 +4842,12 @@
     </row>
     <row r="36" spans="1:15">
       <c r="A36" s="118"/>
-      <c r="B36" s="176"/>
-      <c r="C36" s="176"/>
-      <c r="D36" s="176"/>
-      <c r="E36" s="176"/>
-      <c r="F36" s="176"/>
-      <c r="G36" s="176"/>
+      <c r="B36" s="155"/>
+      <c r="C36" s="155"/>
+      <c r="D36" s="155"/>
+      <c r="E36" s="155"/>
+      <c r="F36" s="155"/>
+      <c r="G36" s="155"/>
       <c r="H36" s="112"/>
       <c r="I36" s="112"/>
       <c r="J36" s="112"/>
@@ -4860,28 +4872,28 @@
       <c r="M37"/>
     </row>
     <row r="38" spans="1:15">
-      <c r="A38" s="153" t="s">
+      <c r="A38" s="175" t="s">
         <v>191</v>
       </c>
-      <c r="B38" s="154"/>
-      <c r="C38" s="154"/>
-      <c r="D38" s="154"/>
-      <c r="E38" s="154"/>
-      <c r="F38" s="154"/>
-      <c r="G38" s="155"/>
+      <c r="B38" s="176"/>
+      <c r="C38" s="176"/>
+      <c r="D38" s="176"/>
+      <c r="E38" s="176"/>
+      <c r="F38" s="176"/>
+      <c r="G38" s="177"/>
     </row>
     <row r="39" spans="1:15">
       <c r="A39" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B39" s="173" t="s">
+      <c r="B39" s="152" t="s">
         <v>186</v>
       </c>
-      <c r="C39" s="173"/>
-      <c r="D39" s="173"/>
-      <c r="E39" s="173"/>
-      <c r="F39" s="173"/>
-      <c r="G39" s="173"/>
+      <c r="C39" s="152"/>
+      <c r="D39" s="152"/>
+      <c r="E39" s="152"/>
+      <c r="F39" s="152"/>
+      <c r="G39" s="152"/>
       <c r="H39" s="105"/>
       <c r="I39" s="105"/>
       <c r="J39" s="105"/>
@@ -4892,12 +4904,12 @@
     </row>
     <row r="40" spans="1:15">
       <c r="A40" s="116"/>
-      <c r="B40" s="167"/>
-      <c r="C40" s="167"/>
-      <c r="D40" s="167"/>
-      <c r="E40" s="167"/>
-      <c r="F40" s="167"/>
-      <c r="G40" s="177"/>
+      <c r="B40" s="156"/>
+      <c r="C40" s="156"/>
+      <c r="D40" s="156"/>
+      <c r="E40" s="156"/>
+      <c r="F40" s="156"/>
+      <c r="G40" s="157"/>
       <c r="H40" s="112"/>
       <c r="I40" s="112"/>
       <c r="J40" s="112"/>
@@ -4908,12 +4920,12 @@
     </row>
     <row r="41" spans="1:15">
       <c r="A41" s="117"/>
-      <c r="B41" s="168"/>
-      <c r="C41" s="168"/>
-      <c r="D41" s="168"/>
-      <c r="E41" s="168"/>
-      <c r="F41" s="168"/>
-      <c r="G41" s="178"/>
+      <c r="B41" s="158"/>
+      <c r="C41" s="158"/>
+      <c r="D41" s="158"/>
+      <c r="E41" s="158"/>
+      <c r="F41" s="158"/>
+      <c r="G41" s="159"/>
       <c r="H41" s="112"/>
       <c r="I41" s="112"/>
       <c r="J41" s="112"/>
@@ -4924,12 +4936,12 @@
     </row>
     <row r="42" spans="1:15">
       <c r="A42" s="118"/>
-      <c r="B42" s="169"/>
-      <c r="C42" s="169"/>
-      <c r="D42" s="169"/>
-      <c r="E42" s="169"/>
-      <c r="F42" s="169"/>
-      <c r="G42" s="179"/>
+      <c r="B42" s="160"/>
+      <c r="C42" s="160"/>
+      <c r="D42" s="160"/>
+      <c r="E42" s="160"/>
+      <c r="F42" s="160"/>
+      <c r="G42" s="161"/>
       <c r="H42" s="112"/>
       <c r="I42" s="112"/>
       <c r="J42" s="112"/>
@@ -4964,226 +4976,295 @@
       <c r="F44" s="5"/>
     </row>
     <row r="45" spans="1:15">
-      <c r="A45" s="140" t="s">
+      <c r="A45" s="165" t="s">
         <v>65</v>
       </c>
-      <c r="B45" s="147"/>
-      <c r="C45" s="140" t="s">
+      <c r="B45" s="171"/>
+      <c r="C45" s="165" t="s">
         <v>66</v>
       </c>
-      <c r="D45" s="141"/>
-      <c r="E45" s="142"/>
+      <c r="D45" s="166"/>
+      <c r="E45" s="167"/>
       <c r="F45" s="29" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:15">
-      <c r="A46" s="148"/>
-      <c r="B46" s="149"/>
-      <c r="C46" s="148"/>
-      <c r="D46" s="170"/>
-      <c r="E46" s="149"/>
+      <c r="A46" s="162"/>
+      <c r="B46" s="164"/>
+      <c r="C46" s="162"/>
+      <c r="D46" s="163"/>
+      <c r="E46" s="164"/>
       <c r="F46" s="49"/>
     </row>
     <row r="47" spans="1:15">
-      <c r="A47" s="138"/>
-      <c r="B47" s="139"/>
-      <c r="C47" s="138"/>
-      <c r="D47" s="171"/>
-      <c r="E47" s="139"/>
+      <c r="A47" s="146"/>
+      <c r="B47" s="148"/>
+      <c r="C47" s="146"/>
+      <c r="D47" s="147"/>
+      <c r="E47" s="148"/>
       <c r="F47" s="49"/>
     </row>
     <row r="48" spans="1:15">
-      <c r="A48" s="138"/>
-      <c r="B48" s="139"/>
-      <c r="C48" s="138"/>
-      <c r="D48" s="171"/>
-      <c r="E48" s="139"/>
+      <c r="A48" s="146"/>
+      <c r="B48" s="148"/>
+      <c r="C48" s="146"/>
+      <c r="D48" s="147"/>
+      <c r="E48" s="148"/>
       <c r="F48" s="49"/>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="138"/>
-      <c r="B49" s="139"/>
-      <c r="C49" s="138"/>
-      <c r="D49" s="171"/>
-      <c r="E49" s="139"/>
+      <c r="A49" s="146"/>
+      <c r="B49" s="148"/>
+      <c r="C49" s="146"/>
+      <c r="D49" s="147"/>
+      <c r="E49" s="148"/>
       <c r="F49" s="49"/>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="138"/>
-      <c r="B50" s="139"/>
-      <c r="C50" s="138"/>
-      <c r="D50" s="171"/>
-      <c r="E50" s="139"/>
+      <c r="A50" s="146"/>
+      <c r="B50" s="148"/>
+      <c r="C50" s="146"/>
+      <c r="D50" s="147"/>
+      <c r="E50" s="148"/>
       <c r="F50" s="49"/>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="138"/>
-      <c r="B51" s="139"/>
-      <c r="C51" s="138"/>
-      <c r="D51" s="171"/>
-      <c r="E51" s="139"/>
+      <c r="A51" s="146"/>
+      <c r="B51" s="148"/>
+      <c r="C51" s="146"/>
+      <c r="D51" s="147"/>
+      <c r="E51" s="148"/>
       <c r="F51" s="49"/>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="138"/>
-      <c r="B52" s="139"/>
-      <c r="C52" s="138"/>
-      <c r="D52" s="171"/>
-      <c r="E52" s="139"/>
+      <c r="A52" s="146"/>
+      <c r="B52" s="148"/>
+      <c r="C52" s="146"/>
+      <c r="D52" s="147"/>
+      <c r="E52" s="148"/>
       <c r="F52" s="49"/>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="138"/>
-      <c r="B53" s="139"/>
-      <c r="C53" s="138"/>
-      <c r="D53" s="171"/>
-      <c r="E53" s="139"/>
+      <c r="A53" s="146"/>
+      <c r="B53" s="148"/>
+      <c r="C53" s="146"/>
+      <c r="D53" s="147"/>
+      <c r="E53" s="148"/>
       <c r="F53" s="49"/>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="138"/>
-      <c r="B54" s="139"/>
-      <c r="C54" s="138"/>
-      <c r="D54" s="171"/>
-      <c r="E54" s="139"/>
+      <c r="A54" s="146"/>
+      <c r="B54" s="148"/>
+      <c r="C54" s="146"/>
+      <c r="D54" s="147"/>
+      <c r="E54" s="148"/>
       <c r="F54" s="49"/>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="138"/>
-      <c r="B55" s="139"/>
-      <c r="C55" s="138"/>
-      <c r="D55" s="171"/>
-      <c r="E55" s="139"/>
+      <c r="A55" s="146"/>
+      <c r="B55" s="148"/>
+      <c r="C55" s="146"/>
+      <c r="D55" s="147"/>
+      <c r="E55" s="148"/>
       <c r="F55" s="49"/>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="138"/>
-      <c r="B56" s="139"/>
-      <c r="C56" s="138"/>
-      <c r="D56" s="171"/>
-      <c r="E56" s="139"/>
+      <c r="A56" s="146"/>
+      <c r="B56" s="148"/>
+      <c r="C56" s="146"/>
+      <c r="D56" s="147"/>
+      <c r="E56" s="148"/>
       <c r="F56" s="49"/>
     </row>
     <row r="57" spans="1:6">
-      <c r="A57" s="138"/>
-      <c r="B57" s="139"/>
-      <c r="C57" s="138"/>
-      <c r="D57" s="171"/>
-      <c r="E57" s="139"/>
+      <c r="A57" s="146"/>
+      <c r="B57" s="148"/>
+      <c r="C57" s="146"/>
+      <c r="D57" s="147"/>
+      <c r="E57" s="148"/>
       <c r="F57" s="49"/>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="138"/>
-      <c r="B58" s="139"/>
-      <c r="C58" s="138"/>
-      <c r="D58" s="171"/>
-      <c r="E58" s="139"/>
+      <c r="A58" s="146"/>
+      <c r="B58" s="148"/>
+      <c r="C58" s="146"/>
+      <c r="D58" s="147"/>
+      <c r="E58" s="148"/>
       <c r="F58" s="49"/>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="138"/>
-      <c r="B59" s="139"/>
-      <c r="C59" s="138"/>
-      <c r="D59" s="171"/>
-      <c r="E59" s="139"/>
+      <c r="A59" s="146"/>
+      <c r="B59" s="148"/>
+      <c r="C59" s="146"/>
+      <c r="D59" s="147"/>
+      <c r="E59" s="148"/>
       <c r="F59" s="49"/>
     </row>
     <row r="60" spans="1:6">
-      <c r="A60" s="138"/>
-      <c r="B60" s="139"/>
-      <c r="C60" s="138"/>
-      <c r="D60" s="171"/>
-      <c r="E60" s="139"/>
+      <c r="A60" s="146"/>
+      <c r="B60" s="148"/>
+      <c r="C60" s="146"/>
+      <c r="D60" s="147"/>
+      <c r="E60" s="148"/>
       <c r="F60" s="49"/>
     </row>
     <row r="61" spans="1:6">
-      <c r="A61" s="138"/>
-      <c r="B61" s="139"/>
-      <c r="C61" s="138"/>
-      <c r="D61" s="171"/>
-      <c r="E61" s="139"/>
+      <c r="A61" s="146"/>
+      <c r="B61" s="148"/>
+      <c r="C61" s="146"/>
+      <c r="D61" s="147"/>
+      <c r="E61" s="148"/>
       <c r="F61" s="49"/>
     </row>
     <row r="62" spans="1:6">
-      <c r="A62" s="138"/>
-      <c r="B62" s="139"/>
-      <c r="C62" s="138"/>
-      <c r="D62" s="171"/>
-      <c r="E62" s="139"/>
+      <c r="A62" s="146"/>
+      <c r="B62" s="148"/>
+      <c r="C62" s="146"/>
+      <c r="D62" s="147"/>
+      <c r="E62" s="148"/>
       <c r="F62" s="49"/>
     </row>
     <row r="63" spans="1:6">
-      <c r="A63" s="138"/>
-      <c r="B63" s="139"/>
-      <c r="C63" s="138"/>
-      <c r="D63" s="171"/>
-      <c r="E63" s="139"/>
+      <c r="A63" s="146"/>
+      <c r="B63" s="148"/>
+      <c r="C63" s="146"/>
+      <c r="D63" s="147"/>
+      <c r="E63" s="148"/>
       <c r="F63" s="49"/>
     </row>
     <row r="64" spans="1:6">
-      <c r="A64" s="138"/>
-      <c r="B64" s="139"/>
-      <c r="C64" s="138"/>
-      <c r="D64" s="171"/>
-      <c r="E64" s="139"/>
+      <c r="A64" s="146"/>
+      <c r="B64" s="148"/>
+      <c r="C64" s="146"/>
+      <c r="D64" s="147"/>
+      <c r="E64" s="148"/>
       <c r="F64" s="49"/>
     </row>
     <row r="65" spans="1:6">
-      <c r="A65" s="138"/>
-      <c r="B65" s="139"/>
-      <c r="C65" s="138"/>
-      <c r="D65" s="171"/>
-      <c r="E65" s="139"/>
+      <c r="A65" s="146"/>
+      <c r="B65" s="148"/>
+      <c r="C65" s="146"/>
+      <c r="D65" s="147"/>
+      <c r="E65" s="148"/>
       <c r="F65" s="49"/>
     </row>
     <row r="66" spans="1:6">
-      <c r="A66" s="138"/>
-      <c r="B66" s="139"/>
-      <c r="C66" s="138"/>
-      <c r="D66" s="171"/>
-      <c r="E66" s="139"/>
+      <c r="A66" s="146"/>
+      <c r="B66" s="148"/>
+      <c r="C66" s="146"/>
+      <c r="D66" s="147"/>
+      <c r="E66" s="148"/>
       <c r="F66" s="49"/>
     </row>
     <row r="67" spans="1:6">
-      <c r="A67" s="138"/>
-      <c r="B67" s="139"/>
-      <c r="C67" s="138"/>
-      <c r="D67" s="171"/>
-      <c r="E67" s="139"/>
+      <c r="A67" s="146"/>
+      <c r="B67" s="148"/>
+      <c r="C67" s="146"/>
+      <c r="D67" s="147"/>
+      <c r="E67" s="148"/>
       <c r="F67" s="49"/>
     </row>
     <row r="68" spans="1:6">
-      <c r="A68" s="138"/>
-      <c r="B68" s="139"/>
-      <c r="C68" s="138"/>
-      <c r="D68" s="171"/>
-      <c r="E68" s="139"/>
+      <c r="A68" s="146"/>
+      <c r="B68" s="148"/>
+      <c r="C68" s="146"/>
+      <c r="D68" s="147"/>
+      <c r="E68" s="148"/>
       <c r="F68" s="49"/>
     </row>
     <row r="69" spans="1:6">
-      <c r="A69" s="138"/>
-      <c r="B69" s="139"/>
-      <c r="C69" s="138"/>
-      <c r="D69" s="171"/>
-      <c r="E69" s="139"/>
+      <c r="A69" s="146"/>
+      <c r="B69" s="148"/>
+      <c r="C69" s="146"/>
+      <c r="D69" s="147"/>
+      <c r="E69" s="148"/>
       <c r="F69" s="49"/>
     </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="165"/>
-      <c r="B70" s="166"/>
-      <c r="C70" s="165"/>
-      <c r="D70" s="172"/>
-      <c r="E70" s="166"/>
+      <c r="A70" s="149"/>
+      <c r="B70" s="151"/>
+      <c r="C70" s="149"/>
+      <c r="D70" s="150"/>
+      <c r="E70" s="151"/>
       <c r="F70" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="95">
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="A38:G38"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C70:E70"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="B41:G41"/>
+    <mergeCell ref="B42:G42"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="C59:E59"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D13:E13"/>
@@ -5200,80 +5281,11 @@
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="A16:C16"/>
     <mergeCell ref="D16:E16"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="C70:E70"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B36:G36"/>
-    <mergeCell ref="B39:G39"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="B41:G41"/>
-    <mergeCell ref="B42:G42"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="C51:E51"/>
-    <mergeCell ref="C52:E52"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="A38:G38"/>
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="1">
@@ -5308,8 +5320,8 @@
   </sheetPr>
   <dimension ref="A1:Z64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C39" sqref="C39:C40"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28:G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -5531,10 +5543,10 @@
         <v>174</v>
       </c>
       <c r="B15" s="122"/>
-      <c r="C15" s="164" t="s">
+      <c r="C15" s="140" t="s">
         <v>175</v>
       </c>
-      <c r="D15" s="164"/>
+      <c r="D15" s="140"/>
       <c r="E15" s="95" t="s">
         <v>176</v>
       </c>
@@ -5549,8 +5561,8 @@
         <v>177</v>
       </c>
       <c r="B16" s="122"/>
-      <c r="C16" s="163"/>
-      <c r="D16" s="164"/>
+      <c r="C16" s="141"/>
+      <c r="D16" s="140"/>
       <c r="E16" s="55" t="s">
         <v>199</v>
       </c>
@@ -5600,15 +5612,15 @@
       <c r="L18"/>
     </row>
     <row r="19" spans="1:22">
-      <c r="A19" s="156" t="s">
+      <c r="A19" s="178" t="s">
         <v>192</v>
       </c>
-      <c r="B19" s="156"/>
-      <c r="C19" s="156"/>
-      <c r="D19" s="156"/>
-      <c r="E19" s="156"/>
-      <c r="F19" s="156"/>
-      <c r="G19" s="156"/>
+      <c r="B19" s="178"/>
+      <c r="C19" s="178"/>
+      <c r="D19" s="178"/>
+      <c r="E19" s="178"/>
+      <c r="F19" s="178"/>
+      <c r="G19" s="178"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -5618,14 +5630,14 @@
       <c r="A20" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B20" s="150" t="s">
+      <c r="B20" s="172" t="s">
         <v>183</v>
       </c>
-      <c r="C20" s="151"/>
-      <c r="D20" s="151"/>
-      <c r="E20" s="151"/>
-      <c r="F20" s="151"/>
-      <c r="G20" s="152"/>
+      <c r="C20" s="173"/>
+      <c r="D20" s="173"/>
+      <c r="E20" s="173"/>
+      <c r="F20" s="173"/>
+      <c r="G20" s="174"/>
       <c r="H20" s="105"/>
       <c r="I20"/>
       <c r="J20"/>
@@ -5643,12 +5655,12 @@
     </row>
     <row r="21" spans="1:22">
       <c r="A21" s="116"/>
-      <c r="B21" s="167"/>
-      <c r="C21" s="167"/>
-      <c r="D21" s="167"/>
-      <c r="E21" s="167"/>
-      <c r="F21" s="167"/>
-      <c r="G21" s="167"/>
+      <c r="B21" s="156"/>
+      <c r="C21" s="156"/>
+      <c r="D21" s="156"/>
+      <c r="E21" s="156"/>
+      <c r="F21" s="156"/>
+      <c r="G21" s="156"/>
       <c r="H21" s="112"/>
       <c r="I21"/>
       <c r="J21"/>
@@ -5666,12 +5678,12 @@
     </row>
     <row r="22" spans="1:22">
       <c r="A22" s="117"/>
-      <c r="B22" s="168"/>
-      <c r="C22" s="168"/>
-      <c r="D22" s="168"/>
-      <c r="E22" s="168"/>
-      <c r="F22" s="168"/>
-      <c r="G22" s="168"/>
+      <c r="B22" s="158"/>
+      <c r="C22" s="158"/>
+      <c r="D22" s="158"/>
+      <c r="E22" s="158"/>
+      <c r="F22" s="158"/>
+      <c r="G22" s="158"/>
       <c r="H22" s="112"/>
       <c r="I22"/>
       <c r="J22"/>
@@ -5689,12 +5701,12 @@
     </row>
     <row r="23" spans="1:22">
       <c r="A23" s="118"/>
-      <c r="B23" s="169"/>
-      <c r="C23" s="169"/>
-      <c r="D23" s="169"/>
-      <c r="E23" s="169"/>
-      <c r="F23" s="169"/>
-      <c r="G23" s="169"/>
+      <c r="B23" s="160"/>
+      <c r="C23" s="160"/>
+      <c r="D23" s="160"/>
+      <c r="E23" s="160"/>
+      <c r="F23" s="160"/>
+      <c r="G23" s="160"/>
       <c r="H23" s="112"/>
       <c r="M23" s="112"/>
       <c r="N23" s="112"/>
@@ -5714,15 +5726,15 @@
       <c r="L24" s="105"/>
     </row>
     <row r="25" spans="1:22">
-      <c r="A25" s="153" t="s">
+      <c r="A25" s="175" t="s">
         <v>193</v>
       </c>
-      <c r="B25" s="154"/>
-      <c r="C25" s="154"/>
-      <c r="D25" s="154"/>
-      <c r="E25" s="154"/>
-      <c r="F25" s="154"/>
-      <c r="G25" s="155"/>
+      <c r="B25" s="176"/>
+      <c r="C25" s="176"/>
+      <c r="D25" s="176"/>
+      <c r="E25" s="176"/>
+      <c r="F25" s="176"/>
+      <c r="G25" s="177"/>
       <c r="I25" s="105"/>
       <c r="J25" s="105"/>
       <c r="K25" s="105"/>
@@ -5732,14 +5744,14 @@
       <c r="A26" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="173" t="s">
+      <c r="B26" s="152" t="s">
         <v>184</v>
       </c>
-      <c r="C26" s="173"/>
-      <c r="D26" s="173"/>
-      <c r="E26" s="173"/>
-      <c r="F26" s="173"/>
-      <c r="G26" s="173"/>
+      <c r="C26" s="152"/>
+      <c r="D26" s="152"/>
+      <c r="E26" s="152"/>
+      <c r="F26" s="152"/>
+      <c r="G26" s="152"/>
       <c r="H26" s="105"/>
       <c r="I26" s="105"/>
       <c r="J26" s="105"/>
@@ -5756,13 +5768,17 @@
       <c r="V26" s="111"/>
     </row>
     <row r="27" spans="1:22">
-      <c r="A27" s="116"/>
-      <c r="B27" s="174"/>
-      <c r="C27" s="174"/>
-      <c r="D27" s="174"/>
-      <c r="E27" s="174"/>
-      <c r="F27" s="174"/>
-      <c r="G27" s="174"/>
+      <c r="A27" s="116">
+        <v>1</v>
+      </c>
+      <c r="B27" s="153" t="s">
+        <v>226</v>
+      </c>
+      <c r="C27" s="153"/>
+      <c r="D27" s="153"/>
+      <c r="E27" s="153"/>
+      <c r="F27" s="153"/>
+      <c r="G27" s="153"/>
       <c r="H27" s="112"/>
       <c r="I27"/>
       <c r="J27"/>
@@ -5780,12 +5796,12 @@
     </row>
     <row r="28" spans="1:22">
       <c r="A28" s="117"/>
-      <c r="B28" s="175"/>
-      <c r="C28" s="175"/>
-      <c r="D28" s="175"/>
-      <c r="E28" s="175"/>
-      <c r="F28" s="175"/>
-      <c r="G28" s="175"/>
+      <c r="B28" s="154"/>
+      <c r="C28" s="154"/>
+      <c r="D28" s="154"/>
+      <c r="E28" s="154"/>
+      <c r="F28" s="154"/>
+      <c r="G28" s="154"/>
       <c r="H28" s="112"/>
       <c r="M28" s="112"/>
       <c r="N28" s="112"/>
@@ -5799,12 +5815,12 @@
     </row>
     <row r="29" spans="1:22">
       <c r="A29" s="118"/>
-      <c r="B29" s="176"/>
-      <c r="C29" s="176"/>
-      <c r="D29" s="176"/>
-      <c r="E29" s="176"/>
-      <c r="F29" s="176"/>
-      <c r="G29" s="176"/>
+      <c r="B29" s="155"/>
+      <c r="C29" s="155"/>
+      <c r="D29" s="155"/>
+      <c r="E29" s="155"/>
+      <c r="F29" s="155"/>
+      <c r="G29" s="155"/>
       <c r="H29" s="112"/>
       <c r="I29" s="105"/>
       <c r="J29" s="105"/>
@@ -5843,15 +5859,15 @@
       <c r="T30"/>
     </row>
     <row r="31" spans="1:22">
-      <c r="A31" s="153" t="s">
+      <c r="A31" s="175" t="s">
         <v>194</v>
       </c>
-      <c r="B31" s="154"/>
-      <c r="C31" s="154"/>
-      <c r="D31" s="154"/>
-      <c r="E31" s="154"/>
-      <c r="F31" s="154"/>
-      <c r="G31" s="155"/>
+      <c r="B31" s="176"/>
+      <c r="C31" s="176"/>
+      <c r="D31" s="176"/>
+      <c r="E31" s="176"/>
+      <c r="F31" s="176"/>
+      <c r="G31" s="177"/>
       <c r="I31" s="112"/>
       <c r="J31" s="112"/>
       <c r="K31" s="112"/>
@@ -5861,14 +5877,14 @@
       <c r="A32" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B32" s="173" t="s">
+      <c r="B32" s="152" t="s">
         <v>186</v>
       </c>
-      <c r="C32" s="173"/>
-      <c r="D32" s="173"/>
-      <c r="E32" s="173"/>
-      <c r="F32" s="173"/>
-      <c r="G32" s="173"/>
+      <c r="C32" s="152"/>
+      <c r="D32" s="152"/>
+      <c r="E32" s="152"/>
+      <c r="F32" s="152"/>
+      <c r="G32" s="152"/>
       <c r="H32" s="105"/>
       <c r="I32" s="112"/>
       <c r="J32" s="112"/>
@@ -5886,12 +5902,12 @@
     </row>
     <row r="33" spans="1:26">
       <c r="A33" s="116"/>
-      <c r="B33" s="167"/>
-      <c r="C33" s="167"/>
-      <c r="D33" s="167"/>
-      <c r="E33" s="167"/>
-      <c r="F33" s="167"/>
-      <c r="G33" s="177"/>
+      <c r="B33" s="156"/>
+      <c r="C33" s="156"/>
+      <c r="D33" s="156"/>
+      <c r="E33" s="156"/>
+      <c r="F33" s="156"/>
+      <c r="G33" s="157"/>
       <c r="H33" s="112"/>
       <c r="I33"/>
       <c r="J33"/>
@@ -5909,12 +5925,12 @@
     </row>
     <row r="34" spans="1:26">
       <c r="A34" s="117"/>
-      <c r="B34" s="168"/>
-      <c r="C34" s="168"/>
-      <c r="D34" s="168"/>
-      <c r="E34" s="168"/>
-      <c r="F34" s="168"/>
-      <c r="G34" s="178"/>
+      <c r="B34" s="158"/>
+      <c r="C34" s="158"/>
+      <c r="D34" s="158"/>
+      <c r="E34" s="158"/>
+      <c r="F34" s="158"/>
+      <c r="G34" s="159"/>
       <c r="H34" s="112"/>
       <c r="M34" s="112"/>
       <c r="N34" s="112"/>
@@ -5928,12 +5944,12 @@
     </row>
     <row r="35" spans="1:26">
       <c r="A35" s="118"/>
-      <c r="B35" s="169"/>
-      <c r="C35" s="169"/>
-      <c r="D35" s="169"/>
-      <c r="E35" s="169"/>
-      <c r="F35" s="169"/>
-      <c r="G35" s="179"/>
+      <c r="B35" s="160"/>
+      <c r="C35" s="160"/>
+      <c r="D35" s="160"/>
+      <c r="E35" s="160"/>
+      <c r="F35" s="160"/>
+      <c r="G35" s="161"/>
       <c r="H35" s="112"/>
       <c r="M35" s="112"/>
       <c r="N35" s="112"/>
@@ -5997,82 +6013,82 @@
       <c r="Z38" s="39"/>
     </row>
     <row r="39" spans="1:26">
-      <c r="A39" s="187" t="s">
+      <c r="A39" s="185" t="s">
         <v>69</v>
       </c>
-      <c r="B39" s="187" t="s">
+      <c r="B39" s="185" t="s">
         <v>0</v>
       </c>
-      <c r="C39" s="189" t="s">
+      <c r="C39" s="187" t="s">
         <v>1</v>
       </c>
-      <c r="D39" s="187" t="s">
+      <c r="D39" s="185" t="s">
         <v>2</v>
       </c>
-      <c r="E39" s="190" t="s">
+      <c r="E39" s="188" t="s">
         <v>161</v>
       </c>
-      <c r="F39" s="190" t="s">
+      <c r="F39" s="188" t="s">
         <v>177</v>
       </c>
-      <c r="G39" s="187" t="s">
+      <c r="G39" s="185" t="s">
         <v>13</v>
       </c>
-      <c r="H39" s="187" t="s">
+      <c r="H39" s="185" t="s">
         <v>116</v>
       </c>
-      <c r="I39" s="194" t="s">
+      <c r="I39" s="192" t="s">
         <v>201</v>
       </c>
-      <c r="J39" s="194" t="s">
+      <c r="J39" s="192" t="s">
         <v>202</v>
       </c>
-      <c r="K39" s="194" t="s">
+      <c r="K39" s="192" t="s">
         <v>203</v>
       </c>
-      <c r="L39" s="195" t="s">
+      <c r="L39" s="193" t="s">
         <v>204</v>
       </c>
-      <c r="M39" s="187" t="s">
+      <c r="M39" s="185" t="s">
         <v>195</v>
       </c>
-      <c r="N39" s="187" t="s">
+      <c r="N39" s="185" t="s">
         <v>210</v>
       </c>
-      <c r="O39" s="189" t="s">
+      <c r="O39" s="187" t="s">
         <v>209</v>
       </c>
-      <c r="P39" s="185" t="s">
+      <c r="P39" s="195" t="s">
         <v>71</v>
       </c>
-      <c r="Q39" s="186"/>
-      <c r="R39" s="185" t="s">
+      <c r="Q39" s="196"/>
+      <c r="R39" s="195" t="s">
         <v>17</v>
       </c>
-      <c r="S39" s="186"/>
+      <c r="S39" s="196"/>
       <c r="T39" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="U39" s="187" t="s">
+      <c r="U39" s="185" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:26">
-      <c r="A40" s="188"/>
-      <c r="B40" s="188"/>
-      <c r="C40" s="188"/>
-      <c r="D40" s="188"/>
-      <c r="E40" s="191"/>
-      <c r="F40" s="192"/>
-      <c r="G40" s="188"/>
-      <c r="H40" s="188"/>
-      <c r="I40" s="194"/>
-      <c r="J40" s="194"/>
-      <c r="K40" s="194"/>
-      <c r="L40" s="196"/>
-      <c r="M40" s="193"/>
-      <c r="N40" s="193"/>
-      <c r="O40" s="193"/>
+      <c r="A40" s="186"/>
+      <c r="B40" s="186"/>
+      <c r="C40" s="186"/>
+      <c r="D40" s="186"/>
+      <c r="E40" s="189"/>
+      <c r="F40" s="190"/>
+      <c r="G40" s="186"/>
+      <c r="H40" s="186"/>
+      <c r="I40" s="192"/>
+      <c r="J40" s="192"/>
+      <c r="K40" s="192"/>
+      <c r="L40" s="194"/>
+      <c r="M40" s="191"/>
+      <c r="N40" s="191"/>
+      <c r="O40" s="191"/>
       <c r="P40" s="29" t="s">
         <v>75</v>
       </c>
@@ -6088,9 +6104,9 @@
       <c r="T40" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="U40" s="188"/>
-    </row>
-    <row r="41" spans="1:26">
+      <c r="U40" s="186"/>
+    </row>
+    <row r="41" spans="1:26" ht="30">
       <c r="A41" s="7">
         <v>1</v>
       </c>
@@ -6113,8 +6129,8 @@
         <v>205</v>
       </c>
       <c r="J41" s="133"/>
-      <c r="K41" s="134" t="s">
-        <v>207</v>
+      <c r="K41" s="206" t="s">
+        <v>225</v>
       </c>
       <c r="L41" s="133"/>
       <c r="M41" s="24" t="s">
@@ -6762,6 +6778,25 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="R39:S39"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="L39:L40"/>
+    <mergeCell ref="N39:N40"/>
+    <mergeCell ref="M39:M40"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="P39:Q39"/>
     <mergeCell ref="B29:G29"/>
     <mergeCell ref="A31:G31"/>
     <mergeCell ref="B32:G32"/>
@@ -6778,28 +6813,9 @@
     <mergeCell ref="I39:I40"/>
     <mergeCell ref="J39:J40"/>
     <mergeCell ref="K39:K40"/>
-    <mergeCell ref="L39:L40"/>
-    <mergeCell ref="N39:N40"/>
-    <mergeCell ref="M39:M40"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="P39:Q39"/>
-    <mergeCell ref="R39:S39"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="A25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
-  <dataValidations disablePrompts="1" count="3">
+  <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>Validate実装パターン</formula1>
     </dataValidation>
@@ -6821,7 +6837,7 @@
   </headerFooter>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000001000000}">
           <x14:formula1>
             <xm:f>config!$D$5:$D$8</xm:f>
@@ -7029,10 +7045,10 @@
         <v>174</v>
       </c>
       <c r="B12" s="122"/>
-      <c r="C12" s="164" t="s">
+      <c r="C12" s="140" t="s">
         <v>175</v>
       </c>
-      <c r="D12" s="164"/>
+      <c r="D12" s="140"/>
       <c r="E12" s="95" t="s">
         <v>176</v>
       </c>
@@ -7047,10 +7063,10 @@
         <v>177</v>
       </c>
       <c r="B13" s="122"/>
-      <c r="C13" s="164" t="s">
+      <c r="C13" s="140" t="s">
         <v>178</v>
       </c>
-      <c r="D13" s="164"/>
+      <c r="D13" s="140"/>
       <c r="E13" s="55"/>
       <c r="F13" s="55"/>
       <c r="G13" s="54"/>
@@ -7090,15 +7106,15 @@
       <c r="L15"/>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="156" t="s">
+      <c r="A16" s="178" t="s">
         <v>192</v>
       </c>
-      <c r="B16" s="156"/>
-      <c r="C16" s="156"/>
-      <c r="D16" s="156"/>
-      <c r="E16" s="156"/>
-      <c r="F16" s="156"/>
-      <c r="G16" s="156"/>
+      <c r="B16" s="178"/>
+      <c r="C16" s="178"/>
+      <c r="D16" s="178"/>
+      <c r="E16" s="178"/>
+      <c r="F16" s="178"/>
+      <c r="G16" s="178"/>
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16"/>
@@ -7109,14 +7125,14 @@
       <c r="A17" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B17" s="150" t="s">
+      <c r="B17" s="172" t="s">
         <v>183</v>
       </c>
-      <c r="C17" s="151"/>
-      <c r="D17" s="151"/>
-      <c r="E17" s="151"/>
-      <c r="F17" s="151"/>
-      <c r="G17" s="152"/>
+      <c r="C17" s="173"/>
+      <c r="D17" s="173"/>
+      <c r="E17" s="173"/>
+      <c r="F17" s="173"/>
+      <c r="G17" s="174"/>
       <c r="H17" s="105"/>
       <c r="I17"/>
       <c r="J17"/>
@@ -7132,12 +7148,12 @@
     </row>
     <row r="18" spans="1:22">
       <c r="A18" s="116"/>
-      <c r="B18" s="167"/>
-      <c r="C18" s="167"/>
-      <c r="D18" s="167"/>
-      <c r="E18" s="167"/>
-      <c r="F18" s="167"/>
-      <c r="G18" s="167"/>
+      <c r="B18" s="156"/>
+      <c r="C18" s="156"/>
+      <c r="D18" s="156"/>
+      <c r="E18" s="156"/>
+      <c r="F18" s="156"/>
+      <c r="G18" s="156"/>
       <c r="H18" s="112"/>
       <c r="I18"/>
       <c r="J18"/>
@@ -7152,12 +7168,12 @@
     </row>
     <row r="19" spans="1:22">
       <c r="A19" s="117"/>
-      <c r="B19" s="168"/>
-      <c r="C19" s="168"/>
-      <c r="D19" s="168"/>
-      <c r="E19" s="168"/>
-      <c r="F19" s="168"/>
-      <c r="G19" s="168"/>
+      <c r="B19" s="158"/>
+      <c r="C19" s="158"/>
+      <c r="D19" s="158"/>
+      <c r="E19" s="158"/>
+      <c r="F19" s="158"/>
+      <c r="G19" s="158"/>
       <c r="H19" s="112"/>
       <c r="I19"/>
       <c r="J19"/>
@@ -7172,12 +7188,12 @@
     </row>
     <row r="20" spans="1:22">
       <c r="A20" s="118"/>
-      <c r="B20" s="169"/>
-      <c r="C20" s="169"/>
-      <c r="D20" s="169"/>
-      <c r="E20" s="169"/>
-      <c r="F20" s="169"/>
-      <c r="G20" s="169"/>
+      <c r="B20" s="160"/>
+      <c r="C20" s="160"/>
+      <c r="D20" s="160"/>
+      <c r="E20" s="160"/>
+      <c r="F20" s="160"/>
+      <c r="G20" s="160"/>
       <c r="H20" s="112"/>
       <c r="I20"/>
       <c r="J20"/>
@@ -7204,15 +7220,15 @@
       <c r="O21" s="112"/>
     </row>
     <row r="22" spans="1:22">
-      <c r="A22" s="153" t="s">
+      <c r="A22" s="175" t="s">
         <v>193</v>
       </c>
-      <c r="B22" s="154"/>
-      <c r="C22" s="154"/>
-      <c r="D22" s="154"/>
-      <c r="E22" s="154"/>
-      <c r="F22" s="154"/>
-      <c r="G22" s="155"/>
+      <c r="B22" s="176"/>
+      <c r="C22" s="176"/>
+      <c r="D22" s="176"/>
+      <c r="E22" s="176"/>
+      <c r="F22" s="176"/>
+      <c r="G22" s="177"/>
       <c r="I22"/>
       <c r="J22"/>
       <c r="K22"/>
@@ -7225,14 +7241,14 @@
       <c r="A23" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B23" s="173" t="s">
+      <c r="B23" s="152" t="s">
         <v>184</v>
       </c>
-      <c r="C23" s="173"/>
-      <c r="D23" s="173"/>
-      <c r="E23" s="173"/>
-      <c r="F23" s="173"/>
-      <c r="G23" s="173"/>
+      <c r="C23" s="152"/>
+      <c r="D23" s="152"/>
+      <c r="E23" s="152"/>
+      <c r="F23" s="152"/>
+      <c r="G23" s="152"/>
       <c r="H23" s="105"/>
       <c r="M23" s="112"/>
       <c r="N23" s="112"/>
@@ -7248,14 +7264,14 @@
       <c r="A24" s="116">
         <v>1</v>
       </c>
-      <c r="B24" s="174" t="s">
+      <c r="B24" s="153" t="s">
         <v>185</v>
       </c>
-      <c r="C24" s="174"/>
-      <c r="D24" s="174"/>
-      <c r="E24" s="174"/>
-      <c r="F24" s="174"/>
-      <c r="G24" s="174"/>
+      <c r="C24" s="153"/>
+      <c r="D24" s="153"/>
+      <c r="E24" s="153"/>
+      <c r="F24" s="153"/>
+      <c r="G24" s="153"/>
       <c r="H24" s="112"/>
       <c r="I24" s="105"/>
       <c r="J24" s="105"/>
@@ -7270,12 +7286,12 @@
     </row>
     <row r="25" spans="1:22">
       <c r="A25" s="117"/>
-      <c r="B25" s="175"/>
-      <c r="C25" s="175"/>
-      <c r="D25" s="175"/>
-      <c r="E25" s="175"/>
-      <c r="F25" s="175"/>
-      <c r="G25" s="175"/>
+      <c r="B25" s="154"/>
+      <c r="C25" s="154"/>
+      <c r="D25" s="154"/>
+      <c r="E25" s="154"/>
+      <c r="F25" s="154"/>
+      <c r="G25" s="154"/>
       <c r="H25" s="112"/>
       <c r="I25" s="105"/>
       <c r="J25" s="105"/>
@@ -7290,12 +7306,12 @@
     </row>
     <row r="26" spans="1:22">
       <c r="A26" s="118"/>
-      <c r="B26" s="176"/>
-      <c r="C26" s="176"/>
-      <c r="D26" s="176"/>
-      <c r="E26" s="176"/>
-      <c r="F26" s="176"/>
-      <c r="G26" s="176"/>
+      <c r="B26" s="155"/>
+      <c r="C26" s="155"/>
+      <c r="D26" s="155"/>
+      <c r="E26" s="155"/>
+      <c r="F26" s="155"/>
+      <c r="G26" s="155"/>
       <c r="H26" s="112"/>
       <c r="I26" s="105"/>
       <c r="J26" s="105"/>
@@ -7334,15 +7350,15 @@
       <c r="T27"/>
     </row>
     <row r="28" spans="1:22">
-      <c r="A28" s="153" t="s">
+      <c r="A28" s="175" t="s">
         <v>194</v>
       </c>
-      <c r="B28" s="154"/>
-      <c r="C28" s="154"/>
-      <c r="D28" s="154"/>
-      <c r="E28" s="154"/>
-      <c r="F28" s="154"/>
-      <c r="G28" s="155"/>
+      <c r="B28" s="176"/>
+      <c r="C28" s="176"/>
+      <c r="D28" s="176"/>
+      <c r="E28" s="176"/>
+      <c r="F28" s="176"/>
+      <c r="G28" s="177"/>
       <c r="M28" s="112"/>
       <c r="N28" s="112"/>
       <c r="O28" s="112"/>
@@ -7351,14 +7367,14 @@
       <c r="A29" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="173" t="s">
+      <c r="B29" s="152" t="s">
         <v>186</v>
       </c>
-      <c r="C29" s="173"/>
-      <c r="D29" s="173"/>
-      <c r="E29" s="173"/>
-      <c r="F29" s="173"/>
-      <c r="G29" s="173"/>
+      <c r="C29" s="152"/>
+      <c r="D29" s="152"/>
+      <c r="E29" s="152"/>
+      <c r="F29" s="152"/>
+      <c r="G29" s="152"/>
       <c r="H29" s="105"/>
       <c r="I29" s="105"/>
       <c r="J29" s="105"/>
@@ -7376,12 +7392,12 @@
     </row>
     <row r="30" spans="1:22">
       <c r="A30" s="116"/>
-      <c r="B30" s="167"/>
-      <c r="C30" s="167"/>
-      <c r="D30" s="167"/>
-      <c r="E30" s="167"/>
-      <c r="F30" s="167"/>
-      <c r="G30" s="177"/>
+      <c r="B30" s="156"/>
+      <c r="C30" s="156"/>
+      <c r="D30" s="156"/>
+      <c r="E30" s="156"/>
+      <c r="F30" s="156"/>
+      <c r="G30" s="157"/>
       <c r="H30" s="112"/>
       <c r="I30" s="112"/>
       <c r="J30" s="112"/>
@@ -7399,12 +7415,12 @@
     </row>
     <row r="31" spans="1:22">
       <c r="A31" s="117"/>
-      <c r="B31" s="168"/>
-      <c r="C31" s="168"/>
-      <c r="D31" s="168"/>
-      <c r="E31" s="168"/>
-      <c r="F31" s="168"/>
-      <c r="G31" s="178"/>
+      <c r="B31" s="158"/>
+      <c r="C31" s="158"/>
+      <c r="D31" s="158"/>
+      <c r="E31" s="158"/>
+      <c r="F31" s="158"/>
+      <c r="G31" s="159"/>
       <c r="H31" s="112"/>
       <c r="I31" s="112"/>
       <c r="J31" s="112"/>
@@ -7419,12 +7435,12 @@
     </row>
     <row r="32" spans="1:22">
       <c r="A32" s="118"/>
-      <c r="B32" s="169"/>
-      <c r="C32" s="169"/>
-      <c r="D32" s="169"/>
-      <c r="E32" s="169"/>
-      <c r="F32" s="169"/>
-      <c r="G32" s="179"/>
+      <c r="B32" s="160"/>
+      <c r="C32" s="160"/>
+      <c r="D32" s="160"/>
+      <c r="E32" s="160"/>
+      <c r="F32" s="160"/>
+      <c r="G32" s="161"/>
       <c r="H32" s="112"/>
       <c r="I32" s="112"/>
       <c r="J32" s="112"/>
@@ -7494,28 +7510,28 @@
       <c r="U35" s="58"/>
     </row>
     <row r="36" spans="1:21" ht="30" customHeight="1">
-      <c r="A36" s="190" t="s">
+      <c r="A36" s="188" t="s">
         <v>118</v>
       </c>
-      <c r="B36" s="190" t="s">
+      <c r="B36" s="188" t="s">
         <v>119</v>
       </c>
       <c r="C36" s="60" t="s">
         <v>120</v>
       </c>
-      <c r="D36" s="190" t="s">
+      <c r="D36" s="188" t="s">
         <v>101</v>
       </c>
-      <c r="E36" s="190" t="s">
+      <c r="E36" s="188" t="s">
         <v>161</v>
       </c>
-      <c r="F36" s="190" t="s">
+      <c r="F36" s="188" t="s">
         <v>177</v>
       </c>
-      <c r="G36" s="190" t="s">
+      <c r="G36" s="188" t="s">
         <v>140</v>
       </c>
-      <c r="H36" s="190" t="s">
+      <c r="H36" s="188" t="s">
         <v>139</v>
       </c>
       <c r="I36" s="200" t="s">
@@ -7527,16 +7543,16 @@
       <c r="K36" s="202" t="s">
         <v>203</v>
       </c>
-      <c r="L36" s="195" t="s">
+      <c r="L36" s="193" t="s">
         <v>204</v>
       </c>
-      <c r="M36" s="187" t="s">
+      <c r="M36" s="185" t="s">
         <v>195</v>
       </c>
-      <c r="N36" s="187" t="s">
+      <c r="N36" s="185" t="s">
         <v>210</v>
       </c>
-      <c r="O36" s="189" t="s">
+      <c r="O36" s="187" t="s">
         <v>209</v>
       </c>
       <c r="P36" s="198" t="s">
@@ -7550,7 +7566,7 @@
       <c r="T36" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="U36" s="190" t="s">
+      <c r="U36" s="188" t="s">
         <v>125</v>
       </c>
     </row>
@@ -7561,16 +7577,16 @@
         <v>121</v>
       </c>
       <c r="D37" s="197"/>
-      <c r="E37" s="192"/>
-      <c r="F37" s="192"/>
+      <c r="E37" s="190"/>
+      <c r="F37" s="190"/>
       <c r="G37" s="197"/>
       <c r="H37" s="197"/>
       <c r="I37" s="201"/>
       <c r="J37" s="203"/>
       <c r="K37" s="203"/>
-      <c r="L37" s="196"/>
-      <c r="M37" s="193"/>
-      <c r="N37" s="193"/>
+      <c r="L37" s="194"/>
+      <c r="M37" s="191"/>
+      <c r="N37" s="191"/>
       <c r="O37" s="204"/>
       <c r="P37" s="62" t="s">
         <v>126</v>
@@ -8243,21 +8259,9 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="A22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="A28:G28"/>
-    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="O36:O37"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="R36:S36"/>
     <mergeCell ref="L36:L37"/>
     <mergeCell ref="B31:G31"/>
     <mergeCell ref="B32:G32"/>
@@ -8274,9 +8278,21 @@
     <mergeCell ref="I36:I37"/>
     <mergeCell ref="J36:J37"/>
     <mergeCell ref="K36:K37"/>
-    <mergeCell ref="O36:O37"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="R36:S36"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="A28:G28"/>
+    <mergeCell ref="B29:G29"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="3">

</xml_diff>

<commit_message>
0.0.23: Required field is added to field list, that is converted to @NotNull annotaion.
</commit_message>
<xml_diff>
--- a/meta/api/BlancoApiPostSample.xlsx
+++ b/meta/api/BlancoApiPostSample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorKt/meta/api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA2C932-B63B-7A4A-9F20-52BF43121B90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C59FBA2-7B7A-5C48-BF75-478F0A3B362A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="180" yWindow="680" windowWidth="21420" windowHeight="17540" tabRatio="860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="232">
   <si>
     <t>項目名</t>
     <rPh sb="0" eb="3">
@@ -2371,10 +2371,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>@NoNull</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>デコレーション</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -2404,7 +2400,7 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>javax.validation.constraints.NoNull</t>
+    <t>@field:Max(10)</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -3789,22 +3785,19 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -3820,34 +3813,37 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="62" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="63" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="65" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="62" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="63" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="65" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5339,8 +5335,8 @@
   </sheetPr>
   <dimension ref="A1:Z66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:G30"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -5577,15 +5573,15 @@
     </row>
     <row r="16" spans="1:19">
       <c r="A16" s="122" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B16" s="122"/>
       <c r="C16" s="164" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D16" s="165"/>
       <c r="E16" s="55" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F16" s="54"/>
       <c r="G16" s="54"/>
@@ -5615,15 +5611,13 @@
     </row>
     <row r="18" spans="1:22">
       <c r="A18" s="122" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B18" s="122"/>
-      <c r="C18" s="164" t="s">
-        <v>226</v>
-      </c>
+      <c r="C18" s="164"/>
       <c r="D18" s="165"/>
       <c r="E18" s="55" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F18" s="54"/>
       <c r="G18" s="54"/>
@@ -5854,12 +5848,8 @@
       <c r="V29"/>
     </row>
     <row r="30" spans="1:22">
-      <c r="A30" s="117">
-        <v>2</v>
-      </c>
-      <c r="B30" s="176" t="s">
-        <v>232</v>
-      </c>
+      <c r="A30" s="117"/>
+      <c r="B30" s="176"/>
       <c r="C30" s="176"/>
       <c r="D30" s="176"/>
       <c r="E30" s="176"/>
@@ -6082,16 +6072,16 @@
       <c r="B41" s="190" t="s">
         <v>0</v>
       </c>
-      <c r="C41" s="193" t="s">
+      <c r="C41" s="192" t="s">
         <v>1</v>
       </c>
       <c r="D41" s="190" t="s">
         <v>2</v>
       </c>
-      <c r="E41" s="194" t="s">
+      <c r="E41" s="193" t="s">
         <v>161</v>
       </c>
-      <c r="F41" s="194" t="s">
+      <c r="F41" s="193" t="s">
         <v>177</v>
       </c>
       <c r="G41" s="190" t="s">
@@ -6109,7 +6099,7 @@
       <c r="K41" s="197" t="s">
         <v>202</v>
       </c>
-      <c r="L41" s="188" t="s">
+      <c r="L41" s="186" t="s">
         <v>203</v>
       </c>
       <c r="M41" s="190" t="s">
@@ -6118,17 +6108,17 @@
       <c r="N41" s="190" t="s">
         <v>209</v>
       </c>
-      <c r="O41" s="193" t="s">
+      <c r="O41" s="192" t="s">
         <v>208</v>
       </c>
-      <c r="P41" s="186" t="s">
+      <c r="P41" s="188" t="s">
         <v>71</v>
       </c>
-      <c r="Q41" s="187"/>
-      <c r="R41" s="186" t="s">
+      <c r="Q41" s="189"/>
+      <c r="R41" s="188" t="s">
         <v>17</v>
       </c>
-      <c r="S41" s="187"/>
+      <c r="S41" s="189"/>
       <c r="T41" s="34" t="s">
         <v>70</v>
       </c>
@@ -6137,21 +6127,21 @@
       </c>
     </row>
     <row r="42" spans="1:26">
-      <c r="A42" s="192"/>
-      <c r="B42" s="192"/>
-      <c r="C42" s="192"/>
-      <c r="D42" s="192"/>
-      <c r="E42" s="195"/>
-      <c r="F42" s="196"/>
-      <c r="G42" s="192"/>
-      <c r="H42" s="192"/>
+      <c r="A42" s="191"/>
+      <c r="B42" s="191"/>
+      <c r="C42" s="191"/>
+      <c r="D42" s="191"/>
+      <c r="E42" s="194"/>
+      <c r="F42" s="195"/>
+      <c r="G42" s="191"/>
+      <c r="H42" s="191"/>
       <c r="I42" s="197"/>
       <c r="J42" s="197"/>
       <c r="K42" s="197"/>
-      <c r="L42" s="189"/>
-      <c r="M42" s="191"/>
-      <c r="N42" s="191"/>
-      <c r="O42" s="191"/>
+      <c r="L42" s="187"/>
+      <c r="M42" s="196"/>
+      <c r="N42" s="196"/>
+      <c r="O42" s="196"/>
       <c r="P42" s="29" t="s">
         <v>75</v>
       </c>
@@ -6167,7 +6157,7 @@
       <c r="T42" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="U42" s="192"/>
+      <c r="U42" s="191"/>
     </row>
     <row r="43" spans="1:26" ht="30">
       <c r="A43" s="7">
@@ -6232,7 +6222,9 @@
       </c>
       <c r="E44" s="25"/>
       <c r="F44" s="25"/>
-      <c r="G44" s="85"/>
+      <c r="G44" s="85" t="s">
+        <v>141</v>
+      </c>
       <c r="H44" s="25"/>
       <c r="I44" s="135" t="s">
         <v>205</v>
@@ -6276,7 +6268,9 @@
       </c>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
-      <c r="G45" s="86"/>
+      <c r="G45" s="86" t="s">
+        <v>141</v>
+      </c>
       <c r="H45" s="26" t="b">
         <v>1</v>
       </c>
@@ -6855,6 +6849,8 @@
     <mergeCell ref="J41:J42"/>
     <mergeCell ref="K41:K42"/>
     <mergeCell ref="M41:M42"/>
+    <mergeCell ref="R41:S41"/>
+    <mergeCell ref="N41:N42"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="P41:Q41"/>
     <mergeCell ref="B31:G31"/>
@@ -6863,7 +6859,6 @@
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
-    <mergeCell ref="R41:S41"/>
     <mergeCell ref="A21:G21"/>
     <mergeCell ref="B22:G22"/>
     <mergeCell ref="B23:G23"/>
@@ -6877,7 +6872,6 @@
     <mergeCell ref="B29:G29"/>
     <mergeCell ref="B30:G30"/>
     <mergeCell ref="L41:L42"/>
-    <mergeCell ref="N41:N42"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="3">
@@ -6934,8 +6928,8 @@
   </sheetPr>
   <dimension ref="A1:V63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="D9" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -7125,15 +7119,15 @@
     </row>
     <row r="13" spans="1:20">
       <c r="A13" s="122" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B13" s="122"/>
       <c r="C13" s="164" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D13" s="165"/>
       <c r="E13" s="55" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F13" s="54"/>
       <c r="G13" s="54"/>
@@ -7163,15 +7157,13 @@
     </row>
     <row r="15" spans="1:20">
       <c r="A15" s="122" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B15" s="122"/>
-      <c r="C15" s="164" t="s">
-        <v>226</v>
-      </c>
+      <c r="C15" s="164"/>
       <c r="D15" s="165"/>
       <c r="E15" s="55" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F15" s="54"/>
       <c r="G15" s="54"/>
@@ -7396,12 +7388,8 @@
       <c r="V26"/>
     </row>
     <row r="27" spans="1:22">
-      <c r="A27" s="117">
-        <v>2</v>
-      </c>
-      <c r="B27" s="176" t="s">
-        <v>232</v>
-      </c>
+      <c r="A27" s="117"/>
+      <c r="B27" s="176"/>
       <c r="C27" s="176"/>
       <c r="D27" s="176"/>
       <c r="E27" s="176"/>
@@ -7625,40 +7613,40 @@
       <c r="U37" s="58"/>
     </row>
     <row r="38" spans="1:22" ht="30" customHeight="1">
-      <c r="A38" s="194" t="s">
+      <c r="A38" s="193" t="s">
         <v>118</v>
       </c>
-      <c r="B38" s="194" t="s">
+      <c r="B38" s="193" t="s">
         <v>119</v>
       </c>
       <c r="C38" s="60" t="s">
         <v>120</v>
       </c>
-      <c r="D38" s="194" t="s">
+      <c r="D38" s="193" t="s">
         <v>101</v>
       </c>
-      <c r="E38" s="194" t="s">
+      <c r="E38" s="193" t="s">
         <v>161</v>
       </c>
-      <c r="F38" s="194" t="s">
+      <c r="F38" s="193" t="s">
         <v>177</v>
       </c>
-      <c r="G38" s="194" t="s">
+      <c r="G38" s="193" t="s">
         <v>140</v>
       </c>
-      <c r="H38" s="194" t="s">
+      <c r="H38" s="193" t="s">
         <v>139</v>
       </c>
-      <c r="I38" s="203" t="s">
+      <c r="I38" s="201" t="s">
         <v>200</v>
       </c>
-      <c r="J38" s="205" t="s">
+      <c r="J38" s="203" t="s">
         <v>201</v>
       </c>
-      <c r="K38" s="205" t="s">
+      <c r="K38" s="203" t="s">
         <v>202</v>
       </c>
-      <c r="L38" s="188" t="s">
+      <c r="L38" s="186" t="s">
         <v>203</v>
       </c>
       <c r="M38" s="190" t="s">
@@ -7667,42 +7655,42 @@
       <c r="N38" s="190" t="s">
         <v>209</v>
       </c>
-      <c r="O38" s="193" t="s">
+      <c r="O38" s="192" t="s">
         <v>208</v>
       </c>
-      <c r="P38" s="202" t="s">
+      <c r="P38" s="199" t="s">
         <v>122</v>
       </c>
       <c r="Q38" s="200"/>
-      <c r="R38" s="199" t="s">
+      <c r="R38" s="206" t="s">
         <v>123</v>
       </c>
       <c r="S38" s="200"/>
       <c r="T38" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="U38" s="194" t="s">
+      <c r="U38" s="193" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="39" spans="1:22" ht="15">
-      <c r="A39" s="201"/>
-      <c r="B39" s="201"/>
+      <c r="A39" s="198"/>
+      <c r="B39" s="198"/>
       <c r="C39" s="61" t="s">
         <v>121</v>
       </c>
-      <c r="D39" s="201"/>
-      <c r="E39" s="196"/>
-      <c r="F39" s="196"/>
-      <c r="G39" s="201"/>
-      <c r="H39" s="201"/>
-      <c r="I39" s="204"/>
-      <c r="J39" s="206"/>
-      <c r="K39" s="206"/>
-      <c r="L39" s="189"/>
-      <c r="M39" s="191"/>
-      <c r="N39" s="191"/>
-      <c r="O39" s="198"/>
+      <c r="D39" s="198"/>
+      <c r="E39" s="195"/>
+      <c r="F39" s="195"/>
+      <c r="G39" s="198"/>
+      <c r="H39" s="198"/>
+      <c r="I39" s="202"/>
+      <c r="J39" s="204"/>
+      <c r="K39" s="204"/>
+      <c r="L39" s="187"/>
+      <c r="M39" s="196"/>
+      <c r="N39" s="196"/>
+      <c r="O39" s="205"/>
       <c r="P39" s="62" t="s">
         <v>126</v>
       </c>
@@ -7718,7 +7706,7 @@
       <c r="T39" s="63" t="s">
         <v>130</v>
       </c>
-      <c r="U39" s="201"/>
+      <c r="U39" s="198"/>
     </row>
     <row r="40" spans="1:22">
       <c r="A40" s="64">
@@ -7778,14 +7766,16 @@
       </c>
       <c r="E41" s="67"/>
       <c r="F41" s="67"/>
-      <c r="G41" s="89"/>
+      <c r="G41" s="89" t="s">
+        <v>141</v>
+      </c>
       <c r="H41" s="67"/>
       <c r="I41" s="135" t="s">
         <v>205</v>
       </c>
       <c r="J41" s="135"/>
       <c r="K41" s="136" t="s">
-        <v>206</v>
+        <v>231</v>
       </c>
       <c r="L41" s="135"/>
       <c r="M41" s="25" t="s">
@@ -7817,7 +7807,9 @@
       </c>
       <c r="E42" s="70"/>
       <c r="F42" s="70"/>
-      <c r="G42" s="90"/>
+      <c r="G42" s="90" t="s">
+        <v>141</v>
+      </c>
       <c r="H42" s="70"/>
       <c r="I42" s="135"/>
       <c r="J42" s="135"/>
@@ -8374,16 +8366,13 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="A24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B26:G26"/>
     <mergeCell ref="B27:G27"/>
     <mergeCell ref="B28:G28"/>
     <mergeCell ref="A30:G30"/>
     <mergeCell ref="B31:G31"/>
+    <mergeCell ref="O38:O39"/>
+    <mergeCell ref="M38:M39"/>
+    <mergeCell ref="R38:S38"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="A18:G18"/>
@@ -8391,6 +8380,15 @@
     <mergeCell ref="B20:G20"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C15:D15"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="A24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="L38:L39"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:G34"/>
     <mergeCell ref="U38:U39"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="B38:B39"/>
@@ -8404,12 +8402,6 @@
     <mergeCell ref="I38:I39"/>
     <mergeCell ref="J38:J39"/>
     <mergeCell ref="K38:K39"/>
-    <mergeCell ref="O38:O39"/>
-    <mergeCell ref="M38:M39"/>
-    <mergeCell ref="R38:S38"/>
-    <mergeCell ref="L38:L39"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B34:G34"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="3">

</xml_diff>

<commit_message>
0.1.1: fieldRequiredKt, nullableKt and fixedValueKt are enabled now.
</commit_message>
<xml_diff>
--- a/meta/api/BlancoApiPostSample.xlsx
+++ b/meta/api/BlancoApiPostSample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorKt/meta/api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C59FBA2-7B7A-5C48-BF75-478F0A3B362A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A844F26F-4813-5C4B-9D54-7BFBA70B4EB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="680" windowWidth="21420" windowHeight="17540" tabRatio="860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15160" yWindow="1200" windowWidth="21420" windowHeight="17540" tabRatio="860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="process" sheetId="19" r:id="rId1"/>
@@ -27,6 +27,7 @@
     <definedName name="isNullable">config!$F$5:$F$6</definedName>
     <definedName name="others">config!$G$5:$G$6</definedName>
     <definedName name="Submit有無">config!$B$5:$B$6</definedName>
+    <definedName name="threeAlters">config!$H$5:$H$7</definedName>
     <definedName name="Validate実装パターン">config!$A$5:$A$6</definedName>
     <definedName name="チェック種別">config!$D$5:$D$49</definedName>
     <definedName name="型">config!#REF!</definedName>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="238">
   <si>
     <t>項目名</t>
     <rPh sb="0" eb="3">
@@ -2401,6 +2402,35 @@
   </si>
   <si>
     <t>@field:Max(10)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>三択</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">サンタク </t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>NOT</t>
+  </si>
+  <si>
+    <t>NOT</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>必須(Kt)</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">ヒッス </t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Nullable(Kt)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>変更不可変数(Kt)</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -3644,12 +3674,87 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="60" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3659,9 +3764,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3674,12 +3776,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3718,84 +3814,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3819,15 +3837,33 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="62" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3838,12 +3874,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="65" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4436,137 +4466,137 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="185" t="s">
+      <c r="A5" s="139" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="185"/>
-      <c r="C5" s="185"/>
-      <c r="D5" s="185"/>
-      <c r="E5" s="185"/>
+      <c r="B5" s="139"/>
+      <c r="C5" s="139"/>
+      <c r="D5" s="139"/>
+      <c r="E5" s="139"/>
       <c r="F5" s="55"/>
       <c r="G5" s="55"/>
       <c r="H5" s="95"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="182" t="s">
+      <c r="A6" s="143" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="183"/>
-      <c r="C6" s="184"/>
-      <c r="D6" s="181" t="s">
+      <c r="B6" s="144"/>
+      <c r="C6" s="145"/>
+      <c r="D6" s="140" t="s">
         <v>197</v>
       </c>
-      <c r="E6" s="181"/>
+      <c r="E6" s="140"/>
       <c r="F6" s="55"/>
       <c r="G6" s="55"/>
       <c r="H6" s="95"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="185" t="s">
+      <c r="A7" s="139" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="185"/>
-      <c r="C7" s="185"/>
-      <c r="D7" s="181" t="s">
+      <c r="B7" s="139"/>
+      <c r="C7" s="139"/>
+      <c r="D7" s="140" t="s">
         <v>166</v>
       </c>
-      <c r="E7" s="181"/>
+      <c r="E7" s="140"/>
       <c r="F7" s="55"/>
       <c r="G7" s="55"/>
       <c r="H7" s="95"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="185" t="s">
+      <c r="A8" s="139" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="185"/>
-      <c r="C8" s="185"/>
-      <c r="D8" s="181" t="s">
+      <c r="B8" s="139"/>
+      <c r="C8" s="139"/>
+      <c r="D8" s="140" t="s">
         <v>162</v>
       </c>
-      <c r="E8" s="181"/>
+      <c r="E8" s="140"/>
       <c r="F8" s="95"/>
       <c r="G8" s="95"/>
       <c r="H8" s="95"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="185" t="s">
+      <c r="A9" s="139" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="185"/>
-      <c r="C9" s="185"/>
-      <c r="D9" s="181" t="s">
+      <c r="B9" s="139"/>
+      <c r="C9" s="139"/>
+      <c r="D9" s="140" t="s">
         <v>100</v>
       </c>
-      <c r="E9" s="181"/>
+      <c r="E9" s="140"/>
       <c r="F9" s="95"/>
       <c r="G9" s="95"/>
       <c r="H9" s="95"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="185" t="s">
+      <c r="A10" s="139" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="185"/>
-      <c r="C10" s="185"/>
-      <c r="D10" s="181"/>
-      <c r="E10" s="181"/>
+      <c r="B10" s="139"/>
+      <c r="C10" s="139"/>
+      <c r="D10" s="140"/>
+      <c r="E10" s="140"/>
       <c r="F10" s="95"/>
       <c r="G10" s="95"/>
       <c r="H10" s="95"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="185" t="s">
+      <c r="A11" s="139" t="s">
         <v>99</v>
       </c>
-      <c r="B11" s="185"/>
-      <c r="C11" s="185"/>
-      <c r="D11" s="181" t="s">
+      <c r="B11" s="139"/>
+      <c r="C11" s="139"/>
+      <c r="D11" s="140" t="s">
         <v>163</v>
       </c>
-      <c r="E11" s="181"/>
+      <c r="E11" s="140"/>
       <c r="F11" s="95"/>
       <c r="G11" s="95"/>
       <c r="H11" s="95"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="144" t="s">
+      <c r="A12" s="146" t="s">
         <v>174</v>
       </c>
-      <c r="B12" s="144"/>
-      <c r="C12" s="144"/>
-      <c r="D12" s="165" t="s">
+      <c r="B12" s="146"/>
+      <c r="C12" s="146"/>
+      <c r="D12" s="141" t="s">
         <v>175</v>
       </c>
-      <c r="E12" s="165"/>
+      <c r="E12" s="141"/>
       <c r="F12" s="95" t="s">
         <v>176</v>
       </c>
       <c r="G12" s="54"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="144" t="s">
+      <c r="A13" s="146" t="s">
         <v>212</v>
       </c>
-      <c r="B13" s="144"/>
-      <c r="C13" s="144"/>
-      <c r="D13" s="165" t="s">
+      <c r="B13" s="146"/>
+      <c r="C13" s="146"/>
+      <c r="D13" s="141" t="s">
         <v>210</v>
       </c>
-      <c r="E13" s="165"/>
+      <c r="E13" s="141"/>
       <c r="F13" s="95" t="s">
         <v>211</v>
       </c>
       <c r="G13" s="54"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="144" t="s">
+      <c r="A14" s="146" t="s">
         <v>177</v>
       </c>
-      <c r="B14" s="144"/>
-      <c r="C14" s="144"/>
-      <c r="D14" s="164"/>
-      <c r="E14" s="165"/>
+      <c r="B14" s="146"/>
+      <c r="C14" s="146"/>
+      <c r="D14" s="142"/>
+      <c r="E14" s="141"/>
       <c r="F14" s="54" t="s">
         <v>198</v>
       </c>
@@ -4574,15 +4604,15 @@
       <c r="H14" s="95"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="144" t="s">
+      <c r="A15" s="146" t="s">
         <v>217</v>
       </c>
-      <c r="B15" s="144"/>
-      <c r="C15" s="144"/>
-      <c r="D15" s="164" t="s">
+      <c r="B15" s="146"/>
+      <c r="C15" s="146"/>
+      <c r="D15" s="142" t="s">
         <v>215</v>
       </c>
-      <c r="E15" s="165"/>
+      <c r="E15" s="141"/>
       <c r="F15" s="54" t="s">
         <v>220</v>
       </c>
@@ -4590,13 +4620,13 @@
       <c r="H15" s="95"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="144" t="s">
+      <c r="A16" s="146" t="s">
         <v>216</v>
       </c>
-      <c r="B16" s="144"/>
-      <c r="C16" s="144"/>
-      <c r="D16" s="164"/>
-      <c r="E16" s="165"/>
+      <c r="B16" s="146"/>
+      <c r="C16" s="146"/>
+      <c r="D16" s="142"/>
+      <c r="E16" s="141"/>
       <c r="F16" s="54" t="s">
         <v>219</v>
       </c>
@@ -4604,13 +4634,13 @@
       <c r="H16" s="95"/>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="144" t="s">
+      <c r="A17" s="146" t="s">
         <v>214</v>
       </c>
-      <c r="B17" s="144"/>
-      <c r="C17" s="144"/>
-      <c r="D17" s="164"/>
-      <c r="E17" s="165"/>
+      <c r="B17" s="146"/>
+      <c r="C17" s="146"/>
+      <c r="D17" s="142"/>
+      <c r="E17" s="141"/>
       <c r="F17" s="54" t="s">
         <v>213</v>
       </c>
@@ -4618,19 +4648,19 @@
       <c r="H17" s="95"/>
     </row>
     <row r="18" spans="1:15">
-      <c r="A18" s="161" t="s">
+      <c r="A18" s="183" t="s">
         <v>143</v>
       </c>
-      <c r="B18" s="162"/>
-      <c r="C18" s="163"/>
+      <c r="B18" s="184"/>
+      <c r="C18" s="185"/>
       <c r="D18" s="114"/>
     </row>
     <row r="19" spans="1:15">
-      <c r="A19" s="145" t="s">
+      <c r="A19" s="169" t="s">
         <v>179</v>
       </c>
-      <c r="B19" s="146"/>
-      <c r="C19" s="147"/>
+      <c r="B19" s="170"/>
+      <c r="C19" s="171"/>
       <c r="D19" s="100"/>
       <c r="E19" t="s">
         <v>180</v>
@@ -4648,15 +4678,15 @@
       <c r="B20" s="6"/>
     </row>
     <row r="21" spans="1:15">
-      <c r="A21" s="158" t="s">
+      <c r="A21" s="180" t="s">
         <v>188</v>
       </c>
-      <c r="B21" s="159"/>
-      <c r="C21" s="159"/>
-      <c r="D21" s="159"/>
-      <c r="E21" s="159"/>
-      <c r="F21" s="159"/>
-      <c r="G21" s="160"/>
+      <c r="B21" s="181"/>
+      <c r="C21" s="181"/>
+      <c r="D21" s="181"/>
+      <c r="E21" s="181"/>
+      <c r="F21" s="181"/>
+      <c r="G21" s="182"/>
       <c r="H21" s="1" t="s">
         <v>223</v>
       </c>
@@ -4707,28 +4737,28 @@
       <c r="C25"/>
     </row>
     <row r="26" spans="1:15">
-      <c r="A26" s="157" t="s">
+      <c r="A26" s="179" t="s">
         <v>189</v>
       </c>
-      <c r="B26" s="157"/>
-      <c r="C26" s="157"/>
-      <c r="D26" s="157"/>
-      <c r="E26" s="157"/>
-      <c r="F26" s="157"/>
-      <c r="G26" s="157"/>
+      <c r="B26" s="179"/>
+      <c r="C26" s="179"/>
+      <c r="D26" s="179"/>
+      <c r="E26" s="179"/>
+      <c r="F26" s="179"/>
+      <c r="G26" s="179"/>
     </row>
     <row r="27" spans="1:15">
       <c r="A27" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B27" s="151" t="s">
+      <c r="B27" s="173" t="s">
         <v>183</v>
       </c>
-      <c r="C27" s="152"/>
-      <c r="D27" s="152"/>
-      <c r="E27" s="152"/>
-      <c r="F27" s="152"/>
-      <c r="G27" s="153"/>
+      <c r="C27" s="174"/>
+      <c r="D27" s="174"/>
+      <c r="E27" s="174"/>
+      <c r="F27" s="174"/>
+      <c r="G27" s="175"/>
       <c r="H27" s="105"/>
       <c r="I27" s="105"/>
       <c r="J27" s="105"/>
@@ -4739,12 +4769,12 @@
     </row>
     <row r="28" spans="1:15">
       <c r="A28" s="116"/>
-      <c r="B28" s="168"/>
-      <c r="C28" s="168"/>
-      <c r="D28" s="168"/>
-      <c r="E28" s="168"/>
-      <c r="F28" s="168"/>
-      <c r="G28" s="168"/>
+      <c r="B28" s="157"/>
+      <c r="C28" s="157"/>
+      <c r="D28" s="157"/>
+      <c r="E28" s="157"/>
+      <c r="F28" s="157"/>
+      <c r="G28" s="157"/>
       <c r="H28" s="112"/>
       <c r="I28" s="112"/>
       <c r="J28" s="112"/>
@@ -4755,12 +4785,12 @@
     </row>
     <row r="29" spans="1:15">
       <c r="A29" s="117"/>
-      <c r="B29" s="169"/>
-      <c r="C29" s="169"/>
-      <c r="D29" s="169"/>
-      <c r="E29" s="169"/>
-      <c r="F29" s="169"/>
-      <c r="G29" s="169"/>
+      <c r="B29" s="159"/>
+      <c r="C29" s="159"/>
+      <c r="D29" s="159"/>
+      <c r="E29" s="159"/>
+      <c r="F29" s="159"/>
+      <c r="G29" s="159"/>
       <c r="H29" s="112"/>
       <c r="I29" s="112"/>
       <c r="J29" s="112"/>
@@ -4771,12 +4801,12 @@
     </row>
     <row r="30" spans="1:15">
       <c r="A30" s="118"/>
-      <c r="B30" s="170"/>
-      <c r="C30" s="170"/>
-      <c r="D30" s="170"/>
-      <c r="E30" s="170"/>
-      <c r="F30" s="170"/>
-      <c r="G30" s="170"/>
+      <c r="B30" s="161"/>
+      <c r="C30" s="161"/>
+      <c r="D30" s="161"/>
+      <c r="E30" s="161"/>
+      <c r="F30" s="161"/>
+      <c r="G30" s="161"/>
       <c r="H30" s="112"/>
       <c r="I30" s="112"/>
       <c r="J30" s="112"/>
@@ -4789,28 +4819,28 @@
       <c r="C31"/>
     </row>
     <row r="32" spans="1:15">
-      <c r="A32" s="154" t="s">
+      <c r="A32" s="176" t="s">
         <v>190</v>
       </c>
-      <c r="B32" s="155"/>
-      <c r="C32" s="155"/>
-      <c r="D32" s="155"/>
-      <c r="E32" s="155"/>
-      <c r="F32" s="155"/>
-      <c r="G32" s="156"/>
+      <c r="B32" s="177"/>
+      <c r="C32" s="177"/>
+      <c r="D32" s="177"/>
+      <c r="E32" s="177"/>
+      <c r="F32" s="177"/>
+      <c r="G32" s="178"/>
     </row>
     <row r="33" spans="1:15">
       <c r="A33" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B33" s="174" t="s">
+      <c r="B33" s="153" t="s">
         <v>184</v>
       </c>
-      <c r="C33" s="174"/>
-      <c r="D33" s="174"/>
-      <c r="E33" s="174"/>
-      <c r="F33" s="174"/>
-      <c r="G33" s="174"/>
+      <c r="C33" s="153"/>
+      <c r="D33" s="153"/>
+      <c r="E33" s="153"/>
+      <c r="F33" s="153"/>
+      <c r="G33" s="153"/>
       <c r="H33" s="105"/>
       <c r="I33" s="105"/>
       <c r="J33" s="105"/>
@@ -4823,14 +4853,14 @@
       <c r="A34" s="116">
         <v>1</v>
       </c>
-      <c r="B34" s="175" t="s">
+      <c r="B34" s="154" t="s">
         <v>218</v>
       </c>
-      <c r="C34" s="175"/>
-      <c r="D34" s="175"/>
-      <c r="E34" s="175"/>
-      <c r="F34" s="175"/>
-      <c r="G34" s="175"/>
+      <c r="C34" s="154"/>
+      <c r="D34" s="154"/>
+      <c r="E34" s="154"/>
+      <c r="F34" s="154"/>
+      <c r="G34" s="154"/>
       <c r="H34" s="112"/>
       <c r="I34" s="112"/>
       <c r="J34" s="112"/>
@@ -4841,12 +4871,12 @@
     </row>
     <row r="35" spans="1:15">
       <c r="A35" s="117"/>
-      <c r="B35" s="176"/>
-      <c r="C35" s="176"/>
-      <c r="D35" s="176"/>
-      <c r="E35" s="176"/>
-      <c r="F35" s="176"/>
-      <c r="G35" s="176"/>
+      <c r="B35" s="155"/>
+      <c r="C35" s="155"/>
+      <c r="D35" s="155"/>
+      <c r="E35" s="155"/>
+      <c r="F35" s="155"/>
+      <c r="G35" s="155"/>
       <c r="H35" s="112"/>
       <c r="I35" s="112"/>
       <c r="J35" s="112"/>
@@ -4857,12 +4887,12 @@
     </row>
     <row r="36" spans="1:15">
       <c r="A36" s="118"/>
-      <c r="B36" s="177"/>
-      <c r="C36" s="177"/>
-      <c r="D36" s="177"/>
-      <c r="E36" s="177"/>
-      <c r="F36" s="177"/>
-      <c r="G36" s="177"/>
+      <c r="B36" s="156"/>
+      <c r="C36" s="156"/>
+      <c r="D36" s="156"/>
+      <c r="E36" s="156"/>
+      <c r="F36" s="156"/>
+      <c r="G36" s="156"/>
       <c r="H36" s="112"/>
       <c r="I36" s="112"/>
       <c r="J36" s="112"/>
@@ -4887,28 +4917,28 @@
       <c r="M37"/>
     </row>
     <row r="38" spans="1:15">
-      <c r="A38" s="154" t="s">
+      <c r="A38" s="176" t="s">
         <v>191</v>
       </c>
-      <c r="B38" s="155"/>
-      <c r="C38" s="155"/>
-      <c r="D38" s="155"/>
-      <c r="E38" s="155"/>
-      <c r="F38" s="155"/>
-      <c r="G38" s="156"/>
+      <c r="B38" s="177"/>
+      <c r="C38" s="177"/>
+      <c r="D38" s="177"/>
+      <c r="E38" s="177"/>
+      <c r="F38" s="177"/>
+      <c r="G38" s="178"/>
     </row>
     <row r="39" spans="1:15">
       <c r="A39" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B39" s="174" t="s">
+      <c r="B39" s="153" t="s">
         <v>186</v>
       </c>
-      <c r="C39" s="174"/>
-      <c r="D39" s="174"/>
-      <c r="E39" s="174"/>
-      <c r="F39" s="174"/>
-      <c r="G39" s="174"/>
+      <c r="C39" s="153"/>
+      <c r="D39" s="153"/>
+      <c r="E39" s="153"/>
+      <c r="F39" s="153"/>
+      <c r="G39" s="153"/>
       <c r="H39" s="105"/>
       <c r="I39" s="105"/>
       <c r="J39" s="105"/>
@@ -4919,12 +4949,12 @@
     </row>
     <row r="40" spans="1:15">
       <c r="A40" s="116"/>
-      <c r="B40" s="168"/>
-      <c r="C40" s="168"/>
-      <c r="D40" s="168"/>
-      <c r="E40" s="168"/>
-      <c r="F40" s="168"/>
-      <c r="G40" s="178"/>
+      <c r="B40" s="157"/>
+      <c r="C40" s="157"/>
+      <c r="D40" s="157"/>
+      <c r="E40" s="157"/>
+      <c r="F40" s="157"/>
+      <c r="G40" s="158"/>
       <c r="H40" s="112"/>
       <c r="I40" s="112"/>
       <c r="J40" s="112"/>
@@ -4935,12 +4965,12 @@
     </row>
     <row r="41" spans="1:15">
       <c r="A41" s="117"/>
-      <c r="B41" s="169"/>
-      <c r="C41" s="169"/>
-      <c r="D41" s="169"/>
-      <c r="E41" s="169"/>
-      <c r="F41" s="169"/>
-      <c r="G41" s="179"/>
+      <c r="B41" s="159"/>
+      <c r="C41" s="159"/>
+      <c r="D41" s="159"/>
+      <c r="E41" s="159"/>
+      <c r="F41" s="159"/>
+      <c r="G41" s="160"/>
       <c r="H41" s="112"/>
       <c r="I41" s="112"/>
       <c r="J41" s="112"/>
@@ -4951,12 +4981,12 @@
     </row>
     <row r="42" spans="1:15">
       <c r="A42" s="118"/>
-      <c r="B42" s="170"/>
-      <c r="C42" s="170"/>
-      <c r="D42" s="170"/>
-      <c r="E42" s="170"/>
-      <c r="F42" s="170"/>
-      <c r="G42" s="180"/>
+      <c r="B42" s="161"/>
+      <c r="C42" s="161"/>
+      <c r="D42" s="161"/>
+      <c r="E42" s="161"/>
+      <c r="F42" s="161"/>
+      <c r="G42" s="162"/>
       <c r="H42" s="112"/>
       <c r="I42" s="112"/>
       <c r="J42" s="112"/>
@@ -4991,226 +5021,295 @@
       <c r="F44" s="5"/>
     </row>
     <row r="45" spans="1:15">
-      <c r="A45" s="141" t="s">
+      <c r="A45" s="166" t="s">
         <v>65</v>
       </c>
-      <c r="B45" s="148"/>
-      <c r="C45" s="141" t="s">
+      <c r="B45" s="172"/>
+      <c r="C45" s="166" t="s">
         <v>66</v>
       </c>
-      <c r="D45" s="142"/>
-      <c r="E45" s="143"/>
+      <c r="D45" s="167"/>
+      <c r="E45" s="168"/>
       <c r="F45" s="29" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:15">
-      <c r="A46" s="149"/>
-      <c r="B46" s="150"/>
-      <c r="C46" s="149"/>
-      <c r="D46" s="171"/>
-      <c r="E46" s="150"/>
+      <c r="A46" s="163"/>
+      <c r="B46" s="165"/>
+      <c r="C46" s="163"/>
+      <c r="D46" s="164"/>
+      <c r="E46" s="165"/>
       <c r="F46" s="49"/>
     </row>
     <row r="47" spans="1:15">
-      <c r="A47" s="139"/>
-      <c r="B47" s="140"/>
-      <c r="C47" s="139"/>
-      <c r="D47" s="172"/>
-      <c r="E47" s="140"/>
+      <c r="A47" s="147"/>
+      <c r="B47" s="149"/>
+      <c r="C47" s="147"/>
+      <c r="D47" s="148"/>
+      <c r="E47" s="149"/>
       <c r="F47" s="49"/>
     </row>
     <row r="48" spans="1:15">
-      <c r="A48" s="139"/>
-      <c r="B48" s="140"/>
-      <c r="C48" s="139"/>
-      <c r="D48" s="172"/>
-      <c r="E48" s="140"/>
+      <c r="A48" s="147"/>
+      <c r="B48" s="149"/>
+      <c r="C48" s="147"/>
+      <c r="D48" s="148"/>
+      <c r="E48" s="149"/>
       <c r="F48" s="49"/>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="139"/>
-      <c r="B49" s="140"/>
-      <c r="C49" s="139"/>
-      <c r="D49" s="172"/>
-      <c r="E49" s="140"/>
+      <c r="A49" s="147"/>
+      <c r="B49" s="149"/>
+      <c r="C49" s="147"/>
+      <c r="D49" s="148"/>
+      <c r="E49" s="149"/>
       <c r="F49" s="49"/>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="139"/>
-      <c r="B50" s="140"/>
-      <c r="C50" s="139"/>
-      <c r="D50" s="172"/>
-      <c r="E50" s="140"/>
+      <c r="A50" s="147"/>
+      <c r="B50" s="149"/>
+      <c r="C50" s="147"/>
+      <c r="D50" s="148"/>
+      <c r="E50" s="149"/>
       <c r="F50" s="49"/>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="139"/>
-      <c r="B51" s="140"/>
-      <c r="C51" s="139"/>
-      <c r="D51" s="172"/>
-      <c r="E51" s="140"/>
+      <c r="A51" s="147"/>
+      <c r="B51" s="149"/>
+      <c r="C51" s="147"/>
+      <c r="D51" s="148"/>
+      <c r="E51" s="149"/>
       <c r="F51" s="49"/>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="139"/>
-      <c r="B52" s="140"/>
-      <c r="C52" s="139"/>
-      <c r="D52" s="172"/>
-      <c r="E52" s="140"/>
+      <c r="A52" s="147"/>
+      <c r="B52" s="149"/>
+      <c r="C52" s="147"/>
+      <c r="D52" s="148"/>
+      <c r="E52" s="149"/>
       <c r="F52" s="49"/>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="139"/>
-      <c r="B53" s="140"/>
-      <c r="C53" s="139"/>
-      <c r="D53" s="172"/>
-      <c r="E53" s="140"/>
+      <c r="A53" s="147"/>
+      <c r="B53" s="149"/>
+      <c r="C53" s="147"/>
+      <c r="D53" s="148"/>
+      <c r="E53" s="149"/>
       <c r="F53" s="49"/>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="139"/>
-      <c r="B54" s="140"/>
-      <c r="C54" s="139"/>
-      <c r="D54" s="172"/>
-      <c r="E54" s="140"/>
+      <c r="A54" s="147"/>
+      <c r="B54" s="149"/>
+      <c r="C54" s="147"/>
+      <c r="D54" s="148"/>
+      <c r="E54" s="149"/>
       <c r="F54" s="49"/>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="139"/>
-      <c r="B55" s="140"/>
-      <c r="C55" s="139"/>
-      <c r="D55" s="172"/>
-      <c r="E55" s="140"/>
+      <c r="A55" s="147"/>
+      <c r="B55" s="149"/>
+      <c r="C55" s="147"/>
+      <c r="D55" s="148"/>
+      <c r="E55" s="149"/>
       <c r="F55" s="49"/>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="139"/>
-      <c r="B56" s="140"/>
-      <c r="C56" s="139"/>
-      <c r="D56" s="172"/>
-      <c r="E56" s="140"/>
+      <c r="A56" s="147"/>
+      <c r="B56" s="149"/>
+      <c r="C56" s="147"/>
+      <c r="D56" s="148"/>
+      <c r="E56" s="149"/>
       <c r="F56" s="49"/>
     </row>
     <row r="57" spans="1:6">
-      <c r="A57" s="139"/>
-      <c r="B57" s="140"/>
-      <c r="C57" s="139"/>
-      <c r="D57" s="172"/>
-      <c r="E57" s="140"/>
+      <c r="A57" s="147"/>
+      <c r="B57" s="149"/>
+      <c r="C57" s="147"/>
+      <c r="D57" s="148"/>
+      <c r="E57" s="149"/>
       <c r="F57" s="49"/>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="139"/>
-      <c r="B58" s="140"/>
-      <c r="C58" s="139"/>
-      <c r="D58" s="172"/>
-      <c r="E58" s="140"/>
+      <c r="A58" s="147"/>
+      <c r="B58" s="149"/>
+      <c r="C58" s="147"/>
+      <c r="D58" s="148"/>
+      <c r="E58" s="149"/>
       <c r="F58" s="49"/>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="139"/>
-      <c r="B59" s="140"/>
-      <c r="C59" s="139"/>
-      <c r="D59" s="172"/>
-      <c r="E59" s="140"/>
+      <c r="A59" s="147"/>
+      <c r="B59" s="149"/>
+      <c r="C59" s="147"/>
+      <c r="D59" s="148"/>
+      <c r="E59" s="149"/>
       <c r="F59" s="49"/>
     </row>
     <row r="60" spans="1:6">
-      <c r="A60" s="139"/>
-      <c r="B60" s="140"/>
-      <c r="C60" s="139"/>
-      <c r="D60" s="172"/>
-      <c r="E60" s="140"/>
+      <c r="A60" s="147"/>
+      <c r="B60" s="149"/>
+      <c r="C60" s="147"/>
+      <c r="D60" s="148"/>
+      <c r="E60" s="149"/>
       <c r="F60" s="49"/>
     </row>
     <row r="61" spans="1:6">
-      <c r="A61" s="139"/>
-      <c r="B61" s="140"/>
-      <c r="C61" s="139"/>
-      <c r="D61" s="172"/>
-      <c r="E61" s="140"/>
+      <c r="A61" s="147"/>
+      <c r="B61" s="149"/>
+      <c r="C61" s="147"/>
+      <c r="D61" s="148"/>
+      <c r="E61" s="149"/>
       <c r="F61" s="49"/>
     </row>
     <row r="62" spans="1:6">
-      <c r="A62" s="139"/>
-      <c r="B62" s="140"/>
-      <c r="C62" s="139"/>
-      <c r="D62" s="172"/>
-      <c r="E62" s="140"/>
+      <c r="A62" s="147"/>
+      <c r="B62" s="149"/>
+      <c r="C62" s="147"/>
+      <c r="D62" s="148"/>
+      <c r="E62" s="149"/>
       <c r="F62" s="49"/>
     </row>
     <row r="63" spans="1:6">
-      <c r="A63" s="139"/>
-      <c r="B63" s="140"/>
-      <c r="C63" s="139"/>
-      <c r="D63" s="172"/>
-      <c r="E63" s="140"/>
+      <c r="A63" s="147"/>
+      <c r="B63" s="149"/>
+      <c r="C63" s="147"/>
+      <c r="D63" s="148"/>
+      <c r="E63" s="149"/>
       <c r="F63" s="49"/>
     </row>
     <row r="64" spans="1:6">
-      <c r="A64" s="139"/>
-      <c r="B64" s="140"/>
-      <c r="C64" s="139"/>
-      <c r="D64" s="172"/>
-      <c r="E64" s="140"/>
+      <c r="A64" s="147"/>
+      <c r="B64" s="149"/>
+      <c r="C64" s="147"/>
+      <c r="D64" s="148"/>
+      <c r="E64" s="149"/>
       <c r="F64" s="49"/>
     </row>
     <row r="65" spans="1:6">
-      <c r="A65" s="139"/>
-      <c r="B65" s="140"/>
-      <c r="C65" s="139"/>
-      <c r="D65" s="172"/>
-      <c r="E65" s="140"/>
+      <c r="A65" s="147"/>
+      <c r="B65" s="149"/>
+      <c r="C65" s="147"/>
+      <c r="D65" s="148"/>
+      <c r="E65" s="149"/>
       <c r="F65" s="49"/>
     </row>
     <row r="66" spans="1:6">
-      <c r="A66" s="139"/>
-      <c r="B66" s="140"/>
-      <c r="C66" s="139"/>
-      <c r="D66" s="172"/>
-      <c r="E66" s="140"/>
+      <c r="A66" s="147"/>
+      <c r="B66" s="149"/>
+      <c r="C66" s="147"/>
+      <c r="D66" s="148"/>
+      <c r="E66" s="149"/>
       <c r="F66" s="49"/>
     </row>
     <row r="67" spans="1:6">
-      <c r="A67" s="139"/>
-      <c r="B67" s="140"/>
-      <c r="C67" s="139"/>
-      <c r="D67" s="172"/>
-      <c r="E67" s="140"/>
+      <c r="A67" s="147"/>
+      <c r="B67" s="149"/>
+      <c r="C67" s="147"/>
+      <c r="D67" s="148"/>
+      <c r="E67" s="149"/>
       <c r="F67" s="49"/>
     </row>
     <row r="68" spans="1:6">
-      <c r="A68" s="139"/>
-      <c r="B68" s="140"/>
-      <c r="C68" s="139"/>
-      <c r="D68" s="172"/>
-      <c r="E68" s="140"/>
+      <c r="A68" s="147"/>
+      <c r="B68" s="149"/>
+      <c r="C68" s="147"/>
+      <c r="D68" s="148"/>
+      <c r="E68" s="149"/>
       <c r="F68" s="49"/>
     </row>
     <row r="69" spans="1:6">
-      <c r="A69" s="139"/>
-      <c r="B69" s="140"/>
-      <c r="C69" s="139"/>
-      <c r="D69" s="172"/>
-      <c r="E69" s="140"/>
+      <c r="A69" s="147"/>
+      <c r="B69" s="149"/>
+      <c r="C69" s="147"/>
+      <c r="D69" s="148"/>
+      <c r="E69" s="149"/>
       <c r="F69" s="49"/>
     </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="166"/>
-      <c r="B70" s="167"/>
-      <c r="C70" s="166"/>
-      <c r="D70" s="173"/>
-      <c r="E70" s="167"/>
+      <c r="A70" s="150"/>
+      <c r="B70" s="152"/>
+      <c r="C70" s="150"/>
+      <c r="D70" s="151"/>
+      <c r="E70" s="152"/>
       <c r="F70" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="95">
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="A38:G38"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C70:E70"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="B41:G41"/>
+    <mergeCell ref="B42:G42"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="C59:E59"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D13:E13"/>
@@ -5227,80 +5326,11 @@
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="A16:C16"/>
     <mergeCell ref="D16:E16"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="C70:E70"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B36:G36"/>
-    <mergeCell ref="B39:G39"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="B41:G41"/>
-    <mergeCell ref="B42:G42"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="C51:E51"/>
-    <mergeCell ref="C52:E52"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="A38:G38"/>
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="1">
@@ -5333,10 +5363,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z66"/>
+  <dimension ref="A1:AC66"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" topLeftCell="F26" workbookViewId="0">
+      <selection activeCell="Q51" sqref="Q51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -5347,52 +5377,55 @@
     <col min="4" max="6" width="20.1640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.5" style="1" customWidth="1"/>
     <col min="8" max="8" width="22.6640625" style="1" customWidth="1"/>
-    <col min="9" max="10" width="20.1640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="32" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.1640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="9.83203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10" style="1" customWidth="1"/>
-    <col min="16" max="16" width="7.1640625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="6.33203125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="6.6640625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="6.83203125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="9" style="1" customWidth="1"/>
-    <col min="21" max="21" width="16.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.83203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="20.1640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="32" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.83203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10" style="1" customWidth="1"/>
+    <col min="19" max="19" width="7.1640625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="6.33203125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="6.6640625" style="1" customWidth="1"/>
     <col min="22" max="22" width="6.83203125" style="1" customWidth="1"/>
-    <col min="23" max="23" width="18.6640625" style="1" customWidth="1"/>
-    <col min="24" max="24" width="43.5" style="1" customWidth="1"/>
-    <col min="25" max="25" width="11.33203125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="6.1640625" style="1" customWidth="1"/>
-    <col min="27" max="27" width="16.1640625" style="1" customWidth="1"/>
-    <col min="28" max="28" width="6.1640625" style="1" customWidth="1"/>
-    <col min="29" max="29" width="18.83203125" style="1" customWidth="1"/>
-    <col min="30" max="30" width="10.33203125" style="1" customWidth="1"/>
-    <col min="31" max="31" width="9.83203125" style="1" customWidth="1"/>
-    <col min="32" max="32" width="8.83203125" style="1"/>
-    <col min="33" max="33" width="9.1640625" style="1" customWidth="1"/>
-    <col min="34" max="16384" width="8.83203125" style="1"/>
+    <col min="23" max="23" width="9" style="1" customWidth="1"/>
+    <col min="24" max="24" width="16.6640625" style="1" customWidth="1"/>
+    <col min="25" max="25" width="6.83203125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="18.6640625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="43.5" style="1" customWidth="1"/>
+    <col min="28" max="28" width="11.33203125" style="1" customWidth="1"/>
+    <col min="29" max="29" width="6.1640625" style="1" customWidth="1"/>
+    <col min="30" max="30" width="16.1640625" style="1" customWidth="1"/>
+    <col min="31" max="31" width="6.1640625" style="1" customWidth="1"/>
+    <col min="32" max="32" width="18.83203125" style="1" customWidth="1"/>
+    <col min="33" max="33" width="10.33203125" style="1" customWidth="1"/>
+    <col min="34" max="34" width="9.83203125" style="1" customWidth="1"/>
+    <col min="35" max="35" width="8.83203125" style="1"/>
+    <col min="36" max="36" width="9.1640625" style="1" customWidth="1"/>
+    <col min="37" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="19">
+    <row r="1" spans="1:22" ht="19">
       <c r="A1" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:22">
       <c r="B2" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:22">
       <c r="B3" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:22">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -5403,11 +5436,14 @@
       <c r="F5" s="54"/>
       <c r="G5" s="28"/>
       <c r="H5" s="28"/>
-      <c r="M5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
       <c r="N5" s="28"/>
-      <c r="O5" s="28"/>
-    </row>
-    <row r="6" spans="1:19">
+      <c r="P5" s="28"/>
+      <c r="Q5" s="28"/>
+      <c r="R5" s="28"/>
+    </row>
+    <row r="6" spans="1:22">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -5421,11 +5457,14 @@
       <c r="F6" s="54"/>
       <c r="G6" s="28"/>
       <c r="H6" s="28"/>
-      <c r="M6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
       <c r="N6" s="28"/>
-      <c r="O6" s="28"/>
-    </row>
-    <row r="7" spans="1:19">
+      <c r="P6" s="28"/>
+      <c r="Q6" s="28"/>
+      <c r="R6" s="28"/>
+    </row>
+    <row r="7" spans="1:22">
       <c r="A7" s="4" t="s">
         <v>81</v>
       </c>
@@ -5438,15 +5477,18 @@
       <c r="F7" s="54"/>
       <c r="G7" s="54"/>
       <c r="H7" s="54"/>
-      <c r="M7" s="54"/>
+      <c r="I7" s="54"/>
+      <c r="J7" s="54"/>
       <c r="N7" s="54"/>
-      <c r="O7" s="54"/>
       <c r="P7" s="54"/>
       <c r="Q7" s="54"/>
       <c r="R7" s="54"/>
-      <c r="S7"/>
-    </row>
-    <row r="8" spans="1:19">
+      <c r="S7" s="54"/>
+      <c r="T7" s="54"/>
+      <c r="U7" s="54"/>
+      <c r="V7"/>
+    </row>
+    <row r="8" spans="1:22">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
@@ -5459,14 +5501,17 @@
       <c r="F8" s="28"/>
       <c r="G8" s="28"/>
       <c r="H8" s="28"/>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="M8" s="28"/>
       <c r="N8" s="28"/>
-      <c r="O8" s="28"/>
-    </row>
-    <row r="9" spans="1:19">
+      <c r="P8" s="28"/>
+      <c r="Q8" s="28"/>
+      <c r="R8" s="28"/>
+    </row>
+    <row r="9" spans="1:22">
       <c r="A9" s="4" t="s">
         <v>155</v>
       </c>
@@ -5479,11 +5524,14 @@
       <c r="F9" s="28"/>
       <c r="G9" s="28"/>
       <c r="H9" s="28"/>
-      <c r="M9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
       <c r="N9" s="28"/>
-      <c r="O9" s="28"/>
-    </row>
-    <row r="10" spans="1:19">
+      <c r="P9" s="28"/>
+      <c r="Q9" s="28"/>
+      <c r="R9" s="28"/>
+    </row>
+    <row r="10" spans="1:22">
       <c r="A10" s="56" t="s">
         <v>156</v>
       </c>
@@ -5493,11 +5541,14 @@
       <c r="E10" s="54"/>
       <c r="F10" s="54"/>
       <c r="H10" s="28"/>
-      <c r="M10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
       <c r="N10" s="28"/>
-      <c r="O10" s="28"/>
-    </row>
-    <row r="11" spans="1:19">
+      <c r="P10" s="28"/>
+      <c r="Q10" s="28"/>
+      <c r="R10" s="28"/>
+    </row>
+    <row r="11" spans="1:22">
       <c r="A11" s="56" t="s">
         <v>157</v>
       </c>
@@ -5507,11 +5558,14 @@
       <c r="E11" s="54"/>
       <c r="F11" s="54"/>
       <c r="H11" s="28"/>
-      <c r="M11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
       <c r="N11" s="28"/>
-      <c r="O11" s="28"/>
-    </row>
-    <row r="12" spans="1:19">
+      <c r="P11" s="28"/>
+      <c r="Q11" s="28"/>
+      <c r="R11" s="28"/>
+    </row>
+    <row r="12" spans="1:22">
       <c r="A12" s="56" t="s">
         <v>158</v>
       </c>
@@ -5521,11 +5575,14 @@
       <c r="E12" s="54"/>
       <c r="F12" s="54"/>
       <c r="H12" s="28"/>
-      <c r="M12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
       <c r="N12" s="28"/>
-      <c r="O12" s="28"/>
-    </row>
-    <row r="13" spans="1:19">
+      <c r="P12" s="28"/>
+      <c r="Q12" s="28"/>
+      <c r="R12" s="28"/>
+    </row>
+    <row r="13" spans="1:22">
       <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
@@ -5536,7 +5593,7 @@
       <c r="F13" s="54"/>
       <c r="G13" s="54"/>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:22">
       <c r="A14" s="4" t="s">
         <v>99</v>
       </c>
@@ -5548,89 +5605,95 @@
       <c r="E14" s="54"/>
       <c r="F14" s="54"/>
       <c r="G14" s="54"/>
-      <c r="I14"/>
-      <c r="J14"/>
       <c r="K14"/>
       <c r="L14"/>
-    </row>
-    <row r="15" spans="1:19">
+      <c r="M14"/>
+      <c r="O14"/>
+    </row>
+    <row r="15" spans="1:22">
       <c r="A15" s="122" t="s">
         <v>174</v>
       </c>
       <c r="B15" s="122"/>
-      <c r="C15" s="165" t="s">
+      <c r="C15" s="141" t="s">
         <v>175</v>
       </c>
-      <c r="D15" s="165"/>
+      <c r="D15" s="141"/>
       <c r="E15" s="95" t="s">
         <v>176</v>
       </c>
       <c r="G15" s="54"/>
-      <c r="I15"/>
-      <c r="J15"/>
       <c r="K15"/>
       <c r="L15"/>
-    </row>
-    <row r="16" spans="1:19">
+      <c r="M15"/>
+      <c r="O15"/>
+    </row>
+    <row r="16" spans="1:22">
       <c r="A16" s="122" t="s">
         <v>226</v>
       </c>
       <c r="B16" s="122"/>
-      <c r="C16" s="164" t="s">
+      <c r="C16" s="142" t="s">
         <v>230</v>
       </c>
-      <c r="D16" s="165"/>
+      <c r="D16" s="141"/>
       <c r="E16" s="55" t="s">
         <v>227</v>
       </c>
       <c r="F16" s="54"/>
       <c r="G16" s="54"/>
       <c r="H16" s="95"/>
-      <c r="I16"/>
-      <c r="J16"/>
+      <c r="I16" s="95"/>
+      <c r="J16" s="95"/>
       <c r="K16"/>
       <c r="L16"/>
-      <c r="M16" s="95"/>
+      <c r="M16"/>
       <c r="N16" s="95"/>
-      <c r="O16" s="95"/>
-    </row>
-    <row r="17" spans="1:22">
+      <c r="O16"/>
+      <c r="P16" s="95"/>
+      <c r="Q16" s="95"/>
+      <c r="R16" s="95"/>
+    </row>
+    <row r="17" spans="1:25">
       <c r="A17" s="122" t="s">
         <v>177</v>
       </c>
       <c r="B17" s="122"/>
-      <c r="C17" s="165" t="s">
+      <c r="C17" s="141" t="s">
         <v>178</v>
       </c>
-      <c r="D17" s="165"/>
+      <c r="D17" s="141"/>
       <c r="E17" s="55"/>
       <c r="F17" s="55"/>
       <c r="G17" s="54"/>
       <c r="H17" s="54"/>
-      <c r="P17" s="95"/>
-    </row>
-    <row r="18" spans="1:22">
+      <c r="S17" s="95"/>
+    </row>
+    <row r="18" spans="1:25">
       <c r="A18" s="122" t="s">
         <v>228</v>
       </c>
       <c r="B18" s="122"/>
-      <c r="C18" s="164"/>
-      <c r="D18" s="165"/>
+      <c r="C18" s="142"/>
+      <c r="D18" s="141"/>
       <c r="E18" s="55" t="s">
         <v>229</v>
       </c>
       <c r="F18" s="54"/>
       <c r="G18" s="54"/>
       <c r="H18" s="95"/>
-      <c r="I18"/>
-      <c r="J18"/>
+      <c r="I18" s="95"/>
+      <c r="J18" s="95"/>
       <c r="K18"/>
       <c r="L18"/>
-      <c r="M18" s="95"/>
+      <c r="M18"/>
       <c r="N18" s="95"/>
-      <c r="O18" s="95"/>
-    </row>
-    <row r="19" spans="1:22">
+      <c r="O18"/>
+      <c r="P18" s="95"/>
+      <c r="Q18" s="95"/>
+      <c r="R18" s="95"/>
+    </row>
+    <row r="19" spans="1:25">
       <c r="A19" s="123" t="s">
         <v>179</v>
       </c>
@@ -5655,156 +5718,171 @@
       <c r="Q19"/>
       <c r="R19"/>
       <c r="S19"/>
-    </row>
-    <row r="20" spans="1:22">
+      <c r="T19"/>
+      <c r="U19"/>
+      <c r="V19"/>
+    </row>
+    <row r="20" spans="1:25">
       <c r="A20" s="6"/>
       <c r="C20" s="28"/>
-      <c r="I20"/>
-      <c r="J20"/>
       <c r="K20"/>
       <c r="L20"/>
-    </row>
-    <row r="21" spans="1:22">
-      <c r="A21" s="157" t="s">
+      <c r="M20"/>
+      <c r="O20"/>
+    </row>
+    <row r="21" spans="1:25">
+      <c r="A21" s="179" t="s">
         <v>192</v>
       </c>
-      <c r="B21" s="157"/>
-      <c r="C21" s="157"/>
-      <c r="D21" s="157"/>
-      <c r="E21" s="157"/>
-      <c r="F21" s="157"/>
-      <c r="G21" s="157"/>
-      <c r="I21"/>
-      <c r="J21"/>
+      <c r="B21" s="179"/>
+      <c r="C21" s="179"/>
+      <c r="D21" s="179"/>
+      <c r="E21" s="179"/>
+      <c r="F21" s="179"/>
+      <c r="G21" s="179"/>
       <c r="K21"/>
       <c r="L21"/>
-    </row>
-    <row r="22" spans="1:22">
+      <c r="M21"/>
+      <c r="O21"/>
+    </row>
+    <row r="22" spans="1:25">
       <c r="A22" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B22" s="151" t="s">
+      <c r="B22" s="173" t="s">
         <v>183</v>
       </c>
-      <c r="C22" s="152"/>
-      <c r="D22" s="152"/>
-      <c r="E22" s="152"/>
-      <c r="F22" s="152"/>
-      <c r="G22" s="153"/>
+      <c r="C22" s="174"/>
+      <c r="D22" s="174"/>
+      <c r="E22" s="174"/>
+      <c r="F22" s="174"/>
+      <c r="G22" s="175"/>
       <c r="H22" s="105"/>
-      <c r="I22"/>
-      <c r="J22"/>
+      <c r="I22" s="105"/>
+      <c r="J22" s="105"/>
       <c r="K22"/>
       <c r="L22"/>
-      <c r="M22" s="105"/>
+      <c r="M22"/>
       <c r="N22" s="105"/>
-      <c r="O22" s="105"/>
+      <c r="O22"/>
       <c r="P22" s="105"/>
       <c r="Q22" s="105"/>
       <c r="R22" s="105"/>
       <c r="S22" s="105"/>
-      <c r="U22" s="111"/>
-      <c r="V22" s="111"/>
-    </row>
-    <row r="23" spans="1:22">
+      <c r="T22" s="105"/>
+      <c r="U22" s="105"/>
+      <c r="V22" s="105"/>
+      <c r="X22" s="111"/>
+      <c r="Y22" s="111"/>
+    </row>
+    <row r="23" spans="1:25">
       <c r="A23" s="116"/>
-      <c r="B23" s="168"/>
-      <c r="C23" s="168"/>
-      <c r="D23" s="168"/>
-      <c r="E23" s="168"/>
-      <c r="F23" s="168"/>
-      <c r="G23" s="168"/>
+      <c r="B23" s="157"/>
+      <c r="C23" s="157"/>
+      <c r="D23" s="157"/>
+      <c r="E23" s="157"/>
+      <c r="F23" s="157"/>
+      <c r="G23" s="157"/>
       <c r="H23" s="112"/>
-      <c r="I23"/>
-      <c r="J23"/>
+      <c r="I23" s="112"/>
+      <c r="J23" s="112"/>
       <c r="K23"/>
       <c r="L23"/>
-      <c r="M23" s="112"/>
+      <c r="M23"/>
       <c r="N23" s="112"/>
-      <c r="O23" s="112"/>
+      <c r="O23"/>
       <c r="P23" s="112"/>
       <c r="Q23" s="112"/>
       <c r="R23" s="112"/>
-      <c r="T23"/>
-      <c r="U23"/>
-      <c r="V23"/>
-    </row>
-    <row r="24" spans="1:22">
+      <c r="S23" s="112"/>
+      <c r="T23" s="112"/>
+      <c r="U23" s="112"/>
+      <c r="W23"/>
+      <c r="X23"/>
+      <c r="Y23"/>
+    </row>
+    <row r="24" spans="1:25">
       <c r="A24" s="117"/>
-      <c r="B24" s="169"/>
-      <c r="C24" s="169"/>
-      <c r="D24" s="169"/>
-      <c r="E24" s="169"/>
-      <c r="F24" s="169"/>
-      <c r="G24" s="169"/>
+      <c r="B24" s="159"/>
+      <c r="C24" s="159"/>
+      <c r="D24" s="159"/>
+      <c r="E24" s="159"/>
+      <c r="F24" s="159"/>
+      <c r="G24" s="159"/>
       <c r="H24" s="112"/>
-      <c r="I24"/>
-      <c r="J24"/>
+      <c r="I24" s="112"/>
+      <c r="J24" s="112"/>
       <c r="K24"/>
       <c r="L24"/>
-      <c r="M24" s="112"/>
+      <c r="M24"/>
       <c r="N24" s="112"/>
-      <c r="O24" s="112"/>
+      <c r="O24"/>
       <c r="P24" s="112"/>
       <c r="Q24" s="112"/>
       <c r="R24" s="112"/>
-      <c r="T24"/>
-      <c r="U24"/>
-      <c r="V24"/>
-    </row>
-    <row r="25" spans="1:22">
+      <c r="S24" s="112"/>
+      <c r="T24" s="112"/>
+      <c r="U24" s="112"/>
+      <c r="W24"/>
+      <c r="X24"/>
+      <c r="Y24"/>
+    </row>
+    <row r="25" spans="1:25">
       <c r="A25" s="118"/>
-      <c r="B25" s="170"/>
-      <c r="C25" s="170"/>
-      <c r="D25" s="170"/>
-      <c r="E25" s="170"/>
-      <c r="F25" s="170"/>
-      <c r="G25" s="170"/>
+      <c r="B25" s="161"/>
+      <c r="C25" s="161"/>
+      <c r="D25" s="161"/>
+      <c r="E25" s="161"/>
+      <c r="F25" s="161"/>
+      <c r="G25" s="161"/>
       <c r="H25" s="112"/>
-      <c r="M25" s="112"/>
+      <c r="I25" s="112"/>
+      <c r="J25" s="112"/>
       <c r="N25" s="112"/>
-      <c r="O25" s="112"/>
       <c r="P25" s="112"/>
       <c r="Q25" s="112"/>
       <c r="R25" s="112"/>
-      <c r="T25"/>
-      <c r="U25"/>
-      <c r="V25"/>
-    </row>
-    <row r="26" spans="1:22">
+      <c r="S25" s="112"/>
+      <c r="T25" s="112"/>
+      <c r="U25" s="112"/>
+      <c r="W25"/>
+      <c r="X25"/>
+      <c r="Y25"/>
+    </row>
+    <row r="26" spans="1:25">
       <c r="C26"/>
-      <c r="I26" s="105"/>
-      <c r="J26" s="105"/>
       <c r="K26" s="105"/>
       <c r="L26" s="105"/>
-    </row>
-    <row r="27" spans="1:22">
-      <c r="A27" s="154" t="s">
+      <c r="M26" s="105"/>
+      <c r="O26" s="105"/>
+    </row>
+    <row r="27" spans="1:25">
+      <c r="A27" s="176" t="s">
         <v>193</v>
       </c>
-      <c r="B27" s="155"/>
-      <c r="C27" s="155"/>
-      <c r="D27" s="155"/>
-      <c r="E27" s="155"/>
-      <c r="F27" s="155"/>
-      <c r="G27" s="156"/>
-      <c r="I27" s="105"/>
-      <c r="J27" s="105"/>
+      <c r="B27" s="177"/>
+      <c r="C27" s="177"/>
+      <c r="D27" s="177"/>
+      <c r="E27" s="177"/>
+      <c r="F27" s="177"/>
+      <c r="G27" s="178"/>
       <c r="K27" s="105"/>
       <c r="L27" s="105"/>
-    </row>
-    <row r="28" spans="1:22">
+      <c r="M27" s="105"/>
+      <c r="O27" s="105"/>
+    </row>
+    <row r="28" spans="1:25">
       <c r="A28" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B28" s="174" t="s">
+      <c r="B28" s="153" t="s">
         <v>184</v>
       </c>
-      <c r="C28" s="174"/>
-      <c r="D28" s="174"/>
-      <c r="E28" s="174"/>
-      <c r="F28" s="174"/>
-      <c r="G28" s="174"/>
+      <c r="C28" s="153"/>
+      <c r="D28" s="153"/>
+      <c r="E28" s="153"/>
+      <c r="F28" s="153"/>
+      <c r="G28" s="153"/>
       <c r="H28" s="105"/>
       <c r="I28" s="105"/>
       <c r="J28" s="105"/>
@@ -5817,79 +5895,91 @@
       <c r="Q28" s="105"/>
       <c r="R28" s="105"/>
       <c r="S28" s="105"/>
-      <c r="U28" s="111"/>
-      <c r="V28" s="111"/>
-    </row>
-    <row r="29" spans="1:22">
+      <c r="T28" s="105"/>
+      <c r="U28" s="105"/>
+      <c r="V28" s="105"/>
+      <c r="X28" s="111"/>
+      <c r="Y28" s="111"/>
+    </row>
+    <row r="29" spans="1:25">
       <c r="A29" s="116">
         <v>1</v>
       </c>
-      <c r="B29" s="175" t="s">
+      <c r="B29" s="154" t="s">
         <v>225</v>
       </c>
-      <c r="C29" s="175"/>
-      <c r="D29" s="175"/>
-      <c r="E29" s="175"/>
-      <c r="F29" s="175"/>
-      <c r="G29" s="175"/>
+      <c r="C29" s="154"/>
+      <c r="D29" s="154"/>
+      <c r="E29" s="154"/>
+      <c r="F29" s="154"/>
+      <c r="G29" s="154"/>
       <c r="H29" s="112"/>
-      <c r="I29"/>
-      <c r="J29"/>
+      <c r="I29" s="112"/>
+      <c r="J29" s="112"/>
       <c r="K29"/>
       <c r="L29"/>
-      <c r="M29" s="112"/>
+      <c r="M29"/>
       <c r="N29" s="112"/>
-      <c r="O29" s="112"/>
+      <c r="O29"/>
       <c r="P29" s="112"/>
       <c r="Q29" s="112"/>
       <c r="R29" s="112"/>
-      <c r="T29"/>
-      <c r="U29"/>
-      <c r="V29"/>
-    </row>
-    <row r="30" spans="1:22">
+      <c r="S29" s="112"/>
+      <c r="T29" s="112"/>
+      <c r="U29" s="112"/>
+      <c r="W29"/>
+      <c r="X29"/>
+      <c r="Y29"/>
+    </row>
+    <row r="30" spans="1:25">
       <c r="A30" s="117"/>
-      <c r="B30" s="176"/>
-      <c r="C30" s="176"/>
-      <c r="D30" s="176"/>
-      <c r="E30" s="176"/>
-      <c r="F30" s="176"/>
-      <c r="G30" s="176"/>
+      <c r="B30" s="155"/>
+      <c r="C30" s="155"/>
+      <c r="D30" s="155"/>
+      <c r="E30" s="155"/>
+      <c r="F30" s="155"/>
+      <c r="G30" s="155"/>
       <c r="H30" s="112"/>
-      <c r="M30" s="112"/>
+      <c r="I30" s="112"/>
+      <c r="J30" s="112"/>
       <c r="N30" s="112"/>
-      <c r="O30" s="112"/>
       <c r="P30" s="112"/>
       <c r="Q30" s="112"/>
       <c r="R30" s="112"/>
-      <c r="T30"/>
-      <c r="U30"/>
-      <c r="V30"/>
-    </row>
-    <row r="31" spans="1:22">
+      <c r="S30" s="112"/>
+      <c r="T30" s="112"/>
+      <c r="U30" s="112"/>
+      <c r="W30"/>
+      <c r="X30"/>
+      <c r="Y30"/>
+    </row>
+    <row r="31" spans="1:25">
       <c r="A31" s="118"/>
-      <c r="B31" s="177"/>
-      <c r="C31" s="177"/>
-      <c r="D31" s="177"/>
-      <c r="E31" s="177"/>
-      <c r="F31" s="177"/>
-      <c r="G31" s="177"/>
+      <c r="B31" s="156"/>
+      <c r="C31" s="156"/>
+      <c r="D31" s="156"/>
+      <c r="E31" s="156"/>
+      <c r="F31" s="156"/>
+      <c r="G31" s="156"/>
       <c r="H31" s="112"/>
-      <c r="I31" s="105"/>
-      <c r="J31" s="105"/>
+      <c r="I31" s="112"/>
+      <c r="J31" s="112"/>
       <c r="K31" s="105"/>
       <c r="L31" s="105"/>
-      <c r="M31" s="112"/>
+      <c r="M31" s="105"/>
       <c r="N31" s="112"/>
-      <c r="O31" s="112"/>
+      <c r="O31" s="105"/>
       <c r="P31" s="112"/>
       <c r="Q31" s="112"/>
       <c r="R31" s="112"/>
-      <c r="T31"/>
-      <c r="U31"/>
-      <c r="V31"/>
-    </row>
-    <row r="32" spans="1:22">
+      <c r="S31" s="112"/>
+      <c r="T31" s="112"/>
+      <c r="U31" s="112"/>
+      <c r="W31"/>
+      <c r="X31"/>
+      <c r="Y31"/>
+    </row>
+    <row r="32" spans="1:25">
       <c r="A32"/>
       <c r="B32"/>
       <c r="C32"/>
@@ -5898,123 +5988,138 @@
       <c r="F32"/>
       <c r="G32"/>
       <c r="H32"/>
-      <c r="I32" s="112"/>
-      <c r="J32" s="112"/>
+      <c r="I32"/>
+      <c r="J32"/>
       <c r="K32" s="112"/>
       <c r="L32" s="112"/>
-      <c r="M32"/>
+      <c r="M32" s="112"/>
       <c r="N32"/>
-      <c r="O32"/>
+      <c r="O32" s="112"/>
       <c r="P32"/>
       <c r="Q32"/>
       <c r="R32"/>
       <c r="S32"/>
       <c r="T32"/>
-    </row>
-    <row r="33" spans="1:26">
-      <c r="A33" s="154" t="s">
+      <c r="U32"/>
+      <c r="V32"/>
+      <c r="W32"/>
+    </row>
+    <row r="33" spans="1:29">
+      <c r="A33" s="176" t="s">
         <v>194</v>
       </c>
-      <c r="B33" s="155"/>
-      <c r="C33" s="155"/>
-      <c r="D33" s="155"/>
-      <c r="E33" s="155"/>
-      <c r="F33" s="155"/>
-      <c r="G33" s="156"/>
-      <c r="I33" s="112"/>
-      <c r="J33" s="112"/>
+      <c r="B33" s="177"/>
+      <c r="C33" s="177"/>
+      <c r="D33" s="177"/>
+      <c r="E33" s="177"/>
+      <c r="F33" s="177"/>
+      <c r="G33" s="178"/>
       <c r="K33" s="112"/>
       <c r="L33" s="112"/>
-    </row>
-    <row r="34" spans="1:26">
+      <c r="M33" s="112"/>
+      <c r="O33" s="112"/>
+    </row>
+    <row r="34" spans="1:29">
       <c r="A34" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="174" t="s">
+      <c r="B34" s="153" t="s">
         <v>186</v>
       </c>
-      <c r="C34" s="174"/>
-      <c r="D34" s="174"/>
-      <c r="E34" s="174"/>
-      <c r="F34" s="174"/>
-      <c r="G34" s="174"/>
+      <c r="C34" s="153"/>
+      <c r="D34" s="153"/>
+      <c r="E34" s="153"/>
+      <c r="F34" s="153"/>
+      <c r="G34" s="153"/>
       <c r="H34" s="105"/>
-      <c r="I34" s="112"/>
-      <c r="J34" s="112"/>
+      <c r="I34" s="105"/>
+      <c r="J34" s="105"/>
       <c r="K34" s="112"/>
       <c r="L34" s="112"/>
-      <c r="M34" s="105"/>
+      <c r="M34" s="112"/>
       <c r="N34" s="105"/>
-      <c r="O34" s="105"/>
+      <c r="O34" s="112"/>
       <c r="P34" s="105"/>
       <c r="Q34" s="105"/>
       <c r="R34" s="105"/>
       <c r="S34" s="105"/>
-      <c r="U34" s="111"/>
-      <c r="V34" s="111"/>
-    </row>
-    <row r="35" spans="1:26">
+      <c r="T34" s="105"/>
+      <c r="U34" s="105"/>
+      <c r="V34" s="105"/>
+      <c r="X34" s="111"/>
+      <c r="Y34" s="111"/>
+    </row>
+    <row r="35" spans="1:29">
       <c r="A35" s="116"/>
-      <c r="B35" s="168"/>
-      <c r="C35" s="168"/>
-      <c r="D35" s="168"/>
-      <c r="E35" s="168"/>
-      <c r="F35" s="168"/>
-      <c r="G35" s="178"/>
+      <c r="B35" s="157"/>
+      <c r="C35" s="157"/>
+      <c r="D35" s="157"/>
+      <c r="E35" s="157"/>
+      <c r="F35" s="157"/>
+      <c r="G35" s="158"/>
       <c r="H35" s="112"/>
-      <c r="I35"/>
-      <c r="J35"/>
+      <c r="I35" s="112"/>
+      <c r="J35" s="112"/>
       <c r="K35"/>
       <c r="L35"/>
-      <c r="M35" s="112"/>
+      <c r="M35"/>
       <c r="N35" s="112"/>
-      <c r="O35" s="112"/>
+      <c r="O35"/>
       <c r="P35" s="112"/>
       <c r="Q35" s="112"/>
       <c r="R35" s="112"/>
-      <c r="T35"/>
-      <c r="U35"/>
-      <c r="V35"/>
-    </row>
-    <row r="36" spans="1:26">
+      <c r="S35" s="112"/>
+      <c r="T35" s="112"/>
+      <c r="U35" s="112"/>
+      <c r="W35"/>
+      <c r="X35"/>
+      <c r="Y35"/>
+    </row>
+    <row r="36" spans="1:29">
       <c r="A36" s="117"/>
-      <c r="B36" s="169"/>
-      <c r="C36" s="169"/>
-      <c r="D36" s="169"/>
-      <c r="E36" s="169"/>
-      <c r="F36" s="169"/>
-      <c r="G36" s="179"/>
+      <c r="B36" s="159"/>
+      <c r="C36" s="159"/>
+      <c r="D36" s="159"/>
+      <c r="E36" s="159"/>
+      <c r="F36" s="159"/>
+      <c r="G36" s="160"/>
       <c r="H36" s="112"/>
-      <c r="M36" s="112"/>
+      <c r="I36" s="112"/>
+      <c r="J36" s="112"/>
       <c r="N36" s="112"/>
-      <c r="O36" s="112"/>
       <c r="P36" s="112"/>
       <c r="Q36" s="112"/>
       <c r="R36" s="112"/>
-      <c r="T36"/>
-      <c r="U36"/>
-      <c r="V36"/>
-    </row>
-    <row r="37" spans="1:26">
+      <c r="S36" s="112"/>
+      <c r="T36" s="112"/>
+      <c r="U36" s="112"/>
+      <c r="W36"/>
+      <c r="X36"/>
+      <c r="Y36"/>
+    </row>
+    <row r="37" spans="1:29">
       <c r="A37" s="118"/>
-      <c r="B37" s="170"/>
-      <c r="C37" s="170"/>
-      <c r="D37" s="170"/>
-      <c r="E37" s="170"/>
-      <c r="F37" s="170"/>
-      <c r="G37" s="180"/>
+      <c r="B37" s="161"/>
+      <c r="C37" s="161"/>
+      <c r="D37" s="161"/>
+      <c r="E37" s="161"/>
+      <c r="F37" s="161"/>
+      <c r="G37" s="162"/>
       <c r="H37" s="112"/>
-      <c r="M37" s="112"/>
+      <c r="I37" s="112"/>
+      <c r="J37" s="112"/>
       <c r="N37" s="112"/>
-      <c r="O37" s="112"/>
       <c r="P37" s="112"/>
       <c r="Q37" s="112"/>
       <c r="R37" s="112"/>
-      <c r="T37"/>
-      <c r="U37"/>
-      <c r="V37"/>
-    </row>
-    <row r="38" spans="1:26">
+      <c r="S37" s="112"/>
+      <c r="T37" s="112"/>
+      <c r="U37" s="112"/>
+      <c r="W37"/>
+      <c r="X37"/>
+      <c r="Y37"/>
+    </row>
+    <row r="38" spans="1:29">
       <c r="A38"/>
       <c r="B38"/>
       <c r="C38"/>
@@ -6023,19 +6128,22 @@
       <c r="F38"/>
       <c r="G38"/>
       <c r="H38"/>
-      <c r="M38"/>
+      <c r="I38"/>
+      <c r="J38"/>
       <c r="N38"/>
-      <c r="O38"/>
       <c r="P38"/>
       <c r="Q38"/>
       <c r="R38"/>
       <c r="S38"/>
       <c r="T38"/>
-    </row>
-    <row r="39" spans="1:26">
+      <c r="U38"/>
+      <c r="V38"/>
+      <c r="W38"/>
+    </row>
+    <row r="39" spans="1:29">
       <c r="A39" s="6"/>
     </row>
-    <row r="40" spans="1:26">
+    <row r="40" spans="1:29">
       <c r="A40" s="19" t="s">
         <v>10</v>
       </c>
@@ -6046,120 +6154,135 @@
       <c r="F40" s="119"/>
       <c r="G40" s="37"/>
       <c r="H40" s="37"/>
-      <c r="I40" s="132"/>
-      <c r="J40" s="132"/>
+      <c r="I40" s="37"/>
+      <c r="J40" s="37"/>
       <c r="K40" s="132"/>
       <c r="L40" s="132"/>
-      <c r="M40" s="37"/>
+      <c r="M40" s="132"/>
       <c r="N40" s="37"/>
-      <c r="O40" s="37"/>
+      <c r="O40" s="132"/>
       <c r="P40" s="37"/>
       <c r="Q40" s="37"/>
       <c r="R40" s="37"/>
       <c r="S40" s="37"/>
       <c r="T40" s="37"/>
-      <c r="U40" s="38"/>
-      <c r="V40" s="55"/>
-      <c r="W40" s="55"/>
-      <c r="X40" s="55"/>
-      <c r="Y40" s="39"/>
-      <c r="Z40" s="39"/>
-    </row>
-    <row r="41" spans="1:26">
-      <c r="A41" s="190" t="s">
+      <c r="U40" s="37"/>
+      <c r="V40" s="37"/>
+      <c r="W40" s="37"/>
+      <c r="X40" s="38"/>
+      <c r="Y40" s="55"/>
+      <c r="Z40" s="55"/>
+      <c r="AA40" s="55"/>
+      <c r="AB40" s="39"/>
+      <c r="AC40" s="39"/>
+    </row>
+    <row r="41" spans="1:29">
+      <c r="A41" s="186" t="s">
         <v>69</v>
       </c>
-      <c r="B41" s="190" t="s">
+      <c r="B41" s="186" t="s">
         <v>0</v>
       </c>
-      <c r="C41" s="192" t="s">
+      <c r="C41" s="188" t="s">
         <v>1</v>
       </c>
-      <c r="D41" s="190" t="s">
+      <c r="D41" s="186" t="s">
         <v>2</v>
       </c>
-      <c r="E41" s="193" t="s">
+      <c r="E41" s="189" t="s">
         <v>161</v>
       </c>
-      <c r="F41" s="193" t="s">
+      <c r="F41" s="189" t="s">
         <v>177</v>
       </c>
-      <c r="G41" s="190" t="s">
+      <c r="G41" s="186" t="s">
         <v>13</v>
       </c>
-      <c r="H41" s="190" t="s">
+      <c r="H41" s="186" t="s">
         <v>116</v>
       </c>
-      <c r="I41" s="197" t="s">
+      <c r="I41" s="186" t="s">
+        <v>195</v>
+      </c>
+      <c r="J41" s="186" t="s">
+        <v>209</v>
+      </c>
+      <c r="K41" s="193" t="s">
         <v>200</v>
       </c>
-      <c r="J41" s="197" t="s">
+      <c r="L41" s="193" t="s">
         <v>201</v>
       </c>
-      <c r="K41" s="197" t="s">
+      <c r="M41" s="193" t="s">
         <v>202</v>
       </c>
-      <c r="L41" s="186" t="s">
+      <c r="N41" s="186" t="s">
+        <v>235</v>
+      </c>
+      <c r="O41" s="196" t="s">
         <v>203</v>
       </c>
-      <c r="M41" s="190" t="s">
-        <v>195</v>
-      </c>
-      <c r="N41" s="190" t="s">
-        <v>209</v>
-      </c>
-      <c r="O41" s="192" t="s">
+      <c r="P41" s="186" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q41" s="186" t="s">
+        <v>237</v>
+      </c>
+      <c r="R41" s="188" t="s">
         <v>208</v>
       </c>
-      <c r="P41" s="188" t="s">
+      <c r="S41" s="194" t="s">
         <v>71</v>
       </c>
-      <c r="Q41" s="189"/>
-      <c r="R41" s="188" t="s">
+      <c r="T41" s="195"/>
+      <c r="U41" s="194" t="s">
         <v>17</v>
       </c>
-      <c r="S41" s="189"/>
-      <c r="T41" s="34" t="s">
+      <c r="V41" s="195"/>
+      <c r="W41" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="U41" s="190" t="s">
+      <c r="X41" s="186" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:26">
-      <c r="A42" s="191"/>
-      <c r="B42" s="191"/>
-      <c r="C42" s="191"/>
-      <c r="D42" s="191"/>
-      <c r="E42" s="194"/>
-      <c r="F42" s="195"/>
-      <c r="G42" s="191"/>
-      <c r="H42" s="191"/>
-      <c r="I42" s="197"/>
-      <c r="J42" s="197"/>
-      <c r="K42" s="197"/>
-      <c r="L42" s="187"/>
-      <c r="M42" s="196"/>
-      <c r="N42" s="196"/>
-      <c r="O42" s="196"/>
-      <c r="P42" s="29" t="s">
+    <row r="42" spans="1:29">
+      <c r="A42" s="187"/>
+      <c r="B42" s="187"/>
+      <c r="C42" s="187"/>
+      <c r="D42" s="187"/>
+      <c r="E42" s="190"/>
+      <c r="F42" s="191"/>
+      <c r="G42" s="187"/>
+      <c r="H42" s="187"/>
+      <c r="I42" s="192"/>
+      <c r="J42" s="192"/>
+      <c r="K42" s="193"/>
+      <c r="L42" s="193"/>
+      <c r="M42" s="193"/>
+      <c r="N42" s="192"/>
+      <c r="O42" s="197"/>
+      <c r="P42" s="192"/>
+      <c r="Q42" s="192"/>
+      <c r="R42" s="192"/>
+      <c r="S42" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="Q42" s="29" t="s">
+      <c r="T42" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="R42" s="29" t="s">
+      <c r="U42" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="S42" s="29" t="s">
+      <c r="V42" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="T42" s="29" t="s">
+      <c r="W42" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="U42" s="191"/>
-    </row>
-    <row r="43" spans="1:26" ht="30">
+      <c r="X42" s="187"/>
+    </row>
+    <row r="43" spans="1:29" ht="30">
       <c r="A43" s="7">
         <v>1</v>
       </c>
@@ -6178,35 +6301,44 @@
         <v>141</v>
       </c>
       <c r="H43" s="24"/>
-      <c r="I43" s="133" t="s">
+      <c r="I43" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="J43" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="K43" s="133" t="s">
         <v>204</v>
       </c>
-      <c r="J43" s="133"/>
-      <c r="K43" s="138" t="s">
+      <c r="L43" s="133"/>
+      <c r="M43" s="138" t="s">
         <v>224</v>
-      </c>
-      <c r="L43" s="133"/>
-      <c r="M43" s="24" t="s">
-        <v>141</v>
       </c>
       <c r="N43" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="O43" s="24" t="s">
+      <c r="O43" s="133"/>
+      <c r="P43" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="P43" s="24">
+      <c r="Q43" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="R43" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="S43" s="24">
         <v>0</v>
       </c>
-      <c r="Q43" s="30">
+      <c r="T43" s="30">
         <v>10</v>
       </c>
-      <c r="R43" s="24"/>
-      <c r="S43" s="30"/>
-      <c r="T43" s="30"/>
-      <c r="U43" s="9"/>
-    </row>
-    <row r="44" spans="1:26">
+      <c r="U43" s="24"/>
+      <c r="V43" s="30"/>
+      <c r="W43" s="30"/>
+      <c r="X43" s="9"/>
+    </row>
+    <row r="44" spans="1:29">
       <c r="A44" s="10">
         <f t="shared" ref="A44:A49" si="0">A43+1</f>
         <v>2</v>
@@ -6226,35 +6358,38 @@
         <v>141</v>
       </c>
       <c r="H44" s="25"/>
-      <c r="I44" s="135" t="s">
+      <c r="I44" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="J44" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="K44" s="135" t="s">
         <v>205</v>
       </c>
-      <c r="J44" s="135"/>
-      <c r="K44" s="136" t="s">
+      <c r="L44" s="135"/>
+      <c r="M44" s="136" t="s">
         <v>206</v>
       </c>
-      <c r="L44" s="135"/>
-      <c r="M44" s="25" t="s">
+      <c r="N44" s="25"/>
+      <c r="O44" s="135"/>
+      <c r="P44" s="25"/>
+      <c r="Q44" s="25"/>
+      <c r="R44" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="N44" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="O44" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="P44" s="21"/>
-      <c r="Q44" s="31"/>
-      <c r="R44" s="21">
+      <c r="S44" s="21"/>
+      <c r="T44" s="31"/>
+      <c r="U44" s="21">
         <v>0</v>
       </c>
-      <c r="S44" s="31">
+      <c r="V44" s="31">
         <v>100</v>
       </c>
-      <c r="T44" s="31"/>
-      <c r="U44" s="12"/>
-    </row>
-    <row r="45" spans="1:26">
+      <c r="W44" s="31"/>
+      <c r="X44" s="12"/>
+    </row>
+    <row r="45" spans="1:29">
       <c r="A45" s="10">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -6274,27 +6409,36 @@
       <c r="H45" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="I45" s="135"/>
-      <c r="J45" s="135"/>
+      <c r="I45" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="J45" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="K45" s="135"/>
       <c r="L45" s="135"/>
-      <c r="M45" s="25" t="s">
+      <c r="M45" s="135"/>
+      <c r="N45" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="O45" s="135"/>
+      <c r="P45" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q45" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="R45" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="N45" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="O45" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="P45" s="21"/>
-      <c r="Q45" s="31"/>
-      <c r="R45" s="21"/>
-      <c r="S45" s="31"/>
+      <c r="S45" s="21"/>
       <c r="T45" s="31"/>
-      <c r="U45" s="14"/>
-    </row>
-    <row r="46" spans="1:26">
+      <c r="U45" s="21"/>
+      <c r="V45" s="31"/>
+      <c r="W45" s="31"/>
+      <c r="X45" s="14"/>
+    </row>
+    <row r="46" spans="1:29">
       <c r="A46" s="10">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -6310,27 +6454,32 @@
       <c r="F46" s="82"/>
       <c r="G46" s="87"/>
       <c r="H46" s="82"/>
-      <c r="I46" s="135"/>
-      <c r="J46" s="135"/>
+      <c r="I46" s="25"/>
+      <c r="J46" s="25"/>
       <c r="K46" s="135"/>
       <c r="L46" s="135"/>
-      <c r="M46" s="25" t="s">
-        <v>141</v>
-      </c>
+      <c r="M46" s="135"/>
       <c r="N46" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="O46" s="25" t="s">
+      <c r="O46" s="135"/>
+      <c r="P46" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="P46" s="21"/>
-      <c r="Q46" s="31"/>
-      <c r="R46" s="21"/>
-      <c r="S46" s="31"/>
+      <c r="Q46" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="R46" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="S46" s="21"/>
       <c r="T46" s="31"/>
-      <c r="U46" s="14"/>
-    </row>
-    <row r="47" spans="1:26">
+      <c r="U46" s="21"/>
+      <c r="V46" s="31"/>
+      <c r="W46" s="31"/>
+      <c r="X46" s="14"/>
+    </row>
+    <row r="47" spans="1:29">
       <c r="A47" s="10">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -6348,29 +6497,28 @@
       <c r="F47" s="26"/>
       <c r="G47" s="86"/>
       <c r="H47" s="26"/>
-      <c r="I47" s="136"/>
-      <c r="J47" s="136"/>
+      <c r="I47" s="25"/>
+      <c r="J47" s="25"/>
       <c r="K47" s="136"/>
       <c r="L47" s="136"/>
-      <c r="M47" s="25" t="s">
+      <c r="M47" s="136"/>
+      <c r="N47" s="25"/>
+      <c r="O47" s="136"/>
+      <c r="P47" s="25"/>
+      <c r="Q47" s="25"/>
+      <c r="R47" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="N47" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="O47" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="P47" s="25"/>
-      <c r="Q47" s="32"/>
-      <c r="R47" s="25"/>
-      <c r="S47" s="32"/>
+      <c r="S47" s="25"/>
       <c r="T47" s="32"/>
-      <c r="U47" s="14" t="s">
+      <c r="U47" s="25"/>
+      <c r="V47" s="32"/>
+      <c r="W47" s="32"/>
+      <c r="X47" s="14" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="48" spans="1:26">
+    <row r="48" spans="1:29">
       <c r="A48" s="10">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -6386,27 +6534,26 @@
       <c r="F48" s="26"/>
       <c r="G48" s="86"/>
       <c r="H48" s="26"/>
-      <c r="I48" s="135"/>
-      <c r="J48" s="135"/>
+      <c r="I48" s="25"/>
+      <c r="J48" s="25"/>
       <c r="K48" s="135"/>
       <c r="L48" s="135"/>
-      <c r="M48" s="25" t="s">
+      <c r="M48" s="135"/>
+      <c r="N48" s="25"/>
+      <c r="O48" s="135"/>
+      <c r="P48" s="25"/>
+      <c r="Q48" s="25"/>
+      <c r="R48" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="N48" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="O48" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="P48" s="21"/>
-      <c r="Q48" s="31"/>
-      <c r="R48" s="21"/>
-      <c r="S48" s="31"/>
+      <c r="S48" s="21"/>
       <c r="T48" s="31"/>
-      <c r="U48" s="14"/>
-    </row>
-    <row r="49" spans="1:21">
+      <c r="U48" s="21"/>
+      <c r="V48" s="31"/>
+      <c r="W48" s="31"/>
+      <c r="X48" s="14"/>
+    </row>
+    <row r="49" spans="1:24">
       <c r="A49" s="10">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -6422,27 +6569,26 @@
       <c r="F49" s="26"/>
       <c r="G49" s="86"/>
       <c r="H49" s="26"/>
-      <c r="I49" s="136"/>
-      <c r="J49" s="136"/>
+      <c r="I49" s="25"/>
+      <c r="J49" s="25"/>
       <c r="K49" s="136"/>
       <c r="L49" s="136"/>
-      <c r="M49" s="25" t="s">
+      <c r="M49" s="136"/>
+      <c r="N49" s="25"/>
+      <c r="O49" s="136"/>
+      <c r="P49" s="25"/>
+      <c r="Q49" s="25"/>
+      <c r="R49" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="N49" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="O49" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="P49" s="21"/>
-      <c r="Q49" s="31"/>
-      <c r="R49" s="21"/>
-      <c r="S49" s="31"/>
+      <c r="S49" s="21"/>
       <c r="T49" s="31"/>
-      <c r="U49" s="14"/>
-    </row>
-    <row r="50" spans="1:21">
+      <c r="U49" s="21"/>
+      <c r="V49" s="31"/>
+      <c r="W49" s="31"/>
+      <c r="X49" s="14"/>
+    </row>
+    <row r="50" spans="1:24">
       <c r="A50" s="10"/>
       <c r="B50" s="22"/>
       <c r="C50" s="13"/>
@@ -6451,21 +6597,24 @@
       <c r="F50" s="26"/>
       <c r="G50" s="86"/>
       <c r="H50" s="26"/>
-      <c r="I50" s="135"/>
-      <c r="J50" s="135"/>
+      <c r="I50" s="25"/>
+      <c r="J50" s="25"/>
       <c r="K50" s="135"/>
       <c r="L50" s="135"/>
-      <c r="M50" s="25"/>
+      <c r="M50" s="135"/>
       <c r="N50" s="25"/>
-      <c r="O50" s="25"/>
-      <c r="P50" s="21"/>
-      <c r="Q50" s="31"/>
-      <c r="R50" s="21"/>
-      <c r="S50" s="31"/>
+      <c r="O50" s="135"/>
+      <c r="P50" s="25"/>
+      <c r="Q50" s="25"/>
+      <c r="R50" s="25"/>
+      <c r="S50" s="21"/>
       <c r="T50" s="31"/>
-      <c r="U50" s="14"/>
-    </row>
-    <row r="51" spans="1:21">
+      <c r="U50" s="21"/>
+      <c r="V50" s="31"/>
+      <c r="W50" s="31"/>
+      <c r="X50" s="14"/>
+    </row>
+    <row r="51" spans="1:24">
       <c r="A51" s="10"/>
       <c r="B51" s="22"/>
       <c r="C51" s="13"/>
@@ -6474,21 +6623,24 @@
       <c r="F51" s="26"/>
       <c r="G51" s="86"/>
       <c r="H51" s="26"/>
-      <c r="I51" s="136"/>
-      <c r="J51" s="136"/>
+      <c r="I51" s="25"/>
+      <c r="J51" s="25"/>
       <c r="K51" s="136"/>
       <c r="L51" s="136"/>
-      <c r="M51" s="25"/>
+      <c r="M51" s="136"/>
       <c r="N51" s="25"/>
-      <c r="O51" s="25"/>
+      <c r="O51" s="136"/>
       <c r="P51" s="25"/>
-      <c r="Q51" s="32"/>
+      <c r="Q51" s="25"/>
       <c r="R51" s="25"/>
-      <c r="S51" s="32"/>
+      <c r="S51" s="25"/>
       <c r="T51" s="32"/>
-      <c r="U51" s="14"/>
-    </row>
-    <row r="52" spans="1:21">
+      <c r="U51" s="25"/>
+      <c r="V51" s="32"/>
+      <c r="W51" s="32"/>
+      <c r="X51" s="14"/>
+    </row>
+    <row r="52" spans="1:24">
       <c r="A52" s="10"/>
       <c r="B52" s="22"/>
       <c r="C52" s="13"/>
@@ -6497,21 +6649,24 @@
       <c r="F52" s="26"/>
       <c r="G52" s="86"/>
       <c r="H52" s="26"/>
-      <c r="I52" s="135"/>
-      <c r="J52" s="135"/>
+      <c r="I52" s="25"/>
+      <c r="J52" s="25"/>
       <c r="K52" s="135"/>
       <c r="L52" s="135"/>
-      <c r="M52" s="25"/>
+      <c r="M52" s="135"/>
       <c r="N52" s="25"/>
-      <c r="O52" s="25"/>
-      <c r="P52" s="21"/>
-      <c r="Q52" s="31"/>
-      <c r="R52" s="21"/>
-      <c r="S52" s="31"/>
+      <c r="O52" s="135"/>
+      <c r="P52" s="25"/>
+      <c r="Q52" s="25"/>
+      <c r="R52" s="25"/>
+      <c r="S52" s="21"/>
       <c r="T52" s="31"/>
-      <c r="U52" s="14"/>
-    </row>
-    <row r="53" spans="1:21">
+      <c r="U52" s="21"/>
+      <c r="V52" s="31"/>
+      <c r="W52" s="31"/>
+      <c r="X52" s="14"/>
+    </row>
+    <row r="53" spans="1:24">
       <c r="A53" s="10"/>
       <c r="B53" s="22"/>
       <c r="C53" s="13"/>
@@ -6520,21 +6675,24 @@
       <c r="F53" s="26"/>
       <c r="G53" s="86"/>
       <c r="H53" s="26"/>
-      <c r="I53" s="135"/>
-      <c r="J53" s="135"/>
+      <c r="I53" s="25"/>
+      <c r="J53" s="25"/>
       <c r="K53" s="135"/>
       <c r="L53" s="135"/>
-      <c r="M53" s="25"/>
+      <c r="M53" s="135"/>
       <c r="N53" s="25"/>
-      <c r="O53" s="25"/>
-      <c r="P53" s="21"/>
-      <c r="Q53" s="31"/>
-      <c r="R53" s="21"/>
-      <c r="S53" s="31"/>
+      <c r="O53" s="135"/>
+      <c r="P53" s="25"/>
+      <c r="Q53" s="25"/>
+      <c r="R53" s="25"/>
+      <c r="S53" s="21"/>
       <c r="T53" s="31"/>
-      <c r="U53" s="14"/>
-    </row>
-    <row r="54" spans="1:21">
+      <c r="U53" s="21"/>
+      <c r="V53" s="31"/>
+      <c r="W53" s="31"/>
+      <c r="X53" s="14"/>
+    </row>
+    <row r="54" spans="1:24">
       <c r="A54" s="10"/>
       <c r="B54" s="22"/>
       <c r="C54" s="13"/>
@@ -6543,21 +6701,24 @@
       <c r="F54" s="26"/>
       <c r="G54" s="86"/>
       <c r="H54" s="26"/>
-      <c r="I54" s="135"/>
-      <c r="J54" s="135"/>
+      <c r="I54" s="25"/>
+      <c r="J54" s="25"/>
       <c r="K54" s="135"/>
       <c r="L54" s="135"/>
-      <c r="M54" s="25"/>
+      <c r="M54" s="135"/>
       <c r="N54" s="25"/>
-      <c r="O54" s="25"/>
-      <c r="P54" s="21"/>
-      <c r="Q54" s="31"/>
-      <c r="R54" s="21"/>
-      <c r="S54" s="31"/>
+      <c r="O54" s="135"/>
+      <c r="P54" s="25"/>
+      <c r="Q54" s="25"/>
+      <c r="R54" s="25"/>
+      <c r="S54" s="21"/>
       <c r="T54" s="31"/>
-      <c r="U54" s="14"/>
-    </row>
-    <row r="55" spans="1:21">
+      <c r="U54" s="21"/>
+      <c r="V54" s="31"/>
+      <c r="W54" s="31"/>
+      <c r="X54" s="14"/>
+    </row>
+    <row r="55" spans="1:24">
       <c r="A55" s="10"/>
       <c r="B55" s="22"/>
       <c r="C55" s="13"/>
@@ -6566,21 +6727,24 @@
       <c r="F55" s="26"/>
       <c r="G55" s="86"/>
       <c r="H55" s="26"/>
-      <c r="I55" s="135"/>
-      <c r="J55" s="135"/>
+      <c r="I55" s="25"/>
+      <c r="J55" s="25"/>
       <c r="K55" s="135"/>
       <c r="L55" s="135"/>
-      <c r="M55" s="25"/>
+      <c r="M55" s="135"/>
       <c r="N55" s="25"/>
-      <c r="O55" s="25"/>
-      <c r="P55" s="21"/>
-      <c r="Q55" s="31"/>
-      <c r="R55" s="21"/>
-      <c r="S55" s="31"/>
+      <c r="O55" s="135"/>
+      <c r="P55" s="25"/>
+      <c r="Q55" s="25"/>
+      <c r="R55" s="25"/>
+      <c r="S55" s="21"/>
       <c r="T55" s="31"/>
-      <c r="U55" s="14"/>
-    </row>
-    <row r="56" spans="1:21">
+      <c r="U55" s="21"/>
+      <c r="V55" s="31"/>
+      <c r="W55" s="31"/>
+      <c r="X55" s="14"/>
+    </row>
+    <row r="56" spans="1:24">
       <c r="A56" s="10"/>
       <c r="B56" s="22"/>
       <c r="C56" s="13"/>
@@ -6589,21 +6753,24 @@
       <c r="F56" s="26"/>
       <c r="G56" s="86"/>
       <c r="H56" s="26"/>
-      <c r="I56" s="135"/>
-      <c r="J56" s="135"/>
+      <c r="I56" s="25"/>
+      <c r="J56" s="25"/>
       <c r="K56" s="135"/>
       <c r="L56" s="135"/>
-      <c r="M56" s="25"/>
+      <c r="M56" s="135"/>
       <c r="N56" s="25"/>
-      <c r="O56" s="25"/>
-      <c r="P56" s="21"/>
-      <c r="Q56" s="31"/>
-      <c r="R56" s="21"/>
-      <c r="S56" s="31"/>
+      <c r="O56" s="135"/>
+      <c r="P56" s="25"/>
+      <c r="Q56" s="25"/>
+      <c r="R56" s="25"/>
+      <c r="S56" s="21"/>
       <c r="T56" s="31"/>
-      <c r="U56" s="14"/>
-    </row>
-    <row r="57" spans="1:21">
+      <c r="U56" s="21"/>
+      <c r="V56" s="31"/>
+      <c r="W56" s="31"/>
+      <c r="X56" s="14"/>
+    </row>
+    <row r="57" spans="1:24">
       <c r="A57" s="10"/>
       <c r="B57" s="22"/>
       <c r="C57" s="13"/>
@@ -6612,21 +6779,24 @@
       <c r="F57" s="26"/>
       <c r="G57" s="86"/>
       <c r="H57" s="26"/>
-      <c r="I57" s="26"/>
-      <c r="J57" s="26"/>
+      <c r="I57" s="25"/>
+      <c r="J57" s="25"/>
       <c r="K57" s="26"/>
       <c r="L57" s="26"/>
-      <c r="M57" s="25"/>
+      <c r="M57" s="26"/>
       <c r="N57" s="25"/>
-      <c r="O57" s="25"/>
+      <c r="O57" s="26"/>
       <c r="P57" s="25"/>
-      <c r="Q57" s="32"/>
+      <c r="Q57" s="25"/>
       <c r="R57" s="25"/>
-      <c r="S57" s="32"/>
+      <c r="S57" s="25"/>
       <c r="T57" s="32"/>
-      <c r="U57" s="14"/>
-    </row>
-    <row r="58" spans="1:21">
+      <c r="U57" s="25"/>
+      <c r="V57" s="32"/>
+      <c r="W57" s="32"/>
+      <c r="X57" s="14"/>
+    </row>
+    <row r="58" spans="1:24">
       <c r="A58" s="10"/>
       <c r="B58" s="22"/>
       <c r="C58" s="13"/>
@@ -6635,21 +6805,24 @@
       <c r="F58" s="26"/>
       <c r="G58" s="86"/>
       <c r="H58" s="26"/>
-      <c r="I58" s="26"/>
-      <c r="J58" s="26"/>
+      <c r="I58" s="25"/>
+      <c r="J58" s="25"/>
       <c r="K58" s="26"/>
       <c r="L58" s="26"/>
-      <c r="M58" s="25"/>
+      <c r="M58" s="26"/>
       <c r="N58" s="25"/>
-      <c r="O58" s="25"/>
-      <c r="P58" s="21"/>
-      <c r="Q58" s="31"/>
-      <c r="R58" s="21"/>
-      <c r="S58" s="31"/>
+      <c r="O58" s="26"/>
+      <c r="P58" s="25"/>
+      <c r="Q58" s="25"/>
+      <c r="R58" s="25"/>
+      <c r="S58" s="21"/>
       <c r="T58" s="31"/>
-      <c r="U58" s="14"/>
-    </row>
-    <row r="59" spans="1:21">
+      <c r="U58" s="21"/>
+      <c r="V58" s="31"/>
+      <c r="W58" s="31"/>
+      <c r="X58" s="14"/>
+    </row>
+    <row r="59" spans="1:24">
       <c r="A59" s="10"/>
       <c r="B59" s="22"/>
       <c r="C59" s="13"/>
@@ -6658,21 +6831,24 @@
       <c r="F59" s="26"/>
       <c r="G59" s="86"/>
       <c r="H59" s="26"/>
-      <c r="I59" s="26"/>
-      <c r="J59" s="26"/>
+      <c r="I59" s="25"/>
+      <c r="J59" s="25"/>
       <c r="K59" s="26"/>
       <c r="L59" s="26"/>
-      <c r="M59" s="25"/>
+      <c r="M59" s="26"/>
       <c r="N59" s="25"/>
-      <c r="O59" s="25"/>
-      <c r="P59" s="21"/>
-      <c r="Q59" s="31"/>
-      <c r="R59" s="21"/>
-      <c r="S59" s="31"/>
+      <c r="O59" s="26"/>
+      <c r="P59" s="25"/>
+      <c r="Q59" s="25"/>
+      <c r="R59" s="25"/>
+      <c r="S59" s="21"/>
       <c r="T59" s="31"/>
-      <c r="U59" s="14"/>
-    </row>
-    <row r="60" spans="1:21">
+      <c r="U59" s="21"/>
+      <c r="V59" s="31"/>
+      <c r="W59" s="31"/>
+      <c r="X59" s="14"/>
+    </row>
+    <row r="60" spans="1:24">
       <c r="A60" s="10"/>
       <c r="B60" s="22"/>
       <c r="C60" s="13"/>
@@ -6681,21 +6857,24 @@
       <c r="F60" s="26"/>
       <c r="G60" s="86"/>
       <c r="H60" s="26"/>
-      <c r="I60" s="26"/>
-      <c r="J60" s="26"/>
+      <c r="I60" s="25"/>
+      <c r="J60" s="25"/>
       <c r="K60" s="26"/>
       <c r="L60" s="26"/>
-      <c r="M60" s="25"/>
+      <c r="M60" s="26"/>
       <c r="N60" s="25"/>
-      <c r="O60" s="25"/>
-      <c r="P60" s="21"/>
-      <c r="Q60" s="31"/>
-      <c r="R60" s="21"/>
-      <c r="S60" s="31"/>
+      <c r="O60" s="26"/>
+      <c r="P60" s="25"/>
+      <c r="Q60" s="25"/>
+      <c r="R60" s="25"/>
+      <c r="S60" s="21"/>
       <c r="T60" s="31"/>
-      <c r="U60" s="14"/>
-    </row>
-    <row r="61" spans="1:21">
+      <c r="U60" s="21"/>
+      <c r="V60" s="31"/>
+      <c r="W60" s="31"/>
+      <c r="X60" s="14"/>
+    </row>
+    <row r="61" spans="1:24">
       <c r="A61" s="10"/>
       <c r="B61" s="22"/>
       <c r="C61" s="13"/>
@@ -6704,21 +6883,24 @@
       <c r="F61" s="26"/>
       <c r="G61" s="86"/>
       <c r="H61" s="26"/>
-      <c r="I61" s="26"/>
-      <c r="J61" s="26"/>
+      <c r="I61" s="25"/>
+      <c r="J61" s="25"/>
       <c r="K61" s="26"/>
       <c r="L61" s="26"/>
-      <c r="M61" s="25"/>
+      <c r="M61" s="26"/>
       <c r="N61" s="25"/>
-      <c r="O61" s="25"/>
-      <c r="P61" s="21"/>
-      <c r="Q61" s="31"/>
-      <c r="R61" s="21"/>
-      <c r="S61" s="31"/>
+      <c r="O61" s="26"/>
+      <c r="P61" s="25"/>
+      <c r="Q61" s="25"/>
+      <c r="R61" s="25"/>
+      <c r="S61" s="21"/>
       <c r="T61" s="31"/>
-      <c r="U61" s="14"/>
-    </row>
-    <row r="62" spans="1:21">
+      <c r="U61" s="21"/>
+      <c r="V61" s="31"/>
+      <c r="W61" s="31"/>
+      <c r="X61" s="14"/>
+    </row>
+    <row r="62" spans="1:24">
       <c r="A62" s="10"/>
       <c r="B62" s="22"/>
       <c r="C62" s="13"/>
@@ -6727,21 +6909,24 @@
       <c r="F62" s="26"/>
       <c r="G62" s="86"/>
       <c r="H62" s="26"/>
-      <c r="I62" s="26"/>
-      <c r="J62" s="26"/>
+      <c r="I62" s="25"/>
+      <c r="J62" s="25"/>
       <c r="K62" s="26"/>
       <c r="L62" s="26"/>
-      <c r="M62" s="25"/>
+      <c r="M62" s="26"/>
       <c r="N62" s="25"/>
-      <c r="O62" s="25"/>
+      <c r="O62" s="26"/>
       <c r="P62" s="25"/>
-      <c r="Q62" s="32"/>
+      <c r="Q62" s="25"/>
       <c r="R62" s="25"/>
-      <c r="S62" s="32"/>
+      <c r="S62" s="25"/>
       <c r="T62" s="32"/>
-      <c r="U62" s="14"/>
-    </row>
-    <row r="63" spans="1:21">
+      <c r="U62" s="25"/>
+      <c r="V62" s="32"/>
+      <c r="W62" s="32"/>
+      <c r="X62" s="14"/>
+    </row>
+    <row r="63" spans="1:24">
       <c r="A63" s="10"/>
       <c r="B63" s="22"/>
       <c r="C63" s="13"/>
@@ -6750,21 +6935,24 @@
       <c r="F63" s="26"/>
       <c r="G63" s="86"/>
       <c r="H63" s="26"/>
-      <c r="I63" s="26"/>
-      <c r="J63" s="26"/>
+      <c r="I63" s="25"/>
+      <c r="J63" s="25"/>
       <c r="K63" s="26"/>
       <c r="L63" s="26"/>
-      <c r="M63" s="25"/>
+      <c r="M63" s="26"/>
       <c r="N63" s="25"/>
-      <c r="O63" s="25"/>
-      <c r="P63" s="21"/>
-      <c r="Q63" s="31"/>
-      <c r="R63" s="21"/>
-      <c r="S63" s="31"/>
+      <c r="O63" s="26"/>
+      <c r="P63" s="25"/>
+      <c r="Q63" s="25"/>
+      <c r="R63" s="25"/>
+      <c r="S63" s="21"/>
       <c r="T63" s="31"/>
-      <c r="U63" s="14"/>
-    </row>
-    <row r="64" spans="1:21">
+      <c r="U63" s="21"/>
+      <c r="V63" s="31"/>
+      <c r="W63" s="31"/>
+      <c r="X63" s="14"/>
+    </row>
+    <row r="64" spans="1:24">
       <c r="A64" s="10"/>
       <c r="B64" s="22"/>
       <c r="C64" s="13"/>
@@ -6773,21 +6961,24 @@
       <c r="F64" s="26"/>
       <c r="G64" s="86"/>
       <c r="H64" s="26"/>
-      <c r="I64" s="26"/>
-      <c r="J64" s="26"/>
+      <c r="I64" s="25"/>
+      <c r="J64" s="25"/>
       <c r="K64" s="26"/>
       <c r="L64" s="26"/>
-      <c r="M64" s="25"/>
+      <c r="M64" s="26"/>
       <c r="N64" s="25"/>
-      <c r="O64" s="25"/>
-      <c r="P64" s="21"/>
-      <c r="Q64" s="31"/>
-      <c r="R64" s="21"/>
-      <c r="S64" s="31"/>
+      <c r="O64" s="26"/>
+      <c r="P64" s="25"/>
+      <c r="Q64" s="25"/>
+      <c r="R64" s="25"/>
+      <c r="S64" s="21"/>
       <c r="T64" s="31"/>
-      <c r="U64" s="14"/>
-    </row>
-    <row r="65" spans="1:21">
+      <c r="U64" s="21"/>
+      <c r="V64" s="31"/>
+      <c r="W64" s="31"/>
+      <c r="X64" s="14"/>
+    </row>
+    <row r="65" spans="1:24">
       <c r="A65" s="10"/>
       <c r="B65" s="22"/>
       <c r="C65" s="13"/>
@@ -6796,21 +6987,24 @@
       <c r="F65" s="26"/>
       <c r="G65" s="86"/>
       <c r="H65" s="26"/>
-      <c r="I65" s="26"/>
-      <c r="J65" s="26"/>
+      <c r="I65" s="25"/>
+      <c r="J65" s="25"/>
       <c r="K65" s="26"/>
       <c r="L65" s="26"/>
-      <c r="M65" s="25"/>
+      <c r="M65" s="26"/>
       <c r="N65" s="25"/>
-      <c r="O65" s="25"/>
+      <c r="O65" s="26"/>
       <c r="P65" s="25"/>
-      <c r="Q65" s="32"/>
+      <c r="Q65" s="25"/>
       <c r="R65" s="25"/>
-      <c r="S65" s="32"/>
+      <c r="S65" s="25"/>
       <c r="T65" s="32"/>
-      <c r="U65" s="14"/>
-    </row>
-    <row r="66" spans="1:21">
+      <c r="U65" s="25"/>
+      <c r="V65" s="32"/>
+      <c r="W65" s="32"/>
+      <c r="X65" s="14"/>
+    </row>
+    <row r="66" spans="1:24">
       <c r="A66" s="15"/>
       <c r="B66" s="23"/>
       <c r="C66" s="16"/>
@@ -6826,33 +7020,28 @@
       <c r="M66" s="27"/>
       <c r="N66" s="27"/>
       <c r="O66" s="27"/>
-      <c r="P66" s="23"/>
-      <c r="Q66" s="33"/>
-      <c r="R66" s="23"/>
-      <c r="S66" s="33"/>
+      <c r="P66" s="27"/>
+      <c r="Q66" s="27"/>
+      <c r="R66" s="27"/>
+      <c r="S66" s="23"/>
       <c r="T66" s="33"/>
-      <c r="U66" s="17"/>
+      <c r="U66" s="23"/>
+      <c r="V66" s="33"/>
+      <c r="W66" s="33"/>
+      <c r="X66" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="37">
-    <mergeCell ref="U41:U42"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="F41:F42"/>
+  <mergeCells count="40">
+    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B30:G30"/>
     <mergeCell ref="O41:O42"/>
     <mergeCell ref="I41:I42"/>
     <mergeCell ref="J41:J42"/>
-    <mergeCell ref="K41:K42"/>
-    <mergeCell ref="M41:M42"/>
-    <mergeCell ref="R41:S41"/>
     <mergeCell ref="N41:N42"/>
     <mergeCell ref="C15:D15"/>
-    <mergeCell ref="P41:Q41"/>
+    <mergeCell ref="S41:T41"/>
     <mergeCell ref="B31:G31"/>
     <mergeCell ref="A33:G33"/>
     <mergeCell ref="B34:G34"/>
@@ -6867,22 +7056,36 @@
     <mergeCell ref="A27:G27"/>
     <mergeCell ref="B28:G28"/>
     <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B36:G36"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="X41:X42"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="R41:R42"/>
+    <mergeCell ref="K41:K42"/>
     <mergeCell ref="L41:L42"/>
+    <mergeCell ref="M41:M42"/>
+    <mergeCell ref="P41:P42"/>
+    <mergeCell ref="U41:V41"/>
+    <mergeCell ref="Q41:Q42"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
-  <dataValidations count="3">
+  <dataValidations count="4">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>Validate実装パターン</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19" xr:uid="{C2D0C7F4-19B0-DB40-AFFD-E6928EE4E5C2}">
       <formula1>isImport</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M43:O66" xr:uid="{1FBC7B49-ABAE-AE4A-8A55-EF1A4EFC4446}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I43:J66 R43:R66" xr:uid="{1FBC7B49-ABAE-AE4A-8A55-EF1A4EFC4446}">
       <formula1>isNullable</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N43:N66 P43:Q66" xr:uid="{672B2DF7-D1C1-234C-A02A-4DFC68BF8F4E}">
+      <formula1>threeAlters</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -6928,7 +7131,7 @@
   </sheetPr>
   <dimension ref="A1:V63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D9" workbookViewId="0">
+    <sheetView topLeftCell="F9" workbookViewId="0">
       <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
@@ -7104,10 +7307,10 @@
         <v>174</v>
       </c>
       <c r="B12" s="122"/>
-      <c r="C12" s="165" t="s">
+      <c r="C12" s="141" t="s">
         <v>175</v>
       </c>
-      <c r="D12" s="165"/>
+      <c r="D12" s="141"/>
       <c r="E12" s="95" t="s">
         <v>176</v>
       </c>
@@ -7122,10 +7325,10 @@
         <v>226</v>
       </c>
       <c r="B13" s="122"/>
-      <c r="C13" s="164" t="s">
+      <c r="C13" s="142" t="s">
         <v>230</v>
       </c>
-      <c r="D13" s="165"/>
+      <c r="D13" s="141"/>
       <c r="E13" s="55" t="s">
         <v>227</v>
       </c>
@@ -7145,10 +7348,10 @@
         <v>177</v>
       </c>
       <c r="B14" s="122"/>
-      <c r="C14" s="165" t="s">
+      <c r="C14" s="141" t="s">
         <v>178</v>
       </c>
-      <c r="D14" s="165"/>
+      <c r="D14" s="141"/>
       <c r="E14" s="55"/>
       <c r="F14" s="55"/>
       <c r="G14" s="54"/>
@@ -7160,8 +7363,8 @@
         <v>228</v>
       </c>
       <c r="B15" s="122"/>
-      <c r="C15" s="164"/>
-      <c r="D15" s="165"/>
+      <c r="C15" s="142"/>
+      <c r="D15" s="141"/>
       <c r="E15" s="55" t="s">
         <v>229</v>
       </c>
@@ -7209,15 +7412,15 @@
       <c r="L17"/>
     </row>
     <row r="18" spans="1:22">
-      <c r="A18" s="157" t="s">
+      <c r="A18" s="179" t="s">
         <v>192</v>
       </c>
-      <c r="B18" s="157"/>
-      <c r="C18" s="157"/>
-      <c r="D18" s="157"/>
-      <c r="E18" s="157"/>
-      <c r="F18" s="157"/>
-      <c r="G18" s="157"/>
+      <c r="B18" s="179"/>
+      <c r="C18" s="179"/>
+      <c r="D18" s="179"/>
+      <c r="E18" s="179"/>
+      <c r="F18" s="179"/>
+      <c r="G18" s="179"/>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
@@ -7228,14 +7431,14 @@
       <c r="A19" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="151" t="s">
+      <c r="B19" s="173" t="s">
         <v>183</v>
       </c>
-      <c r="C19" s="152"/>
-      <c r="D19" s="152"/>
-      <c r="E19" s="152"/>
-      <c r="F19" s="152"/>
-      <c r="G19" s="153"/>
+      <c r="C19" s="174"/>
+      <c r="D19" s="174"/>
+      <c r="E19" s="174"/>
+      <c r="F19" s="174"/>
+      <c r="G19" s="175"/>
       <c r="H19" s="105"/>
       <c r="I19"/>
       <c r="J19"/>
@@ -7251,12 +7454,12 @@
     </row>
     <row r="20" spans="1:22">
       <c r="A20" s="116"/>
-      <c r="B20" s="168"/>
-      <c r="C20" s="168"/>
-      <c r="D20" s="168"/>
-      <c r="E20" s="168"/>
-      <c r="F20" s="168"/>
-      <c r="G20" s="168"/>
+      <c r="B20" s="157"/>
+      <c r="C20" s="157"/>
+      <c r="D20" s="157"/>
+      <c r="E20" s="157"/>
+      <c r="F20" s="157"/>
+      <c r="G20" s="157"/>
       <c r="H20" s="112"/>
       <c r="I20"/>
       <c r="J20"/>
@@ -7271,12 +7474,12 @@
     </row>
     <row r="21" spans="1:22">
       <c r="A21" s="117"/>
-      <c r="B21" s="169"/>
-      <c r="C21" s="169"/>
-      <c r="D21" s="169"/>
-      <c r="E21" s="169"/>
-      <c r="F21" s="169"/>
-      <c r="G21" s="169"/>
+      <c r="B21" s="159"/>
+      <c r="C21" s="159"/>
+      <c r="D21" s="159"/>
+      <c r="E21" s="159"/>
+      <c r="F21" s="159"/>
+      <c r="G21" s="159"/>
       <c r="H21" s="112"/>
       <c r="I21"/>
       <c r="J21"/>
@@ -7291,12 +7494,12 @@
     </row>
     <row r="22" spans="1:22">
       <c r="A22" s="118"/>
-      <c r="B22" s="170"/>
-      <c r="C22" s="170"/>
-      <c r="D22" s="170"/>
-      <c r="E22" s="170"/>
-      <c r="F22" s="170"/>
-      <c r="G22" s="170"/>
+      <c r="B22" s="161"/>
+      <c r="C22" s="161"/>
+      <c r="D22" s="161"/>
+      <c r="E22" s="161"/>
+      <c r="F22" s="161"/>
+      <c r="G22" s="161"/>
       <c r="H22" s="112"/>
       <c r="I22"/>
       <c r="J22"/>
@@ -7323,15 +7526,15 @@
       <c r="O23" s="112"/>
     </row>
     <row r="24" spans="1:22">
-      <c r="A24" s="154" t="s">
+      <c r="A24" s="176" t="s">
         <v>193</v>
       </c>
-      <c r="B24" s="155"/>
-      <c r="C24" s="155"/>
-      <c r="D24" s="155"/>
-      <c r="E24" s="155"/>
-      <c r="F24" s="155"/>
-      <c r="G24" s="156"/>
+      <c r="B24" s="177"/>
+      <c r="C24" s="177"/>
+      <c r="D24" s="177"/>
+      <c r="E24" s="177"/>
+      <c r="F24" s="177"/>
+      <c r="G24" s="178"/>
       <c r="I24"/>
       <c r="J24"/>
       <c r="K24"/>
@@ -7344,14 +7547,14 @@
       <c r="A25" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B25" s="174" t="s">
+      <c r="B25" s="153" t="s">
         <v>184</v>
       </c>
-      <c r="C25" s="174"/>
-      <c r="D25" s="174"/>
-      <c r="E25" s="174"/>
-      <c r="F25" s="174"/>
-      <c r="G25" s="174"/>
+      <c r="C25" s="153"/>
+      <c r="D25" s="153"/>
+      <c r="E25" s="153"/>
+      <c r="F25" s="153"/>
+      <c r="G25" s="153"/>
       <c r="H25" s="105"/>
       <c r="M25" s="112"/>
       <c r="N25" s="112"/>
@@ -7367,14 +7570,14 @@
       <c r="A26" s="116">
         <v>1</v>
       </c>
-      <c r="B26" s="175" t="s">
+      <c r="B26" s="154" t="s">
         <v>185</v>
       </c>
-      <c r="C26" s="175"/>
-      <c r="D26" s="175"/>
-      <c r="E26" s="175"/>
-      <c r="F26" s="175"/>
-      <c r="G26" s="175"/>
+      <c r="C26" s="154"/>
+      <c r="D26" s="154"/>
+      <c r="E26" s="154"/>
+      <c r="F26" s="154"/>
+      <c r="G26" s="154"/>
       <c r="H26" s="112"/>
       <c r="I26" s="105"/>
       <c r="J26" s="105"/>
@@ -7389,12 +7592,12 @@
     </row>
     <row r="27" spans="1:22">
       <c r="A27" s="117"/>
-      <c r="B27" s="176"/>
-      <c r="C27" s="176"/>
-      <c r="D27" s="176"/>
-      <c r="E27" s="176"/>
-      <c r="F27" s="176"/>
-      <c r="G27" s="176"/>
+      <c r="B27" s="155"/>
+      <c r="C27" s="155"/>
+      <c r="D27" s="155"/>
+      <c r="E27" s="155"/>
+      <c r="F27" s="155"/>
+      <c r="G27" s="155"/>
       <c r="H27" s="112"/>
       <c r="I27" s="105"/>
       <c r="J27" s="105"/>
@@ -7409,12 +7612,12 @@
     </row>
     <row r="28" spans="1:22">
       <c r="A28" s="118"/>
-      <c r="B28" s="177"/>
-      <c r="C28" s="177"/>
-      <c r="D28" s="177"/>
-      <c r="E28" s="177"/>
-      <c r="F28" s="177"/>
-      <c r="G28" s="177"/>
+      <c r="B28" s="156"/>
+      <c r="C28" s="156"/>
+      <c r="D28" s="156"/>
+      <c r="E28" s="156"/>
+      <c r="F28" s="156"/>
+      <c r="G28" s="156"/>
       <c r="H28" s="112"/>
       <c r="I28" s="105"/>
       <c r="J28" s="105"/>
@@ -7453,15 +7656,15 @@
       <c r="T29"/>
     </row>
     <row r="30" spans="1:22">
-      <c r="A30" s="154" t="s">
+      <c r="A30" s="176" t="s">
         <v>194</v>
       </c>
-      <c r="B30" s="155"/>
-      <c r="C30" s="155"/>
-      <c r="D30" s="155"/>
-      <c r="E30" s="155"/>
-      <c r="F30" s="155"/>
-      <c r="G30" s="156"/>
+      <c r="B30" s="177"/>
+      <c r="C30" s="177"/>
+      <c r="D30" s="177"/>
+      <c r="E30" s="177"/>
+      <c r="F30" s="177"/>
+      <c r="G30" s="178"/>
       <c r="M30" s="112"/>
       <c r="N30" s="112"/>
       <c r="O30" s="112"/>
@@ -7470,14 +7673,14 @@
       <c r="A31" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B31" s="174" t="s">
+      <c r="B31" s="153" t="s">
         <v>186</v>
       </c>
-      <c r="C31" s="174"/>
-      <c r="D31" s="174"/>
-      <c r="E31" s="174"/>
-      <c r="F31" s="174"/>
-      <c r="G31" s="174"/>
+      <c r="C31" s="153"/>
+      <c r="D31" s="153"/>
+      <c r="E31" s="153"/>
+      <c r="F31" s="153"/>
+      <c r="G31" s="153"/>
       <c r="H31" s="105"/>
       <c r="I31" s="105"/>
       <c r="J31" s="105"/>
@@ -7495,12 +7698,12 @@
     </row>
     <row r="32" spans="1:22">
       <c r="A32" s="116"/>
-      <c r="B32" s="168"/>
-      <c r="C32" s="168"/>
-      <c r="D32" s="168"/>
-      <c r="E32" s="168"/>
-      <c r="F32" s="168"/>
-      <c r="G32" s="178"/>
+      <c r="B32" s="157"/>
+      <c r="C32" s="157"/>
+      <c r="D32" s="157"/>
+      <c r="E32" s="157"/>
+      <c r="F32" s="157"/>
+      <c r="G32" s="158"/>
       <c r="H32" s="112"/>
       <c r="I32" s="112"/>
       <c r="J32" s="112"/>
@@ -7518,12 +7721,12 @@
     </row>
     <row r="33" spans="1:22">
       <c r="A33" s="117"/>
-      <c r="B33" s="169"/>
-      <c r="C33" s="169"/>
-      <c r="D33" s="169"/>
-      <c r="E33" s="169"/>
-      <c r="F33" s="169"/>
-      <c r="G33" s="179"/>
+      <c r="B33" s="159"/>
+      <c r="C33" s="159"/>
+      <c r="D33" s="159"/>
+      <c r="E33" s="159"/>
+      <c r="F33" s="159"/>
+      <c r="G33" s="160"/>
       <c r="H33" s="112"/>
       <c r="I33" s="112"/>
       <c r="J33" s="112"/>
@@ -7538,12 +7741,12 @@
     </row>
     <row r="34" spans="1:22">
       <c r="A34" s="118"/>
-      <c r="B34" s="170"/>
-      <c r="C34" s="170"/>
-      <c r="D34" s="170"/>
-      <c r="E34" s="170"/>
-      <c r="F34" s="170"/>
-      <c r="G34" s="180"/>
+      <c r="B34" s="161"/>
+      <c r="C34" s="161"/>
+      <c r="D34" s="161"/>
+      <c r="E34" s="161"/>
+      <c r="F34" s="161"/>
+      <c r="G34" s="162"/>
       <c r="H34" s="112"/>
       <c r="I34" s="112"/>
       <c r="J34" s="112"/>
@@ -7613,84 +7816,84 @@
       <c r="U37" s="58"/>
     </row>
     <row r="38" spans="1:22" ht="30" customHeight="1">
-      <c r="A38" s="193" t="s">
+      <c r="A38" s="189" t="s">
         <v>118</v>
       </c>
-      <c r="B38" s="193" t="s">
+      <c r="B38" s="189" t="s">
         <v>119</v>
       </c>
       <c r="C38" s="60" t="s">
         <v>120</v>
       </c>
-      <c r="D38" s="193" t="s">
+      <c r="D38" s="189" t="s">
         <v>101</v>
       </c>
-      <c r="E38" s="193" t="s">
+      <c r="E38" s="189" t="s">
         <v>161</v>
       </c>
-      <c r="F38" s="193" t="s">
+      <c r="F38" s="189" t="s">
         <v>177</v>
       </c>
-      <c r="G38" s="193" t="s">
+      <c r="G38" s="189" t="s">
         <v>140</v>
       </c>
-      <c r="H38" s="193" t="s">
+      <c r="H38" s="189" t="s">
         <v>139</v>
       </c>
-      <c r="I38" s="201" t="s">
+      <c r="I38" s="203" t="s">
         <v>200</v>
       </c>
-      <c r="J38" s="203" t="s">
+      <c r="J38" s="205" t="s">
         <v>201</v>
       </c>
-      <c r="K38" s="203" t="s">
+      <c r="K38" s="205" t="s">
         <v>202</v>
       </c>
-      <c r="L38" s="186" t="s">
+      <c r="L38" s="196" t="s">
         <v>203</v>
       </c>
-      <c r="M38" s="190" t="s">
+      <c r="M38" s="186" t="s">
         <v>195</v>
       </c>
-      <c r="N38" s="190" t="s">
+      <c r="N38" s="186" t="s">
         <v>209</v>
       </c>
-      <c r="O38" s="192" t="s">
+      <c r="O38" s="188" t="s">
         <v>208</v>
       </c>
-      <c r="P38" s="199" t="s">
+      <c r="P38" s="202" t="s">
         <v>122</v>
       </c>
       <c r="Q38" s="200"/>
-      <c r="R38" s="206" t="s">
+      <c r="R38" s="199" t="s">
         <v>123</v>
       </c>
       <c r="S38" s="200"/>
       <c r="T38" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="U38" s="193" t="s">
+      <c r="U38" s="189" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="39" spans="1:22" ht="15">
-      <c r="A39" s="198"/>
-      <c r="B39" s="198"/>
+      <c r="A39" s="201"/>
+      <c r="B39" s="201"/>
       <c r="C39" s="61" t="s">
         <v>121</v>
       </c>
-      <c r="D39" s="198"/>
-      <c r="E39" s="195"/>
-      <c r="F39" s="195"/>
-      <c r="G39" s="198"/>
-      <c r="H39" s="198"/>
-      <c r="I39" s="202"/>
-      <c r="J39" s="204"/>
-      <c r="K39" s="204"/>
-      <c r="L39" s="187"/>
-      <c r="M39" s="196"/>
-      <c r="N39" s="196"/>
-      <c r="O39" s="205"/>
+      <c r="D39" s="201"/>
+      <c r="E39" s="191"/>
+      <c r="F39" s="191"/>
+      <c r="G39" s="201"/>
+      <c r="H39" s="201"/>
+      <c r="I39" s="204"/>
+      <c r="J39" s="206"/>
+      <c r="K39" s="206"/>
+      <c r="L39" s="197"/>
+      <c r="M39" s="192"/>
+      <c r="N39" s="192"/>
+      <c r="O39" s="198"/>
       <c r="P39" s="62" t="s">
         <v>126</v>
       </c>
@@ -7706,7 +7909,7 @@
       <c r="T39" s="63" t="s">
         <v>130</v>
       </c>
-      <c r="U39" s="198"/>
+      <c r="U39" s="201"/>
     </row>
     <row r="40" spans="1:22">
       <c r="A40" s="64">
@@ -8366,12 +8569,19 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="A30:G30"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="O38:O39"/>
-    <mergeCell ref="M38:M39"/>
+    <mergeCell ref="U38:U39"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="H38:H39"/>
+    <mergeCell ref="P38:Q38"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="N38:N39"/>
+    <mergeCell ref="I38:I39"/>
+    <mergeCell ref="J38:J39"/>
+    <mergeCell ref="K38:K39"/>
     <mergeCell ref="R38:S38"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C14:D14"/>
@@ -8388,20 +8598,13 @@
     <mergeCell ref="B26:G26"/>
     <mergeCell ref="L38:L39"/>
     <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="A30:G30"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="O38:O39"/>
+    <mergeCell ref="M38:M39"/>
     <mergeCell ref="B34:G34"/>
-    <mergeCell ref="U38:U39"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="H38:H39"/>
-    <mergeCell ref="P38:Q38"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="N38:N39"/>
-    <mergeCell ref="I38:I39"/>
-    <mergeCell ref="J38:J39"/>
-    <mergeCell ref="K38:K39"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="3">
@@ -8781,10 +8984,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -8799,7 +9002,7 @@
     <col min="8" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19">
+    <row r="1" spans="1:8" ht="19">
       <c r="A1" s="18" t="s">
         <v>21</v>
       </c>
@@ -8809,14 +9012,14 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B2" s="42"/>
       <c r="C2" s="42"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" s="43" t="s">
         <v>4</v>
       </c>
@@ -8838,8 +9041,11 @@
       <c r="G4" s="43" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4" s="43" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="44" t="s">
         <v>6</v>
       </c>
@@ -8859,8 +9065,11 @@
       <c r="G5" s="137" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="46" t="s">
         <v>7</v>
       </c>
@@ -8874,8 +9083,11 @@
       <c r="E6" s="66"/>
       <c r="F6" s="66"/>
       <c r="G6" s="66"/>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="B7" s="15"/>
       <c r="C7" s="48" t="s">
         <v>150</v>
@@ -8884,7 +9096,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:8">
       <c r="C8" s="48" t="s">
         <v>151</v>
       </c>
@@ -8892,7 +9104,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:8">
       <c r="D10" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
0.1.2: Client mode is implented for micronaut.
</commit_message>
<xml_diff>
--- a/meta/api/BlancoApiPostSample.xlsx
+++ b/meta/api/BlancoApiPostSample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorKt/meta/api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A844F26F-4813-5C4B-9D54-7BFBA70B4EB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C74319A-EAB5-0E42-9DC7-C3F448825C46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15160" yWindow="1200" windowWidth="21420" windowHeight="17540" tabRatio="860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15160" yWindow="1200" windowWidth="21420" windowHeight="17540" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="process" sheetId="19" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="241">
   <si>
     <t>項目名</t>
     <rPh sb="0" eb="3">
@@ -2431,6 +2431,21 @@
   </si>
   <si>
     <t>変更不可変数(Kt)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>クライアントアノテーション</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>※ Micronaut の Clientモード時に、HttpClient インタフェイスに指定されるアノテーション</t>
+    <rPh sb="45" eb="47">
+      <t xml:space="preserve">シテイサレル </t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>@Client(value = "{\${target.url:`http://192.168.100.109:28000`}", configuration = HttpClientConfiguration::class)</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -4420,9 +4435,9 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O70"/>
+  <dimension ref="A1:O71"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -4648,149 +4663,149 @@
       <c r="H17" s="95"/>
     </row>
     <row r="18" spans="1:15">
-      <c r="A18" s="183" t="s">
+      <c r="A18" s="146" t="s">
+        <v>238</v>
+      </c>
+      <c r="B18" s="146"/>
+      <c r="C18" s="146"/>
+      <c r="D18" s="142" t="s">
+        <v>240</v>
+      </c>
+      <c r="E18" s="141"/>
+      <c r="F18" s="54" t="s">
+        <v>239</v>
+      </c>
+      <c r="G18" s="54"/>
+      <c r="H18" s="95"/>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" s="183" t="s">
         <v>143</v>
       </c>
-      <c r="B18" s="184"/>
-      <c r="C18" s="185"/>
-      <c r="D18" s="114"/>
-    </row>
-    <row r="19" spans="1:15">
-      <c r="A19" s="169" t="s">
+      <c r="B19" s="184"/>
+      <c r="C19" s="185"/>
+      <c r="D19" s="114"/>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="169" t="s">
         <v>179</v>
       </c>
-      <c r="B19" s="170"/>
-      <c r="C19" s="171"/>
-      <c r="D19" s="100"/>
-      <c r="E19" t="s">
+      <c r="B20" s="170"/>
+      <c r="C20" s="171"/>
+      <c r="D20" s="100"/>
+      <c r="E20" t="s">
         <v>180</v>
       </c>
-      <c r="F19"/>
-      <c r="G19"/>
-      <c r="H19"/>
-      <c r="I19"/>
-      <c r="J19"/>
-      <c r="K19"/>
-      <c r="L19"/>
-    </row>
-    <row r="20" spans="1:15">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
+      <c r="F20"/>
+      <c r="G20"/>
+      <c r="H20"/>
+      <c r="I20"/>
+      <c r="J20"/>
+      <c r="K20"/>
+      <c r="L20"/>
     </row>
     <row r="21" spans="1:15">
-      <c r="A21" s="180" t="s">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" s="180" t="s">
         <v>188</v>
       </c>
-      <c r="B21" s="181"/>
-      <c r="C21" s="181"/>
-      <c r="D21" s="181"/>
-      <c r="E21" s="181"/>
-      <c r="F21" s="181"/>
-      <c r="G21" s="182"/>
-      <c r="H21" s="1" t="s">
+      <c r="B22" s="181"/>
+      <c r="C22" s="181"/>
+      <c r="D22" s="181"/>
+      <c r="E22" s="181"/>
+      <c r="F22" s="181"/>
+      <c r="G22" s="182"/>
+      <c r="H22" s="1" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
-      <c r="A22" s="101" t="s">
+    <row r="23" spans="1:15">
+      <c r="A23" s="101" t="s">
         <v>181</v>
       </c>
-      <c r="B22" s="110"/>
-      <c r="C22" s="102"/>
-      <c r="D22" s="103" t="s">
+      <c r="B23" s="110"/>
+      <c r="C23" s="102"/>
+      <c r="D23" s="103" t="s">
         <v>221</v>
       </c>
-      <c r="E22" s="103"/>
-      <c r="F22" s="103"/>
-      <c r="G22" s="104"/>
-      <c r="H22" s="105"/>
-      <c r="I22" s="105"/>
-      <c r="J22" s="105"/>
-      <c r="K22" s="105"/>
-      <c r="L22" s="105"/>
-    </row>
-    <row r="23" spans="1:15">
-      <c r="A23" s="98" t="s">
-        <v>99</v>
-      </c>
-      <c r="B23" s="113"/>
-      <c r="C23" s="99"/>
-      <c r="D23" s="96" t="s">
-        <v>222</v>
-      </c>
-      <c r="E23" s="97"/>
-      <c r="F23" s="97"/>
-      <c r="G23" s="106"/>
+      <c r="E23" s="103"/>
+      <c r="F23" s="103"/>
+      <c r="G23" s="104"/>
+      <c r="H23" s="105"/>
+      <c r="I23" s="105"/>
+      <c r="J23" s="105"/>
+      <c r="K23" s="105"/>
+      <c r="L23" s="105"/>
     </row>
     <row r="24" spans="1:15">
       <c r="A24" s="98" t="s">
-        <v>182</v>
+        <v>99</v>
       </c>
       <c r="B24" s="113"/>
       <c r="C24" s="99"/>
-      <c r="D24" s="107"/>
-      <c r="E24" s="108"/>
-      <c r="F24" s="108"/>
-      <c r="G24" s="109"/>
+      <c r="D24" s="96" t="s">
+        <v>222</v>
+      </c>
+      <c r="E24" s="97"/>
+      <c r="F24" s="97"/>
+      <c r="G24" s="106"/>
     </row>
     <row r="25" spans="1:15">
-      <c r="C25"/>
+      <c r="A25" s="98" t="s">
+        <v>182</v>
+      </c>
+      <c r="B25" s="113"/>
+      <c r="C25" s="99"/>
+      <c r="D25" s="107"/>
+      <c r="E25" s="108"/>
+      <c r="F25" s="108"/>
+      <c r="G25" s="109"/>
     </row>
     <row r="26" spans="1:15">
-      <c r="A26" s="179" t="s">
+      <c r="C26"/>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27" s="179" t="s">
         <v>189</v>
       </c>
-      <c r="B26" s="179"/>
-      <c r="C26" s="179"/>
-      <c r="D26" s="179"/>
-      <c r="E26" s="179"/>
-      <c r="F26" s="179"/>
-      <c r="G26" s="179"/>
-    </row>
-    <row r="27" spans="1:15">
-      <c r="A27" s="115" t="s">
+      <c r="B27" s="179"/>
+      <c r="C27" s="179"/>
+      <c r="D27" s="179"/>
+      <c r="E27" s="179"/>
+      <c r="F27" s="179"/>
+      <c r="G27" s="179"/>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B27" s="173" t="s">
+      <c r="B28" s="173" t="s">
         <v>183</v>
       </c>
-      <c r="C27" s="174"/>
-      <c r="D27" s="174"/>
-      <c r="E27" s="174"/>
-      <c r="F27" s="174"/>
-      <c r="G27" s="175"/>
-      <c r="H27" s="105"/>
-      <c r="I27" s="105"/>
-      <c r="J27" s="105"/>
-      <c r="K27" s="105"/>
-      <c r="L27" s="105"/>
-      <c r="N27" s="111"/>
-      <c r="O27" s="111"/>
-    </row>
-    <row r="28" spans="1:15">
-      <c r="A28" s="116"/>
-      <c r="B28" s="157"/>
-      <c r="C28" s="157"/>
-      <c r="D28" s="157"/>
-      <c r="E28" s="157"/>
-      <c r="F28" s="157"/>
-      <c r="G28" s="157"/>
-      <c r="H28" s="112"/>
-      <c r="I28" s="112"/>
-      <c r="J28" s="112"/>
-      <c r="K28" s="112"/>
-      <c r="M28"/>
-      <c r="N28"/>
-      <c r="O28"/>
+      <c r="C28" s="174"/>
+      <c r="D28" s="174"/>
+      <c r="E28" s="174"/>
+      <c r="F28" s="174"/>
+      <c r="G28" s="175"/>
+      <c r="H28" s="105"/>
+      <c r="I28" s="105"/>
+      <c r="J28" s="105"/>
+      <c r="K28" s="105"/>
+      <c r="L28" s="105"/>
+      <c r="N28" s="111"/>
+      <c r="O28" s="111"/>
     </row>
     <row r="29" spans="1:15">
-      <c r="A29" s="117"/>
-      <c r="B29" s="159"/>
-      <c r="C29" s="159"/>
-      <c r="D29" s="159"/>
-      <c r="E29" s="159"/>
-      <c r="F29" s="159"/>
-      <c r="G29" s="159"/>
+      <c r="A29" s="116"/>
+      <c r="B29" s="157"/>
+      <c r="C29" s="157"/>
+      <c r="D29" s="157"/>
+      <c r="E29" s="157"/>
+      <c r="F29" s="157"/>
+      <c r="G29" s="157"/>
       <c r="H29" s="112"/>
       <c r="I29" s="112"/>
       <c r="J29" s="112"/>
@@ -4800,13 +4815,13 @@
       <c r="O29"/>
     </row>
     <row r="30" spans="1:15">
-      <c r="A30" s="118"/>
-      <c r="B30" s="161"/>
-      <c r="C30" s="161"/>
-      <c r="D30" s="161"/>
-      <c r="E30" s="161"/>
-      <c r="F30" s="161"/>
-      <c r="G30" s="161"/>
+      <c r="A30" s="117"/>
+      <c r="B30" s="159"/>
+      <c r="C30" s="159"/>
+      <c r="D30" s="159"/>
+      <c r="E30" s="159"/>
+      <c r="F30" s="159"/>
+      <c r="G30" s="159"/>
       <c r="H30" s="112"/>
       <c r="I30" s="112"/>
       <c r="J30" s="112"/>
@@ -4816,67 +4831,67 @@
       <c r="O30"/>
     </row>
     <row r="31" spans="1:15">
-      <c r="C31"/>
+      <c r="A31" s="118"/>
+      <c r="B31" s="161"/>
+      <c r="C31" s="161"/>
+      <c r="D31" s="161"/>
+      <c r="E31" s="161"/>
+      <c r="F31" s="161"/>
+      <c r="G31" s="161"/>
+      <c r="H31" s="112"/>
+      <c r="I31" s="112"/>
+      <c r="J31" s="112"/>
+      <c r="K31" s="112"/>
+      <c r="M31"/>
+      <c r="N31"/>
+      <c r="O31"/>
     </row>
     <row r="32" spans="1:15">
-      <c r="A32" s="176" t="s">
+      <c r="C32"/>
+    </row>
+    <row r="33" spans="1:15">
+      <c r="A33" s="176" t="s">
         <v>190</v>
       </c>
-      <c r="B32" s="177"/>
-      <c r="C32" s="177"/>
-      <c r="D32" s="177"/>
-      <c r="E32" s="177"/>
-      <c r="F32" s="177"/>
-      <c r="G32" s="178"/>
-    </row>
-    <row r="33" spans="1:15">
-      <c r="A33" s="115" t="s">
+      <c r="B33" s="177"/>
+      <c r="C33" s="177"/>
+      <c r="D33" s="177"/>
+      <c r="E33" s="177"/>
+      <c r="F33" s="177"/>
+      <c r="G33" s="178"/>
+    </row>
+    <row r="34" spans="1:15">
+      <c r="A34" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B33" s="153" t="s">
+      <c r="B34" s="153" t="s">
         <v>184</v>
       </c>
-      <c r="C33" s="153"/>
-      <c r="D33" s="153"/>
-      <c r="E33" s="153"/>
-      <c r="F33" s="153"/>
-      <c r="G33" s="153"/>
-      <c r="H33" s="105"/>
-      <c r="I33" s="105"/>
-      <c r="J33" s="105"/>
-      <c r="K33" s="105"/>
-      <c r="L33" s="105"/>
-      <c r="N33" s="111"/>
-      <c r="O33" s="111"/>
-    </row>
-    <row r="34" spans="1:15">
-      <c r="A34" s="116">
+      <c r="C34" s="153"/>
+      <c r="D34" s="153"/>
+      <c r="E34" s="153"/>
+      <c r="F34" s="153"/>
+      <c r="G34" s="153"/>
+      <c r="H34" s="105"/>
+      <c r="I34" s="105"/>
+      <c r="J34" s="105"/>
+      <c r="K34" s="105"/>
+      <c r="L34" s="105"/>
+      <c r="N34" s="111"/>
+      <c r="O34" s="111"/>
+    </row>
+    <row r="35" spans="1:15">
+      <c r="A35" s="116">
         <v>1</v>
       </c>
-      <c r="B34" s="154" t="s">
+      <c r="B35" s="154" t="s">
         <v>218</v>
       </c>
-      <c r="C34" s="154"/>
-      <c r="D34" s="154"/>
-      <c r="E34" s="154"/>
-      <c r="F34" s="154"/>
-      <c r="G34" s="154"/>
-      <c r="H34" s="112"/>
-      <c r="I34" s="112"/>
-      <c r="J34" s="112"/>
-      <c r="K34" s="112"/>
-      <c r="M34"/>
-      <c r="N34"/>
-      <c r="O34"/>
-    </row>
-    <row r="35" spans="1:15">
-      <c r="A35" s="117"/>
-      <c r="B35" s="155"/>
-      <c r="C35" s="155"/>
-      <c r="D35" s="155"/>
-      <c r="E35" s="155"/>
-      <c r="F35" s="155"/>
-      <c r="G35" s="155"/>
+      <c r="C35" s="154"/>
+      <c r="D35" s="154"/>
+      <c r="E35" s="154"/>
+      <c r="F35" s="154"/>
+      <c r="G35" s="154"/>
       <c r="H35" s="112"/>
       <c r="I35" s="112"/>
       <c r="J35" s="112"/>
@@ -4886,13 +4901,13 @@
       <c r="O35"/>
     </row>
     <row r="36" spans="1:15">
-      <c r="A36" s="118"/>
-      <c r="B36" s="156"/>
-      <c r="C36" s="156"/>
-      <c r="D36" s="156"/>
-      <c r="E36" s="156"/>
-      <c r="F36" s="156"/>
-      <c r="G36" s="156"/>
+      <c r="A36" s="117"/>
+      <c r="B36" s="155"/>
+      <c r="C36" s="155"/>
+      <c r="D36" s="155"/>
+      <c r="E36" s="155"/>
+      <c r="F36" s="155"/>
+      <c r="G36" s="155"/>
       <c r="H36" s="112"/>
       <c r="I36" s="112"/>
       <c r="J36" s="112"/>
@@ -4902,75 +4917,75 @@
       <c r="O36"/>
     </row>
     <row r="37" spans="1:15">
-      <c r="A37"/>
-      <c r="B37"/>
-      <c r="C37"/>
-      <c r="D37"/>
-      <c r="E37"/>
-      <c r="F37"/>
-      <c r="G37"/>
-      <c r="H37"/>
-      <c r="I37"/>
-      <c r="J37"/>
-      <c r="K37"/>
-      <c r="L37"/>
+      <c r="A37" s="118"/>
+      <c r="B37" s="156"/>
+      <c r="C37" s="156"/>
+      <c r="D37" s="156"/>
+      <c r="E37" s="156"/>
+      <c r="F37" s="156"/>
+      <c r="G37" s="156"/>
+      <c r="H37" s="112"/>
+      <c r="I37" s="112"/>
+      <c r="J37" s="112"/>
+      <c r="K37" s="112"/>
       <c r="M37"/>
+      <c r="N37"/>
+      <c r="O37"/>
     </row>
     <row r="38" spans="1:15">
-      <c r="A38" s="176" t="s">
+      <c r="A38"/>
+      <c r="B38"/>
+      <c r="C38"/>
+      <c r="D38"/>
+      <c r="E38"/>
+      <c r="F38"/>
+      <c r="G38"/>
+      <c r="H38"/>
+      <c r="I38"/>
+      <c r="J38"/>
+      <c r="K38"/>
+      <c r="L38"/>
+      <c r="M38"/>
+    </row>
+    <row r="39" spans="1:15">
+      <c r="A39" s="176" t="s">
         <v>191</v>
       </c>
-      <c r="B38" s="177"/>
-      <c r="C38" s="177"/>
-      <c r="D38" s="177"/>
-      <c r="E38" s="177"/>
-      <c r="F38" s="177"/>
-      <c r="G38" s="178"/>
-    </row>
-    <row r="39" spans="1:15">
-      <c r="A39" s="115" t="s">
+      <c r="B39" s="177"/>
+      <c r="C39" s="177"/>
+      <c r="D39" s="177"/>
+      <c r="E39" s="177"/>
+      <c r="F39" s="177"/>
+      <c r="G39" s="178"/>
+    </row>
+    <row r="40" spans="1:15">
+      <c r="A40" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B39" s="153" t="s">
+      <c r="B40" s="153" t="s">
         <v>186</v>
       </c>
-      <c r="C39" s="153"/>
-      <c r="D39" s="153"/>
-      <c r="E39" s="153"/>
-      <c r="F39" s="153"/>
-      <c r="G39" s="153"/>
-      <c r="H39" s="105"/>
-      <c r="I39" s="105"/>
-      <c r="J39" s="105"/>
-      <c r="K39" s="105"/>
-      <c r="L39" s="105"/>
-      <c r="N39" s="111"/>
-      <c r="O39" s="111"/>
-    </row>
-    <row r="40" spans="1:15">
-      <c r="A40" s="116"/>
-      <c r="B40" s="157"/>
-      <c r="C40" s="157"/>
-      <c r="D40" s="157"/>
-      <c r="E40" s="157"/>
-      <c r="F40" s="157"/>
-      <c r="G40" s="158"/>
-      <c r="H40" s="112"/>
-      <c r="I40" s="112"/>
-      <c r="J40" s="112"/>
-      <c r="K40" s="112"/>
-      <c r="M40"/>
-      <c r="N40"/>
-      <c r="O40"/>
+      <c r="C40" s="153"/>
+      <c r="D40" s="153"/>
+      <c r="E40" s="153"/>
+      <c r="F40" s="153"/>
+      <c r="G40" s="153"/>
+      <c r="H40" s="105"/>
+      <c r="I40" s="105"/>
+      <c r="J40" s="105"/>
+      <c r="K40" s="105"/>
+      <c r="L40" s="105"/>
+      <c r="N40" s="111"/>
+      <c r="O40" s="111"/>
     </row>
     <row r="41" spans="1:15">
-      <c r="A41" s="117"/>
-      <c r="B41" s="159"/>
-      <c r="C41" s="159"/>
-      <c r="D41" s="159"/>
-      <c r="E41" s="159"/>
-      <c r="F41" s="159"/>
-      <c r="G41" s="160"/>
+      <c r="A41" s="116"/>
+      <c r="B41" s="157"/>
+      <c r="C41" s="157"/>
+      <c r="D41" s="157"/>
+      <c r="E41" s="157"/>
+      <c r="F41" s="157"/>
+      <c r="G41" s="158"/>
       <c r="H41" s="112"/>
       <c r="I41" s="112"/>
       <c r="J41" s="112"/>
@@ -4980,13 +4995,13 @@
       <c r="O41"/>
     </row>
     <row r="42" spans="1:15">
-      <c r="A42" s="118"/>
-      <c r="B42" s="161"/>
-      <c r="C42" s="161"/>
-      <c r="D42" s="161"/>
-      <c r="E42" s="161"/>
-      <c r="F42" s="161"/>
-      <c r="G42" s="162"/>
+      <c r="A42" s="117"/>
+      <c r="B42" s="159"/>
+      <c r="C42" s="159"/>
+      <c r="D42" s="159"/>
+      <c r="E42" s="159"/>
+      <c r="F42" s="159"/>
+      <c r="G42" s="160"/>
       <c r="H42" s="112"/>
       <c r="I42" s="112"/>
       <c r="J42" s="112"/>
@@ -4996,58 +5011,66 @@
       <c r="O42"/>
     </row>
     <row r="43" spans="1:15">
-      <c r="A43"/>
-      <c r="B43"/>
-      <c r="C43"/>
-      <c r="D43"/>
-      <c r="E43"/>
-      <c r="F43"/>
-      <c r="G43"/>
-      <c r="H43"/>
-      <c r="I43"/>
-      <c r="J43"/>
-      <c r="K43"/>
-      <c r="L43"/>
+      <c r="A43" s="118"/>
+      <c r="B43" s="161"/>
+      <c r="C43" s="161"/>
+      <c r="D43" s="161"/>
+      <c r="E43" s="161"/>
+      <c r="F43" s="161"/>
+      <c r="G43" s="162"/>
+      <c r="H43" s="112"/>
+      <c r="I43" s="112"/>
+      <c r="J43" s="112"/>
+      <c r="K43" s="112"/>
       <c r="M43"/>
+      <c r="N43"/>
+      <c r="O43"/>
     </row>
     <row r="44" spans="1:15">
-      <c r="A44" s="4" t="s">
+      <c r="A44"/>
+      <c r="B44"/>
+      <c r="C44"/>
+      <c r="D44"/>
+      <c r="E44"/>
+      <c r="F44"/>
+      <c r="G44"/>
+      <c r="H44"/>
+      <c r="I44"/>
+      <c r="J44"/>
+      <c r="K44"/>
+      <c r="L44"/>
+      <c r="M44"/>
+    </row>
+    <row r="45" spans="1:15">
+      <c r="A45" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="5"/>
-    </row>
-    <row r="45" spans="1:15">
-      <c r="A45" s="166" t="s">
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="5"/>
+    </row>
+    <row r="46" spans="1:15">
+      <c r="A46" s="166" t="s">
         <v>65</v>
       </c>
-      <c r="B45" s="172"/>
-      <c r="C45" s="166" t="s">
+      <c r="B46" s="172"/>
+      <c r="C46" s="166" t="s">
         <v>66</v>
       </c>
-      <c r="D45" s="167"/>
-      <c r="E45" s="168"/>
-      <c r="F45" s="29" t="s">
+      <c r="D46" s="167"/>
+      <c r="E46" s="168"/>
+      <c r="F46" s="29" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="46" spans="1:15">
-      <c r="A46" s="163"/>
-      <c r="B46" s="165"/>
-      <c r="C46" s="163"/>
-      <c r="D46" s="164"/>
-      <c r="E46" s="165"/>
-      <c r="F46" s="49"/>
-    </row>
     <row r="47" spans="1:15">
-      <c r="A47" s="147"/>
-      <c r="B47" s="149"/>
-      <c r="C47" s="147"/>
-      <c r="D47" s="148"/>
-      <c r="E47" s="149"/>
+      <c r="A47" s="163"/>
+      <c r="B47" s="165"/>
+      <c r="C47" s="163"/>
+      <c r="D47" s="164"/>
+      <c r="E47" s="165"/>
       <c r="F47" s="49"/>
     </row>
     <row r="48" spans="1:15">
@@ -5227,56 +5250,65 @@
       <c r="F69" s="49"/>
     </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="150"/>
-      <c r="B70" s="152"/>
-      <c r="C70" s="150"/>
-      <c r="D70" s="151"/>
-      <c r="E70" s="152"/>
-      <c r="F70" s="50"/>
+      <c r="A70" s="147"/>
+      <c r="B70" s="149"/>
+      <c r="C70" s="147"/>
+      <c r="D70" s="148"/>
+      <c r="E70" s="149"/>
+      <c r="F70" s="49"/>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" s="150"/>
+      <c r="B71" s="152"/>
+      <c r="C71" s="150"/>
+      <c r="D71" s="151"/>
+      <c r="E71" s="152"/>
+      <c r="F71" s="50"/>
     </row>
   </sheetData>
-  <mergeCells count="95">
-    <mergeCell ref="A52:B52"/>
+  <mergeCells count="97">
     <mergeCell ref="A53:B53"/>
     <mergeCell ref="A54:B54"/>
     <mergeCell ref="A55:B55"/>
     <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A57:B57"/>
     <mergeCell ref="A48:B48"/>
     <mergeCell ref="A49:B49"/>
     <mergeCell ref="A50:B50"/>
     <mergeCell ref="A51:B51"/>
-    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="C46:E46"/>
     <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="A33:G33"/>
+    <mergeCell ref="A39:G39"/>
+    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="A22:G22"/>
     <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="A38:G38"/>
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="A18:C18"/>
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="D17:E17"/>
     <mergeCell ref="A64:B64"/>
     <mergeCell ref="A65:B65"/>
     <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A67:B67"/>
     <mergeCell ref="A58:B58"/>
     <mergeCell ref="A59:B59"/>
     <mergeCell ref="A60:B60"/>
     <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A62:B62"/>
     <mergeCell ref="A68:B68"/>
     <mergeCell ref="A69:B69"/>
     <mergeCell ref="A70:B70"/>
-    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="A71:B71"/>
     <mergeCell ref="B29:G29"/>
     <mergeCell ref="B30:G30"/>
-    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="B31:G31"/>
     <mergeCell ref="C47:E47"/>
     <mergeCell ref="C48:E48"/>
     <mergeCell ref="C49:E49"/>
@@ -5284,43 +5316,44 @@
     <mergeCell ref="C51:E51"/>
     <mergeCell ref="C52:E52"/>
     <mergeCell ref="C53:E53"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="A63:B63"/>
     <mergeCell ref="C61:E61"/>
     <mergeCell ref="C62:E62"/>
     <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C64:E64"/>
     <mergeCell ref="C55:E55"/>
     <mergeCell ref="C56:E56"/>
     <mergeCell ref="C57:E57"/>
     <mergeCell ref="C58:E58"/>
-    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C59:E59"/>
     <mergeCell ref="C70:E70"/>
-    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="C71:E71"/>
     <mergeCell ref="B34:G34"/>
     <mergeCell ref="B35:G35"/>
     <mergeCell ref="B36:G36"/>
-    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="B37:G37"/>
     <mergeCell ref="B40:G40"/>
     <mergeCell ref="B41:G41"/>
     <mergeCell ref="B42:G42"/>
-    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="B43:G43"/>
     <mergeCell ref="C65:E65"/>
     <mergeCell ref="C66:E66"/>
     <mergeCell ref="C67:E67"/>
     <mergeCell ref="C68:E68"/>
-    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C60:E60"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A18:C18"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="D15:E15"/>
@@ -5334,7 +5367,7 @@
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D19" xr:uid="{AA005DBF-E840-AD43-AC91-CD6CE016CB50}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D20" xr:uid="{AA005DBF-E840-AD43-AC91-CD6CE016CB50}">
       <formula1>isImport</formula1>
     </dataValidation>
   </dataValidations>
@@ -5350,7 +5383,7 @@
           <x14:formula1>
             <xm:f>config!$B$5:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>D18</xm:sqref>
+          <xm:sqref>D19</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5365,7 +5398,7 @@
   </sheetPr>
   <dimension ref="A1:AC66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F26" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q51" sqref="Q51"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
0.1.4: fix bug on noAuthentication flag.
</commit_message>
<xml_diff>
--- a/meta/api/BlancoApiPostSample.xlsx
+++ b/meta/api/BlancoApiPostSample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorKt/meta/api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C74319A-EAB5-0E42-9DC7-C3F448825C46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23837E1-F8D1-D949-BE33-FFC93E0CE240}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15160" yWindow="1200" windowWidth="21420" windowHeight="17540" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="241">
   <si>
     <t>項目名</t>
     <rPh sb="0" eb="3">
@@ -3689,148 +3689,163 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="60" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -3846,50 +3861,35 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="62" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="63" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="65" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="62" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="63" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="65" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -4438,7 +4438,7 @@
   <dimension ref="A1:O71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D12" sqref="D12:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -4481,137 +4481,137 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="139" t="s">
+      <c r="A5" s="185" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="139"/>
-      <c r="C5" s="139"/>
-      <c r="D5" s="139"/>
-      <c r="E5" s="139"/>
+      <c r="B5" s="185"/>
+      <c r="C5" s="185"/>
+      <c r="D5" s="185"/>
+      <c r="E5" s="185"/>
       <c r="F5" s="55"/>
       <c r="G5" s="55"/>
       <c r="H5" s="95"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="143" t="s">
+      <c r="A6" s="182" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="144"/>
-      <c r="C6" s="145"/>
-      <c r="D6" s="140" t="s">
+      <c r="B6" s="183"/>
+      <c r="C6" s="184"/>
+      <c r="D6" s="181" t="s">
         <v>197</v>
       </c>
-      <c r="E6" s="140"/>
+      <c r="E6" s="181"/>
       <c r="F6" s="55"/>
       <c r="G6" s="55"/>
       <c r="H6" s="95"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="139" t="s">
+      <c r="A7" s="185" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="139"/>
-      <c r="C7" s="139"/>
-      <c r="D7" s="140" t="s">
+      <c r="B7" s="185"/>
+      <c r="C7" s="185"/>
+      <c r="D7" s="181" t="s">
         <v>166</v>
       </c>
-      <c r="E7" s="140"/>
+      <c r="E7" s="181"/>
       <c r="F7" s="55"/>
       <c r="G7" s="55"/>
       <c r="H7" s="95"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="139" t="s">
+      <c r="A8" s="185" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="139"/>
-      <c r="C8" s="139"/>
-      <c r="D8" s="140" t="s">
+      <c r="B8" s="185"/>
+      <c r="C8" s="185"/>
+      <c r="D8" s="181" t="s">
         <v>162</v>
       </c>
-      <c r="E8" s="140"/>
+      <c r="E8" s="181"/>
       <c r="F8" s="95"/>
       <c r="G8" s="95"/>
       <c r="H8" s="95"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="139" t="s">
+      <c r="A9" s="185" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="139"/>
-      <c r="C9" s="139"/>
-      <c r="D9" s="140" t="s">
+      <c r="B9" s="185"/>
+      <c r="C9" s="185"/>
+      <c r="D9" s="181" t="s">
         <v>100</v>
       </c>
-      <c r="E9" s="140"/>
+      <c r="E9" s="181"/>
       <c r="F9" s="95"/>
       <c r="G9" s="95"/>
       <c r="H9" s="95"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="139" t="s">
+      <c r="A10" s="185" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="139"/>
-      <c r="C10" s="139"/>
-      <c r="D10" s="140"/>
-      <c r="E10" s="140"/>
+      <c r="B10" s="185"/>
+      <c r="C10" s="185"/>
+      <c r="D10" s="181"/>
+      <c r="E10" s="181"/>
       <c r="F10" s="95"/>
       <c r="G10" s="95"/>
       <c r="H10" s="95"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="139" t="s">
+      <c r="A11" s="185" t="s">
         <v>99</v>
       </c>
-      <c r="B11" s="139"/>
-      <c r="C11" s="139"/>
-      <c r="D11" s="140" t="s">
+      <c r="B11" s="185"/>
+      <c r="C11" s="185"/>
+      <c r="D11" s="181" t="s">
         <v>163</v>
       </c>
-      <c r="E11" s="140"/>
+      <c r="E11" s="181"/>
       <c r="F11" s="95"/>
       <c r="G11" s="95"/>
       <c r="H11" s="95"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="146" t="s">
+      <c r="A12" s="144" t="s">
         <v>174</v>
       </c>
-      <c r="B12" s="146"/>
-      <c r="C12" s="146"/>
-      <c r="D12" s="141" t="s">
+      <c r="B12" s="144"/>
+      <c r="C12" s="144"/>
+      <c r="D12" s="165" t="s">
         <v>175</v>
       </c>
-      <c r="E12" s="141"/>
+      <c r="E12" s="165"/>
       <c r="F12" s="95" t="s">
         <v>176</v>
       </c>
       <c r="G12" s="54"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="146" t="s">
+      <c r="A13" s="144" t="s">
         <v>212</v>
       </c>
-      <c r="B13" s="146"/>
-      <c r="C13" s="146"/>
-      <c r="D13" s="141" t="s">
+      <c r="B13" s="144"/>
+      <c r="C13" s="144"/>
+      <c r="D13" s="165" t="s">
         <v>210</v>
       </c>
-      <c r="E13" s="141"/>
+      <c r="E13" s="165"/>
       <c r="F13" s="95" t="s">
         <v>211</v>
       </c>
       <c r="G13" s="54"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="146" t="s">
+      <c r="A14" s="144" t="s">
         <v>177</v>
       </c>
-      <c r="B14" s="146"/>
-      <c r="C14" s="146"/>
-      <c r="D14" s="142"/>
-      <c r="E14" s="141"/>
+      <c r="B14" s="144"/>
+      <c r="C14" s="144"/>
+      <c r="D14" s="164"/>
+      <c r="E14" s="165"/>
       <c r="F14" s="54" t="s">
         <v>198</v>
       </c>
@@ -4619,15 +4619,15 @@
       <c r="H14" s="95"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="146" t="s">
+      <c r="A15" s="144" t="s">
         <v>217</v>
       </c>
-      <c r="B15" s="146"/>
-      <c r="C15" s="146"/>
-      <c r="D15" s="142" t="s">
+      <c r="B15" s="144"/>
+      <c r="C15" s="144"/>
+      <c r="D15" s="164" t="s">
         <v>215</v>
       </c>
-      <c r="E15" s="141"/>
+      <c r="E15" s="165"/>
       <c r="F15" s="54" t="s">
         <v>220</v>
       </c>
@@ -4635,13 +4635,13 @@
       <c r="H15" s="95"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="146" t="s">
+      <c r="A16" s="144" t="s">
         <v>216</v>
       </c>
-      <c r="B16" s="146"/>
-      <c r="C16" s="146"/>
-      <c r="D16" s="142"/>
-      <c r="E16" s="141"/>
+      <c r="B16" s="144"/>
+      <c r="C16" s="144"/>
+      <c r="D16" s="164"/>
+      <c r="E16" s="165"/>
       <c r="F16" s="54" t="s">
         <v>219</v>
       </c>
@@ -4649,13 +4649,13 @@
       <c r="H16" s="95"/>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="146" t="s">
+      <c r="A17" s="144" t="s">
         <v>214</v>
       </c>
-      <c r="B17" s="146"/>
-      <c r="C17" s="146"/>
-      <c r="D17" s="142"/>
-      <c r="E17" s="141"/>
+      <c r="B17" s="144"/>
+      <c r="C17" s="144"/>
+      <c r="D17" s="164"/>
+      <c r="E17" s="165"/>
       <c r="F17" s="54" t="s">
         <v>213</v>
       </c>
@@ -4663,15 +4663,15 @@
       <c r="H17" s="95"/>
     </row>
     <row r="18" spans="1:15">
-      <c r="A18" s="146" t="s">
+      <c r="A18" s="144" t="s">
         <v>238</v>
       </c>
-      <c r="B18" s="146"/>
-      <c r="C18" s="146"/>
-      <c r="D18" s="142" t="s">
+      <c r="B18" s="144"/>
+      <c r="C18" s="144"/>
+      <c r="D18" s="164" t="s">
         <v>240</v>
       </c>
-      <c r="E18" s="141"/>
+      <c r="E18" s="165"/>
       <c r="F18" s="54" t="s">
         <v>239</v>
       </c>
@@ -4679,19 +4679,21 @@
       <c r="H18" s="95"/>
     </row>
     <row r="19" spans="1:15">
-      <c r="A19" s="183" t="s">
+      <c r="A19" s="161" t="s">
         <v>143</v>
       </c>
-      <c r="B19" s="184"/>
-      <c r="C19" s="185"/>
-      <c r="D19" s="114"/>
+      <c r="B19" s="162"/>
+      <c r="C19" s="163"/>
+      <c r="D19" s="114" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="20" spans="1:15">
-      <c r="A20" s="169" t="s">
+      <c r="A20" s="145" t="s">
         <v>179</v>
       </c>
-      <c r="B20" s="170"/>
-      <c r="C20" s="171"/>
+      <c r="B20" s="146"/>
+      <c r="C20" s="147"/>
       <c r="D20" s="100"/>
       <c r="E20" t="s">
         <v>180</v>
@@ -4709,15 +4711,15 @@
       <c r="B21" s="6"/>
     </row>
     <row r="22" spans="1:15">
-      <c r="A22" s="180" t="s">
+      <c r="A22" s="158" t="s">
         <v>188</v>
       </c>
-      <c r="B22" s="181"/>
-      <c r="C22" s="181"/>
-      <c r="D22" s="181"/>
-      <c r="E22" s="181"/>
-      <c r="F22" s="181"/>
-      <c r="G22" s="182"/>
+      <c r="B22" s="159"/>
+      <c r="C22" s="159"/>
+      <c r="D22" s="159"/>
+      <c r="E22" s="159"/>
+      <c r="F22" s="159"/>
+      <c r="G22" s="160"/>
       <c r="H22" s="1" t="s">
         <v>223</v>
       </c>
@@ -4768,28 +4770,28 @@
       <c r="C26"/>
     </row>
     <row r="27" spans="1:15">
-      <c r="A27" s="179" t="s">
+      <c r="A27" s="157" t="s">
         <v>189</v>
       </c>
-      <c r="B27" s="179"/>
-      <c r="C27" s="179"/>
-      <c r="D27" s="179"/>
-      <c r="E27" s="179"/>
-      <c r="F27" s="179"/>
-      <c r="G27" s="179"/>
+      <c r="B27" s="157"/>
+      <c r="C27" s="157"/>
+      <c r="D27" s="157"/>
+      <c r="E27" s="157"/>
+      <c r="F27" s="157"/>
+      <c r="G27" s="157"/>
     </row>
     <row r="28" spans="1:15">
       <c r="A28" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B28" s="173" t="s">
+      <c r="B28" s="151" t="s">
         <v>183</v>
       </c>
-      <c r="C28" s="174"/>
-      <c r="D28" s="174"/>
-      <c r="E28" s="174"/>
-      <c r="F28" s="174"/>
-      <c r="G28" s="175"/>
+      <c r="C28" s="152"/>
+      <c r="D28" s="152"/>
+      <c r="E28" s="152"/>
+      <c r="F28" s="152"/>
+      <c r="G28" s="153"/>
       <c r="H28" s="105"/>
       <c r="I28" s="105"/>
       <c r="J28" s="105"/>
@@ -4800,12 +4802,12 @@
     </row>
     <row r="29" spans="1:15">
       <c r="A29" s="116"/>
-      <c r="B29" s="157"/>
-      <c r="C29" s="157"/>
-      <c r="D29" s="157"/>
-      <c r="E29" s="157"/>
-      <c r="F29" s="157"/>
-      <c r="G29" s="157"/>
+      <c r="B29" s="168"/>
+      <c r="C29" s="168"/>
+      <c r="D29" s="168"/>
+      <c r="E29" s="168"/>
+      <c r="F29" s="168"/>
+      <c r="G29" s="168"/>
       <c r="H29" s="112"/>
       <c r="I29" s="112"/>
       <c r="J29" s="112"/>
@@ -4816,12 +4818,12 @@
     </row>
     <row r="30" spans="1:15">
       <c r="A30" s="117"/>
-      <c r="B30" s="159"/>
-      <c r="C30" s="159"/>
-      <c r="D30" s="159"/>
-      <c r="E30" s="159"/>
-      <c r="F30" s="159"/>
-      <c r="G30" s="159"/>
+      <c r="B30" s="169"/>
+      <c r="C30" s="169"/>
+      <c r="D30" s="169"/>
+      <c r="E30" s="169"/>
+      <c r="F30" s="169"/>
+      <c r="G30" s="169"/>
       <c r="H30" s="112"/>
       <c r="I30" s="112"/>
       <c r="J30" s="112"/>
@@ -4832,12 +4834,12 @@
     </row>
     <row r="31" spans="1:15">
       <c r="A31" s="118"/>
-      <c r="B31" s="161"/>
-      <c r="C31" s="161"/>
-      <c r="D31" s="161"/>
-      <c r="E31" s="161"/>
-      <c r="F31" s="161"/>
-      <c r="G31" s="161"/>
+      <c r="B31" s="170"/>
+      <c r="C31" s="170"/>
+      <c r="D31" s="170"/>
+      <c r="E31" s="170"/>
+      <c r="F31" s="170"/>
+      <c r="G31" s="170"/>
       <c r="H31" s="112"/>
       <c r="I31" s="112"/>
       <c r="J31" s="112"/>
@@ -4850,28 +4852,28 @@
       <c r="C32"/>
     </row>
     <row r="33" spans="1:15">
-      <c r="A33" s="176" t="s">
+      <c r="A33" s="154" t="s">
         <v>190</v>
       </c>
-      <c r="B33" s="177"/>
-      <c r="C33" s="177"/>
-      <c r="D33" s="177"/>
-      <c r="E33" s="177"/>
-      <c r="F33" s="177"/>
-      <c r="G33" s="178"/>
+      <c r="B33" s="155"/>
+      <c r="C33" s="155"/>
+      <c r="D33" s="155"/>
+      <c r="E33" s="155"/>
+      <c r="F33" s="155"/>
+      <c r="G33" s="156"/>
     </row>
     <row r="34" spans="1:15">
       <c r="A34" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="153" t="s">
+      <c r="B34" s="174" t="s">
         <v>184</v>
       </c>
-      <c r="C34" s="153"/>
-      <c r="D34" s="153"/>
-      <c r="E34" s="153"/>
-      <c r="F34" s="153"/>
-      <c r="G34" s="153"/>
+      <c r="C34" s="174"/>
+      <c r="D34" s="174"/>
+      <c r="E34" s="174"/>
+      <c r="F34" s="174"/>
+      <c r="G34" s="174"/>
       <c r="H34" s="105"/>
       <c r="I34" s="105"/>
       <c r="J34" s="105"/>
@@ -4884,14 +4886,14 @@
       <c r="A35" s="116">
         <v>1</v>
       </c>
-      <c r="B35" s="154" t="s">
+      <c r="B35" s="175" t="s">
         <v>218</v>
       </c>
-      <c r="C35" s="154"/>
-      <c r="D35" s="154"/>
-      <c r="E35" s="154"/>
-      <c r="F35" s="154"/>
-      <c r="G35" s="154"/>
+      <c r="C35" s="175"/>
+      <c r="D35" s="175"/>
+      <c r="E35" s="175"/>
+      <c r="F35" s="175"/>
+      <c r="G35" s="175"/>
       <c r="H35" s="112"/>
       <c r="I35" s="112"/>
       <c r="J35" s="112"/>
@@ -4902,12 +4904,12 @@
     </row>
     <row r="36" spans="1:15">
       <c r="A36" s="117"/>
-      <c r="B36" s="155"/>
-      <c r="C36" s="155"/>
-      <c r="D36" s="155"/>
-      <c r="E36" s="155"/>
-      <c r="F36" s="155"/>
-      <c r="G36" s="155"/>
+      <c r="B36" s="176"/>
+      <c r="C36" s="176"/>
+      <c r="D36" s="176"/>
+      <c r="E36" s="176"/>
+      <c r="F36" s="176"/>
+      <c r="G36" s="176"/>
       <c r="H36" s="112"/>
       <c r="I36" s="112"/>
       <c r="J36" s="112"/>
@@ -4918,12 +4920,12 @@
     </row>
     <row r="37" spans="1:15">
       <c r="A37" s="118"/>
-      <c r="B37" s="156"/>
-      <c r="C37" s="156"/>
-      <c r="D37" s="156"/>
-      <c r="E37" s="156"/>
-      <c r="F37" s="156"/>
-      <c r="G37" s="156"/>
+      <c r="B37" s="177"/>
+      <c r="C37" s="177"/>
+      <c r="D37" s="177"/>
+      <c r="E37" s="177"/>
+      <c r="F37" s="177"/>
+      <c r="G37" s="177"/>
       <c r="H37" s="112"/>
       <c r="I37" s="112"/>
       <c r="J37" s="112"/>
@@ -4948,28 +4950,28 @@
       <c r="M38"/>
     </row>
     <row r="39" spans="1:15">
-      <c r="A39" s="176" t="s">
+      <c r="A39" s="154" t="s">
         <v>191</v>
       </c>
-      <c r="B39" s="177"/>
-      <c r="C39" s="177"/>
-      <c r="D39" s="177"/>
-      <c r="E39" s="177"/>
-      <c r="F39" s="177"/>
-      <c r="G39" s="178"/>
+      <c r="B39" s="155"/>
+      <c r="C39" s="155"/>
+      <c r="D39" s="155"/>
+      <c r="E39" s="155"/>
+      <c r="F39" s="155"/>
+      <c r="G39" s="156"/>
     </row>
     <row r="40" spans="1:15">
       <c r="A40" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B40" s="153" t="s">
+      <c r="B40" s="174" t="s">
         <v>186</v>
       </c>
-      <c r="C40" s="153"/>
-      <c r="D40" s="153"/>
-      <c r="E40" s="153"/>
-      <c r="F40" s="153"/>
-      <c r="G40" s="153"/>
+      <c r="C40" s="174"/>
+      <c r="D40" s="174"/>
+      <c r="E40" s="174"/>
+      <c r="F40" s="174"/>
+      <c r="G40" s="174"/>
       <c r="H40" s="105"/>
       <c r="I40" s="105"/>
       <c r="J40" s="105"/>
@@ -4980,12 +4982,12 @@
     </row>
     <row r="41" spans="1:15">
       <c r="A41" s="116"/>
-      <c r="B41" s="157"/>
-      <c r="C41" s="157"/>
-      <c r="D41" s="157"/>
-      <c r="E41" s="157"/>
-      <c r="F41" s="157"/>
-      <c r="G41" s="158"/>
+      <c r="B41" s="168"/>
+      <c r="C41" s="168"/>
+      <c r="D41" s="168"/>
+      <c r="E41" s="168"/>
+      <c r="F41" s="168"/>
+      <c r="G41" s="178"/>
       <c r="H41" s="112"/>
       <c r="I41" s="112"/>
       <c r="J41" s="112"/>
@@ -4996,12 +4998,12 @@
     </row>
     <row r="42" spans="1:15">
       <c r="A42" s="117"/>
-      <c r="B42" s="159"/>
-      <c r="C42" s="159"/>
-      <c r="D42" s="159"/>
-      <c r="E42" s="159"/>
-      <c r="F42" s="159"/>
-      <c r="G42" s="160"/>
+      <c r="B42" s="169"/>
+      <c r="C42" s="169"/>
+      <c r="D42" s="169"/>
+      <c r="E42" s="169"/>
+      <c r="F42" s="169"/>
+      <c r="G42" s="179"/>
       <c r="H42" s="112"/>
       <c r="I42" s="112"/>
       <c r="J42" s="112"/>
@@ -5012,12 +5014,12 @@
     </row>
     <row r="43" spans="1:15">
       <c r="A43" s="118"/>
-      <c r="B43" s="161"/>
-      <c r="C43" s="161"/>
-      <c r="D43" s="161"/>
-      <c r="E43" s="161"/>
-      <c r="F43" s="161"/>
-      <c r="G43" s="162"/>
+      <c r="B43" s="170"/>
+      <c r="C43" s="170"/>
+      <c r="D43" s="170"/>
+      <c r="E43" s="170"/>
+      <c r="F43" s="170"/>
+      <c r="G43" s="180"/>
       <c r="H43" s="112"/>
       <c r="I43" s="112"/>
       <c r="J43" s="112"/>
@@ -5052,231 +5054,292 @@
       <c r="F45" s="5"/>
     </row>
     <row r="46" spans="1:15">
-      <c r="A46" s="166" t="s">
+      <c r="A46" s="141" t="s">
         <v>65</v>
       </c>
-      <c r="B46" s="172"/>
-      <c r="C46" s="166" t="s">
+      <c r="B46" s="148"/>
+      <c r="C46" s="141" t="s">
         <v>66</v>
       </c>
-      <c r="D46" s="167"/>
-      <c r="E46" s="168"/>
+      <c r="D46" s="142"/>
+      <c r="E46" s="143"/>
       <c r="F46" s="29" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="47" spans="1:15">
-      <c r="A47" s="163"/>
-      <c r="B47" s="165"/>
-      <c r="C47" s="163"/>
-      <c r="D47" s="164"/>
-      <c r="E47" s="165"/>
+      <c r="A47" s="149"/>
+      <c r="B47" s="150"/>
+      <c r="C47" s="149"/>
+      <c r="D47" s="171"/>
+      <c r="E47" s="150"/>
       <c r="F47" s="49"/>
     </row>
     <row r="48" spans="1:15">
-      <c r="A48" s="147"/>
-      <c r="B48" s="149"/>
-      <c r="C48" s="147"/>
-      <c r="D48" s="148"/>
-      <c r="E48" s="149"/>
+      <c r="A48" s="139"/>
+      <c r="B48" s="140"/>
+      <c r="C48" s="139"/>
+      <c r="D48" s="172"/>
+      <c r="E48" s="140"/>
       <c r="F48" s="49"/>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="147"/>
-      <c r="B49" s="149"/>
-      <c r="C49" s="147"/>
-      <c r="D49" s="148"/>
-      <c r="E49" s="149"/>
+      <c r="A49" s="139"/>
+      <c r="B49" s="140"/>
+      <c r="C49" s="139"/>
+      <c r="D49" s="172"/>
+      <c r="E49" s="140"/>
       <c r="F49" s="49"/>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="147"/>
-      <c r="B50" s="149"/>
-      <c r="C50" s="147"/>
-      <c r="D50" s="148"/>
-      <c r="E50" s="149"/>
+      <c r="A50" s="139"/>
+      <c r="B50" s="140"/>
+      <c r="C50" s="139"/>
+      <c r="D50" s="172"/>
+      <c r="E50" s="140"/>
       <c r="F50" s="49"/>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="147"/>
-      <c r="B51" s="149"/>
-      <c r="C51" s="147"/>
-      <c r="D51" s="148"/>
-      <c r="E51" s="149"/>
+      <c r="A51" s="139"/>
+      <c r="B51" s="140"/>
+      <c r="C51" s="139"/>
+      <c r="D51" s="172"/>
+      <c r="E51" s="140"/>
       <c r="F51" s="49"/>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="147"/>
-      <c r="B52" s="149"/>
-      <c r="C52" s="147"/>
-      <c r="D52" s="148"/>
-      <c r="E52" s="149"/>
+      <c r="A52" s="139"/>
+      <c r="B52" s="140"/>
+      <c r="C52" s="139"/>
+      <c r="D52" s="172"/>
+      <c r="E52" s="140"/>
       <c r="F52" s="49"/>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="147"/>
-      <c r="B53" s="149"/>
-      <c r="C53" s="147"/>
-      <c r="D53" s="148"/>
-      <c r="E53" s="149"/>
+      <c r="A53" s="139"/>
+      <c r="B53" s="140"/>
+      <c r="C53" s="139"/>
+      <c r="D53" s="172"/>
+      <c r="E53" s="140"/>
       <c r="F53" s="49"/>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="147"/>
-      <c r="B54" s="149"/>
-      <c r="C54" s="147"/>
-      <c r="D54" s="148"/>
-      <c r="E54" s="149"/>
+      <c r="A54" s="139"/>
+      <c r="B54" s="140"/>
+      <c r="C54" s="139"/>
+      <c r="D54" s="172"/>
+      <c r="E54" s="140"/>
       <c r="F54" s="49"/>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="147"/>
-      <c r="B55" s="149"/>
-      <c r="C55" s="147"/>
-      <c r="D55" s="148"/>
-      <c r="E55" s="149"/>
+      <c r="A55" s="139"/>
+      <c r="B55" s="140"/>
+      <c r="C55" s="139"/>
+      <c r="D55" s="172"/>
+      <c r="E55" s="140"/>
       <c r="F55" s="49"/>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="147"/>
-      <c r="B56" s="149"/>
-      <c r="C56" s="147"/>
-      <c r="D56" s="148"/>
-      <c r="E56" s="149"/>
+      <c r="A56" s="139"/>
+      <c r="B56" s="140"/>
+      <c r="C56" s="139"/>
+      <c r="D56" s="172"/>
+      <c r="E56" s="140"/>
       <c r="F56" s="49"/>
     </row>
     <row r="57" spans="1:6">
-      <c r="A57" s="147"/>
-      <c r="B57" s="149"/>
-      <c r="C57" s="147"/>
-      <c r="D57" s="148"/>
-      <c r="E57" s="149"/>
+      <c r="A57" s="139"/>
+      <c r="B57" s="140"/>
+      <c r="C57" s="139"/>
+      <c r="D57" s="172"/>
+      <c r="E57" s="140"/>
       <c r="F57" s="49"/>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="147"/>
-      <c r="B58" s="149"/>
-      <c r="C58" s="147"/>
-      <c r="D58" s="148"/>
-      <c r="E58" s="149"/>
+      <c r="A58" s="139"/>
+      <c r="B58" s="140"/>
+      <c r="C58" s="139"/>
+      <c r="D58" s="172"/>
+      <c r="E58" s="140"/>
       <c r="F58" s="49"/>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="147"/>
-      <c r="B59" s="149"/>
-      <c r="C59" s="147"/>
-      <c r="D59" s="148"/>
-      <c r="E59" s="149"/>
+      <c r="A59" s="139"/>
+      <c r="B59" s="140"/>
+      <c r="C59" s="139"/>
+      <c r="D59" s="172"/>
+      <c r="E59" s="140"/>
       <c r="F59" s="49"/>
     </row>
     <row r="60" spans="1:6">
-      <c r="A60" s="147"/>
-      <c r="B60" s="149"/>
-      <c r="C60" s="147"/>
-      <c r="D60" s="148"/>
-      <c r="E60" s="149"/>
+      <c r="A60" s="139"/>
+      <c r="B60" s="140"/>
+      <c r="C60" s="139"/>
+      <c r="D60" s="172"/>
+      <c r="E60" s="140"/>
       <c r="F60" s="49"/>
     </row>
     <row r="61" spans="1:6">
-      <c r="A61" s="147"/>
-      <c r="B61" s="149"/>
-      <c r="C61" s="147"/>
-      <c r="D61" s="148"/>
-      <c r="E61" s="149"/>
+      <c r="A61" s="139"/>
+      <c r="B61" s="140"/>
+      <c r="C61" s="139"/>
+      <c r="D61" s="172"/>
+      <c r="E61" s="140"/>
       <c r="F61" s="49"/>
     </row>
     <row r="62" spans="1:6">
-      <c r="A62" s="147"/>
-      <c r="B62" s="149"/>
-      <c r="C62" s="147"/>
-      <c r="D62" s="148"/>
-      <c r="E62" s="149"/>
+      <c r="A62" s="139"/>
+      <c r="B62" s="140"/>
+      <c r="C62" s="139"/>
+      <c r="D62" s="172"/>
+      <c r="E62" s="140"/>
       <c r="F62" s="49"/>
     </row>
     <row r="63" spans="1:6">
-      <c r="A63" s="147"/>
-      <c r="B63" s="149"/>
-      <c r="C63" s="147"/>
-      <c r="D63" s="148"/>
-      <c r="E63" s="149"/>
+      <c r="A63" s="139"/>
+      <c r="B63" s="140"/>
+      <c r="C63" s="139"/>
+      <c r="D63" s="172"/>
+      <c r="E63" s="140"/>
       <c r="F63" s="49"/>
     </row>
     <row r="64" spans="1:6">
-      <c r="A64" s="147"/>
-      <c r="B64" s="149"/>
-      <c r="C64" s="147"/>
-      <c r="D64" s="148"/>
-      <c r="E64" s="149"/>
+      <c r="A64" s="139"/>
+      <c r="B64" s="140"/>
+      <c r="C64" s="139"/>
+      <c r="D64" s="172"/>
+      <c r="E64" s="140"/>
       <c r="F64" s="49"/>
     </row>
     <row r="65" spans="1:6">
-      <c r="A65" s="147"/>
-      <c r="B65" s="149"/>
-      <c r="C65" s="147"/>
-      <c r="D65" s="148"/>
-      <c r="E65" s="149"/>
+      <c r="A65" s="139"/>
+      <c r="B65" s="140"/>
+      <c r="C65" s="139"/>
+      <c r="D65" s="172"/>
+      <c r="E65" s="140"/>
       <c r="F65" s="49"/>
     </row>
     <row r="66" spans="1:6">
-      <c r="A66" s="147"/>
-      <c r="B66" s="149"/>
-      <c r="C66" s="147"/>
-      <c r="D66" s="148"/>
-      <c r="E66" s="149"/>
+      <c r="A66" s="139"/>
+      <c r="B66" s="140"/>
+      <c r="C66" s="139"/>
+      <c r="D66" s="172"/>
+      <c r="E66" s="140"/>
       <c r="F66" s="49"/>
     </row>
     <row r="67" spans="1:6">
-      <c r="A67" s="147"/>
-      <c r="B67" s="149"/>
-      <c r="C67" s="147"/>
-      <c r="D67" s="148"/>
-      <c r="E67" s="149"/>
+      <c r="A67" s="139"/>
+      <c r="B67" s="140"/>
+      <c r="C67" s="139"/>
+      <c r="D67" s="172"/>
+      <c r="E67" s="140"/>
       <c r="F67" s="49"/>
     </row>
     <row r="68" spans="1:6">
-      <c r="A68" s="147"/>
-      <c r="B68" s="149"/>
-      <c r="C68" s="147"/>
-      <c r="D68" s="148"/>
-      <c r="E68" s="149"/>
+      <c r="A68" s="139"/>
+      <c r="B68" s="140"/>
+      <c r="C68" s="139"/>
+      <c r="D68" s="172"/>
+      <c r="E68" s="140"/>
       <c r="F68" s="49"/>
     </row>
     <row r="69" spans="1:6">
-      <c r="A69" s="147"/>
-      <c r="B69" s="149"/>
-      <c r="C69" s="147"/>
-      <c r="D69" s="148"/>
-      <c r="E69" s="149"/>
+      <c r="A69" s="139"/>
+      <c r="B69" s="140"/>
+      <c r="C69" s="139"/>
+      <c r="D69" s="172"/>
+      <c r="E69" s="140"/>
       <c r="F69" s="49"/>
     </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="147"/>
-      <c r="B70" s="149"/>
-      <c r="C70" s="147"/>
-      <c r="D70" s="148"/>
-      <c r="E70" s="149"/>
+      <c r="A70" s="139"/>
+      <c r="B70" s="140"/>
+      <c r="C70" s="139"/>
+      <c r="D70" s="172"/>
+      <c r="E70" s="140"/>
       <c r="F70" s="49"/>
     </row>
     <row r="71" spans="1:6">
-      <c r="A71" s="150"/>
-      <c r="B71" s="152"/>
-      <c r="C71" s="150"/>
-      <c r="D71" s="151"/>
-      <c r="E71" s="152"/>
+      <c r="A71" s="166"/>
+      <c r="B71" s="167"/>
+      <c r="C71" s="166"/>
+      <c r="D71" s="173"/>
+      <c r="E71" s="167"/>
       <c r="F71" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="97">
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="C70:E70"/>
+    <mergeCell ref="C71:E71"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="B41:G41"/>
+    <mergeCell ref="B42:G42"/>
+    <mergeCell ref="B43:G43"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
     <mergeCell ref="C46:E46"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="A20:C20"/>
@@ -5293,77 +5356,16 @@
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="D17:E17"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="C51:E51"/>
-    <mergeCell ref="C52:E52"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="C70:E70"/>
-    <mergeCell ref="C71:E71"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B36:G36"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="B41:G41"/>
-    <mergeCell ref="B42:G42"/>
-    <mergeCell ref="B43:G43"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="1">
@@ -5648,10 +5650,10 @@
         <v>174</v>
       </c>
       <c r="B15" s="122"/>
-      <c r="C15" s="141" t="s">
+      <c r="C15" s="165" t="s">
         <v>175</v>
       </c>
-      <c r="D15" s="141"/>
+      <c r="D15" s="165"/>
       <c r="E15" s="95" t="s">
         <v>176</v>
       </c>
@@ -5666,10 +5668,10 @@
         <v>226</v>
       </c>
       <c r="B16" s="122"/>
-      <c r="C16" s="142" t="s">
+      <c r="C16" s="164" t="s">
         <v>230</v>
       </c>
-      <c r="D16" s="141"/>
+      <c r="D16" s="165"/>
       <c r="E16" s="55" t="s">
         <v>227</v>
       </c>
@@ -5692,10 +5694,10 @@
         <v>177</v>
       </c>
       <c r="B17" s="122"/>
-      <c r="C17" s="141" t="s">
+      <c r="C17" s="165" t="s">
         <v>178</v>
       </c>
-      <c r="D17" s="141"/>
+      <c r="D17" s="165"/>
       <c r="E17" s="55"/>
       <c r="F17" s="55"/>
       <c r="G17" s="54"/>
@@ -5707,8 +5709,8 @@
         <v>228</v>
       </c>
       <c r="B18" s="122"/>
-      <c r="C18" s="142"/>
-      <c r="D18" s="141"/>
+      <c r="C18" s="164"/>
+      <c r="D18" s="165"/>
       <c r="E18" s="55" t="s">
         <v>229</v>
       </c>
@@ -5764,15 +5766,15 @@
       <c r="O20"/>
     </row>
     <row r="21" spans="1:25">
-      <c r="A21" s="179" t="s">
+      <c r="A21" s="157" t="s">
         <v>192</v>
       </c>
-      <c r="B21" s="179"/>
-      <c r="C21" s="179"/>
-      <c r="D21" s="179"/>
-      <c r="E21" s="179"/>
-      <c r="F21" s="179"/>
-      <c r="G21" s="179"/>
+      <c r="B21" s="157"/>
+      <c r="C21" s="157"/>
+      <c r="D21" s="157"/>
+      <c r="E21" s="157"/>
+      <c r="F21" s="157"/>
+      <c r="G21" s="157"/>
       <c r="K21"/>
       <c r="L21"/>
       <c r="M21"/>
@@ -5782,14 +5784,14 @@
       <c r="A22" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B22" s="173" t="s">
+      <c r="B22" s="151" t="s">
         <v>183</v>
       </c>
-      <c r="C22" s="174"/>
-      <c r="D22" s="174"/>
-      <c r="E22" s="174"/>
-      <c r="F22" s="174"/>
-      <c r="G22" s="175"/>
+      <c r="C22" s="152"/>
+      <c r="D22" s="152"/>
+      <c r="E22" s="152"/>
+      <c r="F22" s="152"/>
+      <c r="G22" s="153"/>
       <c r="H22" s="105"/>
       <c r="I22" s="105"/>
       <c r="J22" s="105"/>
@@ -5810,12 +5812,12 @@
     </row>
     <row r="23" spans="1:25">
       <c r="A23" s="116"/>
-      <c r="B23" s="157"/>
-      <c r="C23" s="157"/>
-      <c r="D23" s="157"/>
-      <c r="E23" s="157"/>
-      <c r="F23" s="157"/>
-      <c r="G23" s="157"/>
+      <c r="B23" s="168"/>
+      <c r="C23" s="168"/>
+      <c r="D23" s="168"/>
+      <c r="E23" s="168"/>
+      <c r="F23" s="168"/>
+      <c r="G23" s="168"/>
       <c r="H23" s="112"/>
       <c r="I23" s="112"/>
       <c r="J23" s="112"/>
@@ -5836,12 +5838,12 @@
     </row>
     <row r="24" spans="1:25">
       <c r="A24" s="117"/>
-      <c r="B24" s="159"/>
-      <c r="C24" s="159"/>
-      <c r="D24" s="159"/>
-      <c r="E24" s="159"/>
-      <c r="F24" s="159"/>
-      <c r="G24" s="159"/>
+      <c r="B24" s="169"/>
+      <c r="C24" s="169"/>
+      <c r="D24" s="169"/>
+      <c r="E24" s="169"/>
+      <c r="F24" s="169"/>
+      <c r="G24" s="169"/>
       <c r="H24" s="112"/>
       <c r="I24" s="112"/>
       <c r="J24" s="112"/>
@@ -5862,12 +5864,12 @@
     </row>
     <row r="25" spans="1:25">
       <c r="A25" s="118"/>
-      <c r="B25" s="161"/>
-      <c r="C25" s="161"/>
-      <c r="D25" s="161"/>
-      <c r="E25" s="161"/>
-      <c r="F25" s="161"/>
-      <c r="G25" s="161"/>
+      <c r="B25" s="170"/>
+      <c r="C25" s="170"/>
+      <c r="D25" s="170"/>
+      <c r="E25" s="170"/>
+      <c r="F25" s="170"/>
+      <c r="G25" s="170"/>
       <c r="H25" s="112"/>
       <c r="I25" s="112"/>
       <c r="J25" s="112"/>
@@ -5890,15 +5892,15 @@
       <c r="O26" s="105"/>
     </row>
     <row r="27" spans="1:25">
-      <c r="A27" s="176" t="s">
+      <c r="A27" s="154" t="s">
         <v>193</v>
       </c>
-      <c r="B27" s="177"/>
-      <c r="C27" s="177"/>
-      <c r="D27" s="177"/>
-      <c r="E27" s="177"/>
-      <c r="F27" s="177"/>
-      <c r="G27" s="178"/>
+      <c r="B27" s="155"/>
+      <c r="C27" s="155"/>
+      <c r="D27" s="155"/>
+      <c r="E27" s="155"/>
+      <c r="F27" s="155"/>
+      <c r="G27" s="156"/>
       <c r="K27" s="105"/>
       <c r="L27" s="105"/>
       <c r="M27" s="105"/>
@@ -5908,14 +5910,14 @@
       <c r="A28" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B28" s="153" t="s">
+      <c r="B28" s="174" t="s">
         <v>184</v>
       </c>
-      <c r="C28" s="153"/>
-      <c r="D28" s="153"/>
-      <c r="E28" s="153"/>
-      <c r="F28" s="153"/>
-      <c r="G28" s="153"/>
+      <c r="C28" s="174"/>
+      <c r="D28" s="174"/>
+      <c r="E28" s="174"/>
+      <c r="F28" s="174"/>
+      <c r="G28" s="174"/>
       <c r="H28" s="105"/>
       <c r="I28" s="105"/>
       <c r="J28" s="105"/>
@@ -5938,14 +5940,14 @@
       <c r="A29" s="116">
         <v>1</v>
       </c>
-      <c r="B29" s="154" t="s">
+      <c r="B29" s="175" t="s">
         <v>225</v>
       </c>
-      <c r="C29" s="154"/>
-      <c r="D29" s="154"/>
-      <c r="E29" s="154"/>
-      <c r="F29" s="154"/>
-      <c r="G29" s="154"/>
+      <c r="C29" s="175"/>
+      <c r="D29" s="175"/>
+      <c r="E29" s="175"/>
+      <c r="F29" s="175"/>
+      <c r="G29" s="175"/>
       <c r="H29" s="112"/>
       <c r="I29" s="112"/>
       <c r="J29" s="112"/>
@@ -5966,12 +5968,12 @@
     </row>
     <row r="30" spans="1:25">
       <c r="A30" s="117"/>
-      <c r="B30" s="155"/>
-      <c r="C30" s="155"/>
-      <c r="D30" s="155"/>
-      <c r="E30" s="155"/>
-      <c r="F30" s="155"/>
-      <c r="G30" s="155"/>
+      <c r="B30" s="176"/>
+      <c r="C30" s="176"/>
+      <c r="D30" s="176"/>
+      <c r="E30" s="176"/>
+      <c r="F30" s="176"/>
+      <c r="G30" s="176"/>
       <c r="H30" s="112"/>
       <c r="I30" s="112"/>
       <c r="J30" s="112"/>
@@ -5988,12 +5990,12 @@
     </row>
     <row r="31" spans="1:25">
       <c r="A31" s="118"/>
-      <c r="B31" s="156"/>
-      <c r="C31" s="156"/>
-      <c r="D31" s="156"/>
-      <c r="E31" s="156"/>
-      <c r="F31" s="156"/>
-      <c r="G31" s="156"/>
+      <c r="B31" s="177"/>
+      <c r="C31" s="177"/>
+      <c r="D31" s="177"/>
+      <c r="E31" s="177"/>
+      <c r="F31" s="177"/>
+      <c r="G31" s="177"/>
       <c r="H31" s="112"/>
       <c r="I31" s="112"/>
       <c r="J31" s="112"/>
@@ -6038,15 +6040,15 @@
       <c r="W32"/>
     </row>
     <row r="33" spans="1:29">
-      <c r="A33" s="176" t="s">
+      <c r="A33" s="154" t="s">
         <v>194</v>
       </c>
-      <c r="B33" s="177"/>
-      <c r="C33" s="177"/>
-      <c r="D33" s="177"/>
-      <c r="E33" s="177"/>
-      <c r="F33" s="177"/>
-      <c r="G33" s="178"/>
+      <c r="B33" s="155"/>
+      <c r="C33" s="155"/>
+      <c r="D33" s="155"/>
+      <c r="E33" s="155"/>
+      <c r="F33" s="155"/>
+      <c r="G33" s="156"/>
       <c r="K33" s="112"/>
       <c r="L33" s="112"/>
       <c r="M33" s="112"/>
@@ -6056,14 +6058,14 @@
       <c r="A34" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="153" t="s">
+      <c r="B34" s="174" t="s">
         <v>186</v>
       </c>
-      <c r="C34" s="153"/>
-      <c r="D34" s="153"/>
-      <c r="E34" s="153"/>
-      <c r="F34" s="153"/>
-      <c r="G34" s="153"/>
+      <c r="C34" s="174"/>
+      <c r="D34" s="174"/>
+      <c r="E34" s="174"/>
+      <c r="F34" s="174"/>
+      <c r="G34" s="174"/>
       <c r="H34" s="105"/>
       <c r="I34" s="105"/>
       <c r="J34" s="105"/>
@@ -6084,12 +6086,12 @@
     </row>
     <row r="35" spans="1:29">
       <c r="A35" s="116"/>
-      <c r="B35" s="157"/>
-      <c r="C35" s="157"/>
-      <c r="D35" s="157"/>
-      <c r="E35" s="157"/>
-      <c r="F35" s="157"/>
-      <c r="G35" s="158"/>
+      <c r="B35" s="168"/>
+      <c r="C35" s="168"/>
+      <c r="D35" s="168"/>
+      <c r="E35" s="168"/>
+      <c r="F35" s="168"/>
+      <c r="G35" s="178"/>
       <c r="H35" s="112"/>
       <c r="I35" s="112"/>
       <c r="J35" s="112"/>
@@ -6110,12 +6112,12 @@
     </row>
     <row r="36" spans="1:29">
       <c r="A36" s="117"/>
-      <c r="B36" s="159"/>
-      <c r="C36" s="159"/>
-      <c r="D36" s="159"/>
-      <c r="E36" s="159"/>
-      <c r="F36" s="159"/>
-      <c r="G36" s="160"/>
+      <c r="B36" s="169"/>
+      <c r="C36" s="169"/>
+      <c r="D36" s="169"/>
+      <c r="E36" s="169"/>
+      <c r="F36" s="169"/>
+      <c r="G36" s="179"/>
       <c r="H36" s="112"/>
       <c r="I36" s="112"/>
       <c r="J36" s="112"/>
@@ -6132,12 +6134,12 @@
     </row>
     <row r="37" spans="1:29">
       <c r="A37" s="118"/>
-      <c r="B37" s="161"/>
-      <c r="C37" s="161"/>
-      <c r="D37" s="161"/>
-      <c r="E37" s="161"/>
-      <c r="F37" s="161"/>
-      <c r="G37" s="162"/>
+      <c r="B37" s="170"/>
+      <c r="C37" s="170"/>
+      <c r="D37" s="170"/>
+      <c r="E37" s="170"/>
+      <c r="F37" s="170"/>
+      <c r="G37" s="180"/>
       <c r="H37" s="112"/>
       <c r="I37" s="112"/>
       <c r="J37" s="112"/>
@@ -6210,94 +6212,94 @@
       <c r="AC40" s="39"/>
     </row>
     <row r="41" spans="1:29">
-      <c r="A41" s="186" t="s">
+      <c r="A41" s="188" t="s">
         <v>69</v>
       </c>
-      <c r="B41" s="186" t="s">
+      <c r="B41" s="188" t="s">
         <v>0</v>
       </c>
-      <c r="C41" s="188" t="s">
+      <c r="C41" s="193" t="s">
         <v>1</v>
       </c>
-      <c r="D41" s="186" t="s">
+      <c r="D41" s="188" t="s">
         <v>2</v>
       </c>
-      <c r="E41" s="189" t="s">
+      <c r="E41" s="194" t="s">
         <v>161</v>
       </c>
-      <c r="F41" s="189" t="s">
+      <c r="F41" s="194" t="s">
         <v>177</v>
       </c>
-      <c r="G41" s="186" t="s">
+      <c r="G41" s="188" t="s">
         <v>13</v>
       </c>
-      <c r="H41" s="186" t="s">
+      <c r="H41" s="188" t="s">
         <v>116</v>
       </c>
-      <c r="I41" s="186" t="s">
+      <c r="I41" s="188" t="s">
         <v>195</v>
       </c>
-      <c r="J41" s="186" t="s">
+      <c r="J41" s="188" t="s">
         <v>209</v>
       </c>
-      <c r="K41" s="193" t="s">
+      <c r="K41" s="197" t="s">
         <v>200</v>
       </c>
-      <c r="L41" s="193" t="s">
+      <c r="L41" s="197" t="s">
         <v>201</v>
       </c>
-      <c r="M41" s="193" t="s">
+      <c r="M41" s="197" t="s">
         <v>202</v>
       </c>
-      <c r="N41" s="186" t="s">
+      <c r="N41" s="188" t="s">
         <v>235</v>
       </c>
-      <c r="O41" s="196" t="s">
+      <c r="O41" s="186" t="s">
         <v>203</v>
       </c>
-      <c r="P41" s="186" t="s">
+      <c r="P41" s="188" t="s">
         <v>236</v>
       </c>
-      <c r="Q41" s="186" t="s">
+      <c r="Q41" s="188" t="s">
         <v>237</v>
       </c>
-      <c r="R41" s="188" t="s">
+      <c r="R41" s="193" t="s">
         <v>208</v>
       </c>
-      <c r="S41" s="194" t="s">
+      <c r="S41" s="190" t="s">
         <v>71</v>
       </c>
-      <c r="T41" s="195"/>
-      <c r="U41" s="194" t="s">
+      <c r="T41" s="191"/>
+      <c r="U41" s="190" t="s">
         <v>17</v>
       </c>
-      <c r="V41" s="195"/>
+      <c r="V41" s="191"/>
       <c r="W41" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="X41" s="186" t="s">
+      <c r="X41" s="188" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:29">
-      <c r="A42" s="187"/>
-      <c r="B42" s="187"/>
-      <c r="C42" s="187"/>
-      <c r="D42" s="187"/>
-      <c r="E42" s="190"/>
-      <c r="F42" s="191"/>
-      <c r="G42" s="187"/>
-      <c r="H42" s="187"/>
-      <c r="I42" s="192"/>
-      <c r="J42" s="192"/>
-      <c r="K42" s="193"/>
-      <c r="L42" s="193"/>
-      <c r="M42" s="193"/>
-      <c r="N42" s="192"/>
-      <c r="O42" s="197"/>
-      <c r="P42" s="192"/>
-      <c r="Q42" s="192"/>
-      <c r="R42" s="192"/>
+      <c r="A42" s="192"/>
+      <c r="B42" s="192"/>
+      <c r="C42" s="192"/>
+      <c r="D42" s="192"/>
+      <c r="E42" s="195"/>
+      <c r="F42" s="196"/>
+      <c r="G42" s="192"/>
+      <c r="H42" s="192"/>
+      <c r="I42" s="189"/>
+      <c r="J42" s="189"/>
+      <c r="K42" s="197"/>
+      <c r="L42" s="197"/>
+      <c r="M42" s="197"/>
+      <c r="N42" s="189"/>
+      <c r="O42" s="187"/>
+      <c r="P42" s="189"/>
+      <c r="Q42" s="189"/>
+      <c r="R42" s="189"/>
       <c r="S42" s="29" t="s">
         <v>75</v>
       </c>
@@ -6313,7 +6315,7 @@
       <c r="W42" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="X42" s="187"/>
+      <c r="X42" s="192"/>
     </row>
     <row r="43" spans="1:29" ht="30">
       <c r="A43" s="7">
@@ -7065,14 +7067,22 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="B36:G36"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="O41:O42"/>
-    <mergeCell ref="I41:I42"/>
-    <mergeCell ref="J41:J42"/>
-    <mergeCell ref="N41:N42"/>
+    <mergeCell ref="X41:X42"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="R41:R42"/>
+    <mergeCell ref="K41:K42"/>
+    <mergeCell ref="L41:L42"/>
+    <mergeCell ref="M41:M42"/>
+    <mergeCell ref="P41:P42"/>
+    <mergeCell ref="U41:V41"/>
+    <mergeCell ref="Q41:Q42"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="S41:T41"/>
     <mergeCell ref="B31:G31"/>
@@ -7089,22 +7099,14 @@
     <mergeCell ref="A27:G27"/>
     <mergeCell ref="B28:G28"/>
     <mergeCell ref="B35:G35"/>
-    <mergeCell ref="X41:X42"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="R41:R42"/>
-    <mergeCell ref="K41:K42"/>
-    <mergeCell ref="L41:L42"/>
-    <mergeCell ref="M41:M42"/>
-    <mergeCell ref="P41:P42"/>
-    <mergeCell ref="U41:V41"/>
-    <mergeCell ref="Q41:Q42"/>
+    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="O41:O42"/>
+    <mergeCell ref="I41:I42"/>
+    <mergeCell ref="J41:J42"/>
+    <mergeCell ref="N41:N42"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="4">
@@ -7340,10 +7342,10 @@
         <v>174</v>
       </c>
       <c r="B12" s="122"/>
-      <c r="C12" s="141" t="s">
+      <c r="C12" s="165" t="s">
         <v>175</v>
       </c>
-      <c r="D12" s="141"/>
+      <c r="D12" s="165"/>
       <c r="E12" s="95" t="s">
         <v>176</v>
       </c>
@@ -7358,10 +7360,10 @@
         <v>226</v>
       </c>
       <c r="B13" s="122"/>
-      <c r="C13" s="142" t="s">
+      <c r="C13" s="164" t="s">
         <v>230</v>
       </c>
-      <c r="D13" s="141"/>
+      <c r="D13" s="165"/>
       <c r="E13" s="55" t="s">
         <v>227</v>
       </c>
@@ -7381,10 +7383,10 @@
         <v>177</v>
       </c>
       <c r="B14" s="122"/>
-      <c r="C14" s="141" t="s">
+      <c r="C14" s="165" t="s">
         <v>178</v>
       </c>
-      <c r="D14" s="141"/>
+      <c r="D14" s="165"/>
       <c r="E14" s="55"/>
       <c r="F14" s="55"/>
       <c r="G14" s="54"/>
@@ -7396,8 +7398,8 @@
         <v>228</v>
       </c>
       <c r="B15" s="122"/>
-      <c r="C15" s="142"/>
-      <c r="D15" s="141"/>
+      <c r="C15" s="164"/>
+      <c r="D15" s="165"/>
       <c r="E15" s="55" t="s">
         <v>229</v>
       </c>
@@ -7445,15 +7447,15 @@
       <c r="L17"/>
     </row>
     <row r="18" spans="1:22">
-      <c r="A18" s="179" t="s">
+      <c r="A18" s="157" t="s">
         <v>192</v>
       </c>
-      <c r="B18" s="179"/>
-      <c r="C18" s="179"/>
-      <c r="D18" s="179"/>
-      <c r="E18" s="179"/>
-      <c r="F18" s="179"/>
-      <c r="G18" s="179"/>
+      <c r="B18" s="157"/>
+      <c r="C18" s="157"/>
+      <c r="D18" s="157"/>
+      <c r="E18" s="157"/>
+      <c r="F18" s="157"/>
+      <c r="G18" s="157"/>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
@@ -7464,14 +7466,14 @@
       <c r="A19" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="173" t="s">
+      <c r="B19" s="151" t="s">
         <v>183</v>
       </c>
-      <c r="C19" s="174"/>
-      <c r="D19" s="174"/>
-      <c r="E19" s="174"/>
-      <c r="F19" s="174"/>
-      <c r="G19" s="175"/>
+      <c r="C19" s="152"/>
+      <c r="D19" s="152"/>
+      <c r="E19" s="152"/>
+      <c r="F19" s="152"/>
+      <c r="G19" s="153"/>
       <c r="H19" s="105"/>
       <c r="I19"/>
       <c r="J19"/>
@@ -7487,12 +7489,12 @@
     </row>
     <row r="20" spans="1:22">
       <c r="A20" s="116"/>
-      <c r="B20" s="157"/>
-      <c r="C20" s="157"/>
-      <c r="D20" s="157"/>
-      <c r="E20" s="157"/>
-      <c r="F20" s="157"/>
-      <c r="G20" s="157"/>
+      <c r="B20" s="168"/>
+      <c r="C20" s="168"/>
+      <c r="D20" s="168"/>
+      <c r="E20" s="168"/>
+      <c r="F20" s="168"/>
+      <c r="G20" s="168"/>
       <c r="H20" s="112"/>
       <c r="I20"/>
       <c r="J20"/>
@@ -7507,12 +7509,12 @@
     </row>
     <row r="21" spans="1:22">
       <c r="A21" s="117"/>
-      <c r="B21" s="159"/>
-      <c r="C21" s="159"/>
-      <c r="D21" s="159"/>
-      <c r="E21" s="159"/>
-      <c r="F21" s="159"/>
-      <c r="G21" s="159"/>
+      <c r="B21" s="169"/>
+      <c r="C21" s="169"/>
+      <c r="D21" s="169"/>
+      <c r="E21" s="169"/>
+      <c r="F21" s="169"/>
+      <c r="G21" s="169"/>
       <c r="H21" s="112"/>
       <c r="I21"/>
       <c r="J21"/>
@@ -7527,12 +7529,12 @@
     </row>
     <row r="22" spans="1:22">
       <c r="A22" s="118"/>
-      <c r="B22" s="161"/>
-      <c r="C22" s="161"/>
-      <c r="D22" s="161"/>
-      <c r="E22" s="161"/>
-      <c r="F22" s="161"/>
-      <c r="G22" s="161"/>
+      <c r="B22" s="170"/>
+      <c r="C22" s="170"/>
+      <c r="D22" s="170"/>
+      <c r="E22" s="170"/>
+      <c r="F22" s="170"/>
+      <c r="G22" s="170"/>
       <c r="H22" s="112"/>
       <c r="I22"/>
       <c r="J22"/>
@@ -7559,15 +7561,15 @@
       <c r="O23" s="112"/>
     </row>
     <row r="24" spans="1:22">
-      <c r="A24" s="176" t="s">
+      <c r="A24" s="154" t="s">
         <v>193</v>
       </c>
-      <c r="B24" s="177"/>
-      <c r="C24" s="177"/>
-      <c r="D24" s="177"/>
-      <c r="E24" s="177"/>
-      <c r="F24" s="177"/>
-      <c r="G24" s="178"/>
+      <c r="B24" s="155"/>
+      <c r="C24" s="155"/>
+      <c r="D24" s="155"/>
+      <c r="E24" s="155"/>
+      <c r="F24" s="155"/>
+      <c r="G24" s="156"/>
       <c r="I24"/>
       <c r="J24"/>
       <c r="K24"/>
@@ -7580,14 +7582,14 @@
       <c r="A25" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B25" s="153" t="s">
+      <c r="B25" s="174" t="s">
         <v>184</v>
       </c>
-      <c r="C25" s="153"/>
-      <c r="D25" s="153"/>
-      <c r="E25" s="153"/>
-      <c r="F25" s="153"/>
-      <c r="G25" s="153"/>
+      <c r="C25" s="174"/>
+      <c r="D25" s="174"/>
+      <c r="E25" s="174"/>
+      <c r="F25" s="174"/>
+      <c r="G25" s="174"/>
       <c r="H25" s="105"/>
       <c r="M25" s="112"/>
       <c r="N25" s="112"/>
@@ -7603,14 +7605,14 @@
       <c r="A26" s="116">
         <v>1</v>
       </c>
-      <c r="B26" s="154" t="s">
+      <c r="B26" s="175" t="s">
         <v>185</v>
       </c>
-      <c r="C26" s="154"/>
-      <c r="D26" s="154"/>
-      <c r="E26" s="154"/>
-      <c r="F26" s="154"/>
-      <c r="G26" s="154"/>
+      <c r="C26" s="175"/>
+      <c r="D26" s="175"/>
+      <c r="E26" s="175"/>
+      <c r="F26" s="175"/>
+      <c r="G26" s="175"/>
       <c r="H26" s="112"/>
       <c r="I26" s="105"/>
       <c r="J26" s="105"/>
@@ -7625,12 +7627,12 @@
     </row>
     <row r="27" spans="1:22">
       <c r="A27" s="117"/>
-      <c r="B27" s="155"/>
-      <c r="C27" s="155"/>
-      <c r="D27" s="155"/>
-      <c r="E27" s="155"/>
-      <c r="F27" s="155"/>
-      <c r="G27" s="155"/>
+      <c r="B27" s="176"/>
+      <c r="C27" s="176"/>
+      <c r="D27" s="176"/>
+      <c r="E27" s="176"/>
+      <c r="F27" s="176"/>
+      <c r="G27" s="176"/>
       <c r="H27" s="112"/>
       <c r="I27" s="105"/>
       <c r="J27" s="105"/>
@@ -7645,12 +7647,12 @@
     </row>
     <row r="28" spans="1:22">
       <c r="A28" s="118"/>
-      <c r="B28" s="156"/>
-      <c r="C28" s="156"/>
-      <c r="D28" s="156"/>
-      <c r="E28" s="156"/>
-      <c r="F28" s="156"/>
-      <c r="G28" s="156"/>
+      <c r="B28" s="177"/>
+      <c r="C28" s="177"/>
+      <c r="D28" s="177"/>
+      <c r="E28" s="177"/>
+      <c r="F28" s="177"/>
+      <c r="G28" s="177"/>
       <c r="H28" s="112"/>
       <c r="I28" s="105"/>
       <c r="J28" s="105"/>
@@ -7689,15 +7691,15 @@
       <c r="T29"/>
     </row>
     <row r="30" spans="1:22">
-      <c r="A30" s="176" t="s">
+      <c r="A30" s="154" t="s">
         <v>194</v>
       </c>
-      <c r="B30" s="177"/>
-      <c r="C30" s="177"/>
-      <c r="D30" s="177"/>
-      <c r="E30" s="177"/>
-      <c r="F30" s="177"/>
-      <c r="G30" s="178"/>
+      <c r="B30" s="155"/>
+      <c r="C30" s="155"/>
+      <c r="D30" s="155"/>
+      <c r="E30" s="155"/>
+      <c r="F30" s="155"/>
+      <c r="G30" s="156"/>
       <c r="M30" s="112"/>
       <c r="N30" s="112"/>
       <c r="O30" s="112"/>
@@ -7706,14 +7708,14 @@
       <c r="A31" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B31" s="153" t="s">
+      <c r="B31" s="174" t="s">
         <v>186</v>
       </c>
-      <c r="C31" s="153"/>
-      <c r="D31" s="153"/>
-      <c r="E31" s="153"/>
-      <c r="F31" s="153"/>
-      <c r="G31" s="153"/>
+      <c r="C31" s="174"/>
+      <c r="D31" s="174"/>
+      <c r="E31" s="174"/>
+      <c r="F31" s="174"/>
+      <c r="G31" s="174"/>
       <c r="H31" s="105"/>
       <c r="I31" s="105"/>
       <c r="J31" s="105"/>
@@ -7731,12 +7733,12 @@
     </row>
     <row r="32" spans="1:22">
       <c r="A32" s="116"/>
-      <c r="B32" s="157"/>
-      <c r="C32" s="157"/>
-      <c r="D32" s="157"/>
-      <c r="E32" s="157"/>
-      <c r="F32" s="157"/>
-      <c r="G32" s="158"/>
+      <c r="B32" s="168"/>
+      <c r="C32" s="168"/>
+      <c r="D32" s="168"/>
+      <c r="E32" s="168"/>
+      <c r="F32" s="168"/>
+      <c r="G32" s="178"/>
       <c r="H32" s="112"/>
       <c r="I32" s="112"/>
       <c r="J32" s="112"/>
@@ -7754,12 +7756,12 @@
     </row>
     <row r="33" spans="1:22">
       <c r="A33" s="117"/>
-      <c r="B33" s="159"/>
-      <c r="C33" s="159"/>
-      <c r="D33" s="159"/>
-      <c r="E33" s="159"/>
-      <c r="F33" s="159"/>
-      <c r="G33" s="160"/>
+      <c r="B33" s="169"/>
+      <c r="C33" s="169"/>
+      <c r="D33" s="169"/>
+      <c r="E33" s="169"/>
+      <c r="F33" s="169"/>
+      <c r="G33" s="179"/>
       <c r="H33" s="112"/>
       <c r="I33" s="112"/>
       <c r="J33" s="112"/>
@@ -7774,12 +7776,12 @@
     </row>
     <row r="34" spans="1:22">
       <c r="A34" s="118"/>
-      <c r="B34" s="161"/>
-      <c r="C34" s="161"/>
-      <c r="D34" s="161"/>
-      <c r="E34" s="161"/>
-      <c r="F34" s="161"/>
-      <c r="G34" s="162"/>
+      <c r="B34" s="170"/>
+      <c r="C34" s="170"/>
+      <c r="D34" s="170"/>
+      <c r="E34" s="170"/>
+      <c r="F34" s="170"/>
+      <c r="G34" s="180"/>
       <c r="H34" s="112"/>
       <c r="I34" s="112"/>
       <c r="J34" s="112"/>
@@ -7849,84 +7851,84 @@
       <c r="U37" s="58"/>
     </row>
     <row r="38" spans="1:22" ht="30" customHeight="1">
-      <c r="A38" s="189" t="s">
+      <c r="A38" s="194" t="s">
         <v>118</v>
       </c>
-      <c r="B38" s="189" t="s">
+      <c r="B38" s="194" t="s">
         <v>119</v>
       </c>
       <c r="C38" s="60" t="s">
         <v>120</v>
       </c>
-      <c r="D38" s="189" t="s">
+      <c r="D38" s="194" t="s">
         <v>101</v>
       </c>
-      <c r="E38" s="189" t="s">
+      <c r="E38" s="194" t="s">
         <v>161</v>
       </c>
-      <c r="F38" s="189" t="s">
+      <c r="F38" s="194" t="s">
         <v>177</v>
       </c>
-      <c r="G38" s="189" t="s">
+      <c r="G38" s="194" t="s">
         <v>140</v>
       </c>
-      <c r="H38" s="189" t="s">
+      <c r="H38" s="194" t="s">
         <v>139</v>
       </c>
-      <c r="I38" s="203" t="s">
+      <c r="I38" s="201" t="s">
         <v>200</v>
       </c>
-      <c r="J38" s="205" t="s">
+      <c r="J38" s="203" t="s">
         <v>201</v>
       </c>
-      <c r="K38" s="205" t="s">
+      <c r="K38" s="203" t="s">
         <v>202</v>
       </c>
-      <c r="L38" s="196" t="s">
+      <c r="L38" s="186" t="s">
         <v>203</v>
       </c>
-      <c r="M38" s="186" t="s">
+      <c r="M38" s="188" t="s">
         <v>195</v>
       </c>
-      <c r="N38" s="186" t="s">
+      <c r="N38" s="188" t="s">
         <v>209</v>
       </c>
-      <c r="O38" s="188" t="s">
+      <c r="O38" s="193" t="s">
         <v>208</v>
       </c>
-      <c r="P38" s="202" t="s">
+      <c r="P38" s="199" t="s">
         <v>122</v>
       </c>
       <c r="Q38" s="200"/>
-      <c r="R38" s="199" t="s">
+      <c r="R38" s="205" t="s">
         <v>123</v>
       </c>
       <c r="S38" s="200"/>
       <c r="T38" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="U38" s="189" t="s">
+      <c r="U38" s="194" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="39" spans="1:22" ht="15">
-      <c r="A39" s="201"/>
-      <c r="B39" s="201"/>
+      <c r="A39" s="198"/>
+      <c r="B39" s="198"/>
       <c r="C39" s="61" t="s">
         <v>121</v>
       </c>
-      <c r="D39" s="201"/>
-      <c r="E39" s="191"/>
-      <c r="F39" s="191"/>
-      <c r="G39" s="201"/>
-      <c r="H39" s="201"/>
-      <c r="I39" s="204"/>
-      <c r="J39" s="206"/>
-      <c r="K39" s="206"/>
-      <c r="L39" s="197"/>
-      <c r="M39" s="192"/>
-      <c r="N39" s="192"/>
-      <c r="O39" s="198"/>
+      <c r="D39" s="198"/>
+      <c r="E39" s="196"/>
+      <c r="F39" s="196"/>
+      <c r="G39" s="198"/>
+      <c r="H39" s="198"/>
+      <c r="I39" s="202"/>
+      <c r="J39" s="204"/>
+      <c r="K39" s="204"/>
+      <c r="L39" s="187"/>
+      <c r="M39" s="189"/>
+      <c r="N39" s="189"/>
+      <c r="O39" s="206"/>
       <c r="P39" s="62" t="s">
         <v>126</v>
       </c>
@@ -7942,7 +7944,7 @@
       <c r="T39" s="63" t="s">
         <v>130</v>
       </c>
-      <c r="U39" s="201"/>
+      <c r="U39" s="198"/>
     </row>
     <row r="40" spans="1:22">
       <c r="A40" s="64">
@@ -8602,6 +8604,26 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="M38:M39"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="A30:G30"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="A24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A18:G18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C15:D15"/>
     <mergeCell ref="U38:U39"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="B38:B39"/>
@@ -8616,28 +8638,8 @@
     <mergeCell ref="J38:J39"/>
     <mergeCell ref="K38:K39"/>
     <mergeCell ref="R38:S38"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="A18:G18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="A24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B26:G26"/>
     <mergeCell ref="L38:L39"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="A30:G30"/>
-    <mergeCell ref="B31:G31"/>
     <mergeCell ref="O38:O39"/>
-    <mergeCell ref="M38:M39"/>
-    <mergeCell ref="B34:G34"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="3">

</xml_diff>

<commit_message>
0.1.5: NoAuzilliaryAuthentication flag added.
</commit_message>
<xml_diff>
--- a/meta/api/BlancoApiPostSample.xlsx
+++ b/meta/api/BlancoApiPostSample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10212"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorKt/meta/api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23837E1-F8D1-D949-BE33-FFC93E0CE240}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC2A5067-A033-2D43-B747-C2A0113F1718}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15160" yWindow="1200" windowWidth="21420" windowHeight="17540" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="244">
   <si>
     <t>項目名</t>
     <rPh sb="0" eb="3">
@@ -2446,6 +2446,48 @@
   </si>
   <si>
     <t>@Client(value = "{\${target.url:`http://192.168.100.109:28000`}", configuration = HttpClientConfiguration::class)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>※ IPアドレス認証等を想定しています</t>
+    <rPh sb="8" eb="10">
+      <t xml:space="preserve">ニンショウ </t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t xml:space="preserve">トウヲ </t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t xml:space="preserve">ソウテイ </t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>※ 通常のパスワード認証やトークン、シグネチャによる認証を想定しています</t>
+    <rPh sb="2" eb="4">
+      <t xml:space="preserve">ツウジョウノ </t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t xml:space="preserve">ニンショウ </t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t xml:space="preserve">ニンショウ </t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t xml:space="preserve">ソウテイ </t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>補助的な認証が不要なAPI</t>
+    <rPh sb="0" eb="3">
+      <t xml:space="preserve">ホジョテキナ </t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ニンショウ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>フヨウ</t>
+    </rPh>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -3689,12 +3731,87 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="60" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3704,9 +3821,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3719,12 +3833,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3764,88 +3872,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -3861,7 +3888,22 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4435,10 +4477,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O71"/>
+  <dimension ref="A1:O72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12:E12"/>
+      <selection activeCell="A20" sqref="A20:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -4481,137 +4523,137 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="185" t="s">
+      <c r="A5" s="139" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="185"/>
-      <c r="C5" s="185"/>
-      <c r="D5" s="185"/>
-      <c r="E5" s="185"/>
+      <c r="B5" s="139"/>
+      <c r="C5" s="139"/>
+      <c r="D5" s="139"/>
+      <c r="E5" s="139"/>
       <c r="F5" s="55"/>
       <c r="G5" s="55"/>
       <c r="H5" s="95"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="182" t="s">
+      <c r="A6" s="143" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="183"/>
-      <c r="C6" s="184"/>
-      <c r="D6" s="181" t="s">
+      <c r="B6" s="144"/>
+      <c r="C6" s="145"/>
+      <c r="D6" s="140" t="s">
         <v>197</v>
       </c>
-      <c r="E6" s="181"/>
+      <c r="E6" s="140"/>
       <c r="F6" s="55"/>
       <c r="G6" s="55"/>
       <c r="H6" s="95"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="185" t="s">
+      <c r="A7" s="139" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="185"/>
-      <c r="C7" s="185"/>
-      <c r="D7" s="181" t="s">
+      <c r="B7" s="139"/>
+      <c r="C7" s="139"/>
+      <c r="D7" s="140" t="s">
         <v>166</v>
       </c>
-      <c r="E7" s="181"/>
+      <c r="E7" s="140"/>
       <c r="F7" s="55"/>
       <c r="G7" s="55"/>
       <c r="H7" s="95"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="185" t="s">
+      <c r="A8" s="139" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="185"/>
-      <c r="C8" s="185"/>
-      <c r="D8" s="181" t="s">
+      <c r="B8" s="139"/>
+      <c r="C8" s="139"/>
+      <c r="D8" s="140" t="s">
         <v>162</v>
       </c>
-      <c r="E8" s="181"/>
+      <c r="E8" s="140"/>
       <c r="F8" s="95"/>
       <c r="G8" s="95"/>
       <c r="H8" s="95"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="185" t="s">
+      <c r="A9" s="139" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="185"/>
-      <c r="C9" s="185"/>
-      <c r="D9" s="181" t="s">
+      <c r="B9" s="139"/>
+      <c r="C9" s="139"/>
+      <c r="D9" s="140" t="s">
         <v>100</v>
       </c>
-      <c r="E9" s="181"/>
+      <c r="E9" s="140"/>
       <c r="F9" s="95"/>
       <c r="G9" s="95"/>
       <c r="H9" s="95"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="185" t="s">
+      <c r="A10" s="139" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="185"/>
-      <c r="C10" s="185"/>
-      <c r="D10" s="181"/>
-      <c r="E10" s="181"/>
+      <c r="B10" s="139"/>
+      <c r="C10" s="139"/>
+      <c r="D10" s="140"/>
+      <c r="E10" s="140"/>
       <c r="F10" s="95"/>
       <c r="G10" s="95"/>
       <c r="H10" s="95"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="185" t="s">
+      <c r="A11" s="139" t="s">
         <v>99</v>
       </c>
-      <c r="B11" s="185"/>
-      <c r="C11" s="185"/>
-      <c r="D11" s="181" t="s">
+      <c r="B11" s="139"/>
+      <c r="C11" s="139"/>
+      <c r="D11" s="140" t="s">
         <v>163</v>
       </c>
-      <c r="E11" s="181"/>
+      <c r="E11" s="140"/>
       <c r="F11" s="95"/>
       <c r="G11" s="95"/>
       <c r="H11" s="95"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="144" t="s">
+      <c r="A12" s="146" t="s">
         <v>174</v>
       </c>
-      <c r="B12" s="144"/>
-      <c r="C12" s="144"/>
-      <c r="D12" s="165" t="s">
+      <c r="B12" s="146"/>
+      <c r="C12" s="146"/>
+      <c r="D12" s="141" t="s">
         <v>175</v>
       </c>
-      <c r="E12" s="165"/>
+      <c r="E12" s="141"/>
       <c r="F12" s="95" t="s">
         <v>176</v>
       </c>
       <c r="G12" s="54"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="144" t="s">
+      <c r="A13" s="146" t="s">
         <v>212</v>
       </c>
-      <c r="B13" s="144"/>
-      <c r="C13" s="144"/>
-      <c r="D13" s="165" t="s">
+      <c r="B13" s="146"/>
+      <c r="C13" s="146"/>
+      <c r="D13" s="141" t="s">
         <v>210</v>
       </c>
-      <c r="E13" s="165"/>
+      <c r="E13" s="141"/>
       <c r="F13" s="95" t="s">
         <v>211</v>
       </c>
       <c r="G13" s="54"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="144" t="s">
+      <c r="A14" s="146" t="s">
         <v>177</v>
       </c>
-      <c r="B14" s="144"/>
-      <c r="C14" s="144"/>
-      <c r="D14" s="164"/>
-      <c r="E14" s="165"/>
+      <c r="B14" s="146"/>
+      <c r="C14" s="146"/>
+      <c r="D14" s="142"/>
+      <c r="E14" s="141"/>
       <c r="F14" s="54" t="s">
         <v>198</v>
       </c>
@@ -4619,15 +4661,15 @@
       <c r="H14" s="95"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="144" t="s">
+      <c r="A15" s="146" t="s">
         <v>217</v>
       </c>
-      <c r="B15" s="144"/>
-      <c r="C15" s="144"/>
-      <c r="D15" s="164" t="s">
+      <c r="B15" s="146"/>
+      <c r="C15" s="146"/>
+      <c r="D15" s="142" t="s">
         <v>215</v>
       </c>
-      <c r="E15" s="165"/>
+      <c r="E15" s="141"/>
       <c r="F15" s="54" t="s">
         <v>220</v>
       </c>
@@ -4635,13 +4677,13 @@
       <c r="H15" s="95"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="144" t="s">
+      <c r="A16" s="146" t="s">
         <v>216</v>
       </c>
-      <c r="B16" s="144"/>
-      <c r="C16" s="144"/>
-      <c r="D16" s="164"/>
-      <c r="E16" s="165"/>
+      <c r="B16" s="146"/>
+      <c r="C16" s="146"/>
+      <c r="D16" s="142"/>
+      <c r="E16" s="141"/>
       <c r="F16" s="54" t="s">
         <v>219</v>
       </c>
@@ -4649,13 +4691,13 @@
       <c r="H16" s="95"/>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="144" t="s">
+      <c r="A17" s="146" t="s">
         <v>214</v>
       </c>
-      <c r="B17" s="144"/>
-      <c r="C17" s="144"/>
-      <c r="D17" s="164"/>
-      <c r="E17" s="165"/>
+      <c r="B17" s="146"/>
+      <c r="C17" s="146"/>
+      <c r="D17" s="142"/>
+      <c r="E17" s="141"/>
       <c r="F17" s="54" t="s">
         <v>213</v>
       </c>
@@ -4663,15 +4705,15 @@
       <c r="H17" s="95"/>
     </row>
     <row r="18" spans="1:15">
-      <c r="A18" s="144" t="s">
+      <c r="A18" s="146" t="s">
         <v>238</v>
       </c>
-      <c r="B18" s="144"/>
-      <c r="C18" s="144"/>
-      <c r="D18" s="164" t="s">
+      <c r="B18" s="146"/>
+      <c r="C18" s="146"/>
+      <c r="D18" s="142" t="s">
         <v>240</v>
       </c>
-      <c r="E18" s="165"/>
+      <c r="E18" s="141"/>
       <c r="F18" s="54" t="s">
         <v>239</v>
       </c>
@@ -4679,151 +4721,151 @@
       <c r="H18" s="95"/>
     </row>
     <row r="19" spans="1:15">
-      <c r="A19" s="161" t="s">
+      <c r="A19" s="183" t="s">
         <v>143</v>
       </c>
-      <c r="B19" s="162"/>
-      <c r="C19" s="163"/>
+      <c r="B19" s="184"/>
+      <c r="C19" s="185"/>
       <c r="D19" s="114" t="s">
         <v>141</v>
       </c>
+      <c r="E19" s="1" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="20" spans="1:15">
-      <c r="A20" s="145" t="s">
+      <c r="A20" s="183" t="s">
+        <v>243</v>
+      </c>
+      <c r="B20" s="184"/>
+      <c r="C20" s="185"/>
+      <c r="D20" s="114" t="s">
+        <v>141</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" s="169" t="s">
         <v>179</v>
       </c>
-      <c r="B20" s="146"/>
-      <c r="C20" s="147"/>
-      <c r="D20" s="100"/>
-      <c r="E20" t="s">
+      <c r="B21" s="170"/>
+      <c r="C21" s="171"/>
+      <c r="D21" s="100"/>
+      <c r="E21" t="s">
         <v>180</v>
       </c>
-      <c r="F20"/>
-      <c r="G20"/>
-      <c r="H20"/>
-      <c r="I20"/>
-      <c r="J20"/>
-      <c r="K20"/>
-      <c r="L20"/>
-    </row>
-    <row r="21" spans="1:15">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21"/>
+      <c r="K21"/>
+      <c r="L21"/>
     </row>
     <row r="22" spans="1:15">
-      <c r="A22" s="158" t="s">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" s="180" t="s">
         <v>188</v>
       </c>
-      <c r="B22" s="159"/>
-      <c r="C22" s="159"/>
-      <c r="D22" s="159"/>
-      <c r="E22" s="159"/>
-      <c r="F22" s="159"/>
-      <c r="G22" s="160"/>
-      <c r="H22" s="1" t="s">
+      <c r="B23" s="181"/>
+      <c r="C23" s="181"/>
+      <c r="D23" s="181"/>
+      <c r="E23" s="181"/>
+      <c r="F23" s="181"/>
+      <c r="G23" s="182"/>
+      <c r="H23" s="1" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
-      <c r="A23" s="101" t="s">
+    <row r="24" spans="1:15">
+      <c r="A24" s="101" t="s">
         <v>181</v>
       </c>
-      <c r="B23" s="110"/>
-      <c r="C23" s="102"/>
-      <c r="D23" s="103" t="s">
+      <c r="B24" s="110"/>
+      <c r="C24" s="102"/>
+      <c r="D24" s="103" t="s">
         <v>221</v>
       </c>
-      <c r="E23" s="103"/>
-      <c r="F23" s="103"/>
-      <c r="G23" s="104"/>
-      <c r="H23" s="105"/>
-      <c r="I23" s="105"/>
-      <c r="J23" s="105"/>
-      <c r="K23" s="105"/>
-      <c r="L23" s="105"/>
-    </row>
-    <row r="24" spans="1:15">
-      <c r="A24" s="98" t="s">
-        <v>99</v>
-      </c>
-      <c r="B24" s="113"/>
-      <c r="C24" s="99"/>
-      <c r="D24" s="96" t="s">
-        <v>222</v>
-      </c>
-      <c r="E24" s="97"/>
-      <c r="F24" s="97"/>
-      <c r="G24" s="106"/>
+      <c r="E24" s="103"/>
+      <c r="F24" s="103"/>
+      <c r="G24" s="104"/>
+      <c r="H24" s="105"/>
+      <c r="I24" s="105"/>
+      <c r="J24" s="105"/>
+      <c r="K24" s="105"/>
+      <c r="L24" s="105"/>
     </row>
     <row r="25" spans="1:15">
       <c r="A25" s="98" t="s">
-        <v>182</v>
+        <v>99</v>
       </c>
       <c r="B25" s="113"/>
       <c r="C25" s="99"/>
-      <c r="D25" s="107"/>
-      <c r="E25" s="108"/>
-      <c r="F25" s="108"/>
-      <c r="G25" s="109"/>
+      <c r="D25" s="96" t="s">
+        <v>222</v>
+      </c>
+      <c r="E25" s="97"/>
+      <c r="F25" s="97"/>
+      <c r="G25" s="106"/>
     </row>
     <row r="26" spans="1:15">
-      <c r="C26"/>
+      <c r="A26" s="98" t="s">
+        <v>182</v>
+      </c>
+      <c r="B26" s="113"/>
+      <c r="C26" s="99"/>
+      <c r="D26" s="107"/>
+      <c r="E26" s="108"/>
+      <c r="F26" s="108"/>
+      <c r="G26" s="109"/>
     </row>
     <row r="27" spans="1:15">
-      <c r="A27" s="157" t="s">
+      <c r="C27"/>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28" s="179" t="s">
         <v>189</v>
       </c>
-      <c r="B27" s="157"/>
-      <c r="C27" s="157"/>
-      <c r="D27" s="157"/>
-      <c r="E27" s="157"/>
-      <c r="F27" s="157"/>
-      <c r="G27" s="157"/>
-    </row>
-    <row r="28" spans="1:15">
-      <c r="A28" s="115" t="s">
+      <c r="B28" s="179"/>
+      <c r="C28" s="179"/>
+      <c r="D28" s="179"/>
+      <c r="E28" s="179"/>
+      <c r="F28" s="179"/>
+      <c r="G28" s="179"/>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B28" s="151" t="s">
+      <c r="B29" s="173" t="s">
         <v>183</v>
       </c>
-      <c r="C28" s="152"/>
-      <c r="D28" s="152"/>
-      <c r="E28" s="152"/>
-      <c r="F28" s="152"/>
-      <c r="G28" s="153"/>
-      <c r="H28" s="105"/>
-      <c r="I28" s="105"/>
-      <c r="J28" s="105"/>
-      <c r="K28" s="105"/>
-      <c r="L28" s="105"/>
-      <c r="N28" s="111"/>
-      <c r="O28" s="111"/>
-    </row>
-    <row r="29" spans="1:15">
-      <c r="A29" s="116"/>
-      <c r="B29" s="168"/>
-      <c r="C29" s="168"/>
-      <c r="D29" s="168"/>
-      <c r="E29" s="168"/>
-      <c r="F29" s="168"/>
-      <c r="G29" s="168"/>
-      <c r="H29" s="112"/>
-      <c r="I29" s="112"/>
-      <c r="J29" s="112"/>
-      <c r="K29" s="112"/>
-      <c r="M29"/>
-      <c r="N29"/>
-      <c r="O29"/>
+      <c r="C29" s="174"/>
+      <c r="D29" s="174"/>
+      <c r="E29" s="174"/>
+      <c r="F29" s="174"/>
+      <c r="G29" s="175"/>
+      <c r="H29" s="105"/>
+      <c r="I29" s="105"/>
+      <c r="J29" s="105"/>
+      <c r="K29" s="105"/>
+      <c r="L29" s="105"/>
+      <c r="N29" s="111"/>
+      <c r="O29" s="111"/>
     </row>
     <row r="30" spans="1:15">
-      <c r="A30" s="117"/>
-      <c r="B30" s="169"/>
-      <c r="C30" s="169"/>
-      <c r="D30" s="169"/>
-      <c r="E30" s="169"/>
-      <c r="F30" s="169"/>
-      <c r="G30" s="169"/>
+      <c r="A30" s="116"/>
+      <c r="B30" s="157"/>
+      <c r="C30" s="157"/>
+      <c r="D30" s="157"/>
+      <c r="E30" s="157"/>
+      <c r="F30" s="157"/>
+      <c r="G30" s="157"/>
       <c r="H30" s="112"/>
       <c r="I30" s="112"/>
       <c r="J30" s="112"/>
@@ -4833,13 +4875,13 @@
       <c r="O30"/>
     </row>
     <row r="31" spans="1:15">
-      <c r="A31" s="118"/>
-      <c r="B31" s="170"/>
-      <c r="C31" s="170"/>
-      <c r="D31" s="170"/>
-      <c r="E31" s="170"/>
-      <c r="F31" s="170"/>
-      <c r="G31" s="170"/>
+      <c r="A31" s="117"/>
+      <c r="B31" s="159"/>
+      <c r="C31" s="159"/>
+      <c r="D31" s="159"/>
+      <c r="E31" s="159"/>
+      <c r="F31" s="159"/>
+      <c r="G31" s="159"/>
       <c r="H31" s="112"/>
       <c r="I31" s="112"/>
       <c r="J31" s="112"/>
@@ -4849,67 +4891,67 @@
       <c r="O31"/>
     </row>
     <row r="32" spans="1:15">
-      <c r="C32"/>
+      <c r="A32" s="118"/>
+      <c r="B32" s="161"/>
+      <c r="C32" s="161"/>
+      <c r="D32" s="161"/>
+      <c r="E32" s="161"/>
+      <c r="F32" s="161"/>
+      <c r="G32" s="161"/>
+      <c r="H32" s="112"/>
+      <c r="I32" s="112"/>
+      <c r="J32" s="112"/>
+      <c r="K32" s="112"/>
+      <c r="M32"/>
+      <c r="N32"/>
+      <c r="O32"/>
     </row>
     <row r="33" spans="1:15">
-      <c r="A33" s="154" t="s">
+      <c r="C33"/>
+    </row>
+    <row r="34" spans="1:15">
+      <c r="A34" s="176" t="s">
         <v>190</v>
       </c>
-      <c r="B33" s="155"/>
-      <c r="C33" s="155"/>
-      <c r="D33" s="155"/>
-      <c r="E33" s="155"/>
-      <c r="F33" s="155"/>
-      <c r="G33" s="156"/>
-    </row>
-    <row r="34" spans="1:15">
-      <c r="A34" s="115" t="s">
+      <c r="B34" s="177"/>
+      <c r="C34" s="177"/>
+      <c r="D34" s="177"/>
+      <c r="E34" s="177"/>
+      <c r="F34" s="177"/>
+      <c r="G34" s="178"/>
+    </row>
+    <row r="35" spans="1:15">
+      <c r="A35" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="174" t="s">
+      <c r="B35" s="153" t="s">
         <v>184</v>
       </c>
-      <c r="C34" s="174"/>
-      <c r="D34" s="174"/>
-      <c r="E34" s="174"/>
-      <c r="F34" s="174"/>
-      <c r="G34" s="174"/>
-      <c r="H34" s="105"/>
-      <c r="I34" s="105"/>
-      <c r="J34" s="105"/>
-      <c r="K34" s="105"/>
-      <c r="L34" s="105"/>
-      <c r="N34" s="111"/>
-      <c r="O34" s="111"/>
-    </row>
-    <row r="35" spans="1:15">
-      <c r="A35" s="116">
+      <c r="C35" s="153"/>
+      <c r="D35" s="153"/>
+      <c r="E35" s="153"/>
+      <c r="F35" s="153"/>
+      <c r="G35" s="153"/>
+      <c r="H35" s="105"/>
+      <c r="I35" s="105"/>
+      <c r="J35" s="105"/>
+      <c r="K35" s="105"/>
+      <c r="L35" s="105"/>
+      <c r="N35" s="111"/>
+      <c r="O35" s="111"/>
+    </row>
+    <row r="36" spans="1:15">
+      <c r="A36" s="116">
         <v>1</v>
       </c>
-      <c r="B35" s="175" t="s">
+      <c r="B36" s="154" t="s">
         <v>218</v>
       </c>
-      <c r="C35" s="175"/>
-      <c r="D35" s="175"/>
-      <c r="E35" s="175"/>
-      <c r="F35" s="175"/>
-      <c r="G35" s="175"/>
-      <c r="H35" s="112"/>
-      <c r="I35" s="112"/>
-      <c r="J35" s="112"/>
-      <c r="K35" s="112"/>
-      <c r="M35"/>
-      <c r="N35"/>
-      <c r="O35"/>
-    </row>
-    <row r="36" spans="1:15">
-      <c r="A36" s="117"/>
-      <c r="B36" s="176"/>
-      <c r="C36" s="176"/>
-      <c r="D36" s="176"/>
-      <c r="E36" s="176"/>
-      <c r="F36" s="176"/>
-      <c r="G36" s="176"/>
+      <c r="C36" s="154"/>
+      <c r="D36" s="154"/>
+      <c r="E36" s="154"/>
+      <c r="F36" s="154"/>
+      <c r="G36" s="154"/>
       <c r="H36" s="112"/>
       <c r="I36" s="112"/>
       <c r="J36" s="112"/>
@@ -4919,13 +4961,13 @@
       <c r="O36"/>
     </row>
     <row r="37" spans="1:15">
-      <c r="A37" s="118"/>
-      <c r="B37" s="177"/>
-      <c r="C37" s="177"/>
-      <c r="D37" s="177"/>
-      <c r="E37" s="177"/>
-      <c r="F37" s="177"/>
-      <c r="G37" s="177"/>
+      <c r="A37" s="117"/>
+      <c r="B37" s="155"/>
+      <c r="C37" s="155"/>
+      <c r="D37" s="155"/>
+      <c r="E37" s="155"/>
+      <c r="F37" s="155"/>
+      <c r="G37" s="155"/>
       <c r="H37" s="112"/>
       <c r="I37" s="112"/>
       <c r="J37" s="112"/>
@@ -4935,75 +4977,75 @@
       <c r="O37"/>
     </row>
     <row r="38" spans="1:15">
-      <c r="A38"/>
-      <c r="B38"/>
-      <c r="C38"/>
-      <c r="D38"/>
-      <c r="E38"/>
-      <c r="F38"/>
-      <c r="G38"/>
-      <c r="H38"/>
-      <c r="I38"/>
-      <c r="J38"/>
-      <c r="K38"/>
-      <c r="L38"/>
+      <c r="A38" s="118"/>
+      <c r="B38" s="156"/>
+      <c r="C38" s="156"/>
+      <c r="D38" s="156"/>
+      <c r="E38" s="156"/>
+      <c r="F38" s="156"/>
+      <c r="G38" s="156"/>
+      <c r="H38" s="112"/>
+      <c r="I38" s="112"/>
+      <c r="J38" s="112"/>
+      <c r="K38" s="112"/>
       <c r="M38"/>
+      <c r="N38"/>
+      <c r="O38"/>
     </row>
     <row r="39" spans="1:15">
-      <c r="A39" s="154" t="s">
+      <c r="A39"/>
+      <c r="B39"/>
+      <c r="C39"/>
+      <c r="D39"/>
+      <c r="E39"/>
+      <c r="F39"/>
+      <c r="G39"/>
+      <c r="H39"/>
+      <c r="I39"/>
+      <c r="J39"/>
+      <c r="K39"/>
+      <c r="L39"/>
+      <c r="M39"/>
+    </row>
+    <row r="40" spans="1:15">
+      <c r="A40" s="176" t="s">
         <v>191</v>
       </c>
-      <c r="B39" s="155"/>
-      <c r="C39" s="155"/>
-      <c r="D39" s="155"/>
-      <c r="E39" s="155"/>
-      <c r="F39" s="155"/>
-      <c r="G39" s="156"/>
-    </row>
-    <row r="40" spans="1:15">
-      <c r="A40" s="115" t="s">
+      <c r="B40" s="177"/>
+      <c r="C40" s="177"/>
+      <c r="D40" s="177"/>
+      <c r="E40" s="177"/>
+      <c r="F40" s="177"/>
+      <c r="G40" s="178"/>
+    </row>
+    <row r="41" spans="1:15">
+      <c r="A41" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B40" s="174" t="s">
+      <c r="B41" s="153" t="s">
         <v>186</v>
       </c>
-      <c r="C40" s="174"/>
-      <c r="D40" s="174"/>
-      <c r="E40" s="174"/>
-      <c r="F40" s="174"/>
-      <c r="G40" s="174"/>
-      <c r="H40" s="105"/>
-      <c r="I40" s="105"/>
-      <c r="J40" s="105"/>
-      <c r="K40" s="105"/>
-      <c r="L40" s="105"/>
-      <c r="N40" s="111"/>
-      <c r="O40" s="111"/>
-    </row>
-    <row r="41" spans="1:15">
-      <c r="A41" s="116"/>
-      <c r="B41" s="168"/>
-      <c r="C41" s="168"/>
-      <c r="D41" s="168"/>
-      <c r="E41" s="168"/>
-      <c r="F41" s="168"/>
-      <c r="G41" s="178"/>
-      <c r="H41" s="112"/>
-      <c r="I41" s="112"/>
-      <c r="J41" s="112"/>
-      <c r="K41" s="112"/>
-      <c r="M41"/>
-      <c r="N41"/>
-      <c r="O41"/>
+      <c r="C41" s="153"/>
+      <c r="D41" s="153"/>
+      <c r="E41" s="153"/>
+      <c r="F41" s="153"/>
+      <c r="G41" s="153"/>
+      <c r="H41" s="105"/>
+      <c r="I41" s="105"/>
+      <c r="J41" s="105"/>
+      <c r="K41" s="105"/>
+      <c r="L41" s="105"/>
+      <c r="N41" s="111"/>
+      <c r="O41" s="111"/>
     </row>
     <row r="42" spans="1:15">
-      <c r="A42" s="117"/>
-      <c r="B42" s="169"/>
-      <c r="C42" s="169"/>
-      <c r="D42" s="169"/>
-      <c r="E42" s="169"/>
-      <c r="F42" s="169"/>
-      <c r="G42" s="179"/>
+      <c r="A42" s="116"/>
+      <c r="B42" s="157"/>
+      <c r="C42" s="157"/>
+      <c r="D42" s="157"/>
+      <c r="E42" s="157"/>
+      <c r="F42" s="157"/>
+      <c r="G42" s="158"/>
       <c r="H42" s="112"/>
       <c r="I42" s="112"/>
       <c r="J42" s="112"/>
@@ -5013,13 +5055,13 @@
       <c r="O42"/>
     </row>
     <row r="43" spans="1:15">
-      <c r="A43" s="118"/>
-      <c r="B43" s="170"/>
-      <c r="C43" s="170"/>
-      <c r="D43" s="170"/>
-      <c r="E43" s="170"/>
-      <c r="F43" s="170"/>
-      <c r="G43" s="180"/>
+      <c r="A43" s="117"/>
+      <c r="B43" s="159"/>
+      <c r="C43" s="159"/>
+      <c r="D43" s="159"/>
+      <c r="E43" s="159"/>
+      <c r="F43" s="159"/>
+      <c r="G43" s="160"/>
       <c r="H43" s="112"/>
       <c r="I43" s="112"/>
       <c r="J43" s="112"/>
@@ -5029,251 +5071,339 @@
       <c r="O43"/>
     </row>
     <row r="44" spans="1:15">
-      <c r="A44"/>
-      <c r="B44"/>
-      <c r="C44"/>
-      <c r="D44"/>
-      <c r="E44"/>
-      <c r="F44"/>
-      <c r="G44"/>
-      <c r="H44"/>
-      <c r="I44"/>
-      <c r="J44"/>
-      <c r="K44"/>
-      <c r="L44"/>
+      <c r="A44" s="118"/>
+      <c r="B44" s="161"/>
+      <c r="C44" s="161"/>
+      <c r="D44" s="161"/>
+      <c r="E44" s="161"/>
+      <c r="F44" s="161"/>
+      <c r="G44" s="162"/>
+      <c r="H44" s="112"/>
+      <c r="I44" s="112"/>
+      <c r="J44" s="112"/>
+      <c r="K44" s="112"/>
       <c r="M44"/>
+      <c r="N44"/>
+      <c r="O44"/>
     </row>
     <row r="45" spans="1:15">
-      <c r="A45" s="4" t="s">
+      <c r="A45"/>
+      <c r="B45"/>
+      <c r="C45"/>
+      <c r="D45"/>
+      <c r="E45"/>
+      <c r="F45"/>
+      <c r="G45"/>
+      <c r="H45"/>
+      <c r="I45"/>
+      <c r="J45"/>
+      <c r="K45"/>
+      <c r="L45"/>
+      <c r="M45"/>
+    </row>
+    <row r="46" spans="1:15">
+      <c r="A46" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="5"/>
-    </row>
-    <row r="46" spans="1:15">
-      <c r="A46" s="141" t="s">
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="5"/>
+    </row>
+    <row r="47" spans="1:15">
+      <c r="A47" s="166" t="s">
         <v>65</v>
       </c>
-      <c r="B46" s="148"/>
-      <c r="C46" s="141" t="s">
+      <c r="B47" s="172"/>
+      <c r="C47" s="166" t="s">
         <v>66</v>
       </c>
-      <c r="D46" s="142"/>
-      <c r="E46" s="143"/>
-      <c r="F46" s="29" t="s">
+      <c r="D47" s="167"/>
+      <c r="E47" s="168"/>
+      <c r="F47" s="29" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="47" spans="1:15">
-      <c r="A47" s="149"/>
-      <c r="B47" s="150"/>
-      <c r="C47" s="149"/>
-      <c r="D47" s="171"/>
-      <c r="E47" s="150"/>
-      <c r="F47" s="49"/>
-    </row>
     <row r="48" spans="1:15">
-      <c r="A48" s="139"/>
-      <c r="B48" s="140"/>
-      <c r="C48" s="139"/>
-      <c r="D48" s="172"/>
-      <c r="E48" s="140"/>
+      <c r="A48" s="163"/>
+      <c r="B48" s="165"/>
+      <c r="C48" s="163"/>
+      <c r="D48" s="164"/>
+      <c r="E48" s="165"/>
       <c r="F48" s="49"/>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="139"/>
-      <c r="B49" s="140"/>
-      <c r="C49" s="139"/>
-      <c r="D49" s="172"/>
-      <c r="E49" s="140"/>
+      <c r="A49" s="147"/>
+      <c r="B49" s="149"/>
+      <c r="C49" s="147"/>
+      <c r="D49" s="148"/>
+      <c r="E49" s="149"/>
       <c r="F49" s="49"/>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="139"/>
-      <c r="B50" s="140"/>
-      <c r="C50" s="139"/>
-      <c r="D50" s="172"/>
-      <c r="E50" s="140"/>
+      <c r="A50" s="147"/>
+      <c r="B50" s="149"/>
+      <c r="C50" s="147"/>
+      <c r="D50" s="148"/>
+      <c r="E50" s="149"/>
       <c r="F50" s="49"/>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="139"/>
-      <c r="B51" s="140"/>
-      <c r="C51" s="139"/>
-      <c r="D51" s="172"/>
-      <c r="E51" s="140"/>
+      <c r="A51" s="147"/>
+      <c r="B51" s="149"/>
+      <c r="C51" s="147"/>
+      <c r="D51" s="148"/>
+      <c r="E51" s="149"/>
       <c r="F51" s="49"/>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="139"/>
-      <c r="B52" s="140"/>
-      <c r="C52" s="139"/>
-      <c r="D52" s="172"/>
-      <c r="E52" s="140"/>
+      <c r="A52" s="147"/>
+      <c r="B52" s="149"/>
+      <c r="C52" s="147"/>
+      <c r="D52" s="148"/>
+      <c r="E52" s="149"/>
       <c r="F52" s="49"/>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="139"/>
-      <c r="B53" s="140"/>
-      <c r="C53" s="139"/>
-      <c r="D53" s="172"/>
-      <c r="E53" s="140"/>
+      <c r="A53" s="147"/>
+      <c r="B53" s="149"/>
+      <c r="C53" s="147"/>
+      <c r="D53" s="148"/>
+      <c r="E53" s="149"/>
       <c r="F53" s="49"/>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="139"/>
-      <c r="B54" s="140"/>
-      <c r="C54" s="139"/>
-      <c r="D54" s="172"/>
-      <c r="E54" s="140"/>
+      <c r="A54" s="147"/>
+      <c r="B54" s="149"/>
+      <c r="C54" s="147"/>
+      <c r="D54" s="148"/>
+      <c r="E54" s="149"/>
       <c r="F54" s="49"/>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="139"/>
-      <c r="B55" s="140"/>
-      <c r="C55" s="139"/>
-      <c r="D55" s="172"/>
-      <c r="E55" s="140"/>
+      <c r="A55" s="147"/>
+      <c r="B55" s="149"/>
+      <c r="C55" s="147"/>
+      <c r="D55" s="148"/>
+      <c r="E55" s="149"/>
       <c r="F55" s="49"/>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="139"/>
-      <c r="B56" s="140"/>
-      <c r="C56" s="139"/>
-      <c r="D56" s="172"/>
-      <c r="E56" s="140"/>
+      <c r="A56" s="147"/>
+      <c r="B56" s="149"/>
+      <c r="C56" s="147"/>
+      <c r="D56" s="148"/>
+      <c r="E56" s="149"/>
       <c r="F56" s="49"/>
     </row>
     <row r="57" spans="1:6">
-      <c r="A57" s="139"/>
-      <c r="B57" s="140"/>
-      <c r="C57" s="139"/>
-      <c r="D57" s="172"/>
-      <c r="E57" s="140"/>
+      <c r="A57" s="147"/>
+      <c r="B57" s="149"/>
+      <c r="C57" s="147"/>
+      <c r="D57" s="148"/>
+      <c r="E57" s="149"/>
       <c r="F57" s="49"/>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="139"/>
-      <c r="B58" s="140"/>
-      <c r="C58" s="139"/>
-      <c r="D58" s="172"/>
-      <c r="E58" s="140"/>
+      <c r="A58" s="147"/>
+      <c r="B58" s="149"/>
+      <c r="C58" s="147"/>
+      <c r="D58" s="148"/>
+      <c r="E58" s="149"/>
       <c r="F58" s="49"/>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="139"/>
-      <c r="B59" s="140"/>
-      <c r="C59" s="139"/>
-      <c r="D59" s="172"/>
-      <c r="E59" s="140"/>
+      <c r="A59" s="147"/>
+      <c r="B59" s="149"/>
+      <c r="C59" s="147"/>
+      <c r="D59" s="148"/>
+      <c r="E59" s="149"/>
       <c r="F59" s="49"/>
     </row>
     <row r="60" spans="1:6">
-      <c r="A60" s="139"/>
-      <c r="B60" s="140"/>
-      <c r="C60" s="139"/>
-      <c r="D60" s="172"/>
-      <c r="E60" s="140"/>
+      <c r="A60" s="147"/>
+      <c r="B60" s="149"/>
+      <c r="C60" s="147"/>
+      <c r="D60" s="148"/>
+      <c r="E60" s="149"/>
       <c r="F60" s="49"/>
     </row>
     <row r="61" spans="1:6">
-      <c r="A61" s="139"/>
-      <c r="B61" s="140"/>
-      <c r="C61" s="139"/>
-      <c r="D61" s="172"/>
-      <c r="E61" s="140"/>
+      <c r="A61" s="147"/>
+      <c r="B61" s="149"/>
+      <c r="C61" s="147"/>
+      <c r="D61" s="148"/>
+      <c r="E61" s="149"/>
       <c r="F61" s="49"/>
     </row>
     <row r="62" spans="1:6">
-      <c r="A62" s="139"/>
-      <c r="B62" s="140"/>
-      <c r="C62" s="139"/>
-      <c r="D62" s="172"/>
-      <c r="E62" s="140"/>
+      <c r="A62" s="147"/>
+      <c r="B62" s="149"/>
+      <c r="C62" s="147"/>
+      <c r="D62" s="148"/>
+      <c r="E62" s="149"/>
       <c r="F62" s="49"/>
     </row>
     <row r="63" spans="1:6">
-      <c r="A63" s="139"/>
-      <c r="B63" s="140"/>
-      <c r="C63" s="139"/>
-      <c r="D63" s="172"/>
-      <c r="E63" s="140"/>
+      <c r="A63" s="147"/>
+      <c r="B63" s="149"/>
+      <c r="C63" s="147"/>
+      <c r="D63" s="148"/>
+      <c r="E63" s="149"/>
       <c r="F63" s="49"/>
     </row>
     <row r="64" spans="1:6">
-      <c r="A64" s="139"/>
-      <c r="B64" s="140"/>
-      <c r="C64" s="139"/>
-      <c r="D64" s="172"/>
-      <c r="E64" s="140"/>
+      <c r="A64" s="147"/>
+      <c r="B64" s="149"/>
+      <c r="C64" s="147"/>
+      <c r="D64" s="148"/>
+      <c r="E64" s="149"/>
       <c r="F64" s="49"/>
     </row>
     <row r="65" spans="1:6">
-      <c r="A65" s="139"/>
-      <c r="B65" s="140"/>
-      <c r="C65" s="139"/>
-      <c r="D65" s="172"/>
-      <c r="E65" s="140"/>
+      <c r="A65" s="147"/>
+      <c r="B65" s="149"/>
+      <c r="C65" s="147"/>
+      <c r="D65" s="148"/>
+      <c r="E65" s="149"/>
       <c r="F65" s="49"/>
     </row>
     <row r="66" spans="1:6">
-      <c r="A66" s="139"/>
-      <c r="B66" s="140"/>
-      <c r="C66" s="139"/>
-      <c r="D66" s="172"/>
-      <c r="E66" s="140"/>
+      <c r="A66" s="147"/>
+      <c r="B66" s="149"/>
+      <c r="C66" s="147"/>
+      <c r="D66" s="148"/>
+      <c r="E66" s="149"/>
       <c r="F66" s="49"/>
     </row>
     <row r="67" spans="1:6">
-      <c r="A67" s="139"/>
-      <c r="B67" s="140"/>
-      <c r="C67" s="139"/>
-      <c r="D67" s="172"/>
-      <c r="E67" s="140"/>
+      <c r="A67" s="147"/>
+      <c r="B67" s="149"/>
+      <c r="C67" s="147"/>
+      <c r="D67" s="148"/>
+      <c r="E67" s="149"/>
       <c r="F67" s="49"/>
     </row>
     <row r="68" spans="1:6">
-      <c r="A68" s="139"/>
-      <c r="B68" s="140"/>
-      <c r="C68" s="139"/>
-      <c r="D68" s="172"/>
-      <c r="E68" s="140"/>
+      <c r="A68" s="147"/>
+      <c r="B68" s="149"/>
+      <c r="C68" s="147"/>
+      <c r="D68" s="148"/>
+      <c r="E68" s="149"/>
       <c r="F68" s="49"/>
     </row>
     <row r="69" spans="1:6">
-      <c r="A69" s="139"/>
-      <c r="B69" s="140"/>
-      <c r="C69" s="139"/>
-      <c r="D69" s="172"/>
-      <c r="E69" s="140"/>
+      <c r="A69" s="147"/>
+      <c r="B69" s="149"/>
+      <c r="C69" s="147"/>
+      <c r="D69" s="148"/>
+      <c r="E69" s="149"/>
       <c r="F69" s="49"/>
     </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="139"/>
-      <c r="B70" s="140"/>
-      <c r="C70" s="139"/>
-      <c r="D70" s="172"/>
-      <c r="E70" s="140"/>
+      <c r="A70" s="147"/>
+      <c r="B70" s="149"/>
+      <c r="C70" s="147"/>
+      <c r="D70" s="148"/>
+      <c r="E70" s="149"/>
       <c r="F70" s="49"/>
     </row>
     <row r="71" spans="1:6">
-      <c r="A71" s="166"/>
-      <c r="B71" s="167"/>
-      <c r="C71" s="166"/>
-      <c r="D71" s="173"/>
-      <c r="E71" s="167"/>
-      <c r="F71" s="50"/>
+      <c r="A71" s="147"/>
+      <c r="B71" s="149"/>
+      <c r="C71" s="147"/>
+      <c r="D71" s="148"/>
+      <c r="E71" s="149"/>
+      <c r="F71" s="49"/>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="150"/>
+      <c r="B72" s="152"/>
+      <c r="C72" s="150"/>
+      <c r="D72" s="151"/>
+      <c r="E72" s="152"/>
+      <c r="F72" s="50"/>
     </row>
   </sheetData>
-  <mergeCells count="97">
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
+  <mergeCells count="98">
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="A40:G40"/>
+    <mergeCell ref="A28:G28"/>
+    <mergeCell ref="A23:G23"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="C71:E71"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="B41:G41"/>
+    <mergeCell ref="B42:G42"/>
+    <mergeCell ref="B43:G43"/>
+    <mergeCell ref="B44:G44"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C70:E70"/>
+    <mergeCell ref="C61:E61"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D13:E13"/>
@@ -5290,86 +5420,15 @@
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="A16:C16"/>
     <mergeCell ref="D16:E16"/>
-    <mergeCell ref="C70:E70"/>
-    <mergeCell ref="C71:E71"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B36:G36"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="B41:G41"/>
-    <mergeCell ref="B42:G42"/>
-    <mergeCell ref="B43:G43"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="C51:E51"/>
-    <mergeCell ref="C52:E52"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="A33:G33"/>
-    <mergeCell ref="A39:G39"/>
-    <mergeCell ref="A27:G27"/>
-    <mergeCell ref="A22:G22"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D20" xr:uid="{AA005DBF-E840-AD43-AC91-CD6CE016CB50}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D21" xr:uid="{AA005DBF-E840-AD43-AC91-CD6CE016CB50}">
       <formula1>isImport</formula1>
     </dataValidation>
   </dataValidations>
@@ -5385,7 +5444,7 @@
           <x14:formula1>
             <xm:f>config!$B$5:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>D19</xm:sqref>
+          <xm:sqref>D19:D20</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5650,10 +5709,10 @@
         <v>174</v>
       </c>
       <c r="B15" s="122"/>
-      <c r="C15" s="165" t="s">
+      <c r="C15" s="141" t="s">
         <v>175</v>
       </c>
-      <c r="D15" s="165"/>
+      <c r="D15" s="141"/>
       <c r="E15" s="95" t="s">
         <v>176</v>
       </c>
@@ -5668,10 +5727,10 @@
         <v>226</v>
       </c>
       <c r="B16" s="122"/>
-      <c r="C16" s="164" t="s">
+      <c r="C16" s="142" t="s">
         <v>230</v>
       </c>
-      <c r="D16" s="165"/>
+      <c r="D16" s="141"/>
       <c r="E16" s="55" t="s">
         <v>227</v>
       </c>
@@ -5694,10 +5753,10 @@
         <v>177</v>
       </c>
       <c r="B17" s="122"/>
-      <c r="C17" s="165" t="s">
+      <c r="C17" s="141" t="s">
         <v>178</v>
       </c>
-      <c r="D17" s="165"/>
+      <c r="D17" s="141"/>
       <c r="E17" s="55"/>
       <c r="F17" s="55"/>
       <c r="G17" s="54"/>
@@ -5709,8 +5768,8 @@
         <v>228</v>
       </c>
       <c r="B18" s="122"/>
-      <c r="C18" s="164"/>
-      <c r="D18" s="165"/>
+      <c r="C18" s="142"/>
+      <c r="D18" s="141"/>
       <c r="E18" s="55" t="s">
         <v>229</v>
       </c>
@@ -5766,15 +5825,15 @@
       <c r="O20"/>
     </row>
     <row r="21" spans="1:25">
-      <c r="A21" s="157" t="s">
+      <c r="A21" s="179" t="s">
         <v>192</v>
       </c>
-      <c r="B21" s="157"/>
-      <c r="C21" s="157"/>
-      <c r="D21" s="157"/>
-      <c r="E21" s="157"/>
-      <c r="F21" s="157"/>
-      <c r="G21" s="157"/>
+      <c r="B21" s="179"/>
+      <c r="C21" s="179"/>
+      <c r="D21" s="179"/>
+      <c r="E21" s="179"/>
+      <c r="F21" s="179"/>
+      <c r="G21" s="179"/>
       <c r="K21"/>
       <c r="L21"/>
       <c r="M21"/>
@@ -5784,14 +5843,14 @@
       <c r="A22" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B22" s="151" t="s">
+      <c r="B22" s="173" t="s">
         <v>183</v>
       </c>
-      <c r="C22" s="152"/>
-      <c r="D22" s="152"/>
-      <c r="E22" s="152"/>
-      <c r="F22" s="152"/>
-      <c r="G22" s="153"/>
+      <c r="C22" s="174"/>
+      <c r="D22" s="174"/>
+      <c r="E22" s="174"/>
+      <c r="F22" s="174"/>
+      <c r="G22" s="175"/>
       <c r="H22" s="105"/>
       <c r="I22" s="105"/>
       <c r="J22" s="105"/>
@@ -5812,12 +5871,12 @@
     </row>
     <row r="23" spans="1:25">
       <c r="A23" s="116"/>
-      <c r="B23" s="168"/>
-      <c r="C23" s="168"/>
-      <c r="D23" s="168"/>
-      <c r="E23" s="168"/>
-      <c r="F23" s="168"/>
-      <c r="G23" s="168"/>
+      <c r="B23" s="157"/>
+      <c r="C23" s="157"/>
+      <c r="D23" s="157"/>
+      <c r="E23" s="157"/>
+      <c r="F23" s="157"/>
+      <c r="G23" s="157"/>
       <c r="H23" s="112"/>
       <c r="I23" s="112"/>
       <c r="J23" s="112"/>
@@ -5838,12 +5897,12 @@
     </row>
     <row r="24" spans="1:25">
       <c r="A24" s="117"/>
-      <c r="B24" s="169"/>
-      <c r="C24" s="169"/>
-      <c r="D24" s="169"/>
-      <c r="E24" s="169"/>
-      <c r="F24" s="169"/>
-      <c r="G24" s="169"/>
+      <c r="B24" s="159"/>
+      <c r="C24" s="159"/>
+      <c r="D24" s="159"/>
+      <c r="E24" s="159"/>
+      <c r="F24" s="159"/>
+      <c r="G24" s="159"/>
       <c r="H24" s="112"/>
       <c r="I24" s="112"/>
       <c r="J24" s="112"/>
@@ -5864,12 +5923,12 @@
     </row>
     <row r="25" spans="1:25">
       <c r="A25" s="118"/>
-      <c r="B25" s="170"/>
-      <c r="C25" s="170"/>
-      <c r="D25" s="170"/>
-      <c r="E25" s="170"/>
-      <c r="F25" s="170"/>
-      <c r="G25" s="170"/>
+      <c r="B25" s="161"/>
+      <c r="C25" s="161"/>
+      <c r="D25" s="161"/>
+      <c r="E25" s="161"/>
+      <c r="F25" s="161"/>
+      <c r="G25" s="161"/>
       <c r="H25" s="112"/>
       <c r="I25" s="112"/>
       <c r="J25" s="112"/>
@@ -5892,15 +5951,15 @@
       <c r="O26" s="105"/>
     </row>
     <row r="27" spans="1:25">
-      <c r="A27" s="154" t="s">
+      <c r="A27" s="176" t="s">
         <v>193</v>
       </c>
-      <c r="B27" s="155"/>
-      <c r="C27" s="155"/>
-      <c r="D27" s="155"/>
-      <c r="E27" s="155"/>
-      <c r="F27" s="155"/>
-      <c r="G27" s="156"/>
+      <c r="B27" s="177"/>
+      <c r="C27" s="177"/>
+      <c r="D27" s="177"/>
+      <c r="E27" s="177"/>
+      <c r="F27" s="177"/>
+      <c r="G27" s="178"/>
       <c r="K27" s="105"/>
       <c r="L27" s="105"/>
       <c r="M27" s="105"/>
@@ -5910,14 +5969,14 @@
       <c r="A28" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B28" s="174" t="s">
+      <c r="B28" s="153" t="s">
         <v>184</v>
       </c>
-      <c r="C28" s="174"/>
-      <c r="D28" s="174"/>
-      <c r="E28" s="174"/>
-      <c r="F28" s="174"/>
-      <c r="G28" s="174"/>
+      <c r="C28" s="153"/>
+      <c r="D28" s="153"/>
+      <c r="E28" s="153"/>
+      <c r="F28" s="153"/>
+      <c r="G28" s="153"/>
       <c r="H28" s="105"/>
       <c r="I28" s="105"/>
       <c r="J28" s="105"/>
@@ -5940,14 +5999,14 @@
       <c r="A29" s="116">
         <v>1</v>
       </c>
-      <c r="B29" s="175" t="s">
+      <c r="B29" s="154" t="s">
         <v>225</v>
       </c>
-      <c r="C29" s="175"/>
-      <c r="D29" s="175"/>
-      <c r="E29" s="175"/>
-      <c r="F29" s="175"/>
-      <c r="G29" s="175"/>
+      <c r="C29" s="154"/>
+      <c r="D29" s="154"/>
+      <c r="E29" s="154"/>
+      <c r="F29" s="154"/>
+      <c r="G29" s="154"/>
       <c r="H29" s="112"/>
       <c r="I29" s="112"/>
       <c r="J29" s="112"/>
@@ -5968,12 +6027,12 @@
     </row>
     <row r="30" spans="1:25">
       <c r="A30" s="117"/>
-      <c r="B30" s="176"/>
-      <c r="C30" s="176"/>
-      <c r="D30" s="176"/>
-      <c r="E30" s="176"/>
-      <c r="F30" s="176"/>
-      <c r="G30" s="176"/>
+      <c r="B30" s="155"/>
+      <c r="C30" s="155"/>
+      <c r="D30" s="155"/>
+      <c r="E30" s="155"/>
+      <c r="F30" s="155"/>
+      <c r="G30" s="155"/>
       <c r="H30" s="112"/>
       <c r="I30" s="112"/>
       <c r="J30" s="112"/>
@@ -5990,12 +6049,12 @@
     </row>
     <row r="31" spans="1:25">
       <c r="A31" s="118"/>
-      <c r="B31" s="177"/>
-      <c r="C31" s="177"/>
-      <c r="D31" s="177"/>
-      <c r="E31" s="177"/>
-      <c r="F31" s="177"/>
-      <c r="G31" s="177"/>
+      <c r="B31" s="156"/>
+      <c r="C31" s="156"/>
+      <c r="D31" s="156"/>
+      <c r="E31" s="156"/>
+      <c r="F31" s="156"/>
+      <c r="G31" s="156"/>
       <c r="H31" s="112"/>
       <c r="I31" s="112"/>
       <c r="J31" s="112"/>
@@ -6040,15 +6099,15 @@
       <c r="W32"/>
     </row>
     <row r="33" spans="1:29">
-      <c r="A33" s="154" t="s">
+      <c r="A33" s="176" t="s">
         <v>194</v>
       </c>
-      <c r="B33" s="155"/>
-      <c r="C33" s="155"/>
-      <c r="D33" s="155"/>
-      <c r="E33" s="155"/>
-      <c r="F33" s="155"/>
-      <c r="G33" s="156"/>
+      <c r="B33" s="177"/>
+      <c r="C33" s="177"/>
+      <c r="D33" s="177"/>
+      <c r="E33" s="177"/>
+      <c r="F33" s="177"/>
+      <c r="G33" s="178"/>
       <c r="K33" s="112"/>
       <c r="L33" s="112"/>
       <c r="M33" s="112"/>
@@ -6058,14 +6117,14 @@
       <c r="A34" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="174" t="s">
+      <c r="B34" s="153" t="s">
         <v>186</v>
       </c>
-      <c r="C34" s="174"/>
-      <c r="D34" s="174"/>
-      <c r="E34" s="174"/>
-      <c r="F34" s="174"/>
-      <c r="G34" s="174"/>
+      <c r="C34" s="153"/>
+      <c r="D34" s="153"/>
+      <c r="E34" s="153"/>
+      <c r="F34" s="153"/>
+      <c r="G34" s="153"/>
       <c r="H34" s="105"/>
       <c r="I34" s="105"/>
       <c r="J34" s="105"/>
@@ -6086,12 +6145,12 @@
     </row>
     <row r="35" spans="1:29">
       <c r="A35" s="116"/>
-      <c r="B35" s="168"/>
-      <c r="C35" s="168"/>
-      <c r="D35" s="168"/>
-      <c r="E35" s="168"/>
-      <c r="F35" s="168"/>
-      <c r="G35" s="178"/>
+      <c r="B35" s="157"/>
+      <c r="C35" s="157"/>
+      <c r="D35" s="157"/>
+      <c r="E35" s="157"/>
+      <c r="F35" s="157"/>
+      <c r="G35" s="158"/>
       <c r="H35" s="112"/>
       <c r="I35" s="112"/>
       <c r="J35" s="112"/>
@@ -6112,12 +6171,12 @@
     </row>
     <row r="36" spans="1:29">
       <c r="A36" s="117"/>
-      <c r="B36" s="169"/>
-      <c r="C36" s="169"/>
-      <c r="D36" s="169"/>
-      <c r="E36" s="169"/>
-      <c r="F36" s="169"/>
-      <c r="G36" s="179"/>
+      <c r="B36" s="159"/>
+      <c r="C36" s="159"/>
+      <c r="D36" s="159"/>
+      <c r="E36" s="159"/>
+      <c r="F36" s="159"/>
+      <c r="G36" s="160"/>
       <c r="H36" s="112"/>
       <c r="I36" s="112"/>
       <c r="J36" s="112"/>
@@ -6134,12 +6193,12 @@
     </row>
     <row r="37" spans="1:29">
       <c r="A37" s="118"/>
-      <c r="B37" s="170"/>
-      <c r="C37" s="170"/>
-      <c r="D37" s="170"/>
-      <c r="E37" s="170"/>
-      <c r="F37" s="170"/>
-      <c r="G37" s="180"/>
+      <c r="B37" s="161"/>
+      <c r="C37" s="161"/>
+      <c r="D37" s="161"/>
+      <c r="E37" s="161"/>
+      <c r="F37" s="161"/>
+      <c r="G37" s="162"/>
       <c r="H37" s="112"/>
       <c r="I37" s="112"/>
       <c r="J37" s="112"/>
@@ -6212,94 +6271,94 @@
       <c r="AC40" s="39"/>
     </row>
     <row r="41" spans="1:29">
-      <c r="A41" s="188" t="s">
+      <c r="A41" s="186" t="s">
         <v>69</v>
       </c>
-      <c r="B41" s="188" t="s">
+      <c r="B41" s="186" t="s">
         <v>0</v>
       </c>
-      <c r="C41" s="193" t="s">
+      <c r="C41" s="188" t="s">
         <v>1</v>
       </c>
-      <c r="D41" s="188" t="s">
+      <c r="D41" s="186" t="s">
         <v>2</v>
       </c>
-      <c r="E41" s="194" t="s">
+      <c r="E41" s="189" t="s">
         <v>161</v>
       </c>
-      <c r="F41" s="194" t="s">
+      <c r="F41" s="189" t="s">
         <v>177</v>
       </c>
-      <c r="G41" s="188" t="s">
+      <c r="G41" s="186" t="s">
         <v>13</v>
       </c>
-      <c r="H41" s="188" t="s">
+      <c r="H41" s="186" t="s">
         <v>116</v>
       </c>
-      <c r="I41" s="188" t="s">
+      <c r="I41" s="186" t="s">
         <v>195</v>
       </c>
-      <c r="J41" s="188" t="s">
+      <c r="J41" s="186" t="s">
         <v>209</v>
       </c>
-      <c r="K41" s="197" t="s">
+      <c r="K41" s="193" t="s">
         <v>200</v>
       </c>
-      <c r="L41" s="197" t="s">
+      <c r="L41" s="193" t="s">
         <v>201</v>
       </c>
-      <c r="M41" s="197" t="s">
+      <c r="M41" s="193" t="s">
         <v>202</v>
       </c>
-      <c r="N41" s="188" t="s">
+      <c r="N41" s="186" t="s">
         <v>235</v>
       </c>
-      <c r="O41" s="186" t="s">
+      <c r="O41" s="196" t="s">
         <v>203</v>
       </c>
-      <c r="P41" s="188" t="s">
+      <c r="P41" s="186" t="s">
         <v>236</v>
       </c>
-      <c r="Q41" s="188" t="s">
+      <c r="Q41" s="186" t="s">
         <v>237</v>
       </c>
-      <c r="R41" s="193" t="s">
+      <c r="R41" s="188" t="s">
         <v>208</v>
       </c>
-      <c r="S41" s="190" t="s">
+      <c r="S41" s="194" t="s">
         <v>71</v>
       </c>
-      <c r="T41" s="191"/>
-      <c r="U41" s="190" t="s">
+      <c r="T41" s="195"/>
+      <c r="U41" s="194" t="s">
         <v>17</v>
       </c>
-      <c r="V41" s="191"/>
+      <c r="V41" s="195"/>
       <c r="W41" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="X41" s="188" t="s">
+      <c r="X41" s="186" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:29">
-      <c r="A42" s="192"/>
-      <c r="B42" s="192"/>
-      <c r="C42" s="192"/>
-      <c r="D42" s="192"/>
-      <c r="E42" s="195"/>
-      <c r="F42" s="196"/>
-      <c r="G42" s="192"/>
-      <c r="H42" s="192"/>
-      <c r="I42" s="189"/>
-      <c r="J42" s="189"/>
-      <c r="K42" s="197"/>
-      <c r="L42" s="197"/>
-      <c r="M42" s="197"/>
-      <c r="N42" s="189"/>
-      <c r="O42" s="187"/>
-      <c r="P42" s="189"/>
-      <c r="Q42" s="189"/>
-      <c r="R42" s="189"/>
+      <c r="A42" s="187"/>
+      <c r="B42" s="187"/>
+      <c r="C42" s="187"/>
+      <c r="D42" s="187"/>
+      <c r="E42" s="190"/>
+      <c r="F42" s="191"/>
+      <c r="G42" s="187"/>
+      <c r="H42" s="187"/>
+      <c r="I42" s="192"/>
+      <c r="J42" s="192"/>
+      <c r="K42" s="193"/>
+      <c r="L42" s="193"/>
+      <c r="M42" s="193"/>
+      <c r="N42" s="192"/>
+      <c r="O42" s="197"/>
+      <c r="P42" s="192"/>
+      <c r="Q42" s="192"/>
+      <c r="R42" s="192"/>
       <c r="S42" s="29" t="s">
         <v>75</v>
       </c>
@@ -6315,7 +6374,7 @@
       <c r="W42" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="X42" s="192"/>
+      <c r="X42" s="187"/>
     </row>
     <row r="43" spans="1:29" ht="30">
       <c r="A43" s="7">
@@ -7067,6 +7126,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="O41:O42"/>
+    <mergeCell ref="I41:I42"/>
+    <mergeCell ref="J41:J42"/>
+    <mergeCell ref="N41:N42"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="S41:T41"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="A33:G33"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B35:G35"/>
     <mergeCell ref="X41:X42"/>
     <mergeCell ref="A41:A42"/>
     <mergeCell ref="B41:B42"/>
@@ -7083,30 +7166,6 @@
     <mergeCell ref="P41:P42"/>
     <mergeCell ref="U41:V41"/>
     <mergeCell ref="Q41:Q42"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="S41:T41"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="A33:G33"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="A27:G27"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B36:G36"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="O41:O42"/>
-    <mergeCell ref="I41:I42"/>
-    <mergeCell ref="J41:J42"/>
-    <mergeCell ref="N41:N42"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="4">
@@ -7342,10 +7401,10 @@
         <v>174</v>
       </c>
       <c r="B12" s="122"/>
-      <c r="C12" s="165" t="s">
+      <c r="C12" s="141" t="s">
         <v>175</v>
       </c>
-      <c r="D12" s="165"/>
+      <c r="D12" s="141"/>
       <c r="E12" s="95" t="s">
         <v>176</v>
       </c>
@@ -7360,10 +7419,10 @@
         <v>226</v>
       </c>
       <c r="B13" s="122"/>
-      <c r="C13" s="164" t="s">
+      <c r="C13" s="142" t="s">
         <v>230</v>
       </c>
-      <c r="D13" s="165"/>
+      <c r="D13" s="141"/>
       <c r="E13" s="55" t="s">
         <v>227</v>
       </c>
@@ -7383,10 +7442,10 @@
         <v>177</v>
       </c>
       <c r="B14" s="122"/>
-      <c r="C14" s="165" t="s">
+      <c r="C14" s="141" t="s">
         <v>178</v>
       </c>
-      <c r="D14" s="165"/>
+      <c r="D14" s="141"/>
       <c r="E14" s="55"/>
       <c r="F14" s="55"/>
       <c r="G14" s="54"/>
@@ -7398,8 +7457,8 @@
         <v>228</v>
       </c>
       <c r="B15" s="122"/>
-      <c r="C15" s="164"/>
-      <c r="D15" s="165"/>
+      <c r="C15" s="142"/>
+      <c r="D15" s="141"/>
       <c r="E15" s="55" t="s">
         <v>229</v>
       </c>
@@ -7447,15 +7506,15 @@
       <c r="L17"/>
     </row>
     <row r="18" spans="1:22">
-      <c r="A18" s="157" t="s">
+      <c r="A18" s="179" t="s">
         <v>192</v>
       </c>
-      <c r="B18" s="157"/>
-      <c r="C18" s="157"/>
-      <c r="D18" s="157"/>
-      <c r="E18" s="157"/>
-      <c r="F18" s="157"/>
-      <c r="G18" s="157"/>
+      <c r="B18" s="179"/>
+      <c r="C18" s="179"/>
+      <c r="D18" s="179"/>
+      <c r="E18" s="179"/>
+      <c r="F18" s="179"/>
+      <c r="G18" s="179"/>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
@@ -7466,14 +7525,14 @@
       <c r="A19" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="151" t="s">
+      <c r="B19" s="173" t="s">
         <v>183</v>
       </c>
-      <c r="C19" s="152"/>
-      <c r="D19" s="152"/>
-      <c r="E19" s="152"/>
-      <c r="F19" s="152"/>
-      <c r="G19" s="153"/>
+      <c r="C19" s="174"/>
+      <c r="D19" s="174"/>
+      <c r="E19" s="174"/>
+      <c r="F19" s="174"/>
+      <c r="G19" s="175"/>
       <c r="H19" s="105"/>
       <c r="I19"/>
       <c r="J19"/>
@@ -7489,12 +7548,12 @@
     </row>
     <row r="20" spans="1:22">
       <c r="A20" s="116"/>
-      <c r="B20" s="168"/>
-      <c r="C20" s="168"/>
-      <c r="D20" s="168"/>
-      <c r="E20" s="168"/>
-      <c r="F20" s="168"/>
-      <c r="G20" s="168"/>
+      <c r="B20" s="157"/>
+      <c r="C20" s="157"/>
+      <c r="D20" s="157"/>
+      <c r="E20" s="157"/>
+      <c r="F20" s="157"/>
+      <c r="G20" s="157"/>
       <c r="H20" s="112"/>
       <c r="I20"/>
       <c r="J20"/>
@@ -7509,12 +7568,12 @@
     </row>
     <row r="21" spans="1:22">
       <c r="A21" s="117"/>
-      <c r="B21" s="169"/>
-      <c r="C21" s="169"/>
-      <c r="D21" s="169"/>
-      <c r="E21" s="169"/>
-      <c r="F21" s="169"/>
-      <c r="G21" s="169"/>
+      <c r="B21" s="159"/>
+      <c r="C21" s="159"/>
+      <c r="D21" s="159"/>
+      <c r="E21" s="159"/>
+      <c r="F21" s="159"/>
+      <c r="G21" s="159"/>
       <c r="H21" s="112"/>
       <c r="I21"/>
       <c r="J21"/>
@@ -7529,12 +7588,12 @@
     </row>
     <row r="22" spans="1:22">
       <c r="A22" s="118"/>
-      <c r="B22" s="170"/>
-      <c r="C22" s="170"/>
-      <c r="D22" s="170"/>
-      <c r="E22" s="170"/>
-      <c r="F22" s="170"/>
-      <c r="G22" s="170"/>
+      <c r="B22" s="161"/>
+      <c r="C22" s="161"/>
+      <c r="D22" s="161"/>
+      <c r="E22" s="161"/>
+      <c r="F22" s="161"/>
+      <c r="G22" s="161"/>
       <c r="H22" s="112"/>
       <c r="I22"/>
       <c r="J22"/>
@@ -7561,15 +7620,15 @@
       <c r="O23" s="112"/>
     </row>
     <row r="24" spans="1:22">
-      <c r="A24" s="154" t="s">
+      <c r="A24" s="176" t="s">
         <v>193</v>
       </c>
-      <c r="B24" s="155"/>
-      <c r="C24" s="155"/>
-      <c r="D24" s="155"/>
-      <c r="E24" s="155"/>
-      <c r="F24" s="155"/>
-      <c r="G24" s="156"/>
+      <c r="B24" s="177"/>
+      <c r="C24" s="177"/>
+      <c r="D24" s="177"/>
+      <c r="E24" s="177"/>
+      <c r="F24" s="177"/>
+      <c r="G24" s="178"/>
       <c r="I24"/>
       <c r="J24"/>
       <c r="K24"/>
@@ -7582,14 +7641,14 @@
       <c r="A25" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B25" s="174" t="s">
+      <c r="B25" s="153" t="s">
         <v>184</v>
       </c>
-      <c r="C25" s="174"/>
-      <c r="D25" s="174"/>
-      <c r="E25" s="174"/>
-      <c r="F25" s="174"/>
-      <c r="G25" s="174"/>
+      <c r="C25" s="153"/>
+      <c r="D25" s="153"/>
+      <c r="E25" s="153"/>
+      <c r="F25" s="153"/>
+      <c r="G25" s="153"/>
       <c r="H25" s="105"/>
       <c r="M25" s="112"/>
       <c r="N25" s="112"/>
@@ -7605,14 +7664,14 @@
       <c r="A26" s="116">
         <v>1</v>
       </c>
-      <c r="B26" s="175" t="s">
+      <c r="B26" s="154" t="s">
         <v>185</v>
       </c>
-      <c r="C26" s="175"/>
-      <c r="D26" s="175"/>
-      <c r="E26" s="175"/>
-      <c r="F26" s="175"/>
-      <c r="G26" s="175"/>
+      <c r="C26" s="154"/>
+      <c r="D26" s="154"/>
+      <c r="E26" s="154"/>
+      <c r="F26" s="154"/>
+      <c r="G26" s="154"/>
       <c r="H26" s="112"/>
       <c r="I26" s="105"/>
       <c r="J26" s="105"/>
@@ -7627,12 +7686,12 @@
     </row>
     <row r="27" spans="1:22">
       <c r="A27" s="117"/>
-      <c r="B27" s="176"/>
-      <c r="C27" s="176"/>
-      <c r="D27" s="176"/>
-      <c r="E27" s="176"/>
-      <c r="F27" s="176"/>
-      <c r="G27" s="176"/>
+      <c r="B27" s="155"/>
+      <c r="C27" s="155"/>
+      <c r="D27" s="155"/>
+      <c r="E27" s="155"/>
+      <c r="F27" s="155"/>
+      <c r="G27" s="155"/>
       <c r="H27" s="112"/>
       <c r="I27" s="105"/>
       <c r="J27" s="105"/>
@@ -7647,12 +7706,12 @@
     </row>
     <row r="28" spans="1:22">
       <c r="A28" s="118"/>
-      <c r="B28" s="177"/>
-      <c r="C28" s="177"/>
-      <c r="D28" s="177"/>
-      <c r="E28" s="177"/>
-      <c r="F28" s="177"/>
-      <c r="G28" s="177"/>
+      <c r="B28" s="156"/>
+      <c r="C28" s="156"/>
+      <c r="D28" s="156"/>
+      <c r="E28" s="156"/>
+      <c r="F28" s="156"/>
+      <c r="G28" s="156"/>
       <c r="H28" s="112"/>
       <c r="I28" s="105"/>
       <c r="J28" s="105"/>
@@ -7691,15 +7750,15 @@
       <c r="T29"/>
     </row>
     <row r="30" spans="1:22">
-      <c r="A30" s="154" t="s">
+      <c r="A30" s="176" t="s">
         <v>194</v>
       </c>
-      <c r="B30" s="155"/>
-      <c r="C30" s="155"/>
-      <c r="D30" s="155"/>
-      <c r="E30" s="155"/>
-      <c r="F30" s="155"/>
-      <c r="G30" s="156"/>
+      <c r="B30" s="177"/>
+      <c r="C30" s="177"/>
+      <c r="D30" s="177"/>
+      <c r="E30" s="177"/>
+      <c r="F30" s="177"/>
+      <c r="G30" s="178"/>
       <c r="M30" s="112"/>
       <c r="N30" s="112"/>
       <c r="O30" s="112"/>
@@ -7708,14 +7767,14 @@
       <c r="A31" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B31" s="174" t="s">
+      <c r="B31" s="153" t="s">
         <v>186</v>
       </c>
-      <c r="C31" s="174"/>
-      <c r="D31" s="174"/>
-      <c r="E31" s="174"/>
-      <c r="F31" s="174"/>
-      <c r="G31" s="174"/>
+      <c r="C31" s="153"/>
+      <c r="D31" s="153"/>
+      <c r="E31" s="153"/>
+      <c r="F31" s="153"/>
+      <c r="G31" s="153"/>
       <c r="H31" s="105"/>
       <c r="I31" s="105"/>
       <c r="J31" s="105"/>
@@ -7733,12 +7792,12 @@
     </row>
     <row r="32" spans="1:22">
       <c r="A32" s="116"/>
-      <c r="B32" s="168"/>
-      <c r="C32" s="168"/>
-      <c r="D32" s="168"/>
-      <c r="E32" s="168"/>
-      <c r="F32" s="168"/>
-      <c r="G32" s="178"/>
+      <c r="B32" s="157"/>
+      <c r="C32" s="157"/>
+      <c r="D32" s="157"/>
+      <c r="E32" s="157"/>
+      <c r="F32" s="157"/>
+      <c r="G32" s="158"/>
       <c r="H32" s="112"/>
       <c r="I32" s="112"/>
       <c r="J32" s="112"/>
@@ -7756,12 +7815,12 @@
     </row>
     <row r="33" spans="1:22">
       <c r="A33" s="117"/>
-      <c r="B33" s="169"/>
-      <c r="C33" s="169"/>
-      <c r="D33" s="169"/>
-      <c r="E33" s="169"/>
-      <c r="F33" s="169"/>
-      <c r="G33" s="179"/>
+      <c r="B33" s="159"/>
+      <c r="C33" s="159"/>
+      <c r="D33" s="159"/>
+      <c r="E33" s="159"/>
+      <c r="F33" s="159"/>
+      <c r="G33" s="160"/>
       <c r="H33" s="112"/>
       <c r="I33" s="112"/>
       <c r="J33" s="112"/>
@@ -7776,12 +7835,12 @@
     </row>
     <row r="34" spans="1:22">
       <c r="A34" s="118"/>
-      <c r="B34" s="170"/>
-      <c r="C34" s="170"/>
-      <c r="D34" s="170"/>
-      <c r="E34" s="170"/>
-      <c r="F34" s="170"/>
-      <c r="G34" s="180"/>
+      <c r="B34" s="161"/>
+      <c r="C34" s="161"/>
+      <c r="D34" s="161"/>
+      <c r="E34" s="161"/>
+      <c r="F34" s="161"/>
+      <c r="G34" s="162"/>
       <c r="H34" s="112"/>
       <c r="I34" s="112"/>
       <c r="J34" s="112"/>
@@ -7851,28 +7910,28 @@
       <c r="U37" s="58"/>
     </row>
     <row r="38" spans="1:22" ht="30" customHeight="1">
-      <c r="A38" s="194" t="s">
+      <c r="A38" s="189" t="s">
         <v>118</v>
       </c>
-      <c r="B38" s="194" t="s">
+      <c r="B38" s="189" t="s">
         <v>119</v>
       </c>
       <c r="C38" s="60" t="s">
         <v>120</v>
       </c>
-      <c r="D38" s="194" t="s">
+      <c r="D38" s="189" t="s">
         <v>101</v>
       </c>
-      <c r="E38" s="194" t="s">
+      <c r="E38" s="189" t="s">
         <v>161</v>
       </c>
-      <c r="F38" s="194" t="s">
+      <c r="F38" s="189" t="s">
         <v>177</v>
       </c>
-      <c r="G38" s="194" t="s">
+      <c r="G38" s="189" t="s">
         <v>140</v>
       </c>
-      <c r="H38" s="194" t="s">
+      <c r="H38" s="189" t="s">
         <v>139</v>
       </c>
       <c r="I38" s="201" t="s">
@@ -7884,16 +7943,16 @@
       <c r="K38" s="203" t="s">
         <v>202</v>
       </c>
-      <c r="L38" s="186" t="s">
+      <c r="L38" s="196" t="s">
         <v>203</v>
       </c>
-      <c r="M38" s="188" t="s">
+      <c r="M38" s="186" t="s">
         <v>195</v>
       </c>
-      <c r="N38" s="188" t="s">
+      <c r="N38" s="186" t="s">
         <v>209</v>
       </c>
-      <c r="O38" s="193" t="s">
+      <c r="O38" s="188" t="s">
         <v>208</v>
       </c>
       <c r="P38" s="199" t="s">
@@ -7907,7 +7966,7 @@
       <c r="T38" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="U38" s="194" t="s">
+      <c r="U38" s="189" t="s">
         <v>125</v>
       </c>
     </row>
@@ -7918,16 +7977,16 @@
         <v>121</v>
       </c>
       <c r="D39" s="198"/>
-      <c r="E39" s="196"/>
-      <c r="F39" s="196"/>
+      <c r="E39" s="191"/>
+      <c r="F39" s="191"/>
       <c r="G39" s="198"/>
       <c r="H39" s="198"/>
       <c r="I39" s="202"/>
       <c r="J39" s="204"/>
       <c r="K39" s="204"/>
-      <c r="L39" s="187"/>
-      <c r="M39" s="189"/>
-      <c r="N39" s="189"/>
+      <c r="L39" s="197"/>
+      <c r="M39" s="192"/>
+      <c r="N39" s="192"/>
       <c r="O39" s="206"/>
       <c r="P39" s="62" t="s">
         <v>126</v>
@@ -8604,26 +8663,6 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="M38:M39"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="A30:G30"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="A24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="A18:G18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C15:D15"/>
     <mergeCell ref="U38:U39"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="B38:B39"/>
@@ -8640,6 +8679,26 @@
     <mergeCell ref="R38:S38"/>
     <mergeCell ref="L38:L39"/>
     <mergeCell ref="O38:O39"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A18:G18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="A24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="M38:M39"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="A30:G30"/>
+    <mergeCell ref="B31:G31"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="3">

</xml_diff>

<commit_message>
0.1.7: Enable interface for telegrams.
</commit_message>
<xml_diff>
--- a/meta/api/BlancoApiPostSample.xlsx
+++ b/meta/api/BlancoApiPostSample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorKt/meta/api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68AA212-DB56-3047-8A06-26F4F6C162F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E114557-C06D-5E45-AEAB-FBFE191C587D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15160" yWindow="1200" windowWidth="21420" windowHeight="17540" tabRatio="860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="249">
   <si>
     <t>項目名</t>
     <rPh sb="0" eb="3">
@@ -2528,6 +2528,20 @@
     </rPh>
     <rPh sb="48" eb="50">
       <t>カノウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>blanco.restgeneratorkt.NoopInteface</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>電文定義(Kt)・実装</t>
+    <rPh sb="0" eb="4">
+      <t xml:space="preserve">デンブンショリテイギ </t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t xml:space="preserve">ジッソウ </t>
     </rPh>
     <phoneticPr fontId="2"/>
   </si>
@@ -3778,6 +3792,138 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="60" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3787,154 +3933,13 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -3950,9 +3955,24 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3979,12 +3999,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -4576,137 +4590,137 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="185" t="s">
+      <c r="A5" s="141" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="185"/>
-      <c r="C5" s="185"/>
-      <c r="D5" s="185"/>
-      <c r="E5" s="185"/>
+      <c r="B5" s="141"/>
+      <c r="C5" s="141"/>
+      <c r="D5" s="141"/>
+      <c r="E5" s="141"/>
       <c r="F5" s="55"/>
       <c r="G5" s="55"/>
       <c r="H5" s="95"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="182" t="s">
+      <c r="A6" s="145" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="183"/>
-      <c r="C6" s="184"/>
-      <c r="D6" s="181" t="s">
+      <c r="B6" s="146"/>
+      <c r="C6" s="147"/>
+      <c r="D6" s="142" t="s">
         <v>197</v>
       </c>
-      <c r="E6" s="181"/>
+      <c r="E6" s="142"/>
       <c r="F6" s="55"/>
       <c r="G6" s="55"/>
       <c r="H6" s="95"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="185" t="s">
+      <c r="A7" s="141" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="185"/>
-      <c r="C7" s="185"/>
-      <c r="D7" s="181" t="s">
+      <c r="B7" s="141"/>
+      <c r="C7" s="141"/>
+      <c r="D7" s="142" t="s">
         <v>166</v>
       </c>
-      <c r="E7" s="181"/>
+      <c r="E7" s="142"/>
       <c r="F7" s="55"/>
       <c r="G7" s="55"/>
       <c r="H7" s="95"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="185" t="s">
+      <c r="A8" s="141" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="185"/>
-      <c r="C8" s="185"/>
-      <c r="D8" s="181" t="s">
+      <c r="B8" s="141"/>
+      <c r="C8" s="141"/>
+      <c r="D8" s="142" t="s">
         <v>162</v>
       </c>
-      <c r="E8" s="181"/>
+      <c r="E8" s="142"/>
       <c r="F8" s="95"/>
       <c r="G8" s="95"/>
       <c r="H8" s="95"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="185" t="s">
+      <c r="A9" s="141" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="185"/>
-      <c r="C9" s="185"/>
-      <c r="D9" s="181" t="s">
+      <c r="B9" s="141"/>
+      <c r="C9" s="141"/>
+      <c r="D9" s="142" t="s">
         <v>100</v>
       </c>
-      <c r="E9" s="181"/>
+      <c r="E9" s="142"/>
       <c r="F9" s="95"/>
       <c r="G9" s="95"/>
       <c r="H9" s="95"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="185" t="s">
+      <c r="A10" s="141" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="185"/>
-      <c r="C10" s="185"/>
-      <c r="D10" s="181"/>
-      <c r="E10" s="181"/>
+      <c r="B10" s="141"/>
+      <c r="C10" s="141"/>
+      <c r="D10" s="142"/>
+      <c r="E10" s="142"/>
       <c r="F10" s="95"/>
       <c r="G10" s="95"/>
       <c r="H10" s="95"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="185" t="s">
+      <c r="A11" s="141" t="s">
         <v>99</v>
       </c>
-      <c r="B11" s="185"/>
-      <c r="C11" s="185"/>
-      <c r="D11" s="181" t="s">
+      <c r="B11" s="141"/>
+      <c r="C11" s="141"/>
+      <c r="D11" s="142" t="s">
         <v>163</v>
       </c>
-      <c r="E11" s="181"/>
+      <c r="E11" s="142"/>
       <c r="F11" s="95"/>
       <c r="G11" s="95"/>
       <c r="H11" s="95"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="147" t="s">
+      <c r="A12" s="148" t="s">
         <v>174</v>
       </c>
-      <c r="B12" s="147"/>
-      <c r="C12" s="147"/>
-      <c r="D12" s="165" t="s">
+      <c r="B12" s="148"/>
+      <c r="C12" s="148"/>
+      <c r="D12" s="143" t="s">
         <v>175</v>
       </c>
-      <c r="E12" s="165"/>
+      <c r="E12" s="143"/>
       <c r="F12" s="95" t="s">
         <v>176</v>
       </c>
       <c r="G12" s="54"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="147" t="s">
+      <c r="A13" s="148" t="s">
         <v>212</v>
       </c>
-      <c r="B13" s="147"/>
-      <c r="C13" s="147"/>
-      <c r="D13" s="165" t="s">
+      <c r="B13" s="148"/>
+      <c r="C13" s="148"/>
+      <c r="D13" s="143" t="s">
         <v>210</v>
       </c>
-      <c r="E13" s="165"/>
+      <c r="E13" s="143"/>
       <c r="F13" s="95" t="s">
         <v>211</v>
       </c>
       <c r="G13" s="54"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="147" t="s">
+      <c r="A14" s="148" t="s">
         <v>177</v>
       </c>
-      <c r="B14" s="147"/>
-      <c r="C14" s="147"/>
-      <c r="D14" s="164"/>
-      <c r="E14" s="165"/>
+      <c r="B14" s="148"/>
+      <c r="C14" s="148"/>
+      <c r="D14" s="144"/>
+      <c r="E14" s="143"/>
       <c r="F14" s="54" t="s">
         <v>198</v>
       </c>
@@ -4714,15 +4728,15 @@
       <c r="H14" s="95"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="147" t="s">
+      <c r="A15" s="148" t="s">
         <v>217</v>
       </c>
-      <c r="B15" s="147"/>
-      <c r="C15" s="147"/>
-      <c r="D15" s="164" t="s">
+      <c r="B15" s="148"/>
+      <c r="C15" s="148"/>
+      <c r="D15" s="144" t="s">
         <v>215</v>
       </c>
-      <c r="E15" s="165"/>
+      <c r="E15" s="143"/>
       <c r="F15" s="54" t="s">
         <v>220</v>
       </c>
@@ -4730,13 +4744,13 @@
       <c r="H15" s="95"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="147" t="s">
+      <c r="A16" s="148" t="s">
         <v>216</v>
       </c>
-      <c r="B16" s="147"/>
-      <c r="C16" s="147"/>
-      <c r="D16" s="164"/>
-      <c r="E16" s="165"/>
+      <c r="B16" s="148"/>
+      <c r="C16" s="148"/>
+      <c r="D16" s="144"/>
+      <c r="E16" s="143"/>
       <c r="F16" s="54" t="s">
         <v>219</v>
       </c>
@@ -4744,13 +4758,13 @@
       <c r="H16" s="95"/>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="147" t="s">
+      <c r="A17" s="148" t="s">
         <v>214</v>
       </c>
-      <c r="B17" s="147"/>
-      <c r="C17" s="147"/>
-      <c r="D17" s="164"/>
-      <c r="E17" s="165"/>
+      <c r="B17" s="148"/>
+      <c r="C17" s="148"/>
+      <c r="D17" s="144"/>
+      <c r="E17" s="143"/>
       <c r="F17" s="54" t="s">
         <v>213</v>
       </c>
@@ -4758,15 +4772,15 @@
       <c r="H17" s="95"/>
     </row>
     <row r="18" spans="1:15">
-      <c r="A18" s="147" t="s">
+      <c r="A18" s="148" t="s">
         <v>238</v>
       </c>
-      <c r="B18" s="147"/>
-      <c r="C18" s="147"/>
-      <c r="D18" s="164" t="s">
+      <c r="B18" s="148"/>
+      <c r="C18" s="148"/>
+      <c r="D18" s="144" t="s">
         <v>240</v>
       </c>
-      <c r="E18" s="165"/>
+      <c r="E18" s="143"/>
       <c r="F18" s="54" t="s">
         <v>239</v>
       </c>
@@ -4774,11 +4788,11 @@
       <c r="H18" s="95"/>
     </row>
     <row r="19" spans="1:15">
-      <c r="A19" s="139" t="s">
+      <c r="A19" s="183" t="s">
         <v>143</v>
       </c>
-      <c r="B19" s="140"/>
-      <c r="C19" s="141"/>
+      <c r="B19" s="184"/>
+      <c r="C19" s="185"/>
       <c r="D19" s="114" t="s">
         <v>141</v>
       </c>
@@ -4787,11 +4801,11 @@
       </c>
     </row>
     <row r="20" spans="1:15">
-      <c r="A20" s="139" t="s">
+      <c r="A20" s="183" t="s">
         <v>243</v>
       </c>
-      <c r="B20" s="140"/>
-      <c r="C20" s="141"/>
+      <c r="B20" s="184"/>
+      <c r="C20" s="185"/>
       <c r="D20" s="114" t="s">
         <v>141</v>
       </c>
@@ -4800,11 +4814,11 @@
       </c>
     </row>
     <row r="21" spans="1:15">
-      <c r="A21" s="148" t="s">
+      <c r="A21" s="168" t="s">
         <v>179</v>
       </c>
-      <c r="B21" s="149"/>
-      <c r="C21" s="150"/>
+      <c r="B21" s="169"/>
+      <c r="C21" s="170"/>
       <c r="D21" s="100"/>
       <c r="E21" t="s">
         <v>180</v>
@@ -4822,15 +4836,15 @@
       <c r="B22" s="6"/>
     </row>
     <row r="23" spans="1:15">
-      <c r="A23" s="161" t="s">
+      <c r="A23" s="180" t="s">
         <v>188</v>
       </c>
-      <c r="B23" s="162"/>
-      <c r="C23" s="162"/>
-      <c r="D23" s="162"/>
-      <c r="E23" s="162"/>
-      <c r="F23" s="162"/>
-      <c r="G23" s="163"/>
+      <c r="B23" s="181"/>
+      <c r="C23" s="181"/>
+      <c r="D23" s="181"/>
+      <c r="E23" s="181"/>
+      <c r="F23" s="181"/>
+      <c r="G23" s="182"/>
       <c r="H23" s="1" t="s">
         <v>223</v>
       </c>
@@ -4881,28 +4895,28 @@
       <c r="C27"/>
     </row>
     <row r="28" spans="1:15">
-      <c r="A28" s="160" t="s">
+      <c r="A28" s="179" t="s">
         <v>189</v>
       </c>
-      <c r="B28" s="160"/>
-      <c r="C28" s="160"/>
-      <c r="D28" s="160"/>
-      <c r="E28" s="160"/>
-      <c r="F28" s="160"/>
-      <c r="G28" s="160"/>
+      <c r="B28" s="179"/>
+      <c r="C28" s="179"/>
+      <c r="D28" s="179"/>
+      <c r="E28" s="179"/>
+      <c r="F28" s="179"/>
+      <c r="G28" s="179"/>
     </row>
     <row r="29" spans="1:15">
       <c r="A29" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="154" t="s">
+      <c r="B29" s="173" t="s">
         <v>183</v>
       </c>
-      <c r="C29" s="155"/>
-      <c r="D29" s="155"/>
-      <c r="E29" s="155"/>
-      <c r="F29" s="155"/>
-      <c r="G29" s="156"/>
+      <c r="C29" s="174"/>
+      <c r="D29" s="174"/>
+      <c r="E29" s="174"/>
+      <c r="F29" s="174"/>
+      <c r="G29" s="175"/>
       <c r="H29" s="105"/>
       <c r="I29" s="105"/>
       <c r="J29" s="105"/>
@@ -4913,12 +4927,12 @@
     </row>
     <row r="30" spans="1:15">
       <c r="A30" s="116"/>
-      <c r="B30" s="168"/>
-      <c r="C30" s="168"/>
-      <c r="D30" s="168"/>
-      <c r="E30" s="168"/>
-      <c r="F30" s="168"/>
-      <c r="G30" s="168"/>
+      <c r="B30" s="159"/>
+      <c r="C30" s="159"/>
+      <c r="D30" s="159"/>
+      <c r="E30" s="159"/>
+      <c r="F30" s="159"/>
+      <c r="G30" s="159"/>
       <c r="H30" s="112"/>
       <c r="I30" s="112"/>
       <c r="J30" s="112"/>
@@ -4929,12 +4943,12 @@
     </row>
     <row r="31" spans="1:15">
       <c r="A31" s="117"/>
-      <c r="B31" s="169"/>
-      <c r="C31" s="169"/>
-      <c r="D31" s="169"/>
-      <c r="E31" s="169"/>
-      <c r="F31" s="169"/>
-      <c r="G31" s="169"/>
+      <c r="B31" s="161"/>
+      <c r="C31" s="161"/>
+      <c r="D31" s="161"/>
+      <c r="E31" s="161"/>
+      <c r="F31" s="161"/>
+      <c r="G31" s="161"/>
       <c r="H31" s="112"/>
       <c r="I31" s="112"/>
       <c r="J31" s="112"/>
@@ -4945,12 +4959,12 @@
     </row>
     <row r="32" spans="1:15">
       <c r="A32" s="118"/>
-      <c r="B32" s="170"/>
-      <c r="C32" s="170"/>
-      <c r="D32" s="170"/>
-      <c r="E32" s="170"/>
-      <c r="F32" s="170"/>
-      <c r="G32" s="170"/>
+      <c r="B32" s="163"/>
+      <c r="C32" s="163"/>
+      <c r="D32" s="163"/>
+      <c r="E32" s="163"/>
+      <c r="F32" s="163"/>
+      <c r="G32" s="163"/>
       <c r="H32" s="112"/>
       <c r="I32" s="112"/>
       <c r="J32" s="112"/>
@@ -4963,28 +4977,28 @@
       <c r="C33"/>
     </row>
     <row r="34" spans="1:15">
-      <c r="A34" s="157" t="s">
+      <c r="A34" s="176" t="s">
         <v>190</v>
       </c>
-      <c r="B34" s="158"/>
-      <c r="C34" s="158"/>
-      <c r="D34" s="158"/>
-      <c r="E34" s="158"/>
-      <c r="F34" s="158"/>
-      <c r="G34" s="159"/>
+      <c r="B34" s="177"/>
+      <c r="C34" s="177"/>
+      <c r="D34" s="177"/>
+      <c r="E34" s="177"/>
+      <c r="F34" s="177"/>
+      <c r="G34" s="178"/>
     </row>
     <row r="35" spans="1:15">
       <c r="A35" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B35" s="174" t="s">
+      <c r="B35" s="155" t="s">
         <v>184</v>
       </c>
-      <c r="C35" s="174"/>
-      <c r="D35" s="174"/>
-      <c r="E35" s="174"/>
-      <c r="F35" s="174"/>
-      <c r="G35" s="174"/>
+      <c r="C35" s="155"/>
+      <c r="D35" s="155"/>
+      <c r="E35" s="155"/>
+      <c r="F35" s="155"/>
+      <c r="G35" s="155"/>
       <c r="H35" s="105"/>
       <c r="I35" s="105"/>
       <c r="J35" s="105"/>
@@ -4997,14 +5011,14 @@
       <c r="A36" s="116">
         <v>1</v>
       </c>
-      <c r="B36" s="175" t="s">
+      <c r="B36" s="156" t="s">
         <v>218</v>
       </c>
-      <c r="C36" s="175"/>
-      <c r="D36" s="175"/>
-      <c r="E36" s="175"/>
-      <c r="F36" s="175"/>
-      <c r="G36" s="175"/>
+      <c r="C36" s="156"/>
+      <c r="D36" s="156"/>
+      <c r="E36" s="156"/>
+      <c r="F36" s="156"/>
+      <c r="G36" s="156"/>
       <c r="H36" s="112"/>
       <c r="I36" s="112"/>
       <c r="J36" s="112"/>
@@ -5015,12 +5029,12 @@
     </row>
     <row r="37" spans="1:15">
       <c r="A37" s="117"/>
-      <c r="B37" s="176"/>
-      <c r="C37" s="176"/>
-      <c r="D37" s="176"/>
-      <c r="E37" s="176"/>
-      <c r="F37" s="176"/>
-      <c r="G37" s="176"/>
+      <c r="B37" s="157"/>
+      <c r="C37" s="157"/>
+      <c r="D37" s="157"/>
+      <c r="E37" s="157"/>
+      <c r="F37" s="157"/>
+      <c r="G37" s="157"/>
       <c r="H37" s="112"/>
       <c r="I37" s="112"/>
       <c r="J37" s="112"/>
@@ -5031,12 +5045,12 @@
     </row>
     <row r="38" spans="1:15">
       <c r="A38" s="118"/>
-      <c r="B38" s="177"/>
-      <c r="C38" s="177"/>
-      <c r="D38" s="177"/>
-      <c r="E38" s="177"/>
-      <c r="F38" s="177"/>
-      <c r="G38" s="177"/>
+      <c r="B38" s="158"/>
+      <c r="C38" s="158"/>
+      <c r="D38" s="158"/>
+      <c r="E38" s="158"/>
+      <c r="F38" s="158"/>
+      <c r="G38" s="158"/>
       <c r="H38" s="112"/>
       <c r="I38" s="112"/>
       <c r="J38" s="112"/>
@@ -5061,28 +5075,28 @@
       <c r="M39"/>
     </row>
     <row r="40" spans="1:15">
-      <c r="A40" s="157" t="s">
+      <c r="A40" s="176" t="s">
         <v>191</v>
       </c>
-      <c r="B40" s="158"/>
-      <c r="C40" s="158"/>
-      <c r="D40" s="158"/>
-      <c r="E40" s="158"/>
-      <c r="F40" s="158"/>
-      <c r="G40" s="159"/>
+      <c r="B40" s="177"/>
+      <c r="C40" s="177"/>
+      <c r="D40" s="177"/>
+      <c r="E40" s="177"/>
+      <c r="F40" s="177"/>
+      <c r="G40" s="178"/>
     </row>
     <row r="41" spans="1:15">
       <c r="A41" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B41" s="174" t="s">
+      <c r="B41" s="155" t="s">
         <v>186</v>
       </c>
-      <c r="C41" s="174"/>
-      <c r="D41" s="174"/>
-      <c r="E41" s="174"/>
-      <c r="F41" s="174"/>
-      <c r="G41" s="174"/>
+      <c r="C41" s="155"/>
+      <c r="D41" s="155"/>
+      <c r="E41" s="155"/>
+      <c r="F41" s="155"/>
+      <c r="G41" s="155"/>
       <c r="H41" s="105"/>
       <c r="I41" s="105"/>
       <c r="J41" s="105"/>
@@ -5093,12 +5107,12 @@
     </row>
     <row r="42" spans="1:15">
       <c r="A42" s="116"/>
-      <c r="B42" s="168"/>
-      <c r="C42" s="168"/>
-      <c r="D42" s="168"/>
-      <c r="E42" s="168"/>
-      <c r="F42" s="168"/>
-      <c r="G42" s="178"/>
+      <c r="B42" s="159"/>
+      <c r="C42" s="159"/>
+      <c r="D42" s="159"/>
+      <c r="E42" s="159"/>
+      <c r="F42" s="159"/>
+      <c r="G42" s="160"/>
       <c r="H42" s="112"/>
       <c r="I42" s="112"/>
       <c r="J42" s="112"/>
@@ -5109,12 +5123,12 @@
     </row>
     <row r="43" spans="1:15">
       <c r="A43" s="117"/>
-      <c r="B43" s="169"/>
-      <c r="C43" s="169"/>
-      <c r="D43" s="169"/>
-      <c r="E43" s="169"/>
-      <c r="F43" s="169"/>
-      <c r="G43" s="179"/>
+      <c r="B43" s="161"/>
+      <c r="C43" s="161"/>
+      <c r="D43" s="161"/>
+      <c r="E43" s="161"/>
+      <c r="F43" s="161"/>
+      <c r="G43" s="162"/>
       <c r="H43" s="112"/>
       <c r="I43" s="112"/>
       <c r="J43" s="112"/>
@@ -5125,12 +5139,12 @@
     </row>
     <row r="44" spans="1:15">
       <c r="A44" s="118"/>
-      <c r="B44" s="170"/>
-      <c r="C44" s="170"/>
-      <c r="D44" s="170"/>
-      <c r="E44" s="170"/>
-      <c r="F44" s="170"/>
-      <c r="G44" s="180"/>
+      <c r="B44" s="163"/>
+      <c r="C44" s="163"/>
+      <c r="D44" s="163"/>
+      <c r="E44" s="163"/>
+      <c r="F44" s="163"/>
+      <c r="G44" s="164"/>
       <c r="H44" s="112"/>
       <c r="I44" s="112"/>
       <c r="J44" s="112"/>
@@ -5165,226 +5179,298 @@
       <c r="F46" s="5"/>
     </row>
     <row r="47" spans="1:15">
-      <c r="A47" s="144" t="s">
+      <c r="A47" s="171" t="s">
         <v>65</v>
       </c>
-      <c r="B47" s="151"/>
-      <c r="C47" s="144" t="s">
+      <c r="B47" s="172"/>
+      <c r="C47" s="171" t="s">
         <v>66</v>
       </c>
-      <c r="D47" s="145"/>
-      <c r="E47" s="146"/>
+      <c r="D47" s="186"/>
+      <c r="E47" s="187"/>
       <c r="F47" s="29" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="48" spans="1:15">
-      <c r="A48" s="152"/>
-      <c r="B48" s="153"/>
-      <c r="C48" s="152"/>
-      <c r="D48" s="171"/>
-      <c r="E48" s="153"/>
+      <c r="A48" s="165"/>
+      <c r="B48" s="167"/>
+      <c r="C48" s="165"/>
+      <c r="D48" s="166"/>
+      <c r="E48" s="167"/>
       <c r="F48" s="49"/>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="142"/>
-      <c r="B49" s="143"/>
-      <c r="C49" s="142"/>
-      <c r="D49" s="172"/>
-      <c r="E49" s="143"/>
+      <c r="A49" s="149"/>
+      <c r="B49" s="151"/>
+      <c r="C49" s="149"/>
+      <c r="D49" s="150"/>
+      <c r="E49" s="151"/>
       <c r="F49" s="49"/>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="142"/>
-      <c r="B50" s="143"/>
-      <c r="C50" s="142"/>
-      <c r="D50" s="172"/>
-      <c r="E50" s="143"/>
+      <c r="A50" s="149"/>
+      <c r="B50" s="151"/>
+      <c r="C50" s="149"/>
+      <c r="D50" s="150"/>
+      <c r="E50" s="151"/>
       <c r="F50" s="49"/>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="142"/>
-      <c r="B51" s="143"/>
-      <c r="C51" s="142"/>
-      <c r="D51" s="172"/>
-      <c r="E51" s="143"/>
+      <c r="A51" s="149"/>
+      <c r="B51" s="151"/>
+      <c r="C51" s="149"/>
+      <c r="D51" s="150"/>
+      <c r="E51" s="151"/>
       <c r="F51" s="49"/>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="142"/>
-      <c r="B52" s="143"/>
-      <c r="C52" s="142"/>
-      <c r="D52" s="172"/>
-      <c r="E52" s="143"/>
+      <c r="A52" s="149"/>
+      <c r="B52" s="151"/>
+      <c r="C52" s="149"/>
+      <c r="D52" s="150"/>
+      <c r="E52" s="151"/>
       <c r="F52" s="49"/>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="142"/>
-      <c r="B53" s="143"/>
-      <c r="C53" s="142"/>
-      <c r="D53" s="172"/>
-      <c r="E53" s="143"/>
+      <c r="A53" s="149"/>
+      <c r="B53" s="151"/>
+      <c r="C53" s="149"/>
+      <c r="D53" s="150"/>
+      <c r="E53" s="151"/>
       <c r="F53" s="49"/>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="142"/>
-      <c r="B54" s="143"/>
-      <c r="C54" s="142"/>
-      <c r="D54" s="172"/>
-      <c r="E54" s="143"/>
+      <c r="A54" s="149"/>
+      <c r="B54" s="151"/>
+      <c r="C54" s="149"/>
+      <c r="D54" s="150"/>
+      <c r="E54" s="151"/>
       <c r="F54" s="49"/>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="142"/>
-      <c r="B55" s="143"/>
-      <c r="C55" s="142"/>
-      <c r="D55" s="172"/>
-      <c r="E55" s="143"/>
+      <c r="A55" s="149"/>
+      <c r="B55" s="151"/>
+      <c r="C55" s="149"/>
+      <c r="D55" s="150"/>
+      <c r="E55" s="151"/>
       <c r="F55" s="49"/>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="142"/>
-      <c r="B56" s="143"/>
-      <c r="C56" s="142"/>
-      <c r="D56" s="172"/>
-      <c r="E56" s="143"/>
+      <c r="A56" s="149"/>
+      <c r="B56" s="151"/>
+      <c r="C56" s="149"/>
+      <c r="D56" s="150"/>
+      <c r="E56" s="151"/>
       <c r="F56" s="49"/>
     </row>
     <row r="57" spans="1:6">
-      <c r="A57" s="142"/>
-      <c r="B57" s="143"/>
-      <c r="C57" s="142"/>
-      <c r="D57" s="172"/>
-      <c r="E57" s="143"/>
+      <c r="A57" s="149"/>
+      <c r="B57" s="151"/>
+      <c r="C57" s="149"/>
+      <c r="D57" s="150"/>
+      <c r="E57" s="151"/>
       <c r="F57" s="49"/>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="142"/>
-      <c r="B58" s="143"/>
-      <c r="C58" s="142"/>
-      <c r="D58" s="172"/>
-      <c r="E58" s="143"/>
+      <c r="A58" s="149"/>
+      <c r="B58" s="151"/>
+      <c r="C58" s="149"/>
+      <c r="D58" s="150"/>
+      <c r="E58" s="151"/>
       <c r="F58" s="49"/>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="142"/>
-      <c r="B59" s="143"/>
-      <c r="C59" s="142"/>
-      <c r="D59" s="172"/>
-      <c r="E59" s="143"/>
+      <c r="A59" s="149"/>
+      <c r="B59" s="151"/>
+      <c r="C59" s="149"/>
+      <c r="D59" s="150"/>
+      <c r="E59" s="151"/>
       <c r="F59" s="49"/>
     </row>
     <row r="60" spans="1:6">
-      <c r="A60" s="142"/>
-      <c r="B60" s="143"/>
-      <c r="C60" s="142"/>
-      <c r="D60" s="172"/>
-      <c r="E60" s="143"/>
+      <c r="A60" s="149"/>
+      <c r="B60" s="151"/>
+      <c r="C60" s="149"/>
+      <c r="D60" s="150"/>
+      <c r="E60" s="151"/>
       <c r="F60" s="49"/>
     </row>
     <row r="61" spans="1:6">
-      <c r="A61" s="142"/>
-      <c r="B61" s="143"/>
-      <c r="C61" s="142"/>
-      <c r="D61" s="172"/>
-      <c r="E61" s="143"/>
+      <c r="A61" s="149"/>
+      <c r="B61" s="151"/>
+      <c r="C61" s="149"/>
+      <c r="D61" s="150"/>
+      <c r="E61" s="151"/>
       <c r="F61" s="49"/>
     </row>
     <row r="62" spans="1:6">
-      <c r="A62" s="142"/>
-      <c r="B62" s="143"/>
-      <c r="C62" s="142"/>
-      <c r="D62" s="172"/>
-      <c r="E62" s="143"/>
+      <c r="A62" s="149"/>
+      <c r="B62" s="151"/>
+      <c r="C62" s="149"/>
+      <c r="D62" s="150"/>
+      <c r="E62" s="151"/>
       <c r="F62" s="49"/>
     </row>
     <row r="63" spans="1:6">
-      <c r="A63" s="142"/>
-      <c r="B63" s="143"/>
-      <c r="C63" s="142"/>
-      <c r="D63" s="172"/>
-      <c r="E63" s="143"/>
+      <c r="A63" s="149"/>
+      <c r="B63" s="151"/>
+      <c r="C63" s="149"/>
+      <c r="D63" s="150"/>
+      <c r="E63" s="151"/>
       <c r="F63" s="49"/>
     </row>
     <row r="64" spans="1:6">
-      <c r="A64" s="142"/>
-      <c r="B64" s="143"/>
-      <c r="C64" s="142"/>
-      <c r="D64" s="172"/>
-      <c r="E64" s="143"/>
+      <c r="A64" s="149"/>
+      <c r="B64" s="151"/>
+      <c r="C64" s="149"/>
+      <c r="D64" s="150"/>
+      <c r="E64" s="151"/>
       <c r="F64" s="49"/>
     </row>
     <row r="65" spans="1:6">
-      <c r="A65" s="142"/>
-      <c r="B65" s="143"/>
-      <c r="C65" s="142"/>
-      <c r="D65" s="172"/>
-      <c r="E65" s="143"/>
+      <c r="A65" s="149"/>
+      <c r="B65" s="151"/>
+      <c r="C65" s="149"/>
+      <c r="D65" s="150"/>
+      <c r="E65" s="151"/>
       <c r="F65" s="49"/>
     </row>
     <row r="66" spans="1:6">
-      <c r="A66" s="142"/>
-      <c r="B66" s="143"/>
-      <c r="C66" s="142"/>
-      <c r="D66" s="172"/>
-      <c r="E66" s="143"/>
+      <c r="A66" s="149"/>
+      <c r="B66" s="151"/>
+      <c r="C66" s="149"/>
+      <c r="D66" s="150"/>
+      <c r="E66" s="151"/>
       <c r="F66" s="49"/>
     </row>
     <row r="67" spans="1:6">
-      <c r="A67" s="142"/>
-      <c r="B67" s="143"/>
-      <c r="C67" s="142"/>
-      <c r="D67" s="172"/>
-      <c r="E67" s="143"/>
+      <c r="A67" s="149"/>
+      <c r="B67" s="151"/>
+      <c r="C67" s="149"/>
+      <c r="D67" s="150"/>
+      <c r="E67" s="151"/>
       <c r="F67" s="49"/>
     </row>
     <row r="68" spans="1:6">
-      <c r="A68" s="142"/>
-      <c r="B68" s="143"/>
-      <c r="C68" s="142"/>
-      <c r="D68" s="172"/>
-      <c r="E68" s="143"/>
+      <c r="A68" s="149"/>
+      <c r="B68" s="151"/>
+      <c r="C68" s="149"/>
+      <c r="D68" s="150"/>
+      <c r="E68" s="151"/>
       <c r="F68" s="49"/>
     </row>
     <row r="69" spans="1:6">
-      <c r="A69" s="142"/>
-      <c r="B69" s="143"/>
-      <c r="C69" s="142"/>
-      <c r="D69" s="172"/>
-      <c r="E69" s="143"/>
+      <c r="A69" s="149"/>
+      <c r="B69" s="151"/>
+      <c r="C69" s="149"/>
+      <c r="D69" s="150"/>
+      <c r="E69" s="151"/>
       <c r="F69" s="49"/>
     </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="142"/>
-      <c r="B70" s="143"/>
-      <c r="C70" s="142"/>
-      <c r="D70" s="172"/>
-      <c r="E70" s="143"/>
+      <c r="A70" s="149"/>
+      <c r="B70" s="151"/>
+      <c r="C70" s="149"/>
+      <c r="D70" s="150"/>
+      <c r="E70" s="151"/>
       <c r="F70" s="49"/>
     </row>
     <row r="71" spans="1:6">
-      <c r="A71" s="142"/>
-      <c r="B71" s="143"/>
-      <c r="C71" s="142"/>
-      <c r="D71" s="172"/>
-      <c r="E71" s="143"/>
+      <c r="A71" s="149"/>
+      <c r="B71" s="151"/>
+      <c r="C71" s="149"/>
+      <c r="D71" s="150"/>
+      <c r="E71" s="151"/>
       <c r="F71" s="49"/>
     </row>
     <row r="72" spans="1:6">
-      <c r="A72" s="166"/>
-      <c r="B72" s="167"/>
-      <c r="C72" s="166"/>
-      <c r="D72" s="173"/>
-      <c r="E72" s="167"/>
+      <c r="A72" s="152"/>
+      <c r="B72" s="154"/>
+      <c r="C72" s="152"/>
+      <c r="D72" s="153"/>
+      <c r="E72" s="154"/>
       <c r="F72" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="98">
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="A40:G40"/>
+    <mergeCell ref="A28:G28"/>
+    <mergeCell ref="A23:G23"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="C71:E71"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="B41:G41"/>
+    <mergeCell ref="B42:G42"/>
+    <mergeCell ref="B43:G43"/>
+    <mergeCell ref="B44:G44"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C70:E70"/>
+    <mergeCell ref="C61:E61"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D13:E13"/>
@@ -5401,83 +5487,11 @@
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="A16:C16"/>
     <mergeCell ref="D16:E16"/>
-    <mergeCell ref="C71:E71"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B36:G36"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="B41:G41"/>
-    <mergeCell ref="B42:G42"/>
-    <mergeCell ref="B43:G43"/>
-    <mergeCell ref="B44:G44"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="C70:E70"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="C51:E51"/>
-    <mergeCell ref="C52:E52"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="A34:G34"/>
-    <mergeCell ref="A40:G40"/>
-    <mergeCell ref="A28:G28"/>
-    <mergeCell ref="A23:G23"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="1">
@@ -5512,8 +5526,8 @@
   </sheetPr>
   <dimension ref="A1:AC67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -5762,10 +5776,10 @@
         <v>174</v>
       </c>
       <c r="B15" s="122"/>
-      <c r="C15" s="165" t="s">
+      <c r="C15" s="143" t="s">
         <v>175</v>
       </c>
-      <c r="D15" s="165"/>
+      <c r="D15" s="143"/>
       <c r="E15" s="95" t="s">
         <v>176</v>
       </c>
@@ -5780,10 +5794,10 @@
         <v>226</v>
       </c>
       <c r="B16" s="122"/>
-      <c r="C16" s="164" t="s">
+      <c r="C16" s="144" t="s">
         <v>230</v>
       </c>
-      <c r="D16" s="165"/>
+      <c r="D16" s="143"/>
       <c r="E16" s="55" t="s">
         <v>227</v>
       </c>
@@ -5806,10 +5820,10 @@
         <v>177</v>
       </c>
       <c r="B17" s="122"/>
-      <c r="C17" s="165" t="s">
+      <c r="C17" s="143" t="s">
         <v>178</v>
       </c>
-      <c r="D17" s="165"/>
+      <c r="D17" s="143"/>
       <c r="E17" s="55"/>
       <c r="F17" s="55"/>
       <c r="G17" s="54"/>
@@ -5821,8 +5835,8 @@
         <v>228</v>
       </c>
       <c r="B18" s="122"/>
-      <c r="C18" s="164"/>
-      <c r="D18" s="165"/>
+      <c r="C18" s="144"/>
+      <c r="D18" s="143"/>
       <c r="E18" s="55" t="s">
         <v>229</v>
       </c>
@@ -5870,10 +5884,10 @@
       <c r="V19"/>
     </row>
     <row r="20" spans="1:25">
-      <c r="A20" s="207" t="s">
+      <c r="A20" s="139" t="s">
         <v>244</v>
       </c>
-      <c r="B20" s="208"/>
+      <c r="B20" s="140"/>
       <c r="C20" s="100" t="s">
         <v>245</v>
       </c>
@@ -5907,15 +5921,15 @@
       <c r="O21"/>
     </row>
     <row r="22" spans="1:25">
-      <c r="A22" s="160" t="s">
-        <v>192</v>
-      </c>
-      <c r="B22" s="160"/>
-      <c r="C22" s="160"/>
-      <c r="D22" s="160"/>
-      <c r="E22" s="160"/>
-      <c r="F22" s="160"/>
-      <c r="G22" s="160"/>
+      <c r="A22" s="179" t="s">
+        <v>248</v>
+      </c>
+      <c r="B22" s="179"/>
+      <c r="C22" s="179"/>
+      <c r="D22" s="179"/>
+      <c r="E22" s="179"/>
+      <c r="F22" s="179"/>
+      <c r="G22" s="179"/>
       <c r="K22"/>
       <c r="L22"/>
       <c r="M22"/>
@@ -5925,14 +5939,14 @@
       <c r="A23" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B23" s="154" t="s">
+      <c r="B23" s="173" t="s">
         <v>183</v>
       </c>
-      <c r="C23" s="155"/>
-      <c r="D23" s="155"/>
-      <c r="E23" s="155"/>
-      <c r="F23" s="155"/>
-      <c r="G23" s="156"/>
+      <c r="C23" s="174"/>
+      <c r="D23" s="174"/>
+      <c r="E23" s="174"/>
+      <c r="F23" s="174"/>
+      <c r="G23" s="175"/>
       <c r="H23" s="105"/>
       <c r="I23" s="105"/>
       <c r="J23" s="105"/>
@@ -5952,13 +5966,17 @@
       <c r="Y23" s="111"/>
     </row>
     <row r="24" spans="1:25">
-      <c r="A24" s="116"/>
-      <c r="B24" s="168"/>
-      <c r="C24" s="168"/>
-      <c r="D24" s="168"/>
-      <c r="E24" s="168"/>
-      <c r="F24" s="168"/>
-      <c r="G24" s="168"/>
+      <c r="A24" s="116">
+        <v>1</v>
+      </c>
+      <c r="B24" s="156" t="s">
+        <v>247</v>
+      </c>
+      <c r="C24" s="156"/>
+      <c r="D24" s="156"/>
+      <c r="E24" s="156"/>
+      <c r="F24" s="156"/>
+      <c r="G24" s="156"/>
       <c r="H24" s="112"/>
       <c r="I24" s="112"/>
       <c r="J24" s="112"/>
@@ -5979,12 +5997,12 @@
     </row>
     <row r="25" spans="1:25">
       <c r="A25" s="117"/>
-      <c r="B25" s="169"/>
-      <c r="C25" s="169"/>
-      <c r="D25" s="169"/>
-      <c r="E25" s="169"/>
-      <c r="F25" s="169"/>
-      <c r="G25" s="169"/>
+      <c r="B25" s="161"/>
+      <c r="C25" s="161"/>
+      <c r="D25" s="161"/>
+      <c r="E25" s="161"/>
+      <c r="F25" s="161"/>
+      <c r="G25" s="161"/>
       <c r="H25" s="112"/>
       <c r="I25" s="112"/>
       <c r="J25" s="112"/>
@@ -6005,12 +6023,12 @@
     </row>
     <row r="26" spans="1:25">
       <c r="A26" s="118"/>
-      <c r="B26" s="170"/>
-      <c r="C26" s="170"/>
-      <c r="D26" s="170"/>
-      <c r="E26" s="170"/>
-      <c r="F26" s="170"/>
-      <c r="G26" s="170"/>
+      <c r="B26" s="163"/>
+      <c r="C26" s="163"/>
+      <c r="D26" s="163"/>
+      <c r="E26" s="163"/>
+      <c r="F26" s="163"/>
+      <c r="G26" s="163"/>
       <c r="H26" s="112"/>
       <c r="I26" s="112"/>
       <c r="J26" s="112"/>
@@ -6033,15 +6051,15 @@
       <c r="O27" s="105"/>
     </row>
     <row r="28" spans="1:25">
-      <c r="A28" s="157" t="s">
+      <c r="A28" s="176" t="s">
         <v>193</v>
       </c>
-      <c r="B28" s="158"/>
-      <c r="C28" s="158"/>
-      <c r="D28" s="158"/>
-      <c r="E28" s="158"/>
-      <c r="F28" s="158"/>
-      <c r="G28" s="159"/>
+      <c r="B28" s="177"/>
+      <c r="C28" s="177"/>
+      <c r="D28" s="177"/>
+      <c r="E28" s="177"/>
+      <c r="F28" s="177"/>
+      <c r="G28" s="178"/>
       <c r="K28" s="105"/>
       <c r="L28" s="105"/>
       <c r="M28" s="105"/>
@@ -6051,14 +6069,14 @@
       <c r="A29" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="174" t="s">
+      <c r="B29" s="155" t="s">
         <v>184</v>
       </c>
-      <c r="C29" s="174"/>
-      <c r="D29" s="174"/>
-      <c r="E29" s="174"/>
-      <c r="F29" s="174"/>
-      <c r="G29" s="174"/>
+      <c r="C29" s="155"/>
+      <c r="D29" s="155"/>
+      <c r="E29" s="155"/>
+      <c r="F29" s="155"/>
+      <c r="G29" s="155"/>
       <c r="H29" s="105"/>
       <c r="I29" s="105"/>
       <c r="J29" s="105"/>
@@ -6081,14 +6099,14 @@
       <c r="A30" s="116">
         <v>1</v>
       </c>
-      <c r="B30" s="175" t="s">
+      <c r="B30" s="156" t="s">
         <v>225</v>
       </c>
-      <c r="C30" s="175"/>
-      <c r="D30" s="175"/>
-      <c r="E30" s="175"/>
-      <c r="F30" s="175"/>
-      <c r="G30" s="175"/>
+      <c r="C30" s="156"/>
+      <c r="D30" s="156"/>
+      <c r="E30" s="156"/>
+      <c r="F30" s="156"/>
+      <c r="G30" s="156"/>
       <c r="H30" s="112"/>
       <c r="I30" s="112"/>
       <c r="J30" s="112"/>
@@ -6109,12 +6127,12 @@
     </row>
     <row r="31" spans="1:25">
       <c r="A31" s="117"/>
-      <c r="B31" s="176"/>
-      <c r="C31" s="176"/>
-      <c r="D31" s="176"/>
-      <c r="E31" s="176"/>
-      <c r="F31" s="176"/>
-      <c r="G31" s="176"/>
+      <c r="B31" s="157"/>
+      <c r="C31" s="157"/>
+      <c r="D31" s="157"/>
+      <c r="E31" s="157"/>
+      <c r="F31" s="157"/>
+      <c r="G31" s="157"/>
       <c r="H31" s="112"/>
       <c r="I31" s="112"/>
       <c r="J31" s="112"/>
@@ -6131,12 +6149,12 @@
     </row>
     <row r="32" spans="1:25">
       <c r="A32" s="118"/>
-      <c r="B32" s="177"/>
-      <c r="C32" s="177"/>
-      <c r="D32" s="177"/>
-      <c r="E32" s="177"/>
-      <c r="F32" s="177"/>
-      <c r="G32" s="177"/>
+      <c r="B32" s="158"/>
+      <c r="C32" s="158"/>
+      <c r="D32" s="158"/>
+      <c r="E32" s="158"/>
+      <c r="F32" s="158"/>
+      <c r="G32" s="158"/>
       <c r="H32" s="112"/>
       <c r="I32" s="112"/>
       <c r="J32" s="112"/>
@@ -6181,15 +6199,15 @@
       <c r="W33"/>
     </row>
     <row r="34" spans="1:29">
-      <c r="A34" s="157" t="s">
+      <c r="A34" s="176" t="s">
         <v>194</v>
       </c>
-      <c r="B34" s="158"/>
-      <c r="C34" s="158"/>
-      <c r="D34" s="158"/>
-      <c r="E34" s="158"/>
-      <c r="F34" s="158"/>
-      <c r="G34" s="159"/>
+      <c r="B34" s="177"/>
+      <c r="C34" s="177"/>
+      <c r="D34" s="177"/>
+      <c r="E34" s="177"/>
+      <c r="F34" s="177"/>
+      <c r="G34" s="178"/>
       <c r="K34" s="112"/>
       <c r="L34" s="112"/>
       <c r="M34" s="112"/>
@@ -6199,14 +6217,14 @@
       <c r="A35" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B35" s="174" t="s">
+      <c r="B35" s="155" t="s">
         <v>186</v>
       </c>
-      <c r="C35" s="174"/>
-      <c r="D35" s="174"/>
-      <c r="E35" s="174"/>
-      <c r="F35" s="174"/>
-      <c r="G35" s="174"/>
+      <c r="C35" s="155"/>
+      <c r="D35" s="155"/>
+      <c r="E35" s="155"/>
+      <c r="F35" s="155"/>
+      <c r="G35" s="155"/>
       <c r="H35" s="105"/>
       <c r="I35" s="105"/>
       <c r="J35" s="105"/>
@@ -6227,12 +6245,12 @@
     </row>
     <row r="36" spans="1:29">
       <c r="A36" s="116"/>
-      <c r="B36" s="168"/>
-      <c r="C36" s="168"/>
-      <c r="D36" s="168"/>
-      <c r="E36" s="168"/>
-      <c r="F36" s="168"/>
-      <c r="G36" s="178"/>
+      <c r="B36" s="159"/>
+      <c r="C36" s="159"/>
+      <c r="D36" s="159"/>
+      <c r="E36" s="159"/>
+      <c r="F36" s="159"/>
+      <c r="G36" s="160"/>
       <c r="H36" s="112"/>
       <c r="I36" s="112"/>
       <c r="J36" s="112"/>
@@ -6253,12 +6271,12 @@
     </row>
     <row r="37" spans="1:29">
       <c r="A37" s="117"/>
-      <c r="B37" s="169"/>
-      <c r="C37" s="169"/>
-      <c r="D37" s="169"/>
-      <c r="E37" s="169"/>
-      <c r="F37" s="169"/>
-      <c r="G37" s="179"/>
+      <c r="B37" s="161"/>
+      <c r="C37" s="161"/>
+      <c r="D37" s="161"/>
+      <c r="E37" s="161"/>
+      <c r="F37" s="161"/>
+      <c r="G37" s="162"/>
       <c r="H37" s="112"/>
       <c r="I37" s="112"/>
       <c r="J37" s="112"/>
@@ -6275,12 +6293,12 @@
     </row>
     <row r="38" spans="1:29">
       <c r="A38" s="118"/>
-      <c r="B38" s="170"/>
-      <c r="C38" s="170"/>
-      <c r="D38" s="170"/>
-      <c r="E38" s="170"/>
-      <c r="F38" s="170"/>
-      <c r="G38" s="180"/>
+      <c r="B38" s="163"/>
+      <c r="C38" s="163"/>
+      <c r="D38" s="163"/>
+      <c r="E38" s="163"/>
+      <c r="F38" s="163"/>
+      <c r="G38" s="164"/>
       <c r="H38" s="112"/>
       <c r="I38" s="112"/>
       <c r="J38" s="112"/>
@@ -6359,16 +6377,16 @@
       <c r="B42" s="188" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="193" t="s">
+      <c r="C42" s="190" t="s">
         <v>1</v>
       </c>
       <c r="D42" s="188" t="s">
         <v>2</v>
       </c>
-      <c r="E42" s="194" t="s">
+      <c r="E42" s="191" t="s">
         <v>161</v>
       </c>
-      <c r="F42" s="194" t="s">
+      <c r="F42" s="191" t="s">
         <v>177</v>
       </c>
       <c r="G42" s="188" t="s">
@@ -6383,19 +6401,19 @@
       <c r="J42" s="188" t="s">
         <v>209</v>
       </c>
-      <c r="K42" s="197" t="s">
+      <c r="K42" s="195" t="s">
         <v>200</v>
       </c>
-      <c r="L42" s="197" t="s">
+      <c r="L42" s="195" t="s">
         <v>201</v>
       </c>
-      <c r="M42" s="197" t="s">
+      <c r="M42" s="195" t="s">
         <v>202</v>
       </c>
       <c r="N42" s="188" t="s">
         <v>235</v>
       </c>
-      <c r="O42" s="186" t="s">
+      <c r="O42" s="198" t="s">
         <v>203</v>
       </c>
       <c r="P42" s="188" t="s">
@@ -6404,17 +6422,17 @@
       <c r="Q42" s="188" t="s">
         <v>237</v>
       </c>
-      <c r="R42" s="193" t="s">
+      <c r="R42" s="190" t="s">
         <v>208</v>
       </c>
-      <c r="S42" s="190" t="s">
+      <c r="S42" s="196" t="s">
         <v>71</v>
       </c>
-      <c r="T42" s="191"/>
-      <c r="U42" s="190" t="s">
+      <c r="T42" s="197"/>
+      <c r="U42" s="196" t="s">
         <v>17</v>
       </c>
-      <c r="V42" s="191"/>
+      <c r="V42" s="197"/>
       <c r="W42" s="34" t="s">
         <v>70</v>
       </c>
@@ -6423,24 +6441,24 @@
       </c>
     </row>
     <row r="43" spans="1:29">
-      <c r="A43" s="192"/>
-      <c r="B43" s="192"/>
-      <c r="C43" s="192"/>
-      <c r="D43" s="192"/>
-      <c r="E43" s="195"/>
-      <c r="F43" s="196"/>
-      <c r="G43" s="192"/>
-      <c r="H43" s="192"/>
-      <c r="I43" s="189"/>
-      <c r="J43" s="189"/>
-      <c r="K43" s="197"/>
-      <c r="L43" s="197"/>
-      <c r="M43" s="197"/>
-      <c r="N43" s="189"/>
-      <c r="O43" s="187"/>
-      <c r="P43" s="189"/>
-      <c r="Q43" s="189"/>
-      <c r="R43" s="189"/>
+      <c r="A43" s="189"/>
+      <c r="B43" s="189"/>
+      <c r="C43" s="189"/>
+      <c r="D43" s="189"/>
+      <c r="E43" s="192"/>
+      <c r="F43" s="193"/>
+      <c r="G43" s="189"/>
+      <c r="H43" s="189"/>
+      <c r="I43" s="194"/>
+      <c r="J43" s="194"/>
+      <c r="K43" s="195"/>
+      <c r="L43" s="195"/>
+      <c r="M43" s="195"/>
+      <c r="N43" s="194"/>
+      <c r="O43" s="199"/>
+      <c r="P43" s="194"/>
+      <c r="Q43" s="194"/>
+      <c r="R43" s="194"/>
       <c r="S43" s="29" t="s">
         <v>75</v>
       </c>
@@ -6456,7 +6474,7 @@
       <c r="W43" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="X43" s="192"/>
+      <c r="X43" s="189"/>
     </row>
     <row r="44" spans="1:29" ht="30">
       <c r="A44" s="7">
@@ -7208,6 +7226,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="O42:O43"/>
+    <mergeCell ref="I42:I43"/>
+    <mergeCell ref="J42:J43"/>
+    <mergeCell ref="N42:N43"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="S42:T42"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="A28:G28"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B36:G36"/>
     <mergeCell ref="X42:X43"/>
     <mergeCell ref="A42:A43"/>
     <mergeCell ref="B42:B43"/>
@@ -7224,30 +7266,6 @@
     <mergeCell ref="P42:P43"/>
     <mergeCell ref="U42:V42"/>
     <mergeCell ref="Q42:Q43"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="S42:T42"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="A34:G34"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="A22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="A28:G28"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B36:G36"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="O42:O43"/>
-    <mergeCell ref="I42:I43"/>
-    <mergeCell ref="J42:J43"/>
-    <mergeCell ref="N42:N43"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="4">
@@ -7483,10 +7501,10 @@
         <v>174</v>
       </c>
       <c r="B12" s="122"/>
-      <c r="C12" s="165" t="s">
+      <c r="C12" s="143" t="s">
         <v>175</v>
       </c>
-      <c r="D12" s="165"/>
+      <c r="D12" s="143"/>
       <c r="E12" s="95" t="s">
         <v>176</v>
       </c>
@@ -7501,10 +7519,10 @@
         <v>226</v>
       </c>
       <c r="B13" s="122"/>
-      <c r="C13" s="164" t="s">
+      <c r="C13" s="144" t="s">
         <v>230</v>
       </c>
-      <c r="D13" s="165"/>
+      <c r="D13" s="143"/>
       <c r="E13" s="55" t="s">
         <v>227</v>
       </c>
@@ -7524,10 +7542,10 @@
         <v>177</v>
       </c>
       <c r="B14" s="122"/>
-      <c r="C14" s="165" t="s">
+      <c r="C14" s="143" t="s">
         <v>178</v>
       </c>
-      <c r="D14" s="165"/>
+      <c r="D14" s="143"/>
       <c r="E14" s="55"/>
       <c r="F14" s="55"/>
       <c r="G14" s="54"/>
@@ -7539,8 +7557,8 @@
         <v>228</v>
       </c>
       <c r="B15" s="122"/>
-      <c r="C15" s="164"/>
-      <c r="D15" s="165"/>
+      <c r="C15" s="144"/>
+      <c r="D15" s="143"/>
       <c r="E15" s="55" t="s">
         <v>229</v>
       </c>
@@ -7588,15 +7606,15 @@
       <c r="L17"/>
     </row>
     <row r="18" spans="1:22">
-      <c r="A18" s="160" t="s">
+      <c r="A18" s="179" t="s">
         <v>192</v>
       </c>
-      <c r="B18" s="160"/>
-      <c r="C18" s="160"/>
-      <c r="D18" s="160"/>
-      <c r="E18" s="160"/>
-      <c r="F18" s="160"/>
-      <c r="G18" s="160"/>
+      <c r="B18" s="179"/>
+      <c r="C18" s="179"/>
+      <c r="D18" s="179"/>
+      <c r="E18" s="179"/>
+      <c r="F18" s="179"/>
+      <c r="G18" s="179"/>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
@@ -7607,14 +7625,14 @@
       <c r="A19" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="154" t="s">
+      <c r="B19" s="173" t="s">
         <v>183</v>
       </c>
-      <c r="C19" s="155"/>
-      <c r="D19" s="155"/>
-      <c r="E19" s="155"/>
-      <c r="F19" s="155"/>
-      <c r="G19" s="156"/>
+      <c r="C19" s="174"/>
+      <c r="D19" s="174"/>
+      <c r="E19" s="174"/>
+      <c r="F19" s="174"/>
+      <c r="G19" s="175"/>
       <c r="H19" s="105"/>
       <c r="I19"/>
       <c r="J19"/>
@@ -7630,12 +7648,12 @@
     </row>
     <row r="20" spans="1:22">
       <c r="A20" s="116"/>
-      <c r="B20" s="168"/>
-      <c r="C20" s="168"/>
-      <c r="D20" s="168"/>
-      <c r="E20" s="168"/>
-      <c r="F20" s="168"/>
-      <c r="G20" s="168"/>
+      <c r="B20" s="159"/>
+      <c r="C20" s="159"/>
+      <c r="D20" s="159"/>
+      <c r="E20" s="159"/>
+      <c r="F20" s="159"/>
+      <c r="G20" s="159"/>
       <c r="H20" s="112"/>
       <c r="I20"/>
       <c r="J20"/>
@@ -7650,12 +7668,12 @@
     </row>
     <row r="21" spans="1:22">
       <c r="A21" s="117"/>
-      <c r="B21" s="169"/>
-      <c r="C21" s="169"/>
-      <c r="D21" s="169"/>
-      <c r="E21" s="169"/>
-      <c r="F21" s="169"/>
-      <c r="G21" s="169"/>
+      <c r="B21" s="161"/>
+      <c r="C21" s="161"/>
+      <c r="D21" s="161"/>
+      <c r="E21" s="161"/>
+      <c r="F21" s="161"/>
+      <c r="G21" s="161"/>
       <c r="H21" s="112"/>
       <c r="I21"/>
       <c r="J21"/>
@@ -7670,12 +7688,12 @@
     </row>
     <row r="22" spans="1:22">
       <c r="A22" s="118"/>
-      <c r="B22" s="170"/>
-      <c r="C22" s="170"/>
-      <c r="D22" s="170"/>
-      <c r="E22" s="170"/>
-      <c r="F22" s="170"/>
-      <c r="G22" s="170"/>
+      <c r="B22" s="163"/>
+      <c r="C22" s="163"/>
+      <c r="D22" s="163"/>
+      <c r="E22" s="163"/>
+      <c r="F22" s="163"/>
+      <c r="G22" s="163"/>
       <c r="H22" s="112"/>
       <c r="I22"/>
       <c r="J22"/>
@@ -7702,15 +7720,15 @@
       <c r="O23" s="112"/>
     </row>
     <row r="24" spans="1:22">
-      <c r="A24" s="157" t="s">
+      <c r="A24" s="176" t="s">
         <v>193</v>
       </c>
-      <c r="B24" s="158"/>
-      <c r="C24" s="158"/>
-      <c r="D24" s="158"/>
-      <c r="E24" s="158"/>
-      <c r="F24" s="158"/>
-      <c r="G24" s="159"/>
+      <c r="B24" s="177"/>
+      <c r="C24" s="177"/>
+      <c r="D24" s="177"/>
+      <c r="E24" s="177"/>
+      <c r="F24" s="177"/>
+      <c r="G24" s="178"/>
       <c r="I24"/>
       <c r="J24"/>
       <c r="K24"/>
@@ -7723,14 +7741,14 @@
       <c r="A25" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B25" s="174" t="s">
+      <c r="B25" s="155" t="s">
         <v>184</v>
       </c>
-      <c r="C25" s="174"/>
-      <c r="D25" s="174"/>
-      <c r="E25" s="174"/>
-      <c r="F25" s="174"/>
-      <c r="G25" s="174"/>
+      <c r="C25" s="155"/>
+      <c r="D25" s="155"/>
+      <c r="E25" s="155"/>
+      <c r="F25" s="155"/>
+      <c r="G25" s="155"/>
       <c r="H25" s="105"/>
       <c r="M25" s="112"/>
       <c r="N25" s="112"/>
@@ -7746,14 +7764,14 @@
       <c r="A26" s="116">
         <v>1</v>
       </c>
-      <c r="B26" s="175" t="s">
+      <c r="B26" s="156" t="s">
         <v>185</v>
       </c>
-      <c r="C26" s="175"/>
-      <c r="D26" s="175"/>
-      <c r="E26" s="175"/>
-      <c r="F26" s="175"/>
-      <c r="G26" s="175"/>
+      <c r="C26" s="156"/>
+      <c r="D26" s="156"/>
+      <c r="E26" s="156"/>
+      <c r="F26" s="156"/>
+      <c r="G26" s="156"/>
       <c r="H26" s="112"/>
       <c r="I26" s="105"/>
       <c r="J26" s="105"/>
@@ -7768,12 +7786,12 @@
     </row>
     <row r="27" spans="1:22">
       <c r="A27" s="117"/>
-      <c r="B27" s="176"/>
-      <c r="C27" s="176"/>
-      <c r="D27" s="176"/>
-      <c r="E27" s="176"/>
-      <c r="F27" s="176"/>
-      <c r="G27" s="176"/>
+      <c r="B27" s="157"/>
+      <c r="C27" s="157"/>
+      <c r="D27" s="157"/>
+      <c r="E27" s="157"/>
+      <c r="F27" s="157"/>
+      <c r="G27" s="157"/>
       <c r="H27" s="112"/>
       <c r="I27" s="105"/>
       <c r="J27" s="105"/>
@@ -7788,12 +7806,12 @@
     </row>
     <row r="28" spans="1:22">
       <c r="A28" s="118"/>
-      <c r="B28" s="177"/>
-      <c r="C28" s="177"/>
-      <c r="D28" s="177"/>
-      <c r="E28" s="177"/>
-      <c r="F28" s="177"/>
-      <c r="G28" s="177"/>
+      <c r="B28" s="158"/>
+      <c r="C28" s="158"/>
+      <c r="D28" s="158"/>
+      <c r="E28" s="158"/>
+      <c r="F28" s="158"/>
+      <c r="G28" s="158"/>
       <c r="H28" s="112"/>
       <c r="I28" s="105"/>
       <c r="J28" s="105"/>
@@ -7832,15 +7850,15 @@
       <c r="T29"/>
     </row>
     <row r="30" spans="1:22">
-      <c r="A30" s="157" t="s">
+      <c r="A30" s="176" t="s">
         <v>194</v>
       </c>
-      <c r="B30" s="158"/>
-      <c r="C30" s="158"/>
-      <c r="D30" s="158"/>
-      <c r="E30" s="158"/>
-      <c r="F30" s="158"/>
-      <c r="G30" s="159"/>
+      <c r="B30" s="177"/>
+      <c r="C30" s="177"/>
+      <c r="D30" s="177"/>
+      <c r="E30" s="177"/>
+      <c r="F30" s="177"/>
+      <c r="G30" s="178"/>
       <c r="M30" s="112"/>
       <c r="N30" s="112"/>
       <c r="O30" s="112"/>
@@ -7849,14 +7867,14 @@
       <c r="A31" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B31" s="174" t="s">
+      <c r="B31" s="155" t="s">
         <v>186</v>
       </c>
-      <c r="C31" s="174"/>
-      <c r="D31" s="174"/>
-      <c r="E31" s="174"/>
-      <c r="F31" s="174"/>
-      <c r="G31" s="174"/>
+      <c r="C31" s="155"/>
+      <c r="D31" s="155"/>
+      <c r="E31" s="155"/>
+      <c r="F31" s="155"/>
+      <c r="G31" s="155"/>
       <c r="H31" s="105"/>
       <c r="I31" s="105"/>
       <c r="J31" s="105"/>
@@ -7874,12 +7892,12 @@
     </row>
     <row r="32" spans="1:22">
       <c r="A32" s="116"/>
-      <c r="B32" s="168"/>
-      <c r="C32" s="168"/>
-      <c r="D32" s="168"/>
-      <c r="E32" s="168"/>
-      <c r="F32" s="168"/>
-      <c r="G32" s="178"/>
+      <c r="B32" s="159"/>
+      <c r="C32" s="159"/>
+      <c r="D32" s="159"/>
+      <c r="E32" s="159"/>
+      <c r="F32" s="159"/>
+      <c r="G32" s="160"/>
       <c r="H32" s="112"/>
       <c r="I32" s="112"/>
       <c r="J32" s="112"/>
@@ -7897,12 +7915,12 @@
     </row>
     <row r="33" spans="1:22">
       <c r="A33" s="117"/>
-      <c r="B33" s="169"/>
-      <c r="C33" s="169"/>
-      <c r="D33" s="169"/>
-      <c r="E33" s="169"/>
-      <c r="F33" s="169"/>
-      <c r="G33" s="179"/>
+      <c r="B33" s="161"/>
+      <c r="C33" s="161"/>
+      <c r="D33" s="161"/>
+      <c r="E33" s="161"/>
+      <c r="F33" s="161"/>
+      <c r="G33" s="162"/>
       <c r="H33" s="112"/>
       <c r="I33" s="112"/>
       <c r="J33" s="112"/>
@@ -7917,12 +7935,12 @@
     </row>
     <row r="34" spans="1:22">
       <c r="A34" s="118"/>
-      <c r="B34" s="170"/>
-      <c r="C34" s="170"/>
-      <c r="D34" s="170"/>
-      <c r="E34" s="170"/>
-      <c r="F34" s="170"/>
-      <c r="G34" s="180"/>
+      <c r="B34" s="163"/>
+      <c r="C34" s="163"/>
+      <c r="D34" s="163"/>
+      <c r="E34" s="163"/>
+      <c r="F34" s="163"/>
+      <c r="G34" s="164"/>
       <c r="H34" s="112"/>
       <c r="I34" s="112"/>
       <c r="J34" s="112"/>
@@ -7992,40 +8010,40 @@
       <c r="U37" s="58"/>
     </row>
     <row r="38" spans="1:22" ht="30" customHeight="1">
-      <c r="A38" s="194" t="s">
+      <c r="A38" s="191" t="s">
         <v>118</v>
       </c>
-      <c r="B38" s="194" t="s">
+      <c r="B38" s="191" t="s">
         <v>119</v>
       </c>
       <c r="C38" s="60" t="s">
         <v>120</v>
       </c>
-      <c r="D38" s="194" t="s">
+      <c r="D38" s="191" t="s">
         <v>101</v>
       </c>
-      <c r="E38" s="194" t="s">
+      <c r="E38" s="191" t="s">
         <v>161</v>
       </c>
-      <c r="F38" s="194" t="s">
+      <c r="F38" s="191" t="s">
         <v>177</v>
       </c>
-      <c r="G38" s="194" t="s">
+      <c r="G38" s="191" t="s">
         <v>140</v>
       </c>
-      <c r="H38" s="194" t="s">
+      <c r="H38" s="191" t="s">
         <v>139</v>
       </c>
-      <c r="I38" s="201" t="s">
+      <c r="I38" s="203" t="s">
         <v>200</v>
       </c>
-      <c r="J38" s="203" t="s">
+      <c r="J38" s="205" t="s">
         <v>201</v>
       </c>
-      <c r="K38" s="203" t="s">
+      <c r="K38" s="205" t="s">
         <v>202</v>
       </c>
-      <c r="L38" s="186" t="s">
+      <c r="L38" s="198" t="s">
         <v>203</v>
       </c>
       <c r="M38" s="188" t="s">
@@ -8034,42 +8052,42 @@
       <c r="N38" s="188" t="s">
         <v>209</v>
       </c>
-      <c r="O38" s="193" t="s">
+      <c r="O38" s="190" t="s">
         <v>208</v>
       </c>
-      <c r="P38" s="199" t="s">
+      <c r="P38" s="201" t="s">
         <v>122</v>
       </c>
-      <c r="Q38" s="200"/>
-      <c r="R38" s="205" t="s">
+      <c r="Q38" s="202"/>
+      <c r="R38" s="207" t="s">
         <v>123</v>
       </c>
-      <c r="S38" s="200"/>
+      <c r="S38" s="202"/>
       <c r="T38" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="U38" s="194" t="s">
+      <c r="U38" s="191" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="39" spans="1:22" ht="15">
-      <c r="A39" s="198"/>
-      <c r="B39" s="198"/>
+      <c r="A39" s="200"/>
+      <c r="B39" s="200"/>
       <c r="C39" s="61" t="s">
         <v>121</v>
       </c>
-      <c r="D39" s="198"/>
-      <c r="E39" s="196"/>
-      <c r="F39" s="196"/>
-      <c r="G39" s="198"/>
-      <c r="H39" s="198"/>
-      <c r="I39" s="202"/>
-      <c r="J39" s="204"/>
-      <c r="K39" s="204"/>
-      <c r="L39" s="187"/>
-      <c r="M39" s="189"/>
-      <c r="N39" s="189"/>
-      <c r="O39" s="206"/>
+      <c r="D39" s="200"/>
+      <c r="E39" s="193"/>
+      <c r="F39" s="193"/>
+      <c r="G39" s="200"/>
+      <c r="H39" s="200"/>
+      <c r="I39" s="204"/>
+      <c r="J39" s="206"/>
+      <c r="K39" s="206"/>
+      <c r="L39" s="199"/>
+      <c r="M39" s="194"/>
+      <c r="N39" s="194"/>
+      <c r="O39" s="208"/>
       <c r="P39" s="62" t="s">
         <v>126</v>
       </c>
@@ -8085,7 +8103,7 @@
       <c r="T39" s="63" t="s">
         <v>130</v>
       </c>
-      <c r="U39" s="198"/>
+      <c r="U39" s="200"/>
     </row>
     <row r="40" spans="1:22">
       <c r="A40" s="64">
@@ -8745,26 +8763,6 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="M38:M39"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="A30:G30"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="A24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="A18:G18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C15:D15"/>
     <mergeCell ref="U38:U39"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="B38:B39"/>
@@ -8781,6 +8779,26 @@
     <mergeCell ref="R38:S38"/>
     <mergeCell ref="L38:L39"/>
     <mergeCell ref="O38:O39"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A18:G18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="A24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="M38:M39"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="A30:G30"/>
+    <mergeCell ref="B31:G31"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="3">

</xml_diff>

<commit_message>
0.1.8: Adapt override qualifier.
</commit_message>
<xml_diff>
--- a/meta/api/BlancoApiPostSample.xlsx
+++ b/meta/api/BlancoApiPostSample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorKt/meta/api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E114557-C06D-5E45-AEAB-FBFE191C587D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A41E978-512A-FA49-AC60-B1EDC1F1F64A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15160" yWindow="1200" windowWidth="21420" windowHeight="17540" tabRatio="860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="250">
   <si>
     <t>項目名</t>
     <rPh sb="0" eb="3">
@@ -2543,6 +2543,10 @@
     <rPh sb="9" eb="11">
       <t xml:space="preserve">ジッソウ </t>
     </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>オーバーライド</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -5526,8 +5530,8 @@
   </sheetPr>
   <dimension ref="A1:AC67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="O37" workbookViewId="0">
+      <selection activeCell="Z46" sqref="Z46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -5552,8 +5556,8 @@
     <col min="21" max="21" width="6.6640625" style="1" customWidth="1"/>
     <col min="22" max="22" width="6.83203125" style="1" customWidth="1"/>
     <col min="23" max="23" width="9" style="1" customWidth="1"/>
-    <col min="24" max="24" width="16.6640625" style="1" customWidth="1"/>
-    <col min="25" max="25" width="6.83203125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="23.33203125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="19.1640625" style="1" customWidth="1"/>
     <col min="26" max="26" width="18.6640625" style="1" customWidth="1"/>
     <col min="27" max="27" width="43.5" style="1" customWidth="1"/>
     <col min="28" max="28" width="11.33203125" style="1" customWidth="1"/>
@@ -6364,7 +6368,7 @@
       <c r="V41" s="37"/>
       <c r="W41" s="37"/>
       <c r="X41" s="38"/>
-      <c r="Y41" s="55"/>
+      <c r="Y41" s="37"/>
       <c r="Z41" s="55"/>
       <c r="AA41" s="55"/>
       <c r="AB41" s="39"/>
@@ -6438,6 +6442,9 @@
       </c>
       <c r="X42" s="188" t="s">
         <v>8</v>
+      </c>
+      <c r="Y42" s="188" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="43" spans="1:29">
@@ -6475,6 +6482,7 @@
         <v>14</v>
       </c>
       <c r="X43" s="189"/>
+      <c r="Y43" s="194"/>
     </row>
     <row r="44" spans="1:29" ht="30">
       <c r="A44" s="7">
@@ -6531,6 +6539,7 @@
       <c r="V44" s="30"/>
       <c r="W44" s="30"/>
       <c r="X44" s="9"/>
+      <c r="Y44" s="24"/>
     </row>
     <row r="45" spans="1:29">
       <c r="A45" s="10">
@@ -6582,6 +6591,7 @@
       </c>
       <c r="W45" s="31"/>
       <c r="X45" s="12"/>
+      <c r="Y45" s="25"/>
     </row>
     <row r="46" spans="1:29">
       <c r="A46" s="10">
@@ -6631,6 +6641,7 @@
       <c r="V46" s="31"/>
       <c r="W46" s="31"/>
       <c r="X46" s="14"/>
+      <c r="Y46" s="25"/>
     </row>
     <row r="47" spans="1:29">
       <c r="A47" s="10">
@@ -6672,6 +6683,7 @@
       <c r="V47" s="31"/>
       <c r="W47" s="31"/>
       <c r="X47" s="14"/>
+      <c r="Y47" s="25"/>
     </row>
     <row r="48" spans="1:29">
       <c r="A48" s="10">
@@ -6711,8 +6723,9 @@
       <c r="X48" s="14" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="49" spans="1:24">
+      <c r="Y48" s="25"/>
+    </row>
+    <row r="49" spans="1:25">
       <c r="A49" s="10">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -6746,8 +6759,11 @@
       <c r="V49" s="31"/>
       <c r="W49" s="31"/>
       <c r="X49" s="14"/>
-    </row>
-    <row r="50" spans="1:24">
+      <c r="Y49" s="25" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="50" spans="1:25">
       <c r="A50" s="10">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -6781,8 +6797,9 @@
       <c r="V50" s="31"/>
       <c r="W50" s="31"/>
       <c r="X50" s="14"/>
-    </row>
-    <row r="51" spans="1:24">
+      <c r="Y50" s="25"/>
+    </row>
+    <row r="51" spans="1:25">
       <c r="A51" s="10"/>
       <c r="B51" s="22"/>
       <c r="C51" s="13"/>
@@ -6807,8 +6824,9 @@
       <c r="V51" s="31"/>
       <c r="W51" s="31"/>
       <c r="X51" s="14"/>
-    </row>
-    <row r="52" spans="1:24">
+      <c r="Y51" s="25"/>
+    </row>
+    <row r="52" spans="1:25">
       <c r="A52" s="10"/>
       <c r="B52" s="22"/>
       <c r="C52" s="13"/>
@@ -6833,8 +6851,9 @@
       <c r="V52" s="32"/>
       <c r="W52" s="32"/>
       <c r="X52" s="14"/>
-    </row>
-    <row r="53" spans="1:24">
+      <c r="Y52" s="25"/>
+    </row>
+    <row r="53" spans="1:25">
       <c r="A53" s="10"/>
       <c r="B53" s="22"/>
       <c r="C53" s="13"/>
@@ -6859,8 +6878,9 @@
       <c r="V53" s="31"/>
       <c r="W53" s="31"/>
       <c r="X53" s="14"/>
-    </row>
-    <row r="54" spans="1:24">
+      <c r="Y53" s="25"/>
+    </row>
+    <row r="54" spans="1:25">
       <c r="A54" s="10"/>
       <c r="B54" s="22"/>
       <c r="C54" s="13"/>
@@ -6885,8 +6905,9 @@
       <c r="V54" s="31"/>
       <c r="W54" s="31"/>
       <c r="X54" s="14"/>
-    </row>
-    <row r="55" spans="1:24">
+      <c r="Y54" s="25"/>
+    </row>
+    <row r="55" spans="1:25">
       <c r="A55" s="10"/>
       <c r="B55" s="22"/>
       <c r="C55" s="13"/>
@@ -6911,8 +6932,9 @@
       <c r="V55" s="31"/>
       <c r="W55" s="31"/>
       <c r="X55" s="14"/>
-    </row>
-    <row r="56" spans="1:24">
+      <c r="Y55" s="25"/>
+    </row>
+    <row r="56" spans="1:25">
       <c r="A56" s="10"/>
       <c r="B56" s="22"/>
       <c r="C56" s="13"/>
@@ -6937,8 +6959,9 @@
       <c r="V56" s="31"/>
       <c r="W56" s="31"/>
       <c r="X56" s="14"/>
-    </row>
-    <row r="57" spans="1:24">
+      <c r="Y56" s="25"/>
+    </row>
+    <row r="57" spans="1:25">
       <c r="A57" s="10"/>
       <c r="B57" s="22"/>
       <c r="C57" s="13"/>
@@ -6963,8 +6986,9 @@
       <c r="V57" s="31"/>
       <c r="W57" s="31"/>
       <c r="X57" s="14"/>
-    </row>
-    <row r="58" spans="1:24">
+      <c r="Y57" s="25"/>
+    </row>
+    <row r="58" spans="1:25">
       <c r="A58" s="10"/>
       <c r="B58" s="22"/>
       <c r="C58" s="13"/>
@@ -6989,8 +7013,9 @@
       <c r="V58" s="32"/>
       <c r="W58" s="32"/>
       <c r="X58" s="14"/>
-    </row>
-    <row r="59" spans="1:24">
+      <c r="Y58" s="25"/>
+    </row>
+    <row r="59" spans="1:25">
       <c r="A59" s="10"/>
       <c r="B59" s="22"/>
       <c r="C59" s="13"/>
@@ -7015,8 +7040,9 @@
       <c r="V59" s="31"/>
       <c r="W59" s="31"/>
       <c r="X59" s="14"/>
-    </row>
-    <row r="60" spans="1:24">
+      <c r="Y59" s="25"/>
+    </row>
+    <row r="60" spans="1:25">
       <c r="A60" s="10"/>
       <c r="B60" s="22"/>
       <c r="C60" s="13"/>
@@ -7041,8 +7067,9 @@
       <c r="V60" s="31"/>
       <c r="W60" s="31"/>
       <c r="X60" s="14"/>
-    </row>
-    <row r="61" spans="1:24">
+      <c r="Y60" s="25"/>
+    </row>
+    <row r="61" spans="1:25">
       <c r="A61" s="10"/>
       <c r="B61" s="22"/>
       <c r="C61" s="13"/>
@@ -7067,8 +7094,9 @@
       <c r="V61" s="31"/>
       <c r="W61" s="31"/>
       <c r="X61" s="14"/>
-    </row>
-    <row r="62" spans="1:24">
+      <c r="Y61" s="25"/>
+    </row>
+    <row r="62" spans="1:25">
       <c r="A62" s="10"/>
       <c r="B62" s="22"/>
       <c r="C62" s="13"/>
@@ -7093,8 +7121,9 @@
       <c r="V62" s="31"/>
       <c r="W62" s="31"/>
       <c r="X62" s="14"/>
-    </row>
-    <row r="63" spans="1:24">
+      <c r="Y62" s="25"/>
+    </row>
+    <row r="63" spans="1:25">
       <c r="A63" s="10"/>
       <c r="B63" s="22"/>
       <c r="C63" s="13"/>
@@ -7119,8 +7148,9 @@
       <c r="V63" s="32"/>
       <c r="W63" s="32"/>
       <c r="X63" s="14"/>
-    </row>
-    <row r="64" spans="1:24">
+      <c r="Y63" s="25"/>
+    </row>
+    <row r="64" spans="1:25">
       <c r="A64" s="10"/>
       <c r="B64" s="22"/>
       <c r="C64" s="13"/>
@@ -7145,8 +7175,9 @@
       <c r="V64" s="31"/>
       <c r="W64" s="31"/>
       <c r="X64" s="14"/>
-    </row>
-    <row r="65" spans="1:24">
+      <c r="Y64" s="25"/>
+    </row>
+    <row r="65" spans="1:25">
       <c r="A65" s="10"/>
       <c r="B65" s="22"/>
       <c r="C65" s="13"/>
@@ -7171,8 +7202,9 @@
       <c r="V65" s="31"/>
       <c r="W65" s="31"/>
       <c r="X65" s="14"/>
-    </row>
-    <row r="66" spans="1:24">
+      <c r="Y65" s="25"/>
+    </row>
+    <row r="66" spans="1:25">
       <c r="A66" s="10"/>
       <c r="B66" s="22"/>
       <c r="C66" s="13"/>
@@ -7197,8 +7229,9 @@
       <c r="V66" s="32"/>
       <c r="W66" s="32"/>
       <c r="X66" s="14"/>
-    </row>
-    <row r="67" spans="1:24">
+      <c r="Y66" s="25"/>
+    </row>
+    <row r="67" spans="1:25">
       <c r="A67" s="15"/>
       <c r="B67" s="23"/>
       <c r="C67" s="16"/>
@@ -7223,9 +7256,11 @@
       <c r="V67" s="33"/>
       <c r="W67" s="33"/>
       <c r="X67" s="17"/>
+      <c r="Y67" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="40">
+  <mergeCells count="41">
+    <mergeCell ref="Y42:Y43"/>
     <mergeCell ref="B37:G37"/>
     <mergeCell ref="B38:G38"/>
     <mergeCell ref="B30:G30"/>
@@ -7278,7 +7313,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I44:J67 R44:R67" xr:uid="{1FBC7B49-ABAE-AE4A-8A55-EF1A4EFC4446}">
       <formula1>isNullable</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N44:N67 P44:Q67" xr:uid="{672B2DF7-D1C1-234C-A02A-4DFC68BF8F4E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N44:N67 P44:Q67 Y44:Y67" xr:uid="{672B2DF7-D1C1-234C-A02A-4DFC68BF8F4E}">
       <formula1>threeAlters</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>